<commit_message>
add supplier wire frame review
</commit_message>
<xml_diff>
--- a/Requirments/Review.xlsx
+++ b/Requirments/Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI9M-Testing\Core\QA\WorkShop\Online-Mobile-Store-WebSite\Requirments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34B9631-4C29-43CE-B7D1-1D9C9D1F5C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE494EC8-A0A7-4796-A13F-D7DAF19710BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="151">
   <si>
     <t>ID</t>
   </si>
@@ -453,6 +453,27 @@
   </si>
   <si>
     <t>eaa5d9a06cc262045c762d13adc3bd2164cc1ae5</t>
+  </si>
+  <si>
+    <t>Review_WF_Supplier_001</t>
+  </si>
+  <si>
+    <t>error message appears in the same place up right the page for any error in any field of data</t>
+  </si>
+  <si>
+    <t>Wireframe_Supplier_007</t>
+  </si>
+  <si>
+    <t>8e7b04160c24349482edf7e87786b6f640d69018</t>
+  </si>
+  <si>
+    <t>Review_WF_Supplier_002</t>
+  </si>
+  <si>
+    <t>Wireframe_Supplier_008                        Wireframe_Supplier_009</t>
+  </si>
+  <si>
+    <t>you shall update or remove the product using its id, shall be a search bar to search with product id then you can update or remove</t>
   </si>
 </sst>
 </file>
@@ -684,7 +705,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -740,21 +761,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -769,13 +779,27 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1001,8 +1025,8 @@
   </sheetPr>
   <dimension ref="A1:AC905"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60:I60"/>
+    <sheetView tabSelected="1" topLeftCell="E54" workbookViewId="0">
+      <selection activeCell="H62" sqref="H62:I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1012,7 +1036,7 @@
     <col min="3" max="3" width="20.6640625" customWidth="1"/>
     <col min="4" max="4" width="25.5546875" customWidth="1"/>
     <col min="5" max="5" width="97.109375" customWidth="1"/>
-    <col min="6" max="6" width="25.88671875" customWidth="1"/>
+    <col min="6" max="6" width="37.33203125" customWidth="1"/>
     <col min="7" max="7" width="18.5546875" customWidth="1"/>
     <col min="8" max="8" width="34.109375" customWidth="1"/>
     <col min="9" max="9" width="25.6640625" customWidth="1"/>
@@ -1041,14 +1065,14 @@
       <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="43"/>
-      <c r="J1" s="42" t="s">
+      <c r="I1" s="36"/>
+      <c r="J1" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="K1" s="43"/>
+      <c r="K1" s="36"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -1069,19 +1093,19 @@
       <c r="AC1" s="1"/>
     </row>
     <row r="2" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -1123,12 +1147,12 @@
       <c r="G3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="37"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="29" t="s">
+      <c r="H3" s="39"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="K3" s="29"/>
+      <c r="K3" s="37"/>
     </row>
     <row r="4" spans="1:29" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
@@ -1152,12 +1176,12 @@
       <c r="G4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="37"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="29" t="s">
+      <c r="H4" s="39"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="K4" s="29"/>
+      <c r="K4" s="37"/>
     </row>
     <row r="5" spans="1:29" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
@@ -1181,12 +1205,12 @@
       <c r="G5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="37"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="29" t="s">
+      <c r="H5" s="39"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="K5" s="29"/>
+      <c r="K5" s="37"/>
     </row>
     <row r="6" spans="1:29" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
@@ -1210,12 +1234,12 @@
       <c r="G6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="37"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="29" t="s">
+      <c r="H6" s="39"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="K6" s="29"/>
+      <c r="K6" s="37"/>
     </row>
     <row r="7" spans="1:29" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
@@ -1239,12 +1263,12 @@
       <c r="G7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="37"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="29" t="s">
+      <c r="H7" s="39"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="K7" s="29"/>
+      <c r="K7" s="37"/>
     </row>
     <row r="8" spans="1:29" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
@@ -1268,12 +1292,12 @@
       <c r="G8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="37"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="29" t="s">
+      <c r="H8" s="39"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="K8" s="29"/>
+      <c r="K8" s="37"/>
     </row>
     <row r="9" spans="1:29" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
@@ -1297,12 +1321,12 @@
       <c r="G9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="37"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="29" t="s">
+      <c r="H9" s="39"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="K9" s="29"/>
+      <c r="K9" s="37"/>
     </row>
     <row r="10" spans="1:29" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
@@ -1326,12 +1350,12 @@
       <c r="G10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="37"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="29" t="s">
+      <c r="H10" s="39"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="K10" s="29"/>
+      <c r="K10" s="37"/>
     </row>
     <row r="11" spans="1:29" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
@@ -1355,12 +1379,12 @@
       <c r="G11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="37"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="29" t="s">
+      <c r="H11" s="39"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="K11" s="29"/>
+      <c r="K11" s="37"/>
     </row>
     <row r="12" spans="1:29" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
@@ -1384,12 +1408,12 @@
       <c r="G12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="37"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="29" t="s">
+      <c r="H12" s="39"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="K12" s="29"/>
+      <c r="K12" s="37"/>
     </row>
     <row r="13" spans="1:29" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
@@ -1413,12 +1437,12 @@
       <c r="G13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="37"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="29" t="s">
+      <c r="H13" s="39"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="K13" s="29"/>
+      <c r="K13" s="37"/>
     </row>
     <row r="14" spans="1:29" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
@@ -1442,12 +1466,12 @@
       <c r="G14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="37"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="29" t="s">
+      <c r="H14" s="39"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="K14" s="29"/>
+      <c r="K14" s="37"/>
     </row>
     <row r="15" spans="1:29" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
@@ -1469,12 +1493,12 @@
       <c r="G15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="37"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="29" t="s">
+      <c r="H15" s="39"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="29"/>
+      <c r="K15" s="37"/>
     </row>
     <row r="16" spans="1:29" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
@@ -1498,12 +1522,12 @@
       <c r="G16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="37"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="29" t="s">
+      <c r="H16" s="39"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="K16" s="29"/>
+      <c r="K16" s="37"/>
     </row>
     <row r="17" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
@@ -1527,12 +1551,12 @@
       <c r="G17" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="37"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="29" t="s">
+      <c r="H17" s="39"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="29"/>
+      <c r="K17" s="37"/>
     </row>
     <row r="18" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
@@ -1556,12 +1580,12 @@
       <c r="G18" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="37"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="29" t="s">
+      <c r="H18" s="39"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="29"/>
+      <c r="K18" s="37"/>
     </row>
     <row r="19" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
@@ -1585,27 +1609,27 @@
       <c r="G19" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="37"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="29" t="s">
+      <c r="H19" s="39"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="K19" s="29"/>
+      <c r="K19" s="37"/>
     </row>
     <row r="20" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="41"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="34"/>
     </row>
     <row r="21" spans="1:11" s="16" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
@@ -1629,14 +1653,14 @@
       <c r="G21" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H21" s="44" t="s">
+      <c r="H21" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="I21" s="36"/>
-      <c r="J21" s="29" t="s">
+      <c r="I21" s="31"/>
+      <c r="J21" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="K21" s="29"/>
+      <c r="K21" s="37"/>
     </row>
     <row r="22" spans="1:11" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="20" t="s">
@@ -1660,12 +1684,12 @@
       <c r="G22" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="35"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="29" t="s">
+      <c r="H22" s="30"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="K22" s="29"/>
+      <c r="K22" s="37"/>
     </row>
     <row r="23" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
@@ -1689,14 +1713,14 @@
       <c r="G23" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="35" t="s">
+      <c r="H23" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="I23" s="36"/>
-      <c r="J23" s="29" t="s">
+      <c r="I23" s="31"/>
+      <c r="J23" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="K23" s="29"/>
+      <c r="K23" s="37"/>
     </row>
     <row r="24" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
@@ -1724,10 +1748,10 @@
         <v>74</v>
       </c>
       <c r="I24" s="25"/>
-      <c r="J24" s="29" t="s">
+      <c r="J24" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="K24" s="29"/>
+      <c r="K24" s="37"/>
     </row>
     <row r="25" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
@@ -1751,14 +1775,14 @@
       <c r="G25" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="35" t="s">
+      <c r="H25" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="I25" s="36"/>
-      <c r="J25" s="29" t="s">
+      <c r="I25" s="31"/>
+      <c r="J25" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="K25" s="29"/>
+      <c r="K25" s="37"/>
     </row>
     <row r="26" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
@@ -1782,27 +1806,27 @@
       <c r="G26" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H26" s="35"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="29" t="s">
+      <c r="H26" s="30"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="K26" s="29"/>
+      <c r="K26" s="37"/>
     </row>
     <row r="27" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="40"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="40"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="41"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="34"/>
     </row>
     <row r="28" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
@@ -1826,12 +1850,12 @@
       <c r="G28" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H28" s="33"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="33" t="s">
+      <c r="H28" s="43"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="K28" s="34"/>
+      <c r="K28" s="44"/>
     </row>
     <row r="29" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="s">
@@ -1855,14 +1879,14 @@
       <c r="G29" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="35" t="s">
+      <c r="H29" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="I29" s="36"/>
-      <c r="J29" s="32" t="s">
+      <c r="I29" s="31"/>
+      <c r="J29" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="K29" s="29"/>
+      <c r="K29" s="37"/>
     </row>
     <row r="30" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
@@ -1886,12 +1910,12 @@
       <c r="G30" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H30" s="35"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="29" t="s">
+      <c r="H30" s="30"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="K30" s="29"/>
+      <c r="K30" s="37"/>
     </row>
     <row r="31" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
@@ -1915,27 +1939,27 @@
       <c r="G31" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H31" s="35"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="29" t="s">
+      <c r="H31" s="30"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="K31" s="29"/>
+      <c r="K31" s="37"/>
     </row>
     <row r="32" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A32" s="45" t="s">
+      <c r="A32" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="40"/>
-      <c r="K32" s="41"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="34"/>
     </row>
     <row r="33" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
@@ -1959,12 +1983,12 @@
       <c r="G33" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H33" s="35"/>
-      <c r="I33" s="36"/>
-      <c r="J33" s="32" t="s">
+      <c r="H33" s="30"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="K33" s="29"/>
+      <c r="K33" s="37"/>
     </row>
     <row r="34" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
@@ -1988,8 +2012,8 @@
       <c r="G34" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H34" s="35"/>
-      <c r="I34" s="36"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="31"/>
       <c r="J34" s="28" t="s">
         <v>94</v>
       </c>
@@ -2016,12 +2040,12 @@
       <c r="G35" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H35" s="35"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="32" t="s">
+      <c r="H35" s="30"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="K35" s="29"/>
+      <c r="K35" s="37"/>
     </row>
     <row r="36" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A36" s="13" t="s">
@@ -2045,12 +2069,12 @@
       <c r="G36" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H36" s="35"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="32" t="s">
+      <c r="H36" s="30"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="K36" s="29"/>
+      <c r="K36" s="37"/>
     </row>
     <row r="37" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -2074,12 +2098,12 @@
       <c r="G37" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H37" s="35"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="32" t="s">
+      <c r="H37" s="30"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="K37" s="29"/>
+      <c r="K37" s="37"/>
     </row>
     <row r="38" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
@@ -2103,12 +2127,12 @@
       <c r="G38" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H38" s="35"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="32" t="s">
+      <c r="H38" s="30"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="K38" s="29"/>
+      <c r="K38" s="37"/>
     </row>
     <row r="39" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
@@ -2132,12 +2156,12 @@
       <c r="G39" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H39" s="35"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="32" t="s">
+      <c r="H39" s="30"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="K39" s="29"/>
+      <c r="K39" s="37"/>
     </row>
     <row r="40" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
@@ -2161,12 +2185,12 @@
       <c r="G40" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H40" s="35"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="32" t="s">
+      <c r="H40" s="30"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="K40" s="29"/>
+      <c r="K40" s="37"/>
     </row>
     <row r="41" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="13" t="s">
@@ -2190,12 +2214,12 @@
       <c r="G41" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H41" s="35"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="32" t="s">
+      <c r="H41" s="30"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="K41" s="29"/>
+      <c r="K41" s="37"/>
     </row>
     <row r="42" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A42" s="13" t="s">
@@ -2219,12 +2243,12 @@
       <c r="G42" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H42" s="35"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="32" t="s">
+      <c r="H42" s="30"/>
+      <c r="I42" s="31"/>
+      <c r="J42" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="K42" s="29"/>
+      <c r="K42" s="37"/>
     </row>
     <row r="43" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A43" s="13" t="s">
@@ -2248,12 +2272,12 @@
       <c r="G43" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H43" s="35"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="32" t="s">
+      <c r="H43" s="30"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="K43" s="29"/>
+      <c r="K43" s="37"/>
     </row>
     <row r="44" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A44" s="13" t="s">
@@ -2277,12 +2301,12 @@
       <c r="G44" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H44" s="35"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="32" t="s">
+      <c r="H44" s="30"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="K44" s="29"/>
+      <c r="K44" s="37"/>
     </row>
     <row r="45" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="13" t="s">
@@ -2306,12 +2330,12 @@
       <c r="G45" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H45" s="35"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="32" t="s">
+      <c r="H45" s="30"/>
+      <c r="I45" s="31"/>
+      <c r="J45" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="K45" s="29"/>
+      <c r="K45" s="37"/>
     </row>
     <row r="46" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
@@ -2335,12 +2359,12 @@
       <c r="G46" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H46" s="35"/>
-      <c r="I46" s="36"/>
-      <c r="J46" s="32" t="s">
+      <c r="H46" s="30"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="K46" s="29"/>
+      <c r="K46" s="37"/>
     </row>
     <row r="47" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="13" t="s">
@@ -2364,12 +2388,12 @@
       <c r="G47" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H47" s="35"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="32" t="s">
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="K47" s="29"/>
+      <c r="K47" s="37"/>
     </row>
     <row r="48" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A48" s="13" t="s">
@@ -2393,12 +2417,12 @@
       <c r="G48" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H48" s="35"/>
-      <c r="I48" s="36"/>
-      <c r="J48" s="29" t="s">
+      <c r="H48" s="30"/>
+      <c r="I48" s="31"/>
+      <c r="J48" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="K48" s="29"/>
+      <c r="K48" s="37"/>
     </row>
     <row r="49" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A49" s="13"/>
@@ -2408,10 +2432,10 @@
       <c r="E49" s="13"/>
       <c r="F49" s="13"/>
       <c r="G49" s="15"/>
-      <c r="H49" s="35"/>
-      <c r="I49" s="36"/>
-      <c r="J49" s="29"/>
-      <c r="K49" s="29"/>
+      <c r="H49" s="30"/>
+      <c r="I49" s="31"/>
+      <c r="J49" s="37"/>
+      <c r="K49" s="37"/>
     </row>
     <row r="50" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A50" s="13"/>
@@ -2421,10 +2445,10 @@
       <c r="E50" s="13"/>
       <c r="F50" s="13"/>
       <c r="G50" s="15"/>
-      <c r="H50" s="35"/>
-      <c r="I50" s="36"/>
-      <c r="J50" s="29"/>
-      <c r="K50" s="29"/>
+      <c r="H50" s="30"/>
+      <c r="I50" s="31"/>
+      <c r="J50" s="37"/>
+      <c r="K50" s="37"/>
     </row>
     <row r="51" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A51" s="13"/>
@@ -2434,10 +2458,10 @@
       <c r="E51" s="13"/>
       <c r="F51" s="13"/>
       <c r="G51" s="15"/>
-      <c r="H51" s="35"/>
-      <c r="I51" s="36"/>
-      <c r="J51" s="29"/>
-      <c r="K51" s="29"/>
+      <c r="H51" s="30"/>
+      <c r="I51" s="31"/>
+      <c r="J51" s="37"/>
+      <c r="K51" s="37"/>
     </row>
     <row r="52" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A52" s="13"/>
@@ -2447,10 +2471,10 @@
       <c r="E52" s="13"/>
       <c r="F52" s="13"/>
       <c r="G52" s="15"/>
-      <c r="H52" s="35"/>
-      <c r="I52" s="36"/>
-      <c r="J52" s="29"/>
-      <c r="K52" s="29"/>
+      <c r="H52" s="30"/>
+      <c r="I52" s="31"/>
+      <c r="J52" s="37"/>
+      <c r="K52" s="37"/>
     </row>
     <row r="53" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A53" s="13"/>
@@ -2460,10 +2484,10 @@
       <c r="E53" s="13"/>
       <c r="F53" s="13"/>
       <c r="G53" s="15"/>
-      <c r="H53" s="35"/>
-      <c r="I53" s="36"/>
-      <c r="J53" s="29"/>
-      <c r="K53" s="29"/>
+      <c r="H53" s="30"/>
+      <c r="I53" s="31"/>
+      <c r="J53" s="37"/>
+      <c r="K53" s="37"/>
     </row>
     <row r="54" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A54" s="13"/>
@@ -2473,10 +2497,10 @@
       <c r="E54" s="13"/>
       <c r="F54" s="13"/>
       <c r="G54" s="15"/>
-      <c r="H54" s="35"/>
-      <c r="I54" s="36"/>
-      <c r="J54" s="29"/>
-      <c r="K54" s="29"/>
+      <c r="H54" s="30"/>
+      <c r="I54" s="31"/>
+      <c r="J54" s="37"/>
+      <c r="K54" s="37"/>
     </row>
     <row r="55" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A55" s="13"/>
@@ -2486,10 +2510,10 @@
       <c r="E55" s="13"/>
       <c r="F55" s="13"/>
       <c r="G55" s="15"/>
-      <c r="H55" s="35"/>
-      <c r="I55" s="36"/>
-      <c r="J55" s="29"/>
-      <c r="K55" s="29"/>
+      <c r="H55" s="30"/>
+      <c r="I55" s="31"/>
+      <c r="J55" s="37"/>
+      <c r="K55" s="37"/>
     </row>
     <row r="56" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A56" s="13"/>
@@ -2499,10 +2523,10 @@
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
       <c r="G56" s="15"/>
-      <c r="H56" s="35"/>
-      <c r="I56" s="36"/>
-      <c r="J56" s="29"/>
-      <c r="K56" s="29"/>
+      <c r="H56" s="30"/>
+      <c r="I56" s="31"/>
+      <c r="J56" s="37"/>
+      <c r="K56" s="37"/>
     </row>
     <row r="57" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A57" s="13"/>
@@ -2512,10 +2536,10 @@
       <c r="E57" s="13"/>
       <c r="F57" s="13"/>
       <c r="G57" s="15"/>
-      <c r="H57" s="35"/>
-      <c r="I57" s="36"/>
-      <c r="J57" s="29"/>
-      <c r="K57" s="29"/>
+      <c r="H57" s="30"/>
+      <c r="I57" s="31"/>
+      <c r="J57" s="37"/>
+      <c r="K57" s="37"/>
     </row>
     <row r="58" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A58" s="13"/>
@@ -2525,31 +2549,31 @@
       <c r="E58" s="13"/>
       <c r="F58" s="13"/>
       <c r="G58" s="15"/>
-      <c r="H58" s="35"/>
-      <c r="I58" s="36"/>
-      <c r="J58" s="29"/>
-      <c r="K58" s="29"/>
+      <c r="H58" s="30"/>
+      <c r="I58" s="31"/>
+      <c r="J58" s="37"/>
+      <c r="K58" s="37"/>
     </row>
     <row r="59" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A59" s="45" t="s">
+      <c r="A59" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="B59" s="40"/>
-      <c r="C59" s="40"/>
-      <c r="D59" s="40"/>
-      <c r="E59" s="40"/>
-      <c r="F59" s="40"/>
-      <c r="G59" s="40"/>
-      <c r="H59" s="40"/>
-      <c r="I59" s="40"/>
-      <c r="J59" s="40"/>
-      <c r="K59" s="41"/>
+      <c r="B59" s="33"/>
+      <c r="C59" s="33"/>
+      <c r="D59" s="33"/>
+      <c r="E59" s="33"/>
+      <c r="F59" s="33"/>
+      <c r="G59" s="33"/>
+      <c r="H59" s="33"/>
+      <c r="I59" s="33"/>
+      <c r="J59" s="33"/>
+      <c r="K59" s="34"/>
     </row>
     <row r="60" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A60" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="B60" s="46">
+      <c r="B60" s="29">
         <v>45771</v>
       </c>
       <c r="C60" s="13" t="s">
@@ -2565,38 +2589,66 @@
         <v>141</v>
       </c>
       <c r="G60" s="15"/>
-      <c r="H60" s="35"/>
-      <c r="I60" s="36"/>
-      <c r="J60" s="29" t="s">
+      <c r="H60" s="30"/>
+      <c r="I60" s="31"/>
+      <c r="J60" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="K60" s="29"/>
+      <c r="K60" s="37"/>
     </row>
     <row r="61" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A61" s="13"/>
-      <c r="B61" s="13"/>
-      <c r="C61" s="13"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="13"/>
+      <c r="A61" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="B61" s="29">
+        <v>45771</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="F61" s="13" t="s">
+        <v>146</v>
+      </c>
       <c r="G61" s="15"/>
-      <c r="H61" s="35"/>
-      <c r="I61" s="36"/>
-      <c r="J61" s="29"/>
-      <c r="K61" s="29"/>
-    </row>
-    <row r="62" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A62" s="13"/>
-      <c r="B62" s="13"/>
-      <c r="C62" s="13"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
+      <c r="H61" s="30"/>
+      <c r="I61" s="31"/>
+      <c r="J61" s="37" t="s">
+        <v>147</v>
+      </c>
+      <c r="K61" s="37"/>
+    </row>
+    <row r="62" spans="1:11" ht="36" x14ac:dyDescent="0.35">
+      <c r="A62" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B62" s="29">
+        <v>45771</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="E62" s="47" t="s">
+        <v>150</v>
+      </c>
+      <c r="F62" s="47" t="s">
+        <v>149</v>
+      </c>
       <c r="G62" s="15"/>
-      <c r="H62" s="35"/>
-      <c r="I62" s="36"/>
-      <c r="J62" s="29"/>
-      <c r="K62" s="29"/>
+      <c r="H62" s="30"/>
+      <c r="I62" s="31"/>
+      <c r="J62" s="37" t="s">
+        <v>147</v>
+      </c>
+      <c r="K62" s="37"/>
     </row>
     <row r="63" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A63" s="13"/>
@@ -2606,10 +2658,10 @@
       <c r="E63" s="13"/>
       <c r="F63" s="13"/>
       <c r="G63" s="15"/>
-      <c r="H63" s="35"/>
-      <c r="I63" s="36"/>
-      <c r="J63" s="29"/>
-      <c r="K63" s="29"/>
+      <c r="H63" s="30"/>
+      <c r="I63" s="31"/>
+      <c r="J63" s="37"/>
+      <c r="K63" s="37"/>
     </row>
     <row r="64" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A64" s="13"/>
@@ -2621,8 +2673,8 @@
       <c r="G64" s="15"/>
       <c r="H64" s="13"/>
       <c r="I64" s="13"/>
-      <c r="J64" s="29"/>
-      <c r="K64" s="29"/>
+      <c r="J64" s="37"/>
+      <c r="K64" s="37"/>
     </row>
     <row r="65" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A65" s="13"/>
@@ -2634,8 +2686,8 @@
       <c r="G65" s="15"/>
       <c r="H65" s="13"/>
       <c r="I65" s="13"/>
-      <c r="J65" s="29"/>
-      <c r="K65" s="29"/>
+      <c r="J65" s="37"/>
+      <c r="K65" s="37"/>
     </row>
     <row r="66" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A66" s="13"/>
@@ -2647,8 +2699,8 @@
       <c r="G66" s="15"/>
       <c r="H66" s="13"/>
       <c r="I66" s="13"/>
-      <c r="J66" s="29"/>
-      <c r="K66" s="29"/>
+      <c r="J66" s="37"/>
+      <c r="K66" s="37"/>
     </row>
     <row r="67" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A67" s="13"/>
@@ -2660,8 +2712,8 @@
       <c r="G67" s="15"/>
       <c r="H67" s="13"/>
       <c r="I67" s="13"/>
-      <c r="J67" s="29"/>
-      <c r="K67" s="29"/>
+      <c r="J67" s="37"/>
+      <c r="K67" s="37"/>
     </row>
     <row r="68" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A68" s="13"/>
@@ -2673,8 +2725,8 @@
       <c r="G68" s="15"/>
       <c r="H68" s="13"/>
       <c r="I68" s="13"/>
-      <c r="J68" s="29"/>
-      <c r="K68" s="29"/>
+      <c r="J68" s="37"/>
+      <c r="K68" s="37"/>
     </row>
     <row r="69" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A69" s="13"/>
@@ -2686,8 +2738,8 @@
       <c r="G69" s="15"/>
       <c r="H69" s="13"/>
       <c r="I69" s="13"/>
-      <c r="J69" s="29"/>
-      <c r="K69" s="29"/>
+      <c r="J69" s="37"/>
+      <c r="K69" s="37"/>
     </row>
     <row r="70" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A70" s="13"/>
@@ -2699,8 +2751,8 @@
       <c r="G70" s="15"/>
       <c r="H70" s="13"/>
       <c r="I70" s="13"/>
-      <c r="J70" s="29"/>
-      <c r="K70" s="29"/>
+      <c r="J70" s="37"/>
+      <c r="K70" s="37"/>
     </row>
     <row r="71" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A71" s="13"/>
@@ -2712,8 +2764,8 @@
       <c r="G71" s="15"/>
       <c r="H71" s="13"/>
       <c r="I71" s="13"/>
-      <c r="J71" s="29"/>
-      <c r="K71" s="29"/>
+      <c r="J71" s="37"/>
+      <c r="K71" s="37"/>
     </row>
     <row r="72" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A72" s="13"/>
@@ -2725,8 +2777,8 @@
       <c r="G72" s="15"/>
       <c r="H72" s="13"/>
       <c r="I72" s="13"/>
-      <c r="J72" s="29"/>
-      <c r="K72" s="29"/>
+      <c r="J72" s="37"/>
+      <c r="K72" s="37"/>
     </row>
     <row r="73" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A73" s="13"/>
@@ -2738,8 +2790,8 @@
       <c r="G73" s="15"/>
       <c r="H73" s="13"/>
       <c r="I73" s="13"/>
-      <c r="J73" s="29"/>
-      <c r="K73" s="29"/>
+      <c r="J73" s="37"/>
+      <c r="K73" s="37"/>
     </row>
     <row r="74" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A74" s="13"/>
@@ -2751,8 +2803,8 @@
       <c r="G74" s="15"/>
       <c r="H74" s="13"/>
       <c r="I74" s="13"/>
-      <c r="J74" s="29"/>
-      <c r="K74" s="29"/>
+      <c r="J74" s="37"/>
+      <c r="K74" s="37"/>
     </row>
     <row r="75" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A75" s="13"/>
@@ -2764,8 +2816,8 @@
       <c r="G75" s="15"/>
       <c r="H75" s="13"/>
       <c r="I75" s="13"/>
-      <c r="J75" s="29"/>
-      <c r="K75" s="29"/>
+      <c r="J75" s="37"/>
+      <c r="K75" s="37"/>
     </row>
     <row r="76" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A76" s="13"/>
@@ -2777,8 +2829,8 @@
       <c r="G76" s="15"/>
       <c r="H76" s="13"/>
       <c r="I76" s="13"/>
-      <c r="J76" s="29"/>
-      <c r="K76" s="29"/>
+      <c r="J76" s="37"/>
+      <c r="K76" s="37"/>
     </row>
     <row r="77" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A77" s="13"/>
@@ -2790,8 +2842,8 @@
       <c r="G77" s="15"/>
       <c r="H77" s="13"/>
       <c r="I77" s="13"/>
-      <c r="J77" s="29"/>
-      <c r="K77" s="29"/>
+      <c r="J77" s="37"/>
+      <c r="K77" s="37"/>
     </row>
     <row r="78" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A78" s="13"/>
@@ -2803,8 +2855,8 @@
       <c r="G78" s="15"/>
       <c r="H78" s="13"/>
       <c r="I78" s="13"/>
-      <c r="J78" s="29"/>
-      <c r="K78" s="29"/>
+      <c r="J78" s="37"/>
+      <c r="K78" s="37"/>
     </row>
     <row r="79" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A79" s="13"/>
@@ -2816,8 +2868,8 @@
       <c r="G79" s="15"/>
       <c r="H79" s="13"/>
       <c r="I79" s="13"/>
-      <c r="J79" s="29"/>
-      <c r="K79" s="29"/>
+      <c r="J79" s="37"/>
+      <c r="K79" s="37"/>
     </row>
     <row r="80" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A80" s="13"/>
@@ -2829,8 +2881,8 @@
       <c r="G80" s="15"/>
       <c r="H80" s="13"/>
       <c r="I80" s="13"/>
-      <c r="J80" s="29"/>
-      <c r="K80" s="29"/>
+      <c r="J80" s="37"/>
+      <c r="K80" s="37"/>
     </row>
     <row r="81" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A81" s="13"/>
@@ -2842,8 +2894,8 @@
       <c r="G81" s="15"/>
       <c r="H81" s="13"/>
       <c r="I81" s="13"/>
-      <c r="J81" s="29"/>
-      <c r="K81" s="29"/>
+      <c r="J81" s="37"/>
+      <c r="K81" s="37"/>
     </row>
     <row r="82" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A82" s="13"/>
@@ -2855,8 +2907,8 @@
       <c r="G82" s="15"/>
       <c r="H82" s="13"/>
       <c r="I82" s="13"/>
-      <c r="J82" s="29"/>
-      <c r="K82" s="29"/>
+      <c r="J82" s="37"/>
+      <c r="K82" s="37"/>
     </row>
     <row r="83" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A83" s="13"/>
@@ -2868,8 +2920,8 @@
       <c r="G83" s="15"/>
       <c r="H83" s="13"/>
       <c r="I83" s="13"/>
-      <c r="J83" s="29"/>
-      <c r="K83" s="29"/>
+      <c r="J83" s="37"/>
+      <c r="K83" s="37"/>
     </row>
     <row r="84" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A84" s="13"/>
@@ -2881,8 +2933,8 @@
       <c r="G84" s="15"/>
       <c r="H84" s="13"/>
       <c r="I84" s="13"/>
-      <c r="J84" s="29"/>
-      <c r="K84" s="29"/>
+      <c r="J84" s="37"/>
+      <c r="K84" s="37"/>
     </row>
     <row r="85" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A85" s="13"/>
@@ -2894,8 +2946,8 @@
       <c r="G85" s="15"/>
       <c r="H85" s="13"/>
       <c r="I85" s="13"/>
-      <c r="J85" s="29"/>
-      <c r="K85" s="29"/>
+      <c r="J85" s="37"/>
+      <c r="K85" s="37"/>
     </row>
     <row r="86" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A86" s="13"/>
@@ -2907,8 +2959,8 @@
       <c r="G86" s="15"/>
       <c r="H86" s="13"/>
       <c r="I86" s="13"/>
-      <c r="J86" s="29"/>
-      <c r="K86" s="29"/>
+      <c r="J86" s="37"/>
+      <c r="K86" s="37"/>
     </row>
     <row r="87" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A87" s="13"/>
@@ -2920,8 +2972,8 @@
       <c r="G87" s="15"/>
       <c r="H87" s="13"/>
       <c r="I87" s="13"/>
-      <c r="J87" s="29"/>
-      <c r="K87" s="29"/>
+      <c r="J87" s="37"/>
+      <c r="K87" s="37"/>
     </row>
     <row r="88" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A88" s="13"/>
@@ -2933,8 +2985,8 @@
       <c r="G88" s="15"/>
       <c r="H88" s="13"/>
       <c r="I88" s="13"/>
-      <c r="J88" s="29"/>
-      <c r="K88" s="29"/>
+      <c r="J88" s="37"/>
+      <c r="K88" s="37"/>
     </row>
     <row r="89" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A89" s="13"/>
@@ -2946,8 +2998,8 @@
       <c r="G89" s="15"/>
       <c r="H89" s="13"/>
       <c r="I89" s="13"/>
-      <c r="J89" s="29"/>
-      <c r="K89" s="29"/>
+      <c r="J89" s="37"/>
+      <c r="K89" s="37"/>
     </row>
     <row r="90" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A90" s="13"/>
@@ -2959,8 +3011,8 @@
       <c r="G90" s="15"/>
       <c r="H90" s="13"/>
       <c r="I90" s="13"/>
-      <c r="J90" s="29"/>
-      <c r="K90" s="29"/>
+      <c r="J90" s="37"/>
+      <c r="K90" s="37"/>
     </row>
     <row r="91" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A91" s="13"/>
@@ -2972,8 +3024,8 @@
       <c r="G91" s="15"/>
       <c r="H91" s="13"/>
       <c r="I91" s="13"/>
-      <c r="J91" s="29"/>
-      <c r="K91" s="29"/>
+      <c r="J91" s="37"/>
+      <c r="K91" s="37"/>
     </row>
     <row r="92" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A92" s="13"/>
@@ -2985,8 +3037,8 @@
       <c r="G92" s="15"/>
       <c r="H92" s="13"/>
       <c r="I92" s="13"/>
-      <c r="J92" s="29"/>
-      <c r="K92" s="29"/>
+      <c r="J92" s="37"/>
+      <c r="K92" s="37"/>
     </row>
     <row r="93" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A93" s="13"/>
@@ -2998,8 +3050,8 @@
       <c r="G93" s="15"/>
       <c r="H93" s="13"/>
       <c r="I93" s="13"/>
-      <c r="J93" s="29"/>
-      <c r="K93" s="29"/>
+      <c r="J93" s="37"/>
+      <c r="K93" s="37"/>
     </row>
     <row r="94" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A94" s="13"/>
@@ -3011,8 +3063,8 @@
       <c r="G94" s="15"/>
       <c r="H94" s="13"/>
       <c r="I94" s="13"/>
-      <c r="J94" s="29"/>
-      <c r="K94" s="29"/>
+      <c r="J94" s="37"/>
+      <c r="K94" s="37"/>
     </row>
     <row r="95" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A95" s="13"/>
@@ -3024,8 +3076,8 @@
       <c r="G95" s="15"/>
       <c r="H95" s="13"/>
       <c r="I95" s="13"/>
-      <c r="J95" s="29"/>
-      <c r="K95" s="29"/>
+      <c r="J95" s="37"/>
+      <c r="K95" s="37"/>
     </row>
     <row r="96" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A96" s="13"/>
@@ -3037,8 +3089,8 @@
       <c r="G96" s="15"/>
       <c r="H96" s="13"/>
       <c r="I96" s="13"/>
-      <c r="J96" s="29"/>
-      <c r="K96" s="29"/>
+      <c r="J96" s="37"/>
+      <c r="K96" s="37"/>
     </row>
     <row r="97" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A97" s="13"/>
@@ -3050,8 +3102,8 @@
       <c r="G97" s="15"/>
       <c r="H97" s="13"/>
       <c r="I97" s="13"/>
-      <c r="J97" s="29"/>
-      <c r="K97" s="29"/>
+      <c r="J97" s="37"/>
+      <c r="K97" s="37"/>
     </row>
     <row r="98" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A98" s="13"/>
@@ -3063,8 +3115,8 @@
       <c r="G98" s="15"/>
       <c r="H98" s="13"/>
       <c r="I98" s="13"/>
-      <c r="J98" s="29"/>
-      <c r="K98" s="29"/>
+      <c r="J98" s="37"/>
+      <c r="K98" s="37"/>
     </row>
     <row r="99" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A99" s="13"/>
@@ -3076,8 +3128,8 @@
       <c r="G99" s="15"/>
       <c r="H99" s="13"/>
       <c r="I99" s="13"/>
-      <c r="J99" s="29"/>
-      <c r="K99" s="29"/>
+      <c r="J99" s="37"/>
+      <c r="K99" s="37"/>
     </row>
     <row r="100" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A100" s="13"/>
@@ -3089,8 +3141,8 @@
       <c r="G100" s="15"/>
       <c r="H100" s="13"/>
       <c r="I100" s="13"/>
-      <c r="J100" s="29"/>
-      <c r="K100" s="29"/>
+      <c r="J100" s="37"/>
+      <c r="K100" s="37"/>
     </row>
     <row r="101" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A101" s="13"/>
@@ -3102,8 +3154,8 @@
       <c r="G101" s="15"/>
       <c r="H101" s="13"/>
       <c r="I101" s="13"/>
-      <c r="J101" s="29"/>
-      <c r="K101" s="29"/>
+      <c r="J101" s="37"/>
+      <c r="K101" s="37"/>
     </row>
     <row r="102" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A102" s="13"/>
@@ -3115,8 +3167,8 @@
       <c r="G102" s="15"/>
       <c r="H102" s="13"/>
       <c r="I102" s="13"/>
-      <c r="J102" s="29"/>
-      <c r="K102" s="29"/>
+      <c r="J102" s="37"/>
+      <c r="K102" s="37"/>
     </row>
     <row r="103" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A103" s="13"/>
@@ -3128,8 +3180,8 @@
       <c r="G103" s="15"/>
       <c r="H103" s="13"/>
       <c r="I103" s="13"/>
-      <c r="J103" s="29"/>
-      <c r="K103" s="29"/>
+      <c r="J103" s="37"/>
+      <c r="K103" s="37"/>
     </row>
     <row r="104" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A104" s="13"/>
@@ -3141,8 +3193,8 @@
       <c r="G104" s="15"/>
       <c r="H104" s="13"/>
       <c r="I104" s="13"/>
-      <c r="J104" s="29"/>
-      <c r="K104" s="29"/>
+      <c r="J104" s="37"/>
+      <c r="K104" s="37"/>
     </row>
     <row r="105" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A105" s="13"/>
@@ -3154,8 +3206,8 @@
       <c r="G105" s="15"/>
       <c r="H105" s="13"/>
       <c r="I105" s="13"/>
-      <c r="J105" s="29"/>
-      <c r="K105" s="29"/>
+      <c r="J105" s="37"/>
+      <c r="K105" s="37"/>
     </row>
     <row r="106" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A106" s="13"/>
@@ -3167,8 +3219,8 @@
       <c r="G106" s="15"/>
       <c r="H106" s="13"/>
       <c r="I106" s="13"/>
-      <c r="J106" s="29"/>
-      <c r="K106" s="29"/>
+      <c r="J106" s="37"/>
+      <c r="K106" s="37"/>
     </row>
     <row r="107" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A107" s="13"/>
@@ -3180,8 +3232,8 @@
       <c r="G107" s="15"/>
       <c r="H107" s="13"/>
       <c r="I107" s="13"/>
-      <c r="J107" s="29"/>
-      <c r="K107" s="29"/>
+      <c r="J107" s="37"/>
+      <c r="K107" s="37"/>
     </row>
     <row r="108" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A108" s="13"/>
@@ -3193,8 +3245,8 @@
       <c r="G108" s="15"/>
       <c r="H108" s="13"/>
       <c r="I108" s="13"/>
-      <c r="J108" s="29"/>
-      <c r="K108" s="29"/>
+      <c r="J108" s="37"/>
+      <c r="K108" s="37"/>
     </row>
     <row r="109" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A109" s="13"/>
@@ -3206,8 +3258,8 @@
       <c r="G109" s="15"/>
       <c r="H109" s="13"/>
       <c r="I109" s="13"/>
-      <c r="J109" s="29"/>
-      <c r="K109" s="29"/>
+      <c r="J109" s="37"/>
+      <c r="K109" s="37"/>
     </row>
     <row r="110" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A110" s="13"/>
@@ -3219,8 +3271,8 @@
       <c r="G110" s="15"/>
       <c r="H110" s="13"/>
       <c r="I110" s="13"/>
-      <c r="J110" s="29"/>
-      <c r="K110" s="29"/>
+      <c r="J110" s="37"/>
+      <c r="K110" s="37"/>
     </row>
     <row r="111" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A111" s="13"/>
@@ -3232,8 +3284,8 @@
       <c r="G111" s="15"/>
       <c r="H111" s="13"/>
       <c r="I111" s="13"/>
-      <c r="J111" s="29"/>
-      <c r="K111" s="29"/>
+      <c r="J111" s="37"/>
+      <c r="K111" s="37"/>
     </row>
     <row r="112" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A112" s="13"/>
@@ -3245,8 +3297,8 @@
       <c r="G112" s="15"/>
       <c r="H112" s="13"/>
       <c r="I112" s="13"/>
-      <c r="J112" s="29"/>
-      <c r="K112" s="29"/>
+      <c r="J112" s="37"/>
+      <c r="K112" s="37"/>
     </row>
     <row r="113" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A113" s="13"/>
@@ -3258,8 +3310,8 @@
       <c r="G113" s="15"/>
       <c r="H113" s="13"/>
       <c r="I113" s="13"/>
-      <c r="J113" s="29"/>
-      <c r="K113" s="29"/>
+      <c r="J113" s="37"/>
+      <c r="K113" s="37"/>
     </row>
     <row r="114" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A114" s="13"/>
@@ -3271,8 +3323,8 @@
       <c r="G114" s="15"/>
       <c r="H114" s="13"/>
       <c r="I114" s="13"/>
-      <c r="J114" s="29"/>
-      <c r="K114" s="29"/>
+      <c r="J114" s="37"/>
+      <c r="K114" s="37"/>
     </row>
     <row r="115" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A115" s="13"/>
@@ -3284,8 +3336,8 @@
       <c r="G115" s="15"/>
       <c r="H115" s="13"/>
       <c r="I115" s="13"/>
-      <c r="J115" s="29"/>
-      <c r="K115" s="29"/>
+      <c r="J115" s="37"/>
+      <c r="K115" s="37"/>
     </row>
     <row r="116" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A116" s="13"/>
@@ -3297,8 +3349,8 @@
       <c r="G116" s="15"/>
       <c r="H116" s="13"/>
       <c r="I116" s="13"/>
-      <c r="J116" s="29"/>
-      <c r="K116" s="29"/>
+      <c r="J116" s="37"/>
+      <c r="K116" s="37"/>
     </row>
     <row r="117" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A117" s="13"/>
@@ -3310,8 +3362,8 @@
       <c r="G117" s="15"/>
       <c r="H117" s="13"/>
       <c r="I117" s="13"/>
-      <c r="J117" s="29"/>
-      <c r="K117" s="29"/>
+      <c r="J117" s="37"/>
+      <c r="K117" s="37"/>
     </row>
     <row r="118" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A118" s="13"/>
@@ -3323,8 +3375,8 @@
       <c r="G118" s="15"/>
       <c r="H118" s="13"/>
       <c r="I118" s="13"/>
-      <c r="J118" s="29"/>
-      <c r="K118" s="29"/>
+      <c r="J118" s="37"/>
+      <c r="K118" s="37"/>
     </row>
     <row r="119" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A119" s="13"/>
@@ -3336,8 +3388,8 @@
       <c r="G119" s="15"/>
       <c r="H119" s="13"/>
       <c r="I119" s="13"/>
-      <c r="J119" s="29"/>
-      <c r="K119" s="29"/>
+      <c r="J119" s="37"/>
+      <c r="K119" s="37"/>
     </row>
     <row r="120" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A120" s="13"/>
@@ -3349,8 +3401,8 @@
       <c r="G120" s="15"/>
       <c r="H120" s="13"/>
       <c r="I120" s="13"/>
-      <c r="J120" s="29"/>
-      <c r="K120" s="29"/>
+      <c r="J120" s="37"/>
+      <c r="K120" s="37"/>
     </row>
     <row r="121" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A121" s="13"/>
@@ -3362,8 +3414,8 @@
       <c r="G121" s="15"/>
       <c r="H121" s="13"/>
       <c r="I121" s="13"/>
-      <c r="J121" s="29"/>
-      <c r="K121" s="29"/>
+      <c r="J121" s="37"/>
+      <c r="K121" s="37"/>
     </row>
     <row r="122" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A122" s="13"/>
@@ -3375,8 +3427,8 @@
       <c r="G122" s="15"/>
       <c r="H122" s="13"/>
       <c r="I122" s="13"/>
-      <c r="J122" s="29"/>
-      <c r="K122" s="29"/>
+      <c r="J122" s="37"/>
+      <c r="K122" s="37"/>
     </row>
     <row r="123" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A123" s="13"/>
@@ -3388,8 +3440,8 @@
       <c r="G123" s="15"/>
       <c r="H123" s="13"/>
       <c r="I123" s="13"/>
-      <c r="J123" s="29"/>
-      <c r="K123" s="29"/>
+      <c r="J123" s="37"/>
+      <c r="K123" s="37"/>
     </row>
     <row r="124" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A124" s="13"/>
@@ -3401,8 +3453,8 @@
       <c r="G124" s="15"/>
       <c r="H124" s="13"/>
       <c r="I124" s="13"/>
-      <c r="J124" s="29"/>
-      <c r="K124" s="29"/>
+      <c r="J124" s="37"/>
+      <c r="K124" s="37"/>
     </row>
     <row r="125" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A125" s="13"/>
@@ -3414,8 +3466,8 @@
       <c r="G125" s="15"/>
       <c r="H125" s="13"/>
       <c r="I125" s="13"/>
-      <c r="J125" s="29"/>
-      <c r="K125" s="29"/>
+      <c r="J125" s="37"/>
+      <c r="K125" s="37"/>
     </row>
     <row r="126" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A126" s="13"/>
@@ -3427,8 +3479,8 @@
       <c r="G126" s="15"/>
       <c r="H126" s="13"/>
       <c r="I126" s="13"/>
-      <c r="J126" s="29"/>
-      <c r="K126" s="29"/>
+      <c r="J126" s="37"/>
+      <c r="K126" s="37"/>
     </row>
     <row r="127" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A127" s="13"/>
@@ -3440,8 +3492,8 @@
       <c r="G127" s="15"/>
       <c r="H127" s="13"/>
       <c r="I127" s="13"/>
-      <c r="J127" s="29"/>
-      <c r="K127" s="29"/>
+      <c r="J127" s="37"/>
+      <c r="K127" s="37"/>
     </row>
     <row r="128" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A128" s="13"/>
@@ -3453,8 +3505,8 @@
       <c r="G128" s="15"/>
       <c r="H128" s="13"/>
       <c r="I128" s="13"/>
-      <c r="J128" s="29"/>
-      <c r="K128" s="29"/>
+      <c r="J128" s="37"/>
+      <c r="K128" s="37"/>
     </row>
     <row r="129" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A129" s="13"/>
@@ -3466,8 +3518,8 @@
       <c r="G129" s="15"/>
       <c r="H129" s="13"/>
       <c r="I129" s="13"/>
-      <c r="J129" s="29"/>
-      <c r="K129" s="29"/>
+      <c r="J129" s="37"/>
+      <c r="K129" s="37"/>
     </row>
     <row r="130" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A130" s="13"/>
@@ -3479,8 +3531,8 @@
       <c r="G130" s="15"/>
       <c r="H130" s="13"/>
       <c r="I130" s="13"/>
-      <c r="J130" s="29"/>
-      <c r="K130" s="29"/>
+      <c r="J130" s="37"/>
+      <c r="K130" s="37"/>
     </row>
     <row r="131" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A131" s="13"/>
@@ -3492,8 +3544,8 @@
       <c r="G131" s="15"/>
       <c r="H131" s="13"/>
       <c r="I131" s="13"/>
-      <c r="J131" s="29"/>
-      <c r="K131" s="29"/>
+      <c r="J131" s="37"/>
+      <c r="K131" s="37"/>
     </row>
     <row r="132" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A132" s="13"/>
@@ -3505,8 +3557,8 @@
       <c r="G132" s="15"/>
       <c r="H132" s="13"/>
       <c r="I132" s="13"/>
-      <c r="J132" s="29"/>
-      <c r="K132" s="29"/>
+      <c r="J132" s="37"/>
+      <c r="K132" s="37"/>
     </row>
     <row r="133" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A133" s="13"/>
@@ -3518,8 +3570,8 @@
       <c r="G133" s="15"/>
       <c r="H133" s="13"/>
       <c r="I133" s="13"/>
-      <c r="J133" s="29"/>
-      <c r="K133" s="29"/>
+      <c r="J133" s="37"/>
+      <c r="K133" s="37"/>
     </row>
     <row r="134" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A134" s="13"/>
@@ -3531,8 +3583,8 @@
       <c r="G134" s="15"/>
       <c r="H134" s="13"/>
       <c r="I134" s="13"/>
-      <c r="J134" s="29"/>
-      <c r="K134" s="29"/>
+      <c r="J134" s="37"/>
+      <c r="K134" s="37"/>
     </row>
     <row r="135" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A135" s="13"/>
@@ -3544,8 +3596,8 @@
       <c r="G135" s="15"/>
       <c r="H135" s="13"/>
       <c r="I135" s="13"/>
-      <c r="J135" s="29"/>
-      <c r="K135" s="29"/>
+      <c r="J135" s="37"/>
+      <c r="K135" s="37"/>
     </row>
     <row r="136" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A136" s="13"/>
@@ -3557,8 +3609,8 @@
       <c r="G136" s="15"/>
       <c r="H136" s="13"/>
       <c r="I136" s="13"/>
-      <c r="J136" s="29"/>
-      <c r="K136" s="29"/>
+      <c r="J136" s="37"/>
+      <c r="K136" s="37"/>
     </row>
     <row r="137" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A137" s="13"/>
@@ -3570,8 +3622,8 @@
       <c r="G137" s="15"/>
       <c r="H137" s="13"/>
       <c r="I137" s="13"/>
-      <c r="J137" s="29"/>
-      <c r="K137" s="29"/>
+      <c r="J137" s="37"/>
+      <c r="K137" s="37"/>
     </row>
     <row r="138" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A138" s="13"/>
@@ -3583,8 +3635,8 @@
       <c r="G138" s="15"/>
       <c r="H138" s="13"/>
       <c r="I138" s="13"/>
-      <c r="J138" s="29"/>
-      <c r="K138" s="29"/>
+      <c r="J138" s="37"/>
+      <c r="K138" s="37"/>
     </row>
     <row r="139" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A139" s="13"/>
@@ -3596,8 +3648,8 @@
       <c r="G139" s="15"/>
       <c r="H139" s="13"/>
       <c r="I139" s="13"/>
-      <c r="J139" s="29"/>
-      <c r="K139" s="29"/>
+      <c r="J139" s="37"/>
+      <c r="K139" s="37"/>
     </row>
     <row r="140" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A140" s="13"/>
@@ -3609,8 +3661,8 @@
       <c r="G140" s="15"/>
       <c r="H140" s="13"/>
       <c r="I140" s="13"/>
-      <c r="J140" s="29"/>
-      <c r="K140" s="29"/>
+      <c r="J140" s="37"/>
+      <c r="K140" s="37"/>
     </row>
     <row r="141" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A141" s="13"/>
@@ -3622,8 +3674,8 @@
       <c r="G141" s="15"/>
       <c r="H141" s="13"/>
       <c r="I141" s="13"/>
-      <c r="J141" s="29"/>
-      <c r="K141" s="29"/>
+      <c r="J141" s="37"/>
+      <c r="K141" s="37"/>
     </row>
     <row r="142" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A142" s="13"/>
@@ -3635,8 +3687,8 @@
       <c r="G142" s="15"/>
       <c r="H142" s="13"/>
       <c r="I142" s="13"/>
-      <c r="J142" s="29"/>
-      <c r="K142" s="29"/>
+      <c r="J142" s="37"/>
+      <c r="K142" s="37"/>
     </row>
     <row r="143" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A143" s="13"/>
@@ -3648,8 +3700,8 @@
       <c r="G143" s="15"/>
       <c r="H143" s="13"/>
       <c r="I143" s="13"/>
-      <c r="J143" s="29"/>
-      <c r="K143" s="29"/>
+      <c r="J143" s="37"/>
+      <c r="K143" s="37"/>
     </row>
     <row r="144" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A144" s="13"/>
@@ -3661,8 +3713,8 @@
       <c r="G144" s="15"/>
       <c r="H144" s="13"/>
       <c r="I144" s="13"/>
-      <c r="J144" s="29"/>
-      <c r="K144" s="29"/>
+      <c r="J144" s="37"/>
+      <c r="K144" s="37"/>
     </row>
     <row r="145" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A145" s="13"/>
@@ -3674,8 +3726,8 @@
       <c r="G145" s="15"/>
       <c r="H145" s="13"/>
       <c r="I145" s="13"/>
-      <c r="J145" s="29"/>
-      <c r="K145" s="29"/>
+      <c r="J145" s="37"/>
+      <c r="K145" s="37"/>
     </row>
     <row r="146" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A146" s="13"/>
@@ -3687,8 +3739,8 @@
       <c r="G146" s="15"/>
       <c r="H146" s="13"/>
       <c r="I146" s="13"/>
-      <c r="J146" s="29"/>
-      <c r="K146" s="29"/>
+      <c r="J146" s="37"/>
+      <c r="K146" s="37"/>
     </row>
     <row r="147" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A147" s="13"/>
@@ -3700,8 +3752,8 @@
       <c r="G147" s="15"/>
       <c r="H147" s="13"/>
       <c r="I147" s="13"/>
-      <c r="J147" s="29"/>
-      <c r="K147" s="29"/>
+      <c r="J147" s="37"/>
+      <c r="K147" s="37"/>
     </row>
     <row r="148" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A148" s="13"/>
@@ -3713,8 +3765,8 @@
       <c r="G148" s="15"/>
       <c r="H148" s="13"/>
       <c r="I148" s="13"/>
-      <c r="J148" s="29"/>
-      <c r="K148" s="29"/>
+      <c r="J148" s="37"/>
+      <c r="K148" s="37"/>
     </row>
     <row r="149" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A149" s="13"/>
@@ -3726,8 +3778,8 @@
       <c r="G149" s="15"/>
       <c r="H149" s="13"/>
       <c r="I149" s="13"/>
-      <c r="J149" s="29"/>
-      <c r="K149" s="29"/>
+      <c r="J149" s="37"/>
+      <c r="K149" s="37"/>
     </row>
     <row r="150" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A150" s="13"/>
@@ -3739,8 +3791,8 @@
       <c r="G150" s="15"/>
       <c r="H150" s="13"/>
       <c r="I150" s="13"/>
-      <c r="J150" s="29"/>
-      <c r="K150" s="29"/>
+      <c r="J150" s="37"/>
+      <c r="K150" s="37"/>
     </row>
     <row r="151" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A151" s="13"/>
@@ -3752,8 +3804,8 @@
       <c r="G151" s="15"/>
       <c r="H151" s="13"/>
       <c r="I151" s="13"/>
-      <c r="J151" s="29"/>
-      <c r="K151" s="29"/>
+      <c r="J151" s="37"/>
+      <c r="K151" s="37"/>
     </row>
     <row r="152" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A152" s="13"/>
@@ -3765,8 +3817,8 @@
       <c r="G152" s="15"/>
       <c r="H152" s="13"/>
       <c r="I152" s="13"/>
-      <c r="J152" s="29"/>
-      <c r="K152" s="29"/>
+      <c r="J152" s="37"/>
+      <c r="K152" s="37"/>
     </row>
     <row r="153" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A153" s="13"/>
@@ -3778,8 +3830,8 @@
       <c r="G153" s="15"/>
       <c r="H153" s="13"/>
       <c r="I153" s="13"/>
-      <c r="J153" s="29"/>
-      <c r="K153" s="29"/>
+      <c r="J153" s="37"/>
+      <c r="K153" s="37"/>
     </row>
     <row r="154" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A154" s="13"/>
@@ -3791,8 +3843,8 @@
       <c r="G154" s="15"/>
       <c r="H154" s="13"/>
       <c r="I154" s="13"/>
-      <c r="J154" s="29"/>
-      <c r="K154" s="29"/>
+      <c r="J154" s="37"/>
+      <c r="K154" s="37"/>
     </row>
     <row r="155" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A155" s="13"/>
@@ -3804,8 +3856,8 @@
       <c r="G155" s="15"/>
       <c r="H155" s="13"/>
       <c r="I155" s="13"/>
-      <c r="J155" s="29"/>
-      <c r="K155" s="29"/>
+      <c r="J155" s="37"/>
+      <c r="K155" s="37"/>
     </row>
     <row r="156" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A156" s="13"/>
@@ -3817,8 +3869,8 @@
       <c r="G156" s="15"/>
       <c r="H156" s="13"/>
       <c r="I156" s="13"/>
-      <c r="J156" s="29"/>
-      <c r="K156" s="29"/>
+      <c r="J156" s="37"/>
+      <c r="K156" s="37"/>
     </row>
     <row r="157" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A157" s="13"/>
@@ -3830,8 +3882,8 @@
       <c r="G157" s="15"/>
       <c r="H157" s="13"/>
       <c r="I157" s="13"/>
-      <c r="J157" s="29"/>
-      <c r="K157" s="29"/>
+      <c r="J157" s="37"/>
+      <c r="K157" s="37"/>
     </row>
     <row r="158" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A158" s="13"/>
@@ -3843,8 +3895,8 @@
       <c r="G158" s="15"/>
       <c r="H158" s="13"/>
       <c r="I158" s="13"/>
-      <c r="J158" s="29"/>
-      <c r="K158" s="29"/>
+      <c r="J158" s="37"/>
+      <c r="K158" s="37"/>
     </row>
     <row r="159" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A159" s="13"/>
@@ -3856,8 +3908,8 @@
       <c r="G159" s="15"/>
       <c r="H159" s="13"/>
       <c r="I159" s="13"/>
-      <c r="J159" s="29"/>
-      <c r="K159" s="29"/>
+      <c r="J159" s="37"/>
+      <c r="K159" s="37"/>
     </row>
     <row r="160" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A160" s="13"/>
@@ -3869,8 +3921,8 @@
       <c r="G160" s="15"/>
       <c r="H160" s="13"/>
       <c r="I160" s="13"/>
-      <c r="J160" s="29"/>
-      <c r="K160" s="29"/>
+      <c r="J160" s="37"/>
+      <c r="K160" s="37"/>
     </row>
     <row r="161" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A161" s="13"/>
@@ -3882,8 +3934,8 @@
       <c r="G161" s="15"/>
       <c r="H161" s="13"/>
       <c r="I161" s="13"/>
-      <c r="J161" s="29"/>
-      <c r="K161" s="29"/>
+      <c r="J161" s="37"/>
+      <c r="K161" s="37"/>
     </row>
     <row r="162" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A162" s="13"/>
@@ -3895,8 +3947,8 @@
       <c r="G162" s="15"/>
       <c r="H162" s="13"/>
       <c r="I162" s="13"/>
-      <c r="J162" s="29"/>
-      <c r="K162" s="29"/>
+      <c r="J162" s="37"/>
+      <c r="K162" s="37"/>
     </row>
     <row r="163" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A163" s="13"/>
@@ -3908,8 +3960,8 @@
       <c r="G163" s="15"/>
       <c r="H163" s="13"/>
       <c r="I163" s="13"/>
-      <c r="J163" s="29"/>
-      <c r="K163" s="29"/>
+      <c r="J163" s="37"/>
+      <c r="K163" s="37"/>
     </row>
     <row r="164" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A164" s="13"/>
@@ -3921,8 +3973,8 @@
       <c r="G164" s="15"/>
       <c r="H164" s="13"/>
       <c r="I164" s="13"/>
-      <c r="J164" s="29"/>
-      <c r="K164" s="29"/>
+      <c r="J164" s="37"/>
+      <c r="K164" s="37"/>
     </row>
     <row r="165" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A165" s="13"/>
@@ -3934,8 +3986,8 @@
       <c r="G165" s="15"/>
       <c r="H165" s="13"/>
       <c r="I165" s="13"/>
-      <c r="J165" s="29"/>
-      <c r="K165" s="29"/>
+      <c r="J165" s="37"/>
+      <c r="K165" s="37"/>
     </row>
     <row r="166" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A166" s="13"/>
@@ -3947,8 +3999,8 @@
       <c r="G166" s="15"/>
       <c r="H166" s="13"/>
       <c r="I166" s="13"/>
-      <c r="J166" s="29"/>
-      <c r="K166" s="29"/>
+      <c r="J166" s="37"/>
+      <c r="K166" s="37"/>
     </row>
     <row r="167" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A167" s="13"/>
@@ -3960,8 +4012,8 @@
       <c r="G167" s="15"/>
       <c r="H167" s="13"/>
       <c r="I167" s="13"/>
-      <c r="J167" s="29"/>
-      <c r="K167" s="29"/>
+      <c r="J167" s="37"/>
+      <c r="K167" s="37"/>
     </row>
     <row r="168" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A168" s="13"/>
@@ -3973,8 +4025,8 @@
       <c r="G168" s="15"/>
       <c r="H168" s="13"/>
       <c r="I168" s="13"/>
-      <c r="J168" s="29"/>
-      <c r="K168" s="29"/>
+      <c r="J168" s="37"/>
+      <c r="K168" s="37"/>
     </row>
     <row r="169" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A169" s="13"/>
@@ -3986,8 +4038,8 @@
       <c r="G169" s="15"/>
       <c r="H169" s="13"/>
       <c r="I169" s="13"/>
-      <c r="J169" s="29"/>
-      <c r="K169" s="29"/>
+      <c r="J169" s="37"/>
+      <c r="K169" s="37"/>
     </row>
     <row r="170" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A170" s="13"/>
@@ -3999,8 +4051,8 @@
       <c r="G170" s="15"/>
       <c r="H170" s="13"/>
       <c r="I170" s="13"/>
-      <c r="J170" s="29"/>
-      <c r="K170" s="29"/>
+      <c r="J170" s="37"/>
+      <c r="K170" s="37"/>
     </row>
     <row r="171" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A171" s="13"/>
@@ -4012,8 +4064,8 @@
       <c r="G171" s="15"/>
       <c r="H171" s="13"/>
       <c r="I171" s="13"/>
-      <c r="J171" s="29"/>
-      <c r="K171" s="29"/>
+      <c r="J171" s="37"/>
+      <c r="K171" s="37"/>
     </row>
     <row r="172" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A172" s="13"/>
@@ -4025,8 +4077,8 @@
       <c r="G172" s="15"/>
       <c r="H172" s="13"/>
       <c r="I172" s="13"/>
-      <c r="J172" s="29"/>
-      <c r="K172" s="29"/>
+      <c r="J172" s="37"/>
+      <c r="K172" s="37"/>
     </row>
     <row r="173" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A173" s="13"/>
@@ -4038,8 +4090,8 @@
       <c r="G173" s="15"/>
       <c r="H173" s="13"/>
       <c r="I173" s="13"/>
-      <c r="J173" s="29"/>
-      <c r="K173" s="29"/>
+      <c r="J173" s="37"/>
+      <c r="K173" s="37"/>
     </row>
     <row r="174" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A174" s="13"/>
@@ -4051,8 +4103,8 @@
       <c r="G174" s="15"/>
       <c r="H174" s="13"/>
       <c r="I174" s="13"/>
-      <c r="J174" s="29"/>
-      <c r="K174" s="29"/>
+      <c r="J174" s="37"/>
+      <c r="K174" s="37"/>
     </row>
     <row r="175" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A175" s="13"/>
@@ -4064,8 +4116,8 @@
       <c r="G175" s="15"/>
       <c r="H175" s="13"/>
       <c r="I175" s="13"/>
-      <c r="J175" s="29"/>
-      <c r="K175" s="29"/>
+      <c r="J175" s="37"/>
+      <c r="K175" s="37"/>
     </row>
     <row r="176" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A176" s="13"/>
@@ -4077,8 +4129,8 @@
       <c r="G176" s="15"/>
       <c r="H176" s="13"/>
       <c r="I176" s="13"/>
-      <c r="J176" s="29"/>
-      <c r="K176" s="29"/>
+      <c r="J176" s="37"/>
+      <c r="K176" s="37"/>
     </row>
     <row r="177" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A177" s="13"/>
@@ -4090,8 +4142,8 @@
       <c r="G177" s="15"/>
       <c r="H177" s="13"/>
       <c r="I177" s="13"/>
-      <c r="J177" s="29"/>
-      <c r="K177" s="29"/>
+      <c r="J177" s="37"/>
+      <c r="K177" s="37"/>
     </row>
     <row r="178" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A178" s="13"/>
@@ -4103,8 +4155,8 @@
       <c r="G178" s="15"/>
       <c r="H178" s="13"/>
       <c r="I178" s="13"/>
-      <c r="J178" s="29"/>
-      <c r="K178" s="29"/>
+      <c r="J178" s="37"/>
+      <c r="K178" s="37"/>
     </row>
     <row r="179" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A179" s="13"/>
@@ -4116,8 +4168,8 @@
       <c r="G179" s="15"/>
       <c r="H179" s="13"/>
       <c r="I179" s="13"/>
-      <c r="J179" s="29"/>
-      <c r="K179" s="29"/>
+      <c r="J179" s="37"/>
+      <c r="K179" s="37"/>
     </row>
     <row r="180" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A180" s="13"/>
@@ -4129,8 +4181,8 @@
       <c r="G180" s="15"/>
       <c r="H180" s="13"/>
       <c r="I180" s="13"/>
-      <c r="J180" s="29"/>
-      <c r="K180" s="29"/>
+      <c r="J180" s="37"/>
+      <c r="K180" s="37"/>
     </row>
     <row r="181" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A181" s="13"/>
@@ -4142,8 +4194,8 @@
       <c r="G181" s="15"/>
       <c r="H181" s="13"/>
       <c r="I181" s="13"/>
-      <c r="J181" s="29"/>
-      <c r="K181" s="29"/>
+      <c r="J181" s="37"/>
+      <c r="K181" s="37"/>
     </row>
     <row r="182" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A182" s="13"/>
@@ -4155,8 +4207,8 @@
       <c r="G182" s="15"/>
       <c r="H182" s="13"/>
       <c r="I182" s="13"/>
-      <c r="J182" s="29"/>
-      <c r="K182" s="29"/>
+      <c r="J182" s="37"/>
+      <c r="K182" s="37"/>
     </row>
     <row r="183" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A183" s="13"/>
@@ -4168,8 +4220,8 @@
       <c r="G183" s="15"/>
       <c r="H183" s="13"/>
       <c r="I183" s="13"/>
-      <c r="J183" s="29"/>
-      <c r="K183" s="29"/>
+      <c r="J183" s="37"/>
+      <c r="K183" s="37"/>
     </row>
     <row r="184" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A184" s="13"/>
@@ -4181,8 +4233,8 @@
       <c r="G184" s="15"/>
       <c r="H184" s="13"/>
       <c r="I184" s="13"/>
-      <c r="J184" s="29"/>
-      <c r="K184" s="29"/>
+      <c r="J184" s="37"/>
+      <c r="K184" s="37"/>
     </row>
     <row r="185" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A185" s="13"/>
@@ -4194,8 +4246,8 @@
       <c r="G185" s="15"/>
       <c r="H185" s="13"/>
       <c r="I185" s="13"/>
-      <c r="J185" s="29"/>
-      <c r="K185" s="29"/>
+      <c r="J185" s="37"/>
+      <c r="K185" s="37"/>
     </row>
     <row r="186" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A186" s="13"/>
@@ -4207,8 +4259,8 @@
       <c r="G186" s="15"/>
       <c r="H186" s="13"/>
       <c r="I186" s="13"/>
-      <c r="J186" s="29"/>
-      <c r="K186" s="29"/>
+      <c r="J186" s="37"/>
+      <c r="K186" s="37"/>
     </row>
     <row r="187" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A187" s="13"/>
@@ -4220,8 +4272,8 @@
       <c r="G187" s="15"/>
       <c r="H187" s="13"/>
       <c r="I187" s="13"/>
-      <c r="J187" s="29"/>
-      <c r="K187" s="29"/>
+      <c r="J187" s="37"/>
+      <c r="K187" s="37"/>
     </row>
     <row r="188" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A188" s="13"/>
@@ -4233,8 +4285,8 @@
       <c r="G188" s="15"/>
       <c r="H188" s="13"/>
       <c r="I188" s="13"/>
-      <c r="J188" s="29"/>
-      <c r="K188" s="29"/>
+      <c r="J188" s="37"/>
+      <c r="K188" s="37"/>
     </row>
     <row r="189" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A189" s="13"/>
@@ -4246,8 +4298,8 @@
       <c r="G189" s="15"/>
       <c r="H189" s="13"/>
       <c r="I189" s="13"/>
-      <c r="J189" s="29"/>
-      <c r="K189" s="29"/>
+      <c r="J189" s="37"/>
+      <c r="K189" s="37"/>
     </row>
     <row r="190" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A190" s="13"/>
@@ -4259,8 +4311,8 @@
       <c r="G190" s="15"/>
       <c r="H190" s="13"/>
       <c r="I190" s="13"/>
-      <c r="J190" s="29"/>
-      <c r="K190" s="29"/>
+      <c r="J190" s="37"/>
+      <c r="K190" s="37"/>
     </row>
     <row r="191" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A191" s="13"/>
@@ -4272,8 +4324,8 @@
       <c r="G191" s="15"/>
       <c r="H191" s="13"/>
       <c r="I191" s="13"/>
-      <c r="J191" s="29"/>
-      <c r="K191" s="29"/>
+      <c r="J191" s="37"/>
+      <c r="K191" s="37"/>
     </row>
     <row r="192" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A192" s="13"/>
@@ -4285,8 +4337,8 @@
       <c r="G192" s="15"/>
       <c r="H192" s="13"/>
       <c r="I192" s="13"/>
-      <c r="J192" s="29"/>
-      <c r="K192" s="29"/>
+      <c r="J192" s="37"/>
+      <c r="K192" s="37"/>
     </row>
     <row r="193" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A193" s="13"/>
@@ -4298,8 +4350,8 @@
       <c r="G193" s="15"/>
       <c r="H193" s="13"/>
       <c r="I193" s="13"/>
-      <c r="J193" s="29"/>
-      <c r="K193" s="29"/>
+      <c r="J193" s="37"/>
+      <c r="K193" s="37"/>
     </row>
     <row r="194" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A194" s="13"/>
@@ -4311,8 +4363,8 @@
       <c r="G194" s="15"/>
       <c r="H194" s="13"/>
       <c r="I194" s="13"/>
-      <c r="J194" s="29"/>
-      <c r="K194" s="29"/>
+      <c r="J194" s="37"/>
+      <c r="K194" s="37"/>
     </row>
     <row r="195" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A195" s="13"/>
@@ -4324,8 +4376,8 @@
       <c r="G195" s="15"/>
       <c r="H195" s="13"/>
       <c r="I195" s="13"/>
-      <c r="J195" s="29"/>
-      <c r="K195" s="29"/>
+      <c r="J195" s="37"/>
+      <c r="K195" s="37"/>
     </row>
     <row r="196" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A196" s="13"/>
@@ -4337,8 +4389,8 @@
       <c r="G196" s="15"/>
       <c r="H196" s="13"/>
       <c r="I196" s="13"/>
-      <c r="J196" s="29"/>
-      <c r="K196" s="29"/>
+      <c r="J196" s="37"/>
+      <c r="K196" s="37"/>
     </row>
     <row r="197" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A197" s="13"/>
@@ -4350,8 +4402,8 @@
       <c r="G197" s="15"/>
       <c r="H197" s="13"/>
       <c r="I197" s="13"/>
-      <c r="J197" s="29"/>
-      <c r="K197" s="29"/>
+      <c r="J197" s="37"/>
+      <c r="K197" s="37"/>
     </row>
     <row r="198" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A198" s="13"/>
@@ -4363,8 +4415,8 @@
       <c r="G198" s="15"/>
       <c r="H198" s="13"/>
       <c r="I198" s="13"/>
-      <c r="J198" s="29"/>
-      <c r="K198" s="29"/>
+      <c r="J198" s="37"/>
+      <c r="K198" s="37"/>
     </row>
     <row r="199" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A199" s="13"/>
@@ -4376,8 +4428,8 @@
       <c r="G199" s="15"/>
       <c r="H199" s="13"/>
       <c r="I199" s="13"/>
-      <c r="J199" s="29"/>
-      <c r="K199" s="29"/>
+      <c r="J199" s="37"/>
+      <c r="K199" s="37"/>
     </row>
     <row r="200" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A200" s="13"/>
@@ -4389,8 +4441,8 @@
       <c r="G200" s="15"/>
       <c r="H200" s="13"/>
       <c r="I200" s="13"/>
-      <c r="J200" s="29"/>
-      <c r="K200" s="29"/>
+      <c r="J200" s="37"/>
+      <c r="K200" s="37"/>
     </row>
     <row r="201" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A201" s="13"/>
@@ -4402,8 +4454,8 @@
       <c r="G201" s="15"/>
       <c r="H201" s="13"/>
       <c r="I201" s="13"/>
-      <c r="J201" s="29"/>
-      <c r="K201" s="29"/>
+      <c r="J201" s="37"/>
+      <c r="K201" s="37"/>
     </row>
     <row r="202" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A202" s="13"/>
@@ -4415,8 +4467,8 @@
       <c r="G202" s="15"/>
       <c r="H202" s="13"/>
       <c r="I202" s="13"/>
-      <c r="J202" s="29"/>
-      <c r="K202" s="29"/>
+      <c r="J202" s="37"/>
+      <c r="K202" s="37"/>
     </row>
     <row r="203" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A203" s="13"/>
@@ -4428,8 +4480,8 @@
       <c r="G203" s="15"/>
       <c r="H203" s="13"/>
       <c r="I203" s="13"/>
-      <c r="J203" s="29"/>
-      <c r="K203" s="29"/>
+      <c r="J203" s="37"/>
+      <c r="K203" s="37"/>
     </row>
     <row r="204" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A204" s="13"/>
@@ -4441,8 +4493,8 @@
       <c r="G204" s="15"/>
       <c r="H204" s="13"/>
       <c r="I204" s="13"/>
-      <c r="J204" s="29"/>
-      <c r="K204" s="29"/>
+      <c r="J204" s="37"/>
+      <c r="K204" s="37"/>
     </row>
     <row r="205" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A205" s="13"/>
@@ -4454,8 +4506,8 @@
       <c r="G205" s="15"/>
       <c r="H205" s="13"/>
       <c r="I205" s="13"/>
-      <c r="J205" s="29"/>
-      <c r="K205" s="29"/>
+      <c r="J205" s="37"/>
+      <c r="K205" s="37"/>
     </row>
     <row r="206" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A206" s="13"/>
@@ -4467,8 +4519,8 @@
       <c r="G206" s="15"/>
       <c r="H206" s="13"/>
       <c r="I206" s="13"/>
-      <c r="J206" s="29"/>
-      <c r="K206" s="29"/>
+      <c r="J206" s="37"/>
+      <c r="K206" s="37"/>
     </row>
     <row r="207" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A207" s="13"/>
@@ -4480,8 +4532,8 @@
       <c r="G207" s="15"/>
       <c r="H207" s="13"/>
       <c r="I207" s="13"/>
-      <c r="J207" s="29"/>
-      <c r="K207" s="29"/>
+      <c r="J207" s="37"/>
+      <c r="K207" s="37"/>
     </row>
     <row r="208" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A208" s="13"/>
@@ -4493,8 +4545,8 @@
       <c r="G208" s="15"/>
       <c r="H208" s="13"/>
       <c r="I208" s="13"/>
-      <c r="J208" s="29"/>
-      <c r="K208" s="29"/>
+      <c r="J208" s="37"/>
+      <c r="K208" s="37"/>
     </row>
     <row r="209" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A209" s="13"/>
@@ -4506,8 +4558,8 @@
       <c r="G209" s="15"/>
       <c r="H209" s="13"/>
       <c r="I209" s="13"/>
-      <c r="J209" s="29"/>
-      <c r="K209" s="29"/>
+      <c r="J209" s="37"/>
+      <c r="K209" s="37"/>
     </row>
     <row r="210" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A210" s="13"/>
@@ -4519,8 +4571,8 @@
       <c r="G210" s="15"/>
       <c r="H210" s="13"/>
       <c r="I210" s="13"/>
-      <c r="J210" s="29"/>
-      <c r="K210" s="29"/>
+      <c r="J210" s="37"/>
+      <c r="K210" s="37"/>
     </row>
     <row r="211" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A211" s="13"/>
@@ -4532,8 +4584,8 @@
       <c r="G211" s="15"/>
       <c r="H211" s="13"/>
       <c r="I211" s="13"/>
-      <c r="J211" s="29"/>
-      <c r="K211" s="29"/>
+      <c r="J211" s="37"/>
+      <c r="K211" s="37"/>
     </row>
     <row r="212" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A212" s="13"/>
@@ -4545,8 +4597,8 @@
       <c r="G212" s="15"/>
       <c r="H212" s="13"/>
       <c r="I212" s="13"/>
-      <c r="J212" s="29"/>
-      <c r="K212" s="29"/>
+      <c r="J212" s="37"/>
+      <c r="K212" s="37"/>
     </row>
     <row r="213" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A213" s="13"/>
@@ -4558,8 +4610,8 @@
       <c r="G213" s="15"/>
       <c r="H213" s="13"/>
       <c r="I213" s="13"/>
-      <c r="J213" s="29"/>
-      <c r="K213" s="29"/>
+      <c r="J213" s="37"/>
+      <c r="K213" s="37"/>
     </row>
     <row r="214" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A214" s="13"/>
@@ -4571,8 +4623,8 @@
       <c r="G214" s="15"/>
       <c r="H214" s="13"/>
       <c r="I214" s="13"/>
-      <c r="J214" s="29"/>
-      <c r="K214" s="29"/>
+      <c r="J214" s="37"/>
+      <c r="K214" s="37"/>
     </row>
     <row r="215" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A215" s="13"/>
@@ -4584,8 +4636,8 @@
       <c r="G215" s="15"/>
       <c r="H215" s="13"/>
       <c r="I215" s="13"/>
-      <c r="J215" s="29"/>
-      <c r="K215" s="29"/>
+      <c r="J215" s="37"/>
+      <c r="K215" s="37"/>
     </row>
     <row r="216" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A216" s="13"/>
@@ -4597,8 +4649,8 @@
       <c r="G216" s="15"/>
       <c r="H216" s="13"/>
       <c r="I216" s="13"/>
-      <c r="J216" s="29"/>
-      <c r="K216" s="29"/>
+      <c r="J216" s="37"/>
+      <c r="K216" s="37"/>
     </row>
     <row r="217" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A217" s="13"/>
@@ -4610,8 +4662,8 @@
       <c r="G217" s="15"/>
       <c r="H217" s="13"/>
       <c r="I217" s="13"/>
-      <c r="J217" s="29"/>
-      <c r="K217" s="29"/>
+      <c r="J217" s="37"/>
+      <c r="K217" s="37"/>
     </row>
     <row r="218" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A218" s="13"/>
@@ -4623,8 +4675,8 @@
       <c r="G218" s="15"/>
       <c r="H218" s="13"/>
       <c r="I218" s="13"/>
-      <c r="J218" s="29"/>
-      <c r="K218" s="29"/>
+      <c r="J218" s="37"/>
+      <c r="K218" s="37"/>
     </row>
     <row r="219" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A219" s="13"/>
@@ -4636,8 +4688,8 @@
       <c r="G219" s="15"/>
       <c r="H219" s="13"/>
       <c r="I219" s="13"/>
-      <c r="J219" s="29"/>
-      <c r="K219" s="29"/>
+      <c r="J219" s="37"/>
+      <c r="K219" s="37"/>
     </row>
     <row r="220" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A220" s="13"/>
@@ -4649,8 +4701,8 @@
       <c r="G220" s="15"/>
       <c r="H220" s="13"/>
       <c r="I220" s="13"/>
-      <c r="J220" s="29"/>
-      <c r="K220" s="29"/>
+      <c r="J220" s="37"/>
+      <c r="K220" s="37"/>
     </row>
     <row r="221" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A221" s="13"/>
@@ -4662,8 +4714,8 @@
       <c r="G221" s="15"/>
       <c r="H221" s="13"/>
       <c r="I221" s="13"/>
-      <c r="J221" s="29"/>
-      <c r="K221" s="29"/>
+      <c r="J221" s="37"/>
+      <c r="K221" s="37"/>
     </row>
     <row r="222" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A222" s="13"/>
@@ -4675,8 +4727,8 @@
       <c r="G222" s="15"/>
       <c r="H222" s="13"/>
       <c r="I222" s="13"/>
-      <c r="J222" s="29"/>
-      <c r="K222" s="29"/>
+      <c r="J222" s="37"/>
+      <c r="K222" s="37"/>
     </row>
     <row r="223" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A223" s="13"/>
@@ -4688,8 +4740,8 @@
       <c r="G223" s="15"/>
       <c r="H223" s="13"/>
       <c r="I223" s="13"/>
-      <c r="J223" s="29"/>
-      <c r="K223" s="29"/>
+      <c r="J223" s="37"/>
+      <c r="K223" s="37"/>
     </row>
     <row r="224" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A224" s="13"/>
@@ -4701,8 +4753,8 @@
       <c r="G224" s="15"/>
       <c r="H224" s="13"/>
       <c r="I224" s="13"/>
-      <c r="J224" s="29"/>
-      <c r="K224" s="29"/>
+      <c r="J224" s="37"/>
+      <c r="K224" s="37"/>
     </row>
     <row r="225" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A225" s="13"/>
@@ -4714,8 +4766,8 @@
       <c r="G225" s="15"/>
       <c r="H225" s="13"/>
       <c r="I225" s="13"/>
-      <c r="J225" s="29"/>
-      <c r="K225" s="29"/>
+      <c r="J225" s="37"/>
+      <c r="K225" s="37"/>
     </row>
     <row r="226" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A226" s="13"/>
@@ -4727,8 +4779,8 @@
       <c r="G226" s="15"/>
       <c r="H226" s="13"/>
       <c r="I226" s="13"/>
-      <c r="J226" s="29"/>
-      <c r="K226" s="29"/>
+      <c r="J226" s="37"/>
+      <c r="K226" s="37"/>
     </row>
     <row r="227" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A227" s="13"/>
@@ -4740,8 +4792,8 @@
       <c r="G227" s="15"/>
       <c r="H227" s="13"/>
       <c r="I227" s="13"/>
-      <c r="J227" s="29"/>
-      <c r="K227" s="29"/>
+      <c r="J227" s="37"/>
+      <c r="K227" s="37"/>
     </row>
     <row r="228" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A228" s="13"/>
@@ -4753,8 +4805,8 @@
       <c r="G228" s="15"/>
       <c r="H228" s="13"/>
       <c r="I228" s="13"/>
-      <c r="J228" s="29"/>
-      <c r="K228" s="29"/>
+      <c r="J228" s="37"/>
+      <c r="K228" s="37"/>
     </row>
     <row r="229" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A229" s="13"/>
@@ -4766,8 +4818,8 @@
       <c r="G229" s="15"/>
       <c r="H229" s="13"/>
       <c r="I229" s="13"/>
-      <c r="J229" s="29"/>
-      <c r="K229" s="29"/>
+      <c r="J229" s="37"/>
+      <c r="K229" s="37"/>
     </row>
     <row r="230" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A230" s="13"/>
@@ -4779,8 +4831,8 @@
       <c r="G230" s="15"/>
       <c r="H230" s="13"/>
       <c r="I230" s="13"/>
-      <c r="J230" s="29"/>
-      <c r="K230" s="29"/>
+      <c r="J230" s="37"/>
+      <c r="K230" s="37"/>
     </row>
     <row r="231" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="G231" s="2"/>
@@ -6809,20 +6861,254 @@
     </row>
   </sheetData>
   <mergeCells count="286">
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="A59:K59"/>
+    <mergeCell ref="J229:K229"/>
+    <mergeCell ref="J230:K230"/>
+    <mergeCell ref="J220:K220"/>
+    <mergeCell ref="J221:K221"/>
+    <mergeCell ref="J222:K222"/>
+    <mergeCell ref="J223:K223"/>
+    <mergeCell ref="J224:K224"/>
+    <mergeCell ref="J225:K225"/>
+    <mergeCell ref="J226:K226"/>
+    <mergeCell ref="J227:K227"/>
+    <mergeCell ref="J228:K228"/>
+    <mergeCell ref="J211:K211"/>
+    <mergeCell ref="J212:K212"/>
+    <mergeCell ref="J213:K213"/>
+    <mergeCell ref="J214:K214"/>
+    <mergeCell ref="J215:K215"/>
+    <mergeCell ref="J216:K216"/>
+    <mergeCell ref="J217:K217"/>
+    <mergeCell ref="J218:K218"/>
+    <mergeCell ref="J219:K219"/>
+    <mergeCell ref="J202:K202"/>
+    <mergeCell ref="J203:K203"/>
+    <mergeCell ref="J204:K204"/>
+    <mergeCell ref="J205:K205"/>
+    <mergeCell ref="J206:K206"/>
+    <mergeCell ref="J207:K207"/>
+    <mergeCell ref="J208:K208"/>
+    <mergeCell ref="J209:K209"/>
+    <mergeCell ref="J210:K210"/>
+    <mergeCell ref="J193:K193"/>
+    <mergeCell ref="J194:K194"/>
+    <mergeCell ref="J195:K195"/>
+    <mergeCell ref="J196:K196"/>
+    <mergeCell ref="J197:K197"/>
+    <mergeCell ref="J198:K198"/>
+    <mergeCell ref="J199:K199"/>
+    <mergeCell ref="J200:K200"/>
+    <mergeCell ref="J201:K201"/>
+    <mergeCell ref="J184:K184"/>
+    <mergeCell ref="J185:K185"/>
+    <mergeCell ref="J186:K186"/>
+    <mergeCell ref="J187:K187"/>
+    <mergeCell ref="J188:K188"/>
+    <mergeCell ref="J189:K189"/>
+    <mergeCell ref="J190:K190"/>
+    <mergeCell ref="J191:K191"/>
+    <mergeCell ref="J192:K192"/>
+    <mergeCell ref="J175:K175"/>
+    <mergeCell ref="J176:K176"/>
+    <mergeCell ref="J177:K177"/>
+    <mergeCell ref="J178:K178"/>
+    <mergeCell ref="J179:K179"/>
+    <mergeCell ref="J180:K180"/>
+    <mergeCell ref="J181:K181"/>
+    <mergeCell ref="J182:K182"/>
+    <mergeCell ref="J183:K183"/>
+    <mergeCell ref="J166:K166"/>
+    <mergeCell ref="J167:K167"/>
+    <mergeCell ref="J168:K168"/>
+    <mergeCell ref="J169:K169"/>
+    <mergeCell ref="J170:K170"/>
+    <mergeCell ref="J171:K171"/>
+    <mergeCell ref="J172:K172"/>
+    <mergeCell ref="J173:K173"/>
+    <mergeCell ref="J174:K174"/>
+    <mergeCell ref="J157:K157"/>
+    <mergeCell ref="J158:K158"/>
+    <mergeCell ref="J159:K159"/>
+    <mergeCell ref="J160:K160"/>
+    <mergeCell ref="J161:K161"/>
+    <mergeCell ref="J162:K162"/>
+    <mergeCell ref="J163:K163"/>
+    <mergeCell ref="J164:K164"/>
+    <mergeCell ref="J165:K165"/>
+    <mergeCell ref="J148:K148"/>
+    <mergeCell ref="J149:K149"/>
+    <mergeCell ref="J150:K150"/>
+    <mergeCell ref="J151:K151"/>
+    <mergeCell ref="J152:K152"/>
+    <mergeCell ref="J153:K153"/>
+    <mergeCell ref="J154:K154"/>
+    <mergeCell ref="J155:K155"/>
+    <mergeCell ref="J156:K156"/>
+    <mergeCell ref="J139:K139"/>
+    <mergeCell ref="J140:K140"/>
+    <mergeCell ref="J141:K141"/>
+    <mergeCell ref="J142:K142"/>
+    <mergeCell ref="J143:K143"/>
+    <mergeCell ref="J144:K144"/>
+    <mergeCell ref="J145:K145"/>
+    <mergeCell ref="J146:K146"/>
+    <mergeCell ref="J147:K147"/>
+    <mergeCell ref="J130:K130"/>
+    <mergeCell ref="J131:K131"/>
+    <mergeCell ref="J132:K132"/>
+    <mergeCell ref="J133:K133"/>
+    <mergeCell ref="J134:K134"/>
+    <mergeCell ref="J135:K135"/>
+    <mergeCell ref="J136:K136"/>
+    <mergeCell ref="J137:K137"/>
+    <mergeCell ref="J138:K138"/>
+    <mergeCell ref="J121:K121"/>
+    <mergeCell ref="J122:K122"/>
+    <mergeCell ref="J123:K123"/>
+    <mergeCell ref="J124:K124"/>
+    <mergeCell ref="J125:K125"/>
+    <mergeCell ref="J126:K126"/>
+    <mergeCell ref="J127:K127"/>
+    <mergeCell ref="J128:K128"/>
+    <mergeCell ref="J129:K129"/>
+    <mergeCell ref="J112:K112"/>
+    <mergeCell ref="J113:K113"/>
+    <mergeCell ref="J114:K114"/>
+    <mergeCell ref="J115:K115"/>
+    <mergeCell ref="J116:K116"/>
+    <mergeCell ref="J117:K117"/>
+    <mergeCell ref="J118:K118"/>
+    <mergeCell ref="J119:K119"/>
+    <mergeCell ref="J120:K120"/>
+    <mergeCell ref="J103:K103"/>
+    <mergeCell ref="J104:K104"/>
+    <mergeCell ref="J105:K105"/>
+    <mergeCell ref="J106:K106"/>
+    <mergeCell ref="J107:K107"/>
+    <mergeCell ref="J108:K108"/>
+    <mergeCell ref="J109:K109"/>
+    <mergeCell ref="J110:K110"/>
+    <mergeCell ref="J111:K111"/>
+    <mergeCell ref="J94:K94"/>
+    <mergeCell ref="J95:K95"/>
+    <mergeCell ref="J96:K96"/>
+    <mergeCell ref="J97:K97"/>
+    <mergeCell ref="J98:K98"/>
+    <mergeCell ref="J99:K99"/>
+    <mergeCell ref="J100:K100"/>
+    <mergeCell ref="J101:K101"/>
+    <mergeCell ref="J102:K102"/>
+    <mergeCell ref="J87:K87"/>
+    <mergeCell ref="J88:K88"/>
+    <mergeCell ref="J72:K72"/>
+    <mergeCell ref="J73:K73"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="J74:K74"/>
+    <mergeCell ref="J75:K75"/>
+    <mergeCell ref="J76:K76"/>
+    <mergeCell ref="J77:K77"/>
+    <mergeCell ref="J78:K78"/>
+    <mergeCell ref="J79:K79"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="J55:K55"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="J60:K60"/>
+    <mergeCell ref="J61:K61"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J89:K89"/>
+    <mergeCell ref="J90:K90"/>
+    <mergeCell ref="J91:K91"/>
+    <mergeCell ref="J92:K92"/>
+    <mergeCell ref="J93:K93"/>
+    <mergeCell ref="J63:K63"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J71:K71"/>
+    <mergeCell ref="J80:K80"/>
+    <mergeCell ref="J81:K81"/>
+    <mergeCell ref="J82:K82"/>
+    <mergeCell ref="J83:K83"/>
+    <mergeCell ref="J84:K84"/>
+    <mergeCell ref="J85:K85"/>
+    <mergeCell ref="J86:K86"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="J52:K52"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="A20:K20"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="A27:K27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
     <mergeCell ref="H35:I35"/>
     <mergeCell ref="H36:I36"/>
     <mergeCell ref="H37:I37"/>
@@ -6847,254 +7133,20 @@
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A20:K20"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="J51:K51"/>
-    <mergeCell ref="J52:K52"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="A27:K27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J89:K89"/>
-    <mergeCell ref="J90:K90"/>
-    <mergeCell ref="J91:K91"/>
-    <mergeCell ref="J92:K92"/>
-    <mergeCell ref="J93:K93"/>
-    <mergeCell ref="J63:K63"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J67:K67"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="J71:K71"/>
-    <mergeCell ref="J80:K80"/>
-    <mergeCell ref="J81:K81"/>
-    <mergeCell ref="J82:K82"/>
-    <mergeCell ref="J83:K83"/>
-    <mergeCell ref="J84:K84"/>
-    <mergeCell ref="J85:K85"/>
-    <mergeCell ref="J86:K86"/>
-    <mergeCell ref="J87:K87"/>
-    <mergeCell ref="J88:K88"/>
-    <mergeCell ref="J72:K72"/>
-    <mergeCell ref="J73:K73"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="J74:K74"/>
-    <mergeCell ref="J75:K75"/>
-    <mergeCell ref="J76:K76"/>
-    <mergeCell ref="J77:K77"/>
-    <mergeCell ref="J78:K78"/>
-    <mergeCell ref="J79:K79"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="J55:K55"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="J60:K60"/>
-    <mergeCell ref="J61:K61"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J94:K94"/>
-    <mergeCell ref="J95:K95"/>
-    <mergeCell ref="J96:K96"/>
-    <mergeCell ref="J97:K97"/>
-    <mergeCell ref="J98:K98"/>
-    <mergeCell ref="J99:K99"/>
-    <mergeCell ref="J100:K100"/>
-    <mergeCell ref="J101:K101"/>
-    <mergeCell ref="J102:K102"/>
-    <mergeCell ref="J103:K103"/>
-    <mergeCell ref="J104:K104"/>
-    <mergeCell ref="J105:K105"/>
-    <mergeCell ref="J106:K106"/>
-    <mergeCell ref="J107:K107"/>
-    <mergeCell ref="J108:K108"/>
-    <mergeCell ref="J109:K109"/>
-    <mergeCell ref="J110:K110"/>
-    <mergeCell ref="J111:K111"/>
-    <mergeCell ref="J112:K112"/>
-    <mergeCell ref="J113:K113"/>
-    <mergeCell ref="J114:K114"/>
-    <mergeCell ref="J115:K115"/>
-    <mergeCell ref="J116:K116"/>
-    <mergeCell ref="J117:K117"/>
-    <mergeCell ref="J118:K118"/>
-    <mergeCell ref="J119:K119"/>
-    <mergeCell ref="J120:K120"/>
-    <mergeCell ref="J121:K121"/>
-    <mergeCell ref="J122:K122"/>
-    <mergeCell ref="J123:K123"/>
-    <mergeCell ref="J124:K124"/>
-    <mergeCell ref="J125:K125"/>
-    <mergeCell ref="J126:K126"/>
-    <mergeCell ref="J127:K127"/>
-    <mergeCell ref="J128:K128"/>
-    <mergeCell ref="J129:K129"/>
-    <mergeCell ref="J130:K130"/>
-    <mergeCell ref="J131:K131"/>
-    <mergeCell ref="J132:K132"/>
-    <mergeCell ref="J133:K133"/>
-    <mergeCell ref="J134:K134"/>
-    <mergeCell ref="J135:K135"/>
-    <mergeCell ref="J136:K136"/>
-    <mergeCell ref="J137:K137"/>
-    <mergeCell ref="J138:K138"/>
-    <mergeCell ref="J139:K139"/>
-    <mergeCell ref="J140:K140"/>
-    <mergeCell ref="J141:K141"/>
-    <mergeCell ref="J142:K142"/>
-    <mergeCell ref="J143:K143"/>
-    <mergeCell ref="J144:K144"/>
-    <mergeCell ref="J145:K145"/>
-    <mergeCell ref="J146:K146"/>
-    <mergeCell ref="J147:K147"/>
-    <mergeCell ref="J148:K148"/>
-    <mergeCell ref="J149:K149"/>
-    <mergeCell ref="J150:K150"/>
-    <mergeCell ref="J151:K151"/>
-    <mergeCell ref="J152:K152"/>
-    <mergeCell ref="J153:K153"/>
-    <mergeCell ref="J154:K154"/>
-    <mergeCell ref="J155:K155"/>
-    <mergeCell ref="J156:K156"/>
-    <mergeCell ref="J157:K157"/>
-    <mergeCell ref="J158:K158"/>
-    <mergeCell ref="J159:K159"/>
-    <mergeCell ref="J160:K160"/>
-    <mergeCell ref="J161:K161"/>
-    <mergeCell ref="J162:K162"/>
-    <mergeCell ref="J163:K163"/>
-    <mergeCell ref="J164:K164"/>
-    <mergeCell ref="J165:K165"/>
-    <mergeCell ref="J166:K166"/>
-    <mergeCell ref="J167:K167"/>
-    <mergeCell ref="J168:K168"/>
-    <mergeCell ref="J169:K169"/>
-    <mergeCell ref="J170:K170"/>
-    <mergeCell ref="J171:K171"/>
-    <mergeCell ref="J172:K172"/>
-    <mergeCell ref="J173:K173"/>
-    <mergeCell ref="J174:K174"/>
-    <mergeCell ref="J175:K175"/>
-    <mergeCell ref="J176:K176"/>
-    <mergeCell ref="J177:K177"/>
-    <mergeCell ref="J178:K178"/>
-    <mergeCell ref="J179:K179"/>
-    <mergeCell ref="J180:K180"/>
-    <mergeCell ref="J181:K181"/>
-    <mergeCell ref="J182:K182"/>
-    <mergeCell ref="J183:K183"/>
-    <mergeCell ref="J184:K184"/>
-    <mergeCell ref="J185:K185"/>
-    <mergeCell ref="J186:K186"/>
-    <mergeCell ref="J187:K187"/>
-    <mergeCell ref="J188:K188"/>
-    <mergeCell ref="J189:K189"/>
-    <mergeCell ref="J190:K190"/>
-    <mergeCell ref="J191:K191"/>
-    <mergeCell ref="J192:K192"/>
-    <mergeCell ref="J193:K193"/>
-    <mergeCell ref="J194:K194"/>
-    <mergeCell ref="J195:K195"/>
-    <mergeCell ref="J196:K196"/>
-    <mergeCell ref="J197:K197"/>
-    <mergeCell ref="J198:K198"/>
-    <mergeCell ref="J199:K199"/>
-    <mergeCell ref="J200:K200"/>
-    <mergeCell ref="J201:K201"/>
-    <mergeCell ref="J202:K202"/>
-    <mergeCell ref="J203:K203"/>
-    <mergeCell ref="J204:K204"/>
-    <mergeCell ref="J205:K205"/>
-    <mergeCell ref="J206:K206"/>
-    <mergeCell ref="J207:K207"/>
-    <mergeCell ref="J208:K208"/>
-    <mergeCell ref="J209:K209"/>
-    <mergeCell ref="J210:K210"/>
-    <mergeCell ref="J211:K211"/>
-    <mergeCell ref="J212:K212"/>
-    <mergeCell ref="J213:K213"/>
-    <mergeCell ref="J214:K214"/>
-    <mergeCell ref="J215:K215"/>
-    <mergeCell ref="J216:K216"/>
-    <mergeCell ref="J217:K217"/>
-    <mergeCell ref="J218:K218"/>
-    <mergeCell ref="J219:K219"/>
-    <mergeCell ref="J229:K229"/>
-    <mergeCell ref="J230:K230"/>
-    <mergeCell ref="J220:K220"/>
-    <mergeCell ref="J221:K221"/>
-    <mergeCell ref="J222:K222"/>
-    <mergeCell ref="J223:K223"/>
-    <mergeCell ref="J224:K224"/>
-    <mergeCell ref="J225:K225"/>
-    <mergeCell ref="J226:K226"/>
-    <mergeCell ref="J227:K227"/>
-    <mergeCell ref="J228:K228"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="A59:K59"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Doc: Added Review for cart and order history Wireframes
</commit_message>
<xml_diff>
--- a/Requirments/Review.xlsx
+++ b/Requirments/Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Requirments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA0AC72-5361-4672-9488-4F4F9662C3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CD1ED2-2FF2-4874-B4D5-3628277262C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="161">
   <si>
     <t>ID</t>
   </si>
@@ -487,6 +487,25 @@
   </si>
   <si>
     <t>Review_TC_Client_001</t>
+  </si>
+  <si>
+    <t>Review_WF_OrderHistory_001</t>
+  </si>
+  <si>
+    <t>c6f01a322014a391cd5f759d3365a7b7b0cbe67a</t>
+  </si>
+  <si>
+    <t>Wireframe_OrderHistory_001  
+Wireframe_OrderHistory_002</t>
+  </si>
+  <si>
+    <t>Review_WF_ShoppingCart_001</t>
+  </si>
+  <si>
+    <t>what is the message that should be shown when the item deleted from the cart</t>
+  </si>
+  <si>
+    <t>Wireframe_Cart_005</t>
   </si>
 </sst>
 </file>
@@ -718,7 +737,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -774,21 +793,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -797,23 +810,28 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1039,13 +1057,13 @@
   </sheetPr>
   <dimension ref="A1:AC906"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="M65" sqref="M65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="36" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" customWidth="1"/>
@@ -1079,14 +1097,14 @@
       <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="45" t="s">
+      <c r="I1" s="37"/>
+      <c r="J1" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="K1" s="46"/>
+      <c r="K1" s="37"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -1107,19 +1125,19 @@
       <c r="AC1" s="1"/>
     </row>
     <row r="2" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -1161,12 +1179,12 @@
       <c r="G3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="43"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="31" t="s">
+      <c r="H3" s="40"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K3" s="31"/>
+      <c r="K3" s="38"/>
     </row>
     <row r="4" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
@@ -1190,12 +1208,12 @@
       <c r="G4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="31" t="s">
+      <c r="H4" s="40"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K4" s="31"/>
+      <c r="K4" s="38"/>
     </row>
     <row r="5" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
@@ -1219,12 +1237,12 @@
       <c r="G5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="43"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="31" t="s">
+      <c r="H5" s="40"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K5" s="31"/>
+      <c r="K5" s="38"/>
     </row>
     <row r="6" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
@@ -1248,12 +1266,12 @@
       <c r="G6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="43"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="31" t="s">
+      <c r="H6" s="40"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K6" s="31"/>
+      <c r="K6" s="38"/>
     </row>
     <row r="7" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -1277,12 +1295,12 @@
       <c r="G7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="43"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="31" t="s">
+      <c r="H7" s="40"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K7" s="31"/>
+      <c r="K7" s="38"/>
     </row>
     <row r="8" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
@@ -1306,12 +1324,12 @@
       <c r="G8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="43"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="31" t="s">
+      <c r="H8" s="40"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K8" s="31"/>
+      <c r="K8" s="38"/>
     </row>
     <row r="9" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
@@ -1335,12 +1353,12 @@
       <c r="G9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="43"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="31" t="s">
+      <c r="H9" s="40"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K9" s="31"/>
+      <c r="K9" s="38"/>
     </row>
     <row r="10" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
@@ -1364,12 +1382,12 @@
       <c r="G10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="43"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="31" t="s">
+      <c r="H10" s="40"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K10" s="31"/>
+      <c r="K10" s="38"/>
     </row>
     <row r="11" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
@@ -1393,12 +1411,12 @@
       <c r="G11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="43"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="31" t="s">
+      <c r="H11" s="40"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K11" s="31"/>
+      <c r="K11" s="38"/>
     </row>
     <row r="12" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
@@ -1422,12 +1440,12 @@
       <c r="G12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="43"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="31" t="s">
+      <c r="H12" s="40"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K12" s="31"/>
+      <c r="K12" s="38"/>
     </row>
     <row r="13" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
@@ -1451,12 +1469,12 @@
       <c r="G13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="43"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="31" t="s">
+      <c r="H13" s="40"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K13" s="31"/>
+      <c r="K13" s="38"/>
     </row>
     <row r="14" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
@@ -1480,12 +1498,12 @@
       <c r="G14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="43"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="31" t="s">
+      <c r="H14" s="40"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K14" s="31"/>
+      <c r="K14" s="38"/>
     </row>
     <row r="15" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
@@ -1507,12 +1525,12 @@
       <c r="G15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="43"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="31" t="s">
+      <c r="H15" s="40"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="31"/>
+      <c r="K15" s="38"/>
     </row>
     <row r="16" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
@@ -1536,12 +1554,12 @@
       <c r="G16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="43"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="31" t="s">
+      <c r="H16" s="40"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K16" s="31"/>
+      <c r="K16" s="38"/>
     </row>
     <row r="17" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
@@ -1565,12 +1583,12 @@
       <c r="G17" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="43"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="31" t="s">
+      <c r="H17" s="40"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="31"/>
+      <c r="K17" s="38"/>
     </row>
     <row r="18" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
@@ -1594,12 +1612,12 @@
       <c r="G18" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="43"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="31" t="s">
+      <c r="H18" s="40"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="31"/>
+      <c r="K18" s="38"/>
     </row>
     <row r="19" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
@@ -1623,27 +1641,27 @@
       <c r="G19" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="43"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="31" t="s">
+      <c r="H19" s="40"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K19" s="31"/>
+      <c r="K19" s="38"/>
     </row>
     <row r="20" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="39"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="35"/>
     </row>
     <row r="21" spans="1:11" s="16" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
@@ -1667,14 +1685,14 @@
       <c r="G21" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H21" s="40" t="s">
+      <c r="H21" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I21" s="36"/>
-      <c r="J21" s="31" t="s">
+      <c r="I21" s="31"/>
+      <c r="J21" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="K21" s="31"/>
+      <c r="K21" s="38"/>
     </row>
     <row r="22" spans="1:11" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
@@ -1698,12 +1716,12 @@
       <c r="G22" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="35"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="31" t="s">
+      <c r="H22" s="32"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="K22" s="31"/>
+      <c r="K22" s="38"/>
     </row>
     <row r="23" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
@@ -1727,14 +1745,14 @@
       <c r="G23" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="35" t="s">
+      <c r="H23" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="I23" s="36"/>
-      <c r="J23" s="31" t="s">
+      <c r="I23" s="31"/>
+      <c r="J23" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="K23" s="31"/>
+      <c r="K23" s="38"/>
     </row>
     <row r="24" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
@@ -1762,10 +1780,10 @@
         <v>74</v>
       </c>
       <c r="I24" s="25"/>
-      <c r="J24" s="31" t="s">
+      <c r="J24" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="K24" s="31"/>
+      <c r="K24" s="38"/>
     </row>
     <row r="25" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
@@ -1789,14 +1807,14 @@
       <c r="G25" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="35" t="s">
+      <c r="H25" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="I25" s="36"/>
-      <c r="J25" s="31" t="s">
+      <c r="I25" s="31"/>
+      <c r="J25" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="K25" s="31"/>
+      <c r="K25" s="38"/>
     </row>
     <row r="26" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
@@ -1820,27 +1838,27 @@
       <c r="G26" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H26" s="35"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="31" t="s">
+      <c r="H26" s="32"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="K26" s="31"/>
+      <c r="K26" s="38"/>
     </row>
     <row r="27" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="39"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="35"/>
     </row>
     <row r="28" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
@@ -1864,12 +1882,12 @@
       <c r="G28" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H28" s="41"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="41" t="s">
+      <c r="H28" s="43"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="K28" s="42"/>
+      <c r="K28" s="44"/>
     </row>
     <row r="29" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
@@ -1893,14 +1911,14 @@
       <c r="G29" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="35" t="s">
+      <c r="H29" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="I29" s="36"/>
-      <c r="J29" s="34" t="s">
+      <c r="I29" s="31"/>
+      <c r="J29" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="K29" s="31"/>
+      <c r="K29" s="38"/>
     </row>
     <row r="30" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
@@ -1924,12 +1942,12 @@
       <c r="G30" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H30" s="35"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="31" t="s">
+      <c r="H30" s="32"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="K30" s="31"/>
+      <c r="K30" s="38"/>
     </row>
     <row r="31" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
@@ -1955,10 +1973,10 @@
       </c>
       <c r="H31" s="24"/>
       <c r="I31" s="25"/>
-      <c r="J31" s="48" t="s">
+      <c r="J31" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="K31" s="42"/>
+      <c r="K31" s="44"/>
     </row>
     <row r="32" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
@@ -1982,27 +2000,27 @@
       <c r="G32" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H32" s="35"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="31" t="s">
+      <c r="H32" s="32"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="K32" s="31"/>
+      <c r="K32" s="38"/>
     </row>
     <row r="33" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="38"/>
-      <c r="J33" s="38"/>
-      <c r="K33" s="39"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="35"/>
     </row>
     <row r="34" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
@@ -2026,12 +2044,12 @@
       <c r="G34" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H34" s="35"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="34" t="s">
+      <c r="H34" s="32"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K34" s="31"/>
+      <c r="K34" s="38"/>
     </row>
     <row r="35" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
@@ -2055,8 +2073,8 @@
       <c r="G35" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H35" s="35"/>
-      <c r="I35" s="36"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="31"/>
       <c r="J35" s="28" t="s">
         <v>94</v>
       </c>
@@ -2083,12 +2101,12 @@
       <c r="G36" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H36" s="35"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="34" t="s">
+      <c r="H36" s="32"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K36" s="31"/>
+      <c r="K36" s="38"/>
     </row>
     <row r="37" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
@@ -2112,12 +2130,12 @@
       <c r="G37" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H37" s="35"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="34" t="s">
+      <c r="H37" s="32"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K37" s="31"/>
+      <c r="K37" s="38"/>
     </row>
     <row r="38" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
@@ -2141,12 +2159,12 @@
       <c r="G38" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H38" s="35"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="34" t="s">
+      <c r="H38" s="32"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K38" s="31"/>
+      <c r="K38" s="38"/>
     </row>
     <row r="39" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
@@ -2170,12 +2188,12 @@
       <c r="G39" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H39" s="35"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="34" t="s">
+      <c r="H39" s="32"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K39" s="31"/>
+      <c r="K39" s="38"/>
     </row>
     <row r="40" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
@@ -2199,12 +2217,12 @@
       <c r="G40" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H40" s="35"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="34" t="s">
+      <c r="H40" s="32"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K40" s="31"/>
+      <c r="K40" s="38"/>
     </row>
     <row r="41" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
@@ -2228,12 +2246,12 @@
       <c r="G41" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H41" s="35"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="34" t="s">
+      <c r="H41" s="32"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K41" s="31"/>
+      <c r="K41" s="38"/>
     </row>
     <row r="42" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
@@ -2257,12 +2275,12 @@
       <c r="G42" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H42" s="35"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="34" t="s">
+      <c r="H42" s="32"/>
+      <c r="I42" s="31"/>
+      <c r="J42" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K42" s="31"/>
+      <c r="K42" s="38"/>
     </row>
     <row r="43" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
@@ -2286,12 +2304,12 @@
       <c r="G43" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H43" s="35"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="34" t="s">
+      <c r="H43" s="32"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K43" s="31"/>
+      <c r="K43" s="38"/>
     </row>
     <row r="44" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
@@ -2315,12 +2333,12 @@
       <c r="G44" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H44" s="35"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="34" t="s">
+      <c r="H44" s="32"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K44" s="31"/>
+      <c r="K44" s="38"/>
     </row>
     <row r="45" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
@@ -2344,12 +2362,12 @@
       <c r="G45" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H45" s="35"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="34" t="s">
+      <c r="H45" s="32"/>
+      <c r="I45" s="31"/>
+      <c r="J45" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K45" s="31"/>
+      <c r="K45" s="38"/>
     </row>
     <row r="46" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
@@ -2373,12 +2391,12 @@
       <c r="G46" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H46" s="35"/>
-      <c r="I46" s="36"/>
-      <c r="J46" s="34" t="s">
+      <c r="H46" s="32"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K46" s="31"/>
+      <c r="K46" s="38"/>
     </row>
     <row r="47" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
@@ -2402,12 +2420,12 @@
       <c r="G47" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H47" s="35"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="34" t="s">
+      <c r="H47" s="32"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K47" s="31"/>
+      <c r="K47" s="38"/>
     </row>
     <row r="48" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
@@ -2431,12 +2449,12 @@
       <c r="G48" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H48" s="35"/>
-      <c r="I48" s="36"/>
-      <c r="J48" s="34" t="s">
+      <c r="H48" s="32"/>
+      <c r="I48" s="31"/>
+      <c r="J48" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="K48" s="31"/>
+      <c r="K48" s="38"/>
     </row>
     <row r="49" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
@@ -2460,12 +2478,12 @@
       <c r="G49" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H49" s="35"/>
-      <c r="I49" s="36"/>
-      <c r="J49" s="31" t="s">
+      <c r="H49" s="32"/>
+      <c r="I49" s="31"/>
+      <c r="J49" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="K49" s="31"/>
+      <c r="K49" s="38"/>
     </row>
     <row r="50" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
@@ -2487,12 +2505,12 @@
       <c r="G50" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H50" s="35"/>
-      <c r="I50" s="36"/>
-      <c r="J50" s="31" t="s">
+      <c r="H50" s="32"/>
+      <c r="I50" s="31"/>
+      <c r="J50" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="K50" s="31"/>
+      <c r="K50" s="38"/>
     </row>
     <row r="51" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
@@ -2514,12 +2532,12 @@
       <c r="G51" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H51" s="35"/>
-      <c r="I51" s="36"/>
-      <c r="J51" s="31" t="s">
+      <c r="H51" s="32"/>
+      <c r="I51" s="31"/>
+      <c r="J51" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="K51" s="31"/>
+      <c r="K51" s="38"/>
     </row>
     <row r="52" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A52" s="13"/>
@@ -2529,10 +2547,10 @@
       <c r="E52" s="13"/>
       <c r="F52" s="13"/>
       <c r="G52" s="15"/>
-      <c r="H52" s="35"/>
-      <c r="I52" s="36"/>
-      <c r="J52" s="31"/>
-      <c r="K52" s="31"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="31"/>
+      <c r="J52" s="38"/>
+      <c r="K52" s="38"/>
     </row>
     <row r="53" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A53" s="13"/>
@@ -2542,10 +2560,10 @@
       <c r="E53" s="13"/>
       <c r="F53" s="13"/>
       <c r="G53" s="15"/>
-      <c r="H53" s="35"/>
-      <c r="I53" s="36"/>
-      <c r="J53" s="31"/>
-      <c r="K53" s="31"/>
+      <c r="H53" s="32"/>
+      <c r="I53" s="31"/>
+      <c r="J53" s="38"/>
+      <c r="K53" s="38"/>
     </row>
     <row r="54" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A54" s="13"/>
@@ -2555,10 +2573,10 @@
       <c r="E54" s="13"/>
       <c r="F54" s="13"/>
       <c r="G54" s="15"/>
-      <c r="H54" s="35"/>
-      <c r="I54" s="36"/>
-      <c r="J54" s="31"/>
-      <c r="K54" s="31"/>
+      <c r="H54" s="32"/>
+      <c r="I54" s="31"/>
+      <c r="J54" s="38"/>
+      <c r="K54" s="38"/>
     </row>
     <row r="55" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A55" s="13"/>
@@ -2568,10 +2586,10 @@
       <c r="E55" s="13"/>
       <c r="F55" s="13"/>
       <c r="G55" s="15"/>
-      <c r="H55" s="35"/>
-      <c r="I55" s="36"/>
-      <c r="J55" s="31"/>
-      <c r="K55" s="31"/>
+      <c r="H55" s="32"/>
+      <c r="I55" s="31"/>
+      <c r="J55" s="38"/>
+      <c r="K55" s="38"/>
     </row>
     <row r="56" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A56" s="13"/>
@@ -2581,10 +2599,10 @@
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
       <c r="G56" s="15"/>
-      <c r="H56" s="35"/>
-      <c r="I56" s="36"/>
-      <c r="J56" s="31"/>
-      <c r="K56" s="31"/>
+      <c r="H56" s="32"/>
+      <c r="I56" s="31"/>
+      <c r="J56" s="38"/>
+      <c r="K56" s="38"/>
     </row>
     <row r="57" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A57" s="13"/>
@@ -2594,10 +2612,10 @@
       <c r="E57" s="13"/>
       <c r="F57" s="13"/>
       <c r="G57" s="15"/>
-      <c r="H57" s="35"/>
-      <c r="I57" s="36"/>
-      <c r="J57" s="31"/>
-      <c r="K57" s="31"/>
+      <c r="H57" s="32"/>
+      <c r="I57" s="31"/>
+      <c r="J57" s="38"/>
+      <c r="K57" s="38"/>
     </row>
     <row r="58" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A58" s="13"/>
@@ -2607,10 +2625,10 @@
       <c r="E58" s="13"/>
       <c r="F58" s="13"/>
       <c r="G58" s="15"/>
-      <c r="H58" s="35"/>
-      <c r="I58" s="36"/>
-      <c r="J58" s="31"/>
-      <c r="K58" s="31"/>
+      <c r="H58" s="32"/>
+      <c r="I58" s="31"/>
+      <c r="J58" s="38"/>
+      <c r="K58" s="38"/>
     </row>
     <row r="59" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A59" s="13"/>
@@ -2620,34 +2638,34 @@
       <c r="E59" s="13"/>
       <c r="F59" s="13"/>
       <c r="G59" s="15"/>
-      <c r="H59" s="35"/>
-      <c r="I59" s="36"/>
-      <c r="J59" s="31"/>
-      <c r="K59" s="31"/>
+      <c r="H59" s="32"/>
+      <c r="I59" s="31"/>
+      <c r="J59" s="38"/>
+      <c r="K59" s="38"/>
     </row>
     <row r="60" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A60" s="47" t="s">
+      <c r="A60" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="B60" s="38"/>
-      <c r="C60" s="38"/>
-      <c r="D60" s="38"/>
-      <c r="E60" s="38"/>
-      <c r="F60" s="38"/>
-      <c r="G60" s="38"/>
-      <c r="H60" s="38"/>
-      <c r="I60" s="38"/>
-      <c r="J60" s="38"/>
-      <c r="K60" s="39"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="34"/>
+      <c r="D60" s="34"/>
+      <c r="E60" s="34"/>
+      <c r="F60" s="34"/>
+      <c r="G60" s="34"/>
+      <c r="H60" s="34"/>
+      <c r="I60" s="34"/>
+      <c r="J60" s="34"/>
+      <c r="K60" s="35"/>
     </row>
     <row r="61" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A61" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="B61" s="29">
+      <c r="B61" s="17">
         <v>45771</v>
       </c>
-      <c r="C61" s="13" t="s">
+      <c r="C61" s="18" t="s">
         <v>138</v>
       </c>
       <c r="D61" s="13" t="s">
@@ -2662,21 +2680,21 @@
       <c r="G61" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H61" s="35"/>
-      <c r="I61" s="36"/>
-      <c r="J61" s="31" t="s">
+      <c r="H61" s="32"/>
+      <c r="I61" s="31"/>
+      <c r="J61" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="K61" s="31"/>
+      <c r="K61" s="38"/>
     </row>
     <row r="62" spans="1:11" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="B62" s="29">
+      <c r="B62" s="17">
         <v>45771</v>
       </c>
-      <c r="C62" s="13" t="s">
+      <c r="C62" s="18" t="s">
         <v>138</v>
       </c>
       <c r="D62" s="13" t="s">
@@ -2691,550 +2709,582 @@
       <c r="G62" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="H62" s="40" t="s">
+      <c r="H62" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="I62" s="36"/>
-      <c r="J62" s="31" t="s">
+      <c r="I62" s="31"/>
+      <c r="J62" s="38" t="s">
         <v>147</v>
       </c>
-      <c r="K62" s="31"/>
+      <c r="K62" s="38"/>
     </row>
     <row r="63" spans="1:11" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="B63" s="29">
+      <c r="B63" s="17">
         <v>45771</v>
       </c>
-      <c r="C63" s="13" t="s">
+      <c r="C63" s="18" t="s">
         <v>138</v>
       </c>
       <c r="D63" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="E63" s="30" t="s">
+      <c r="E63" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="F63" s="30" t="s">
+      <c r="F63" s="29" t="s">
         <v>149</v>
       </c>
       <c r="G63" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H63" s="35"/>
-      <c r="I63" s="36"/>
-      <c r="J63" s="31" t="s">
+      <c r="H63" s="32"/>
+      <c r="I63" s="31"/>
+      <c r="J63" s="38" t="s">
         <v>147</v>
       </c>
-      <c r="K63" s="31"/>
-    </row>
-    <row r="64" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A64" s="13"/>
-      <c r="B64" s="13"/>
-      <c r="C64" s="13"/>
-      <c r="D64" s="13"/>
-      <c r="E64" s="13"/>
-      <c r="F64" s="13"/>
-      <c r="G64" s="15"/>
-      <c r="H64" s="35"/>
-      <c r="I64" s="36"/>
-      <c r="J64" s="31"/>
-      <c r="K64" s="31"/>
+      <c r="K63" s="38"/>
+    </row>
+    <row r="64" spans="1:11" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A64" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B64" s="17">
+        <v>45771</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="F64" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="G64" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H64" s="32"/>
+      <c r="I64" s="31"/>
+      <c r="J64" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="K64" s="38"/>
     </row>
     <row r="65" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A65" s="13"/>
-      <c r="B65" s="13"/>
-      <c r="C65" s="13"/>
-      <c r="D65" s="13"/>
-      <c r="E65" s="13"/>
-      <c r="F65" s="13"/>
-      <c r="G65" s="15"/>
-      <c r="H65" s="13"/>
-      <c r="I65" s="13"/>
-      <c r="J65" s="31"/>
-      <c r="K65" s="31"/>
+      <c r="A65" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B65" s="17">
+        <v>45771</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="F65" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="G65" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H65" s="32"/>
+      <c r="I65" s="31"/>
+      <c r="J65" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="K65" s="38"/>
     </row>
     <row r="66" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A66" s="13"/>
-      <c r="B66" s="13"/>
-      <c r="C66" s="13"/>
+      <c r="B66" s="18"/>
+      <c r="C66" s="18"/>
       <c r="D66" s="13"/>
       <c r="E66" s="13"/>
       <c r="F66" s="13"/>
       <c r="G66" s="15"/>
-      <c r="H66" s="13"/>
-      <c r="I66" s="13"/>
-      <c r="J66" s="31"/>
-      <c r="K66" s="31"/>
+      <c r="H66" s="32"/>
+      <c r="I66" s="31"/>
+      <c r="J66" s="38"/>
+      <c r="K66" s="38"/>
     </row>
     <row r="67" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A67" s="13"/>
-      <c r="B67" s="13"/>
-      <c r="C67" s="13"/>
+      <c r="B67" s="18"/>
+      <c r="C67" s="18"/>
       <c r="D67" s="13"/>
       <c r="E67" s="13"/>
       <c r="F67" s="13"/>
       <c r="G67" s="15"/>
-      <c r="H67" s="13"/>
-      <c r="I67" s="13"/>
-      <c r="J67" s="31"/>
-      <c r="K67" s="31"/>
+      <c r="H67" s="32"/>
+      <c r="I67" s="31"/>
+      <c r="J67" s="38"/>
+      <c r="K67" s="38"/>
     </row>
     <row r="68" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A68" s="13"/>
-      <c r="B68" s="13"/>
-      <c r="C68" s="13"/>
+      <c r="B68" s="18"/>
+      <c r="C68" s="18"/>
       <c r="D68" s="13"/>
       <c r="E68" s="13"/>
       <c r="F68" s="13"/>
       <c r="G68" s="15"/>
-      <c r="H68" s="13"/>
-      <c r="I68" s="13"/>
-      <c r="J68" s="31"/>
-      <c r="K68" s="31"/>
+      <c r="H68" s="32"/>
+      <c r="I68" s="31"/>
+      <c r="J68" s="38"/>
+      <c r="K68" s="38"/>
     </row>
     <row r="69" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A69" s="13"/>
-      <c r="B69" s="13"/>
-      <c r="C69" s="13"/>
+      <c r="B69" s="18"/>
+      <c r="C69" s="18"/>
       <c r="D69" s="13"/>
       <c r="E69" s="13"/>
       <c r="F69" s="13"/>
       <c r="G69" s="15"/>
-      <c r="H69" s="13"/>
-      <c r="I69" s="13"/>
-      <c r="J69" s="31"/>
-      <c r="K69" s="31"/>
+      <c r="H69" s="32"/>
+      <c r="I69" s="31"/>
+      <c r="J69" s="38"/>
+      <c r="K69" s="38"/>
     </row>
     <row r="70" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A70" s="13"/>
-      <c r="B70" s="13"/>
-      <c r="C70" s="13"/>
+      <c r="B70" s="18"/>
+      <c r="C70" s="18"/>
       <c r="D70" s="13"/>
       <c r="E70" s="13"/>
       <c r="F70" s="13"/>
       <c r="G70" s="15"/>
-      <c r="H70" s="13"/>
-      <c r="I70" s="13"/>
-      <c r="J70" s="31"/>
-      <c r="K70" s="31"/>
+      <c r="H70" s="32"/>
+      <c r="I70" s="31"/>
+      <c r="J70" s="38"/>
+      <c r="K70" s="38"/>
     </row>
     <row r="71" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A71" s="13"/>
-      <c r="B71" s="13"/>
-      <c r="C71" s="13"/>
+      <c r="B71" s="18"/>
+      <c r="C71" s="18"/>
       <c r="D71" s="13"/>
       <c r="E71" s="13"/>
       <c r="F71" s="13"/>
       <c r="G71" s="15"/>
-      <c r="H71" s="13"/>
-      <c r="I71" s="13"/>
-      <c r="J71" s="31"/>
-      <c r="K71" s="31"/>
+      <c r="H71" s="32"/>
+      <c r="I71" s="31"/>
+      <c r="J71" s="38"/>
+      <c r="K71" s="38"/>
     </row>
     <row r="72" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A72" s="13"/>
-      <c r="B72" s="13"/>
-      <c r="C72" s="13"/>
+      <c r="B72" s="18"/>
+      <c r="C72" s="18"/>
       <c r="D72" s="13"/>
       <c r="E72" s="13"/>
       <c r="F72" s="13"/>
       <c r="G72" s="15"/>
-      <c r="H72" s="13"/>
-      <c r="I72" s="13"/>
-      <c r="J72" s="31"/>
-      <c r="K72" s="31"/>
+      <c r="H72" s="32"/>
+      <c r="I72" s="31"/>
+      <c r="J72" s="38"/>
+      <c r="K72" s="38"/>
     </row>
     <row r="73" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A73" s="13"/>
-      <c r="B73" s="13"/>
-      <c r="C73" s="13"/>
+      <c r="B73" s="18"/>
+      <c r="C73" s="18"/>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
       <c r="F73" s="13"/>
       <c r="G73" s="15"/>
-      <c r="H73" s="13"/>
-      <c r="I73" s="13"/>
-      <c r="J73" s="31"/>
-      <c r="K73" s="31"/>
+      <c r="H73" s="32"/>
+      <c r="I73" s="31"/>
+      <c r="J73" s="38"/>
+      <c r="K73" s="38"/>
     </row>
     <row r="74" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A74" s="13"/>
-      <c r="B74" s="13"/>
-      <c r="C74" s="13"/>
+      <c r="B74" s="18"/>
+      <c r="C74" s="18"/>
       <c r="D74" s="13"/>
       <c r="E74" s="13"/>
       <c r="F74" s="13"/>
       <c r="G74" s="15"/>
-      <c r="H74" s="13"/>
-      <c r="I74" s="13"/>
-      <c r="J74" s="31"/>
-      <c r="K74" s="31"/>
+      <c r="H74" s="32"/>
+      <c r="I74" s="31"/>
+      <c r="J74" s="38"/>
+      <c r="K74" s="38"/>
     </row>
     <row r="75" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A75" s="13"/>
-      <c r="B75" s="13"/>
-      <c r="C75" s="13"/>
+      <c r="B75" s="18"/>
+      <c r="C75" s="18"/>
       <c r="D75" s="13"/>
       <c r="E75" s="13"/>
       <c r="F75" s="13"/>
       <c r="G75" s="15"/>
-      <c r="H75" s="13"/>
-      <c r="I75" s="13"/>
-      <c r="J75" s="31"/>
-      <c r="K75" s="31"/>
+      <c r="H75" s="32"/>
+      <c r="I75" s="31"/>
+      <c r="J75" s="38"/>
+      <c r="K75" s="38"/>
     </row>
     <row r="76" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A76" s="13"/>
-      <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
+      <c r="B76" s="18"/>
+      <c r="C76" s="18"/>
       <c r="D76" s="13"/>
       <c r="E76" s="13"/>
       <c r="F76" s="13"/>
       <c r="G76" s="15"/>
-      <c r="H76" s="13"/>
-      <c r="I76" s="13"/>
-      <c r="J76" s="31"/>
-      <c r="K76" s="31"/>
+      <c r="H76" s="32"/>
+      <c r="I76" s="31"/>
+      <c r="J76" s="38"/>
+      <c r="K76" s="38"/>
     </row>
     <row r="77" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A77" s="13"/>
-      <c r="B77" s="13"/>
-      <c r="C77" s="13"/>
+      <c r="B77" s="18"/>
+      <c r="C77" s="18"/>
       <c r="D77" s="13"/>
       <c r="E77" s="13"/>
       <c r="F77" s="13"/>
       <c r="G77" s="15"/>
-      <c r="H77" s="13"/>
-      <c r="I77" s="13"/>
-      <c r="J77" s="31"/>
-      <c r="K77" s="31"/>
+      <c r="H77" s="32"/>
+      <c r="I77" s="31"/>
+      <c r="J77" s="38"/>
+      <c r="K77" s="38"/>
     </row>
     <row r="78" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A78" s="13"/>
-      <c r="B78" s="13"/>
-      <c r="C78" s="13"/>
+      <c r="B78" s="18"/>
+      <c r="C78" s="18"/>
       <c r="D78" s="13"/>
       <c r="E78" s="13"/>
       <c r="F78" s="13"/>
       <c r="G78" s="15"/>
-      <c r="H78" s="13"/>
-      <c r="I78" s="13"/>
-      <c r="J78" s="31"/>
-      <c r="K78" s="31"/>
+      <c r="H78" s="32"/>
+      <c r="I78" s="31"/>
+      <c r="J78" s="38"/>
+      <c r="K78" s="38"/>
     </row>
     <row r="79" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A79" s="13"/>
-      <c r="B79" s="13"/>
-      <c r="C79" s="13"/>
+      <c r="B79" s="18"/>
+      <c r="C79" s="18"/>
       <c r="D79" s="13"/>
       <c r="E79" s="13"/>
       <c r="F79" s="13"/>
       <c r="G79" s="15"/>
-      <c r="H79" s="13"/>
-      <c r="I79" s="13"/>
-      <c r="J79" s="31"/>
-      <c r="K79" s="31"/>
+      <c r="H79" s="32"/>
+      <c r="I79" s="31"/>
+      <c r="J79" s="38"/>
+      <c r="K79" s="38"/>
     </row>
     <row r="80" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A80" s="13"/>
-      <c r="B80" s="13"/>
-      <c r="C80" s="13"/>
+      <c r="B80" s="18"/>
+      <c r="C80" s="18"/>
       <c r="D80" s="13"/>
       <c r="E80" s="13"/>
       <c r="F80" s="13"/>
       <c r="G80" s="15"/>
-      <c r="H80" s="13"/>
-      <c r="I80" s="13"/>
-      <c r="J80" s="31"/>
-      <c r="K80" s="31"/>
+      <c r="H80" s="32"/>
+      <c r="I80" s="31"/>
+      <c r="J80" s="38"/>
+      <c r="K80" s="38"/>
     </row>
     <row r="81" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A81" s="13"/>
-      <c r="B81" s="13"/>
-      <c r="C81" s="13"/>
+      <c r="B81" s="18"/>
+      <c r="C81" s="18"/>
       <c r="D81" s="13"/>
       <c r="E81" s="13"/>
       <c r="F81" s="13"/>
       <c r="G81" s="15"/>
-      <c r="H81" s="13"/>
-      <c r="I81" s="13"/>
-      <c r="J81" s="31"/>
-      <c r="K81" s="31"/>
+      <c r="H81" s="32"/>
+      <c r="I81" s="31"/>
+      <c r="J81" s="38"/>
+      <c r="K81" s="38"/>
     </row>
     <row r="82" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A82" s="13"/>
-      <c r="B82" s="13"/>
-      <c r="C82" s="13"/>
+      <c r="B82" s="18"/>
+      <c r="C82" s="18"/>
       <c r="D82" s="13"/>
       <c r="E82" s="13"/>
       <c r="F82" s="13"/>
       <c r="G82" s="15"/>
-      <c r="H82" s="13"/>
-      <c r="I82" s="13"/>
-      <c r="J82" s="31"/>
-      <c r="K82" s="31"/>
+      <c r="H82" s="32"/>
+      <c r="I82" s="31"/>
+      <c r="J82" s="38"/>
+      <c r="K82" s="38"/>
     </row>
     <row r="83" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A83" s="13"/>
-      <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
+      <c r="B83" s="18"/>
+      <c r="C83" s="18"/>
       <c r="D83" s="13"/>
       <c r="E83" s="13"/>
       <c r="F83" s="13"/>
       <c r="G83" s="15"/>
-      <c r="H83" s="13"/>
-      <c r="I83" s="13"/>
-      <c r="J83" s="31"/>
-      <c r="K83" s="31"/>
+      <c r="H83" s="32"/>
+      <c r="I83" s="31"/>
+      <c r="J83" s="38"/>
+      <c r="K83" s="38"/>
     </row>
     <row r="84" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A84" s="13"/>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
+      <c r="B84" s="18"/>
+      <c r="C84" s="18"/>
       <c r="D84" s="13"/>
       <c r="E84" s="13"/>
       <c r="F84" s="13"/>
       <c r="G84" s="15"/>
-      <c r="H84" s="13"/>
-      <c r="I84" s="13"/>
-      <c r="J84" s="31"/>
-      <c r="K84" s="31"/>
+      <c r="H84" s="32"/>
+      <c r="I84" s="31"/>
+      <c r="J84" s="38"/>
+      <c r="K84" s="38"/>
     </row>
     <row r="85" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A85" s="13"/>
-      <c r="B85" s="13"/>
-      <c r="C85" s="13"/>
+      <c r="B85" s="18"/>
+      <c r="C85" s="18"/>
       <c r="D85" s="13"/>
       <c r="E85" s="13"/>
       <c r="F85" s="13"/>
       <c r="G85" s="15"/>
-      <c r="H85" s="13"/>
-      <c r="I85" s="13"/>
-      <c r="J85" s="31"/>
-      <c r="K85" s="31"/>
+      <c r="H85" s="32"/>
+      <c r="I85" s="31"/>
+      <c r="J85" s="38"/>
+      <c r="K85" s="38"/>
     </row>
     <row r="86" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A86" s="13"/>
-      <c r="B86" s="13"/>
-      <c r="C86" s="13"/>
+      <c r="B86" s="18"/>
+      <c r="C86" s="18"/>
       <c r="D86" s="13"/>
       <c r="E86" s="13"/>
       <c r="F86" s="13"/>
       <c r="G86" s="15"/>
-      <c r="H86" s="13"/>
-      <c r="I86" s="13"/>
-      <c r="J86" s="31"/>
-      <c r="K86" s="31"/>
+      <c r="H86" s="32"/>
+      <c r="I86" s="31"/>
+      <c r="J86" s="38"/>
+      <c r="K86" s="38"/>
     </row>
     <row r="87" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A87" s="13"/>
-      <c r="B87" s="13"/>
-      <c r="C87" s="13"/>
+      <c r="B87" s="18"/>
+      <c r="C87" s="18"/>
       <c r="D87" s="13"/>
       <c r="E87" s="13"/>
       <c r="F87" s="13"/>
       <c r="G87" s="15"/>
-      <c r="H87" s="13"/>
-      <c r="I87" s="13"/>
-      <c r="J87" s="31"/>
-      <c r="K87" s="31"/>
+      <c r="H87" s="32"/>
+      <c r="I87" s="31"/>
+      <c r="J87" s="38"/>
+      <c r="K87" s="38"/>
     </row>
     <row r="88" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A88" s="13"/>
-      <c r="B88" s="13"/>
-      <c r="C88" s="13"/>
+      <c r="B88" s="18"/>
+      <c r="C88" s="18"/>
       <c r="D88" s="13"/>
       <c r="E88" s="13"/>
       <c r="F88" s="13"/>
       <c r="G88" s="15"/>
-      <c r="H88" s="13"/>
-      <c r="I88" s="13"/>
-      <c r="J88" s="31"/>
-      <c r="K88" s="31"/>
+      <c r="H88" s="32"/>
+      <c r="I88" s="31"/>
+      <c r="J88" s="38"/>
+      <c r="K88" s="38"/>
     </row>
     <row r="89" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A89" s="13"/>
-      <c r="B89" s="13"/>
-      <c r="C89" s="13"/>
+      <c r="B89" s="18"/>
+      <c r="C89" s="18"/>
       <c r="D89" s="13"/>
       <c r="E89" s="13"/>
       <c r="F89" s="13"/>
       <c r="G89" s="15"/>
-      <c r="H89" s="13"/>
-      <c r="I89" s="13"/>
-      <c r="J89" s="31"/>
-      <c r="K89" s="31"/>
+      <c r="H89" s="32"/>
+      <c r="I89" s="31"/>
+      <c r="J89" s="38"/>
+      <c r="K89" s="38"/>
     </row>
     <row r="90" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A90" s="13"/>
-      <c r="B90" s="13"/>
-      <c r="C90" s="13"/>
+      <c r="B90" s="18"/>
+      <c r="C90" s="18"/>
       <c r="D90" s="13"/>
       <c r="E90" s="13"/>
       <c r="F90" s="13"/>
       <c r="G90" s="15"/>
-      <c r="H90" s="13"/>
-      <c r="I90" s="13"/>
-      <c r="J90" s="31"/>
-      <c r="K90" s="31"/>
+      <c r="H90" s="32"/>
+      <c r="I90" s="31"/>
+      <c r="J90" s="38"/>
+      <c r="K90" s="38"/>
     </row>
     <row r="91" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A91" s="13"/>
-      <c r="B91" s="13"/>
-      <c r="C91" s="13"/>
+      <c r="B91" s="18"/>
+      <c r="C91" s="18"/>
       <c r="D91" s="13"/>
       <c r="E91" s="13"/>
       <c r="F91" s="13"/>
       <c r="G91" s="15"/>
-      <c r="H91" s="13"/>
-      <c r="I91" s="13"/>
-      <c r="J91" s="31"/>
-      <c r="K91" s="31"/>
+      <c r="H91" s="32"/>
+      <c r="I91" s="31"/>
+      <c r="J91" s="38"/>
+      <c r="K91" s="38"/>
     </row>
     <row r="92" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A92" s="13"/>
-      <c r="B92" s="13"/>
-      <c r="C92" s="13"/>
+      <c r="B92" s="18"/>
+      <c r="C92" s="18"/>
       <c r="D92" s="13"/>
       <c r="E92" s="13"/>
       <c r="F92" s="13"/>
       <c r="G92" s="15"/>
-      <c r="H92" s="13"/>
-      <c r="I92" s="13"/>
-      <c r="J92" s="31"/>
-      <c r="K92" s="31"/>
+      <c r="H92" s="32"/>
+      <c r="I92" s="31"/>
+      <c r="J92" s="38"/>
+      <c r="K92" s="38"/>
     </row>
     <row r="93" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A93" s="13"/>
-      <c r="B93" s="13"/>
-      <c r="C93" s="13"/>
+      <c r="B93" s="18"/>
+      <c r="C93" s="18"/>
       <c r="D93" s="13"/>
       <c r="E93" s="13"/>
       <c r="F93" s="13"/>
       <c r="G93" s="15"/>
-      <c r="H93" s="13"/>
-      <c r="I93" s="13"/>
-      <c r="J93" s="31"/>
-      <c r="K93" s="31"/>
+      <c r="H93" s="32"/>
+      <c r="I93" s="31"/>
+      <c r="J93" s="38"/>
+      <c r="K93" s="38"/>
     </row>
     <row r="94" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A94" s="13"/>
-      <c r="B94" s="13"/>
-      <c r="C94" s="13"/>
+      <c r="B94" s="18"/>
+      <c r="C94" s="18"/>
       <c r="D94" s="13"/>
       <c r="E94" s="13"/>
       <c r="F94" s="13"/>
       <c r="G94" s="15"/>
-      <c r="H94" s="13"/>
-      <c r="I94" s="13"/>
-      <c r="J94" s="31"/>
-      <c r="K94" s="31"/>
+      <c r="H94" s="32"/>
+      <c r="I94" s="31"/>
+      <c r="J94" s="38"/>
+      <c r="K94" s="38"/>
     </row>
     <row r="95" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A95" s="13"/>
-      <c r="B95" s="13"/>
-      <c r="C95" s="13"/>
+      <c r="B95" s="18"/>
+      <c r="C95" s="18"/>
       <c r="D95" s="13"/>
       <c r="E95" s="13"/>
       <c r="F95" s="13"/>
       <c r="G95" s="15"/>
-      <c r="H95" s="13"/>
-      <c r="I95" s="13"/>
-      <c r="J95" s="31"/>
-      <c r="K95" s="31"/>
+      <c r="H95" s="32"/>
+      <c r="I95" s="31"/>
+      <c r="J95" s="38"/>
+      <c r="K95" s="38"/>
     </row>
     <row r="96" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A96" s="13"/>
-      <c r="B96" s="13"/>
-      <c r="C96" s="13"/>
+      <c r="B96" s="18"/>
+      <c r="C96" s="18"/>
       <c r="D96" s="13"/>
       <c r="E96" s="13"/>
       <c r="F96" s="13"/>
       <c r="G96" s="15"/>
-      <c r="H96" s="13"/>
-      <c r="I96" s="13"/>
-      <c r="J96" s="31"/>
-      <c r="K96" s="31"/>
+      <c r="H96" s="32"/>
+      <c r="I96" s="31"/>
+      <c r="J96" s="38"/>
+      <c r="K96" s="38"/>
     </row>
     <row r="97" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A97" s="13"/>
-      <c r="B97" s="13"/>
-      <c r="C97" s="13"/>
+      <c r="B97" s="18"/>
+      <c r="C97" s="18"/>
       <c r="D97" s="13"/>
       <c r="E97" s="13"/>
       <c r="F97" s="13"/>
       <c r="G97" s="15"/>
-      <c r="H97" s="13"/>
-      <c r="I97" s="13"/>
-      <c r="J97" s="31"/>
-      <c r="K97" s="31"/>
+      <c r="H97" s="32"/>
+      <c r="I97" s="31"/>
+      <c r="J97" s="38"/>
+      <c r="K97" s="38"/>
     </row>
     <row r="98" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A98" s="13"/>
-      <c r="B98" s="13"/>
-      <c r="C98" s="13"/>
+      <c r="B98" s="18"/>
+      <c r="C98" s="18"/>
       <c r="D98" s="13"/>
       <c r="E98" s="13"/>
       <c r="F98" s="13"/>
       <c r="G98" s="15"/>
-      <c r="H98" s="13"/>
-      <c r="I98" s="13"/>
-      <c r="J98" s="31"/>
-      <c r="K98" s="31"/>
+      <c r="H98" s="32"/>
+      <c r="I98" s="31"/>
+      <c r="J98" s="38"/>
+      <c r="K98" s="38"/>
     </row>
     <row r="99" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A99" s="13"/>
-      <c r="B99" s="13"/>
-      <c r="C99" s="13"/>
+      <c r="B99" s="18"/>
+      <c r="C99" s="18"/>
       <c r="D99" s="13"/>
       <c r="E99" s="13"/>
       <c r="F99" s="13"/>
       <c r="G99" s="15"/>
-      <c r="H99" s="13"/>
-      <c r="I99" s="13"/>
-      <c r="J99" s="31"/>
-      <c r="K99" s="31"/>
+      <c r="H99" s="32"/>
+      <c r="I99" s="31"/>
+      <c r="J99" s="38"/>
+      <c r="K99" s="38"/>
     </row>
     <row r="100" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A100" s="13"/>
-      <c r="B100" s="13"/>
-      <c r="C100" s="13"/>
+      <c r="B100" s="18"/>
+      <c r="C100" s="18"/>
       <c r="D100" s="13"/>
       <c r="E100" s="13"/>
       <c r="F100" s="13"/>
       <c r="G100" s="15"/>
-      <c r="H100" s="13"/>
-      <c r="I100" s="13"/>
-      <c r="J100" s="31"/>
-      <c r="K100" s="31"/>
+      <c r="H100" s="32"/>
+      <c r="I100" s="31"/>
+      <c r="J100" s="38"/>
+      <c r="K100" s="38"/>
     </row>
     <row r="101" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A101" s="13"/>
-      <c r="B101" s="13"/>
-      <c r="C101" s="13"/>
+      <c r="B101" s="18"/>
+      <c r="C101" s="18"/>
       <c r="D101" s="13"/>
       <c r="E101" s="13"/>
       <c r="F101" s="13"/>
       <c r="G101" s="15"/>
-      <c r="H101" s="13"/>
-      <c r="I101" s="13"/>
-      <c r="J101" s="31"/>
-      <c r="K101" s="31"/>
+      <c r="H101" s="32"/>
+      <c r="I101" s="31"/>
+      <c r="J101" s="38"/>
+      <c r="K101" s="38"/>
     </row>
     <row r="102" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A102" s="13"/>
-      <c r="B102" s="13"/>
-      <c r="C102" s="13"/>
+      <c r="B102" s="18"/>
+      <c r="C102" s="18"/>
       <c r="D102" s="13"/>
       <c r="E102" s="13"/>
       <c r="F102" s="13"/>
       <c r="G102" s="15"/>
-      <c r="H102" s="13"/>
-      <c r="I102" s="13"/>
-      <c r="J102" s="31"/>
-      <c r="K102" s="31"/>
+      <c r="H102" s="32"/>
+      <c r="I102" s="31"/>
+      <c r="J102" s="38"/>
+      <c r="K102" s="38"/>
     </row>
     <row r="103" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A103" s="13"/>
@@ -3244,10 +3294,10 @@
       <c r="E103" s="13"/>
       <c r="F103" s="13"/>
       <c r="G103" s="15"/>
-      <c r="H103" s="13"/>
-      <c r="I103" s="13"/>
-      <c r="J103" s="31"/>
-      <c r="K103" s="31"/>
+      <c r="H103" s="32"/>
+      <c r="I103" s="31"/>
+      <c r="J103" s="38"/>
+      <c r="K103" s="38"/>
     </row>
     <row r="104" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A104" s="13"/>
@@ -3257,10 +3307,10 @@
       <c r="E104" s="13"/>
       <c r="F104" s="13"/>
       <c r="G104" s="15"/>
-      <c r="H104" s="13"/>
-      <c r="I104" s="13"/>
-      <c r="J104" s="31"/>
-      <c r="K104" s="31"/>
+      <c r="H104" s="32"/>
+      <c r="I104" s="31"/>
+      <c r="J104" s="38"/>
+      <c r="K104" s="38"/>
     </row>
     <row r="105" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A105" s="13"/>
@@ -3270,10 +3320,10 @@
       <c r="E105" s="13"/>
       <c r="F105" s="13"/>
       <c r="G105" s="15"/>
-      <c r="H105" s="13"/>
-      <c r="I105" s="13"/>
-      <c r="J105" s="31"/>
-      <c r="K105" s="31"/>
+      <c r="H105" s="32"/>
+      <c r="I105" s="31"/>
+      <c r="J105" s="38"/>
+      <c r="K105" s="38"/>
     </row>
     <row r="106" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A106" s="13"/>
@@ -3283,10 +3333,10 @@
       <c r="E106" s="13"/>
       <c r="F106" s="13"/>
       <c r="G106" s="15"/>
-      <c r="H106" s="13"/>
-      <c r="I106" s="13"/>
-      <c r="J106" s="31"/>
-      <c r="K106" s="31"/>
+      <c r="H106" s="32"/>
+      <c r="I106" s="31"/>
+      <c r="J106" s="38"/>
+      <c r="K106" s="38"/>
     </row>
     <row r="107" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A107" s="13"/>
@@ -3296,10 +3346,10 @@
       <c r="E107" s="13"/>
       <c r="F107" s="13"/>
       <c r="G107" s="15"/>
-      <c r="H107" s="13"/>
-      <c r="I107" s="13"/>
-      <c r="J107" s="31"/>
-      <c r="K107" s="31"/>
+      <c r="H107" s="32"/>
+      <c r="I107" s="31"/>
+      <c r="J107" s="38"/>
+      <c r="K107" s="38"/>
     </row>
     <row r="108" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A108" s="13"/>
@@ -3309,10 +3359,10 @@
       <c r="E108" s="13"/>
       <c r="F108" s="13"/>
       <c r="G108" s="15"/>
-      <c r="H108" s="13"/>
-      <c r="I108" s="13"/>
-      <c r="J108" s="31"/>
-      <c r="K108" s="31"/>
+      <c r="H108" s="32"/>
+      <c r="I108" s="31"/>
+      <c r="J108" s="38"/>
+      <c r="K108" s="38"/>
     </row>
     <row r="109" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A109" s="13"/>
@@ -3322,10 +3372,10 @@
       <c r="E109" s="13"/>
       <c r="F109" s="13"/>
       <c r="G109" s="15"/>
-      <c r="H109" s="13"/>
-      <c r="I109" s="13"/>
-      <c r="J109" s="31"/>
-      <c r="K109" s="31"/>
+      <c r="H109" s="32"/>
+      <c r="I109" s="31"/>
+      <c r="J109" s="38"/>
+      <c r="K109" s="38"/>
     </row>
     <row r="110" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A110" s="13"/>
@@ -3335,10 +3385,10 @@
       <c r="E110" s="13"/>
       <c r="F110" s="13"/>
       <c r="G110" s="15"/>
-      <c r="H110" s="13"/>
-      <c r="I110" s="13"/>
-      <c r="J110" s="31"/>
-      <c r="K110" s="31"/>
+      <c r="H110" s="32"/>
+      <c r="I110" s="31"/>
+      <c r="J110" s="38"/>
+      <c r="K110" s="38"/>
     </row>
     <row r="111" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A111" s="13"/>
@@ -3348,10 +3398,10 @@
       <c r="E111" s="13"/>
       <c r="F111" s="13"/>
       <c r="G111" s="15"/>
-      <c r="H111" s="13"/>
-      <c r="I111" s="13"/>
-      <c r="J111" s="31"/>
-      <c r="K111" s="31"/>
+      <c r="H111" s="32"/>
+      <c r="I111" s="31"/>
+      <c r="J111" s="38"/>
+      <c r="K111" s="38"/>
     </row>
     <row r="112" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A112" s="13"/>
@@ -3361,10 +3411,10 @@
       <c r="E112" s="13"/>
       <c r="F112" s="13"/>
       <c r="G112" s="15"/>
-      <c r="H112" s="13"/>
-      <c r="I112" s="13"/>
-      <c r="J112" s="31"/>
-      <c r="K112" s="31"/>
+      <c r="H112" s="32"/>
+      <c r="I112" s="31"/>
+      <c r="J112" s="38"/>
+      <c r="K112" s="38"/>
     </row>
     <row r="113" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A113" s="13"/>
@@ -3374,10 +3424,10 @@
       <c r="E113" s="13"/>
       <c r="F113" s="13"/>
       <c r="G113" s="15"/>
-      <c r="H113" s="13"/>
-      <c r="I113" s="13"/>
-      <c r="J113" s="31"/>
-      <c r="K113" s="31"/>
+      <c r="H113" s="32"/>
+      <c r="I113" s="31"/>
+      <c r="J113" s="38"/>
+      <c r="K113" s="38"/>
     </row>
     <row r="114" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A114" s="13"/>
@@ -3387,10 +3437,10 @@
       <c r="E114" s="13"/>
       <c r="F114" s="13"/>
       <c r="G114" s="15"/>
-      <c r="H114" s="13"/>
-      <c r="I114" s="13"/>
-      <c r="J114" s="31"/>
-      <c r="K114" s="31"/>
+      <c r="H114" s="32"/>
+      <c r="I114" s="31"/>
+      <c r="J114" s="38"/>
+      <c r="K114" s="38"/>
     </row>
     <row r="115" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A115" s="13"/>
@@ -3400,10 +3450,10 @@
       <c r="E115" s="13"/>
       <c r="F115" s="13"/>
       <c r="G115" s="15"/>
-      <c r="H115" s="13"/>
-      <c r="I115" s="13"/>
-      <c r="J115" s="31"/>
-      <c r="K115" s="31"/>
+      <c r="H115" s="32"/>
+      <c r="I115" s="31"/>
+      <c r="J115" s="38"/>
+      <c r="K115" s="38"/>
     </row>
     <row r="116" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A116" s="13"/>
@@ -3413,10 +3463,10 @@
       <c r="E116" s="13"/>
       <c r="F116" s="13"/>
       <c r="G116" s="15"/>
-      <c r="H116" s="13"/>
-      <c r="I116" s="13"/>
-      <c r="J116" s="31"/>
-      <c r="K116" s="31"/>
+      <c r="H116" s="32"/>
+      <c r="I116" s="31"/>
+      <c r="J116" s="38"/>
+      <c r="K116" s="38"/>
     </row>
     <row r="117" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A117" s="13"/>
@@ -3426,10 +3476,10 @@
       <c r="E117" s="13"/>
       <c r="F117" s="13"/>
       <c r="G117" s="15"/>
-      <c r="H117" s="13"/>
-      <c r="I117" s="13"/>
-      <c r="J117" s="31"/>
-      <c r="K117" s="31"/>
+      <c r="H117" s="32"/>
+      <c r="I117" s="31"/>
+      <c r="J117" s="38"/>
+      <c r="K117" s="38"/>
     </row>
     <row r="118" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A118" s="13"/>
@@ -3439,10 +3489,10 @@
       <c r="E118" s="13"/>
       <c r="F118" s="13"/>
       <c r="G118" s="15"/>
-      <c r="H118" s="13"/>
-      <c r="I118" s="13"/>
-      <c r="J118" s="31"/>
-      <c r="K118" s="31"/>
+      <c r="H118" s="32"/>
+      <c r="I118" s="31"/>
+      <c r="J118" s="38"/>
+      <c r="K118" s="38"/>
     </row>
     <row r="119" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A119" s="13"/>
@@ -3452,10 +3502,10 @@
       <c r="E119" s="13"/>
       <c r="F119" s="13"/>
       <c r="G119" s="15"/>
-      <c r="H119" s="13"/>
-      <c r="I119" s="13"/>
-      <c r="J119" s="31"/>
-      <c r="K119" s="31"/>
+      <c r="H119" s="32"/>
+      <c r="I119" s="31"/>
+      <c r="J119" s="38"/>
+      <c r="K119" s="38"/>
     </row>
     <row r="120" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A120" s="13"/>
@@ -3465,10 +3515,10 @@
       <c r="E120" s="13"/>
       <c r="F120" s="13"/>
       <c r="G120" s="15"/>
-      <c r="H120" s="13"/>
-      <c r="I120" s="13"/>
-      <c r="J120" s="31"/>
-      <c r="K120" s="31"/>
+      <c r="H120" s="32"/>
+      <c r="I120" s="31"/>
+      <c r="J120" s="38"/>
+      <c r="K120" s="38"/>
     </row>
     <row r="121" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A121" s="13"/>
@@ -3478,10 +3528,10 @@
       <c r="E121" s="13"/>
       <c r="F121" s="13"/>
       <c r="G121" s="15"/>
-      <c r="H121" s="13"/>
-      <c r="I121" s="13"/>
-      <c r="J121" s="31"/>
-      <c r="K121" s="31"/>
+      <c r="H121" s="32"/>
+      <c r="I121" s="31"/>
+      <c r="J121" s="38"/>
+      <c r="K121" s="38"/>
     </row>
     <row r="122" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A122" s="13"/>
@@ -3491,10 +3541,10 @@
       <c r="E122" s="13"/>
       <c r="F122" s="13"/>
       <c r="G122" s="15"/>
-      <c r="H122" s="13"/>
-      <c r="I122" s="13"/>
-      <c r="J122" s="31"/>
-      <c r="K122" s="31"/>
+      <c r="H122" s="32"/>
+      <c r="I122" s="31"/>
+      <c r="J122" s="38"/>
+      <c r="K122" s="38"/>
     </row>
     <row r="123" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A123" s="13"/>
@@ -3504,10 +3554,10 @@
       <c r="E123" s="13"/>
       <c r="F123" s="13"/>
       <c r="G123" s="15"/>
-      <c r="H123" s="13"/>
-      <c r="I123" s="13"/>
-      <c r="J123" s="31"/>
-      <c r="K123" s="31"/>
+      <c r="H123" s="32"/>
+      <c r="I123" s="31"/>
+      <c r="J123" s="38"/>
+      <c r="K123" s="38"/>
     </row>
     <row r="124" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A124" s="13"/>
@@ -3517,10 +3567,10 @@
       <c r="E124" s="13"/>
       <c r="F124" s="13"/>
       <c r="G124" s="15"/>
-      <c r="H124" s="13"/>
-      <c r="I124" s="13"/>
-      <c r="J124" s="31"/>
-      <c r="K124" s="31"/>
+      <c r="H124" s="32"/>
+      <c r="I124" s="31"/>
+      <c r="J124" s="38"/>
+      <c r="K124" s="38"/>
     </row>
     <row r="125" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A125" s="13"/>
@@ -3530,10 +3580,10 @@
       <c r="E125" s="13"/>
       <c r="F125" s="13"/>
       <c r="G125" s="15"/>
-      <c r="H125" s="13"/>
-      <c r="I125" s="13"/>
-      <c r="J125" s="31"/>
-      <c r="K125" s="31"/>
+      <c r="H125" s="32"/>
+      <c r="I125" s="31"/>
+      <c r="J125" s="38"/>
+      <c r="K125" s="38"/>
     </row>
     <row r="126" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A126" s="13"/>
@@ -3543,10 +3593,10 @@
       <c r="E126" s="13"/>
       <c r="F126" s="13"/>
       <c r="G126" s="15"/>
-      <c r="H126" s="13"/>
-      <c r="I126" s="13"/>
-      <c r="J126" s="31"/>
-      <c r="K126" s="31"/>
+      <c r="H126" s="32"/>
+      <c r="I126" s="31"/>
+      <c r="J126" s="38"/>
+      <c r="K126" s="38"/>
     </row>
     <row r="127" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A127" s="13"/>
@@ -3556,10 +3606,10 @@
       <c r="E127" s="13"/>
       <c r="F127" s="13"/>
       <c r="G127" s="15"/>
-      <c r="H127" s="13"/>
-      <c r="I127" s="13"/>
-      <c r="J127" s="31"/>
-      <c r="K127" s="31"/>
+      <c r="H127" s="32"/>
+      <c r="I127" s="31"/>
+      <c r="J127" s="38"/>
+      <c r="K127" s="38"/>
     </row>
     <row r="128" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A128" s="13"/>
@@ -3569,10 +3619,10 @@
       <c r="E128" s="13"/>
       <c r="F128" s="13"/>
       <c r="G128" s="15"/>
-      <c r="H128" s="13"/>
-      <c r="I128" s="13"/>
-      <c r="J128" s="31"/>
-      <c r="K128" s="31"/>
+      <c r="H128" s="32"/>
+      <c r="I128" s="31"/>
+      <c r="J128" s="38"/>
+      <c r="K128" s="38"/>
     </row>
     <row r="129" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A129" s="13"/>
@@ -3582,10 +3632,10 @@
       <c r="E129" s="13"/>
       <c r="F129" s="13"/>
       <c r="G129" s="15"/>
-      <c r="H129" s="13"/>
-      <c r="I129" s="13"/>
-      <c r="J129" s="31"/>
-      <c r="K129" s="31"/>
+      <c r="H129" s="32"/>
+      <c r="I129" s="31"/>
+      <c r="J129" s="38"/>
+      <c r="K129" s="38"/>
     </row>
     <row r="130" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A130" s="13"/>
@@ -3597,8 +3647,8 @@
       <c r="G130" s="15"/>
       <c r="H130" s="13"/>
       <c r="I130" s="13"/>
-      <c r="J130" s="31"/>
-      <c r="K130" s="31"/>
+      <c r="J130" s="38"/>
+      <c r="K130" s="38"/>
     </row>
     <row r="131" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A131" s="13"/>
@@ -3610,8 +3660,8 @@
       <c r="G131" s="15"/>
       <c r="H131" s="13"/>
       <c r="I131" s="13"/>
-      <c r="J131" s="31"/>
-      <c r="K131" s="31"/>
+      <c r="J131" s="38"/>
+      <c r="K131" s="38"/>
     </row>
     <row r="132" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A132" s="13"/>
@@ -3623,8 +3673,8 @@
       <c r="G132" s="15"/>
       <c r="H132" s="13"/>
       <c r="I132" s="13"/>
-      <c r="J132" s="31"/>
-      <c r="K132" s="31"/>
+      <c r="J132" s="38"/>
+      <c r="K132" s="38"/>
     </row>
     <row r="133" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A133" s="13"/>
@@ -3636,8 +3686,8 @@
       <c r="G133" s="15"/>
       <c r="H133" s="13"/>
       <c r="I133" s="13"/>
-      <c r="J133" s="31"/>
-      <c r="K133" s="31"/>
+      <c r="J133" s="38"/>
+      <c r="K133" s="38"/>
     </row>
     <row r="134" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A134" s="13"/>
@@ -3649,8 +3699,8 @@
       <c r="G134" s="15"/>
       <c r="H134" s="13"/>
       <c r="I134" s="13"/>
-      <c r="J134" s="31"/>
-      <c r="K134" s="31"/>
+      <c r="J134" s="38"/>
+      <c r="K134" s="38"/>
     </row>
     <row r="135" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A135" s="13"/>
@@ -3662,8 +3712,8 @@
       <c r="G135" s="15"/>
       <c r="H135" s="13"/>
       <c r="I135" s="13"/>
-      <c r="J135" s="31"/>
-      <c r="K135" s="31"/>
+      <c r="J135" s="38"/>
+      <c r="K135" s="38"/>
     </row>
     <row r="136" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A136" s="13"/>
@@ -3675,8 +3725,8 @@
       <c r="G136" s="15"/>
       <c r="H136" s="13"/>
       <c r="I136" s="13"/>
-      <c r="J136" s="31"/>
-      <c r="K136" s="31"/>
+      <c r="J136" s="38"/>
+      <c r="K136" s="38"/>
     </row>
     <row r="137" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A137" s="13"/>
@@ -3688,8 +3738,8 @@
       <c r="G137" s="15"/>
       <c r="H137" s="13"/>
       <c r="I137" s="13"/>
-      <c r="J137" s="31"/>
-      <c r="K137" s="31"/>
+      <c r="J137" s="38"/>
+      <c r="K137" s="38"/>
     </row>
     <row r="138" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A138" s="13"/>
@@ -3701,8 +3751,8 @@
       <c r="G138" s="15"/>
       <c r="H138" s="13"/>
       <c r="I138" s="13"/>
-      <c r="J138" s="31"/>
-      <c r="K138" s="31"/>
+      <c r="J138" s="38"/>
+      <c r="K138" s="38"/>
     </row>
     <row r="139" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A139" s="13"/>
@@ -3714,8 +3764,8 @@
       <c r="G139" s="15"/>
       <c r="H139" s="13"/>
       <c r="I139" s="13"/>
-      <c r="J139" s="31"/>
-      <c r="K139" s="31"/>
+      <c r="J139" s="38"/>
+      <c r="K139" s="38"/>
     </row>
     <row r="140" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A140" s="13"/>
@@ -3727,8 +3777,8 @@
       <c r="G140" s="15"/>
       <c r="H140" s="13"/>
       <c r="I140" s="13"/>
-      <c r="J140" s="31"/>
-      <c r="K140" s="31"/>
+      <c r="J140" s="38"/>
+      <c r="K140" s="38"/>
     </row>
     <row r="141" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A141" s="13"/>
@@ -3740,8 +3790,8 @@
       <c r="G141" s="15"/>
       <c r="H141" s="13"/>
       <c r="I141" s="13"/>
-      <c r="J141" s="31"/>
-      <c r="K141" s="31"/>
+      <c r="J141" s="38"/>
+      <c r="K141" s="38"/>
     </row>
     <row r="142" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A142" s="13"/>
@@ -3753,8 +3803,8 @@
       <c r="G142" s="15"/>
       <c r="H142" s="13"/>
       <c r="I142" s="13"/>
-      <c r="J142" s="31"/>
-      <c r="K142" s="31"/>
+      <c r="J142" s="38"/>
+      <c r="K142" s="38"/>
     </row>
     <row r="143" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A143" s="13"/>
@@ -3766,8 +3816,8 @@
       <c r="G143" s="15"/>
       <c r="H143" s="13"/>
       <c r="I143" s="13"/>
-      <c r="J143" s="31"/>
-      <c r="K143" s="31"/>
+      <c r="J143" s="38"/>
+      <c r="K143" s="38"/>
     </row>
     <row r="144" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A144" s="13"/>
@@ -3779,8 +3829,8 @@
       <c r="G144" s="15"/>
       <c r="H144" s="13"/>
       <c r="I144" s="13"/>
-      <c r="J144" s="31"/>
-      <c r="K144" s="31"/>
+      <c r="J144" s="38"/>
+      <c r="K144" s="38"/>
     </row>
     <row r="145" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A145" s="13"/>
@@ -3792,8 +3842,8 @@
       <c r="G145" s="15"/>
       <c r="H145" s="13"/>
       <c r="I145" s="13"/>
-      <c r="J145" s="31"/>
-      <c r="K145" s="31"/>
+      <c r="J145" s="38"/>
+      <c r="K145" s="38"/>
     </row>
     <row r="146" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A146" s="13"/>
@@ -3805,8 +3855,8 @@
       <c r="G146" s="15"/>
       <c r="H146" s="13"/>
       <c r="I146" s="13"/>
-      <c r="J146" s="31"/>
-      <c r="K146" s="31"/>
+      <c r="J146" s="38"/>
+      <c r="K146" s="38"/>
     </row>
     <row r="147" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A147" s="13"/>
@@ -3818,8 +3868,8 @@
       <c r="G147" s="15"/>
       <c r="H147" s="13"/>
       <c r="I147" s="13"/>
-      <c r="J147" s="31"/>
-      <c r="K147" s="31"/>
+      <c r="J147" s="38"/>
+      <c r="K147" s="38"/>
     </row>
     <row r="148" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A148" s="13"/>
@@ -3831,8 +3881,8 @@
       <c r="G148" s="15"/>
       <c r="H148" s="13"/>
       <c r="I148" s="13"/>
-      <c r="J148" s="31"/>
-      <c r="K148" s="31"/>
+      <c r="J148" s="38"/>
+      <c r="K148" s="38"/>
     </row>
     <row r="149" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A149" s="13"/>
@@ -3844,8 +3894,8 @@
       <c r="G149" s="15"/>
       <c r="H149" s="13"/>
       <c r="I149" s="13"/>
-      <c r="J149" s="31"/>
-      <c r="K149" s="31"/>
+      <c r="J149" s="38"/>
+      <c r="K149" s="38"/>
     </row>
     <row r="150" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A150" s="13"/>
@@ -3857,8 +3907,8 @@
       <c r="G150" s="15"/>
       <c r="H150" s="13"/>
       <c r="I150" s="13"/>
-      <c r="J150" s="31"/>
-      <c r="K150" s="31"/>
+      <c r="J150" s="38"/>
+      <c r="K150" s="38"/>
     </row>
     <row r="151" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A151" s="13"/>
@@ -3870,8 +3920,8 @@
       <c r="G151" s="15"/>
       <c r="H151" s="13"/>
       <c r="I151" s="13"/>
-      <c r="J151" s="31"/>
-      <c r="K151" s="31"/>
+      <c r="J151" s="38"/>
+      <c r="K151" s="38"/>
     </row>
     <row r="152" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A152" s="13"/>
@@ -3883,8 +3933,8 @@
       <c r="G152" s="15"/>
       <c r="H152" s="13"/>
       <c r="I152" s="13"/>
-      <c r="J152" s="31"/>
-      <c r="K152" s="31"/>
+      <c r="J152" s="38"/>
+      <c r="K152" s="38"/>
     </row>
     <row r="153" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A153" s="13"/>
@@ -3896,8 +3946,8 @@
       <c r="G153" s="15"/>
       <c r="H153" s="13"/>
       <c r="I153" s="13"/>
-      <c r="J153" s="31"/>
-      <c r="K153" s="31"/>
+      <c r="J153" s="38"/>
+      <c r="K153" s="38"/>
     </row>
     <row r="154" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A154" s="13"/>
@@ -3909,8 +3959,8 @@
       <c r="G154" s="15"/>
       <c r="H154" s="13"/>
       <c r="I154" s="13"/>
-      <c r="J154" s="31"/>
-      <c r="K154" s="31"/>
+      <c r="J154" s="38"/>
+      <c r="K154" s="38"/>
     </row>
     <row r="155" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A155" s="13"/>
@@ -3922,8 +3972,8 @@
       <c r="G155" s="15"/>
       <c r="H155" s="13"/>
       <c r="I155" s="13"/>
-      <c r="J155" s="31"/>
-      <c r="K155" s="31"/>
+      <c r="J155" s="38"/>
+      <c r="K155" s="38"/>
     </row>
     <row r="156" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A156" s="13"/>
@@ -3935,8 +3985,8 @@
       <c r="G156" s="15"/>
       <c r="H156" s="13"/>
       <c r="I156" s="13"/>
-      <c r="J156" s="31"/>
-      <c r="K156" s="31"/>
+      <c r="J156" s="38"/>
+      <c r="K156" s="38"/>
     </row>
     <row r="157" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A157" s="13"/>
@@ -3948,8 +3998,8 @@
       <c r="G157" s="15"/>
       <c r="H157" s="13"/>
       <c r="I157" s="13"/>
-      <c r="J157" s="31"/>
-      <c r="K157" s="31"/>
+      <c r="J157" s="38"/>
+      <c r="K157" s="38"/>
     </row>
     <row r="158" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A158" s="13"/>
@@ -3961,8 +4011,8 @@
       <c r="G158" s="15"/>
       <c r="H158" s="13"/>
       <c r="I158" s="13"/>
-      <c r="J158" s="31"/>
-      <c r="K158" s="31"/>
+      <c r="J158" s="38"/>
+      <c r="K158" s="38"/>
     </row>
     <row r="159" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A159" s="13"/>
@@ -3974,8 +4024,8 @@
       <c r="G159" s="15"/>
       <c r="H159" s="13"/>
       <c r="I159" s="13"/>
-      <c r="J159" s="31"/>
-      <c r="K159" s="31"/>
+      <c r="J159" s="38"/>
+      <c r="K159" s="38"/>
     </row>
     <row r="160" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A160" s="13"/>
@@ -3987,8 +4037,8 @@
       <c r="G160" s="15"/>
       <c r="H160" s="13"/>
       <c r="I160" s="13"/>
-      <c r="J160" s="31"/>
-      <c r="K160" s="31"/>
+      <c r="J160" s="38"/>
+      <c r="K160" s="38"/>
     </row>
     <row r="161" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A161" s="13"/>
@@ -4000,8 +4050,8 @@
       <c r="G161" s="15"/>
       <c r="H161" s="13"/>
       <c r="I161" s="13"/>
-      <c r="J161" s="31"/>
-      <c r="K161" s="31"/>
+      <c r="J161" s="38"/>
+      <c r="K161" s="38"/>
     </row>
     <row r="162" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A162" s="13"/>
@@ -4013,8 +4063,8 @@
       <c r="G162" s="15"/>
       <c r="H162" s="13"/>
       <c r="I162" s="13"/>
-      <c r="J162" s="31"/>
-      <c r="K162" s="31"/>
+      <c r="J162" s="38"/>
+      <c r="K162" s="38"/>
     </row>
     <row r="163" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A163" s="13"/>
@@ -4026,8 +4076,8 @@
       <c r="G163" s="15"/>
       <c r="H163" s="13"/>
       <c r="I163" s="13"/>
-      <c r="J163" s="31"/>
-      <c r="K163" s="31"/>
+      <c r="J163" s="38"/>
+      <c r="K163" s="38"/>
     </row>
     <row r="164" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A164" s="13"/>
@@ -4039,8 +4089,8 @@
       <c r="G164" s="15"/>
       <c r="H164" s="13"/>
       <c r="I164" s="13"/>
-      <c r="J164" s="31"/>
-      <c r="K164" s="31"/>
+      <c r="J164" s="38"/>
+      <c r="K164" s="38"/>
     </row>
     <row r="165" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A165" s="13"/>
@@ -4052,8 +4102,8 @@
       <c r="G165" s="15"/>
       <c r="H165" s="13"/>
       <c r="I165" s="13"/>
-      <c r="J165" s="31"/>
-      <c r="K165" s="31"/>
+      <c r="J165" s="38"/>
+      <c r="K165" s="38"/>
     </row>
     <row r="166" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A166" s="13"/>
@@ -4065,8 +4115,8 @@
       <c r="G166" s="15"/>
       <c r="H166" s="13"/>
       <c r="I166" s="13"/>
-      <c r="J166" s="31"/>
-      <c r="K166" s="31"/>
+      <c r="J166" s="38"/>
+      <c r="K166" s="38"/>
     </row>
     <row r="167" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A167" s="13"/>
@@ -4078,8 +4128,8 @@
       <c r="G167" s="15"/>
       <c r="H167" s="13"/>
       <c r="I167" s="13"/>
-      <c r="J167" s="31"/>
-      <c r="K167" s="31"/>
+      <c r="J167" s="38"/>
+      <c r="K167" s="38"/>
     </row>
     <row r="168" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A168" s="13"/>
@@ -4091,8 +4141,8 @@
       <c r="G168" s="15"/>
       <c r="H168" s="13"/>
       <c r="I168" s="13"/>
-      <c r="J168" s="31"/>
-      <c r="K168" s="31"/>
+      <c r="J168" s="38"/>
+      <c r="K168" s="38"/>
     </row>
     <row r="169" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A169" s="13"/>
@@ -4104,8 +4154,8 @@
       <c r="G169" s="15"/>
       <c r="H169" s="13"/>
       <c r="I169" s="13"/>
-      <c r="J169" s="31"/>
-      <c r="K169" s="31"/>
+      <c r="J169" s="38"/>
+      <c r="K169" s="38"/>
     </row>
     <row r="170" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A170" s="13"/>
@@ -4117,8 +4167,8 @@
       <c r="G170" s="15"/>
       <c r="H170" s="13"/>
       <c r="I170" s="13"/>
-      <c r="J170" s="31"/>
-      <c r="K170" s="31"/>
+      <c r="J170" s="38"/>
+      <c r="K170" s="38"/>
     </row>
     <row r="171" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A171" s="13"/>
@@ -4130,8 +4180,8 @@
       <c r="G171" s="15"/>
       <c r="H171" s="13"/>
       <c r="I171" s="13"/>
-      <c r="J171" s="31"/>
-      <c r="K171" s="31"/>
+      <c r="J171" s="38"/>
+      <c r="K171" s="38"/>
     </row>
     <row r="172" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A172" s="13"/>
@@ -4143,8 +4193,8 @@
       <c r="G172" s="15"/>
       <c r="H172" s="13"/>
       <c r="I172" s="13"/>
-      <c r="J172" s="31"/>
-      <c r="K172" s="31"/>
+      <c r="J172" s="38"/>
+      <c r="K172" s="38"/>
     </row>
     <row r="173" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A173" s="13"/>
@@ -4156,8 +4206,8 @@
       <c r="G173" s="15"/>
       <c r="H173" s="13"/>
       <c r="I173" s="13"/>
-      <c r="J173" s="31"/>
-      <c r="K173" s="31"/>
+      <c r="J173" s="38"/>
+      <c r="K173" s="38"/>
     </row>
     <row r="174" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A174" s="13"/>
@@ -4169,8 +4219,8 @@
       <c r="G174" s="15"/>
       <c r="H174" s="13"/>
       <c r="I174" s="13"/>
-      <c r="J174" s="31"/>
-      <c r="K174" s="31"/>
+      <c r="J174" s="38"/>
+      <c r="K174" s="38"/>
     </row>
     <row r="175" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A175" s="13"/>
@@ -4182,8 +4232,8 @@
       <c r="G175" s="15"/>
       <c r="H175" s="13"/>
       <c r="I175" s="13"/>
-      <c r="J175" s="31"/>
-      <c r="K175" s="31"/>
+      <c r="J175" s="38"/>
+      <c r="K175" s="38"/>
     </row>
     <row r="176" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A176" s="13"/>
@@ -4195,8 +4245,8 @@
       <c r="G176" s="15"/>
       <c r="H176" s="13"/>
       <c r="I176" s="13"/>
-      <c r="J176" s="31"/>
-      <c r="K176" s="31"/>
+      <c r="J176" s="38"/>
+      <c r="K176" s="38"/>
     </row>
     <row r="177" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A177" s="13"/>
@@ -4208,8 +4258,8 @@
       <c r="G177" s="15"/>
       <c r="H177" s="13"/>
       <c r="I177" s="13"/>
-      <c r="J177" s="31"/>
-      <c r="K177" s="31"/>
+      <c r="J177" s="38"/>
+      <c r="K177" s="38"/>
     </row>
     <row r="178" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A178" s="13"/>
@@ -4221,8 +4271,8 @@
       <c r="G178" s="15"/>
       <c r="H178" s="13"/>
       <c r="I178" s="13"/>
-      <c r="J178" s="31"/>
-      <c r="K178" s="31"/>
+      <c r="J178" s="38"/>
+      <c r="K178" s="38"/>
     </row>
     <row r="179" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A179" s="13"/>
@@ -4234,8 +4284,8 @@
       <c r="G179" s="15"/>
       <c r="H179" s="13"/>
       <c r="I179" s="13"/>
-      <c r="J179" s="31"/>
-      <c r="K179" s="31"/>
+      <c r="J179" s="38"/>
+      <c r="K179" s="38"/>
     </row>
     <row r="180" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A180" s="13"/>
@@ -4247,8 +4297,8 @@
       <c r="G180" s="15"/>
       <c r="H180" s="13"/>
       <c r="I180" s="13"/>
-      <c r="J180" s="31"/>
-      <c r="K180" s="31"/>
+      <c r="J180" s="38"/>
+      <c r="K180" s="38"/>
     </row>
     <row r="181" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A181" s="13"/>
@@ -4260,8 +4310,8 @@
       <c r="G181" s="15"/>
       <c r="H181" s="13"/>
       <c r="I181" s="13"/>
-      <c r="J181" s="31"/>
-      <c r="K181" s="31"/>
+      <c r="J181" s="38"/>
+      <c r="K181" s="38"/>
     </row>
     <row r="182" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A182" s="13"/>
@@ -4273,8 +4323,8 @@
       <c r="G182" s="15"/>
       <c r="H182" s="13"/>
       <c r="I182" s="13"/>
-      <c r="J182" s="31"/>
-      <c r="K182" s="31"/>
+      <c r="J182" s="38"/>
+      <c r="K182" s="38"/>
     </row>
     <row r="183" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A183" s="13"/>
@@ -4286,8 +4336,8 @@
       <c r="G183" s="15"/>
       <c r="H183" s="13"/>
       <c r="I183" s="13"/>
-      <c r="J183" s="31"/>
-      <c r="K183" s="31"/>
+      <c r="J183" s="38"/>
+      <c r="K183" s="38"/>
     </row>
     <row r="184" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A184" s="13"/>
@@ -4299,8 +4349,8 @@
       <c r="G184" s="15"/>
       <c r="H184" s="13"/>
       <c r="I184" s="13"/>
-      <c r="J184" s="31"/>
-      <c r="K184" s="31"/>
+      <c r="J184" s="38"/>
+      <c r="K184" s="38"/>
     </row>
     <row r="185" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A185" s="13"/>
@@ -4312,8 +4362,8 @@
       <c r="G185" s="15"/>
       <c r="H185" s="13"/>
       <c r="I185" s="13"/>
-      <c r="J185" s="31"/>
-      <c r="K185" s="31"/>
+      <c r="J185" s="38"/>
+      <c r="K185" s="38"/>
     </row>
     <row r="186" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A186" s="13"/>
@@ -4325,8 +4375,8 @@
       <c r="G186" s="15"/>
       <c r="H186" s="13"/>
       <c r="I186" s="13"/>
-      <c r="J186" s="31"/>
-      <c r="K186" s="31"/>
+      <c r="J186" s="38"/>
+      <c r="K186" s="38"/>
     </row>
     <row r="187" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A187" s="13"/>
@@ -4338,8 +4388,8 @@
       <c r="G187" s="15"/>
       <c r="H187" s="13"/>
       <c r="I187" s="13"/>
-      <c r="J187" s="31"/>
-      <c r="K187" s="31"/>
+      <c r="J187" s="38"/>
+      <c r="K187" s="38"/>
     </row>
     <row r="188" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A188" s="13"/>
@@ -4351,8 +4401,8 @@
       <c r="G188" s="15"/>
       <c r="H188" s="13"/>
       <c r="I188" s="13"/>
-      <c r="J188" s="31"/>
-      <c r="K188" s="31"/>
+      <c r="J188" s="38"/>
+      <c r="K188" s="38"/>
     </row>
     <row r="189" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A189" s="13"/>
@@ -4364,8 +4414,8 @@
       <c r="G189" s="15"/>
       <c r="H189" s="13"/>
       <c r="I189" s="13"/>
-      <c r="J189" s="31"/>
-      <c r="K189" s="31"/>
+      <c r="J189" s="38"/>
+      <c r="K189" s="38"/>
     </row>
     <row r="190" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A190" s="13"/>
@@ -4377,8 +4427,8 @@
       <c r="G190" s="15"/>
       <c r="H190" s="13"/>
       <c r="I190" s="13"/>
-      <c r="J190" s="31"/>
-      <c r="K190" s="31"/>
+      <c r="J190" s="38"/>
+      <c r="K190" s="38"/>
     </row>
     <row r="191" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A191" s="13"/>
@@ -4390,8 +4440,8 @@
       <c r="G191" s="15"/>
       <c r="H191" s="13"/>
       <c r="I191" s="13"/>
-      <c r="J191" s="31"/>
-      <c r="K191" s="31"/>
+      <c r="J191" s="38"/>
+      <c r="K191" s="38"/>
     </row>
     <row r="192" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A192" s="13"/>
@@ -4403,8 +4453,8 @@
       <c r="G192" s="15"/>
       <c r="H192" s="13"/>
       <c r="I192" s="13"/>
-      <c r="J192" s="31"/>
-      <c r="K192" s="31"/>
+      <c r="J192" s="38"/>
+      <c r="K192" s="38"/>
     </row>
     <row r="193" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A193" s="13"/>
@@ -4416,8 +4466,8 @@
       <c r="G193" s="15"/>
       <c r="H193" s="13"/>
       <c r="I193" s="13"/>
-      <c r="J193" s="31"/>
-      <c r="K193" s="31"/>
+      <c r="J193" s="38"/>
+      <c r="K193" s="38"/>
     </row>
     <row r="194" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A194" s="13"/>
@@ -4429,8 +4479,8 @@
       <c r="G194" s="15"/>
       <c r="H194" s="13"/>
       <c r="I194" s="13"/>
-      <c r="J194" s="31"/>
-      <c r="K194" s="31"/>
+      <c r="J194" s="38"/>
+      <c r="K194" s="38"/>
     </row>
     <row r="195" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A195" s="13"/>
@@ -4442,8 +4492,8 @@
       <c r="G195" s="15"/>
       <c r="H195" s="13"/>
       <c r="I195" s="13"/>
-      <c r="J195" s="31"/>
-      <c r="K195" s="31"/>
+      <c r="J195" s="38"/>
+      <c r="K195" s="38"/>
     </row>
     <row r="196" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A196" s="13"/>
@@ -4455,8 +4505,8 @@
       <c r="G196" s="15"/>
       <c r="H196" s="13"/>
       <c r="I196" s="13"/>
-      <c r="J196" s="31"/>
-      <c r="K196" s="31"/>
+      <c r="J196" s="38"/>
+      <c r="K196" s="38"/>
     </row>
     <row r="197" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A197" s="13"/>
@@ -4468,8 +4518,8 @@
       <c r="G197" s="15"/>
       <c r="H197" s="13"/>
       <c r="I197" s="13"/>
-      <c r="J197" s="31"/>
-      <c r="K197" s="31"/>
+      <c r="J197" s="38"/>
+      <c r="K197" s="38"/>
     </row>
     <row r="198" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A198" s="13"/>
@@ -4481,8 +4531,8 @@
       <c r="G198" s="15"/>
       <c r="H198" s="13"/>
       <c r="I198" s="13"/>
-      <c r="J198" s="31"/>
-      <c r="K198" s="31"/>
+      <c r="J198" s="38"/>
+      <c r="K198" s="38"/>
     </row>
     <row r="199" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A199" s="13"/>
@@ -4494,8 +4544,8 @@
       <c r="G199" s="15"/>
       <c r="H199" s="13"/>
       <c r="I199" s="13"/>
-      <c r="J199" s="31"/>
-      <c r="K199" s="31"/>
+      <c r="J199" s="38"/>
+      <c r="K199" s="38"/>
     </row>
     <row r="200" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A200" s="13"/>
@@ -4507,8 +4557,8 @@
       <c r="G200" s="15"/>
       <c r="H200" s="13"/>
       <c r="I200" s="13"/>
-      <c r="J200" s="31"/>
-      <c r="K200" s="31"/>
+      <c r="J200" s="38"/>
+      <c r="K200" s="38"/>
     </row>
     <row r="201" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A201" s="13"/>
@@ -4520,8 +4570,8 @@
       <c r="G201" s="15"/>
       <c r="H201" s="13"/>
       <c r="I201" s="13"/>
-      <c r="J201" s="31"/>
-      <c r="K201" s="31"/>
+      <c r="J201" s="38"/>
+      <c r="K201" s="38"/>
     </row>
     <row r="202" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A202" s="13"/>
@@ -4533,8 +4583,8 @@
       <c r="G202" s="15"/>
       <c r="H202" s="13"/>
       <c r="I202" s="13"/>
-      <c r="J202" s="31"/>
-      <c r="K202" s="31"/>
+      <c r="J202" s="38"/>
+      <c r="K202" s="38"/>
     </row>
     <row r="203" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A203" s="13"/>
@@ -4546,8 +4596,8 @@
       <c r="G203" s="15"/>
       <c r="H203" s="13"/>
       <c r="I203" s="13"/>
-      <c r="J203" s="31"/>
-      <c r="K203" s="31"/>
+      <c r="J203" s="38"/>
+      <c r="K203" s="38"/>
     </row>
     <row r="204" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A204" s="13"/>
@@ -4559,8 +4609,8 @@
       <c r="G204" s="15"/>
       <c r="H204" s="13"/>
       <c r="I204" s="13"/>
-      <c r="J204" s="31"/>
-      <c r="K204" s="31"/>
+      <c r="J204" s="38"/>
+      <c r="K204" s="38"/>
     </row>
     <row r="205" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A205" s="13"/>
@@ -4572,8 +4622,8 @@
       <c r="G205" s="15"/>
       <c r="H205" s="13"/>
       <c r="I205" s="13"/>
-      <c r="J205" s="31"/>
-      <c r="K205" s="31"/>
+      <c r="J205" s="38"/>
+      <c r="K205" s="38"/>
     </row>
     <row r="206" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A206" s="13"/>
@@ -4585,8 +4635,8 @@
       <c r="G206" s="15"/>
       <c r="H206" s="13"/>
       <c r="I206" s="13"/>
-      <c r="J206" s="31"/>
-      <c r="K206" s="31"/>
+      <c r="J206" s="38"/>
+      <c r="K206" s="38"/>
     </row>
     <row r="207" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A207" s="13"/>
@@ -4598,8 +4648,8 @@
       <c r="G207" s="15"/>
       <c r="H207" s="13"/>
       <c r="I207" s="13"/>
-      <c r="J207" s="31"/>
-      <c r="K207" s="31"/>
+      <c r="J207" s="38"/>
+      <c r="K207" s="38"/>
     </row>
     <row r="208" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A208" s="13"/>
@@ -4611,8 +4661,8 @@
       <c r="G208" s="15"/>
       <c r="H208" s="13"/>
       <c r="I208" s="13"/>
-      <c r="J208" s="31"/>
-      <c r="K208" s="31"/>
+      <c r="J208" s="38"/>
+      <c r="K208" s="38"/>
     </row>
     <row r="209" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A209" s="13"/>
@@ -4624,8 +4674,8 @@
       <c r="G209" s="15"/>
       <c r="H209" s="13"/>
       <c r="I209" s="13"/>
-      <c r="J209" s="31"/>
-      <c r="K209" s="31"/>
+      <c r="J209" s="38"/>
+      <c r="K209" s="38"/>
     </row>
     <row r="210" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A210" s="13"/>
@@ -4637,8 +4687,8 @@
       <c r="G210" s="15"/>
       <c r="H210" s="13"/>
       <c r="I210" s="13"/>
-      <c r="J210" s="31"/>
-      <c r="K210" s="31"/>
+      <c r="J210" s="38"/>
+      <c r="K210" s="38"/>
     </row>
     <row r="211" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A211" s="13"/>
@@ -4650,8 +4700,8 @@
       <c r="G211" s="15"/>
       <c r="H211" s="13"/>
       <c r="I211" s="13"/>
-      <c r="J211" s="31"/>
-      <c r="K211" s="31"/>
+      <c r="J211" s="38"/>
+      <c r="K211" s="38"/>
     </row>
     <row r="212" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A212" s="13"/>
@@ -4663,8 +4713,8 @@
       <c r="G212" s="15"/>
       <c r="H212" s="13"/>
       <c r="I212" s="13"/>
-      <c r="J212" s="31"/>
-      <c r="K212" s="31"/>
+      <c r="J212" s="38"/>
+      <c r="K212" s="38"/>
     </row>
     <row r="213" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A213" s="13"/>
@@ -4676,8 +4726,8 @@
       <c r="G213" s="15"/>
       <c r="H213" s="13"/>
       <c r="I213" s="13"/>
-      <c r="J213" s="31"/>
-      <c r="K213" s="31"/>
+      <c r="J213" s="38"/>
+      <c r="K213" s="38"/>
     </row>
     <row r="214" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A214" s="13"/>
@@ -4689,8 +4739,8 @@
       <c r="G214" s="15"/>
       <c r="H214" s="13"/>
       <c r="I214" s="13"/>
-      <c r="J214" s="31"/>
-      <c r="K214" s="31"/>
+      <c r="J214" s="38"/>
+      <c r="K214" s="38"/>
     </row>
     <row r="215" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A215" s="13"/>
@@ -4702,8 +4752,8 @@
       <c r="G215" s="15"/>
       <c r="H215" s="13"/>
       <c r="I215" s="13"/>
-      <c r="J215" s="31"/>
-      <c r="K215" s="31"/>
+      <c r="J215" s="38"/>
+      <c r="K215" s="38"/>
     </row>
     <row r="216" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A216" s="13"/>
@@ -4715,8 +4765,8 @@
       <c r="G216" s="15"/>
       <c r="H216" s="13"/>
       <c r="I216" s="13"/>
-      <c r="J216" s="31"/>
-      <c r="K216" s="31"/>
+      <c r="J216" s="38"/>
+      <c r="K216" s="38"/>
     </row>
     <row r="217" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A217" s="13"/>
@@ -4728,8 +4778,8 @@
       <c r="G217" s="15"/>
       <c r="H217" s="13"/>
       <c r="I217" s="13"/>
-      <c r="J217" s="31"/>
-      <c r="K217" s="31"/>
+      <c r="J217" s="38"/>
+      <c r="K217" s="38"/>
     </row>
     <row r="218" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A218" s="13"/>
@@ -4741,8 +4791,8 @@
       <c r="G218" s="15"/>
       <c r="H218" s="13"/>
       <c r="I218" s="13"/>
-      <c r="J218" s="31"/>
-      <c r="K218" s="31"/>
+      <c r="J218" s="38"/>
+      <c r="K218" s="38"/>
     </row>
     <row r="219" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A219" s="13"/>
@@ -4754,8 +4804,8 @@
       <c r="G219" s="15"/>
       <c r="H219" s="13"/>
       <c r="I219" s="13"/>
-      <c r="J219" s="31"/>
-      <c r="K219" s="31"/>
+      <c r="J219" s="38"/>
+      <c r="K219" s="38"/>
     </row>
     <row r="220" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A220" s="13"/>
@@ -4767,8 +4817,8 @@
       <c r="G220" s="15"/>
       <c r="H220" s="13"/>
       <c r="I220" s="13"/>
-      <c r="J220" s="31"/>
-      <c r="K220" s="31"/>
+      <c r="J220" s="38"/>
+      <c r="K220" s="38"/>
     </row>
     <row r="221" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A221" s="13"/>
@@ -4780,8 +4830,8 @@
       <c r="G221" s="15"/>
       <c r="H221" s="13"/>
       <c r="I221" s="13"/>
-      <c r="J221" s="31"/>
-      <c r="K221" s="31"/>
+      <c r="J221" s="38"/>
+      <c r="K221" s="38"/>
     </row>
     <row r="222" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A222" s="13"/>
@@ -4793,8 +4843,8 @@
       <c r="G222" s="15"/>
       <c r="H222" s="13"/>
       <c r="I222" s="13"/>
-      <c r="J222" s="31"/>
-      <c r="K222" s="31"/>
+      <c r="J222" s="38"/>
+      <c r="K222" s="38"/>
     </row>
     <row r="223" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A223" s="13"/>
@@ -4806,8 +4856,8 @@
       <c r="G223" s="15"/>
       <c r="H223" s="13"/>
       <c r="I223" s="13"/>
-      <c r="J223" s="31"/>
-      <c r="K223" s="31"/>
+      <c r="J223" s="38"/>
+      <c r="K223" s="38"/>
     </row>
     <row r="224" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A224" s="13"/>
@@ -4819,8 +4869,8 @@
       <c r="G224" s="15"/>
       <c r="H224" s="13"/>
       <c r="I224" s="13"/>
-      <c r="J224" s="31"/>
-      <c r="K224" s="31"/>
+      <c r="J224" s="38"/>
+      <c r="K224" s="38"/>
     </row>
     <row r="225" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A225" s="13"/>
@@ -4832,8 +4882,8 @@
       <c r="G225" s="15"/>
       <c r="H225" s="13"/>
       <c r="I225" s="13"/>
-      <c r="J225" s="31"/>
-      <c r="K225" s="31"/>
+      <c r="J225" s="38"/>
+      <c r="K225" s="38"/>
     </row>
     <row r="226" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A226" s="13"/>
@@ -4845,8 +4895,8 @@
       <c r="G226" s="15"/>
       <c r="H226" s="13"/>
       <c r="I226" s="13"/>
-      <c r="J226" s="31"/>
-      <c r="K226" s="31"/>
+      <c r="J226" s="38"/>
+      <c r="K226" s="38"/>
     </row>
     <row r="227" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A227" s="13"/>
@@ -4858,8 +4908,8 @@
       <c r="G227" s="15"/>
       <c r="H227" s="13"/>
       <c r="I227" s="13"/>
-      <c r="J227" s="31"/>
-      <c r="K227" s="31"/>
+      <c r="J227" s="38"/>
+      <c r="K227" s="38"/>
     </row>
     <row r="228" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A228" s="13"/>
@@ -4871,8 +4921,8 @@
       <c r="G228" s="15"/>
       <c r="H228" s="13"/>
       <c r="I228" s="13"/>
-      <c r="J228" s="31"/>
-      <c r="K228" s="31"/>
+      <c r="J228" s="38"/>
+      <c r="K228" s="38"/>
     </row>
     <row r="229" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A229" s="13"/>
@@ -4884,8 +4934,8 @@
       <c r="G229" s="15"/>
       <c r="H229" s="13"/>
       <c r="I229" s="13"/>
-      <c r="J229" s="31"/>
-      <c r="K229" s="31"/>
+      <c r="J229" s="38"/>
+      <c r="K229" s="38"/>
     </row>
     <row r="230" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A230" s="13"/>
@@ -4897,8 +4947,8 @@
       <c r="G230" s="15"/>
       <c r="H230" s="13"/>
       <c r="I230" s="13"/>
-      <c r="J230" s="31"/>
-      <c r="K230" s="31"/>
+      <c r="J230" s="38"/>
+      <c r="K230" s="38"/>
     </row>
     <row r="231" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A231" s="13"/>
@@ -4910,8 +4960,8 @@
       <c r="G231" s="15"/>
       <c r="H231" s="13"/>
       <c r="I231" s="13"/>
-      <c r="J231" s="31"/>
-      <c r="K231" s="31"/>
+      <c r="J231" s="38"/>
+      <c r="K231" s="38"/>
     </row>
     <row r="232" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G232" s="2"/>
@@ -6939,21 +6989,321 @@
       <c r="G906" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="287">
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="A60:K60"/>
+  <mergeCells count="352">
+    <mergeCell ref="H128:I128"/>
+    <mergeCell ref="H129:I129"/>
+    <mergeCell ref="H119:I119"/>
+    <mergeCell ref="H120:I120"/>
+    <mergeCell ref="H121:I121"/>
+    <mergeCell ref="H122:I122"/>
+    <mergeCell ref="H123:I123"/>
+    <mergeCell ref="H124:I124"/>
+    <mergeCell ref="H125:I125"/>
+    <mergeCell ref="H126:I126"/>
+    <mergeCell ref="H127:I127"/>
+    <mergeCell ref="H110:I110"/>
+    <mergeCell ref="H111:I111"/>
+    <mergeCell ref="H112:I112"/>
+    <mergeCell ref="H113:I113"/>
+    <mergeCell ref="H114:I114"/>
+    <mergeCell ref="H115:I115"/>
+    <mergeCell ref="H116:I116"/>
+    <mergeCell ref="H117:I117"/>
+    <mergeCell ref="H118:I118"/>
+    <mergeCell ref="H101:I101"/>
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="H103:I103"/>
+    <mergeCell ref="H104:I104"/>
+    <mergeCell ref="H105:I105"/>
+    <mergeCell ref="H106:I106"/>
+    <mergeCell ref="H107:I107"/>
+    <mergeCell ref="H108:I108"/>
+    <mergeCell ref="H109:I109"/>
+    <mergeCell ref="H92:I92"/>
+    <mergeCell ref="H93:I93"/>
+    <mergeCell ref="H94:I94"/>
+    <mergeCell ref="H95:I95"/>
+    <mergeCell ref="H96:I96"/>
+    <mergeCell ref="H97:I97"/>
+    <mergeCell ref="H98:I98"/>
+    <mergeCell ref="H99:I99"/>
+    <mergeCell ref="H100:I100"/>
+    <mergeCell ref="H83:I83"/>
+    <mergeCell ref="H84:I84"/>
+    <mergeCell ref="H85:I85"/>
+    <mergeCell ref="H86:I86"/>
+    <mergeCell ref="H87:I87"/>
+    <mergeCell ref="H88:I88"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="H90:I90"/>
+    <mergeCell ref="H91:I91"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="H78:I78"/>
+    <mergeCell ref="H79:I79"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="H82:I82"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="H68:I68"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="J230:K230"/>
+    <mergeCell ref="J231:K231"/>
+    <mergeCell ref="J221:K221"/>
+    <mergeCell ref="J222:K222"/>
+    <mergeCell ref="J223:K223"/>
+    <mergeCell ref="J224:K224"/>
+    <mergeCell ref="J225:K225"/>
+    <mergeCell ref="J226:K226"/>
+    <mergeCell ref="J227:K227"/>
+    <mergeCell ref="J228:K228"/>
+    <mergeCell ref="J229:K229"/>
+    <mergeCell ref="J212:K212"/>
+    <mergeCell ref="J213:K213"/>
+    <mergeCell ref="J214:K214"/>
+    <mergeCell ref="J215:K215"/>
+    <mergeCell ref="J216:K216"/>
+    <mergeCell ref="J217:K217"/>
+    <mergeCell ref="J218:K218"/>
+    <mergeCell ref="J219:K219"/>
+    <mergeCell ref="J220:K220"/>
+    <mergeCell ref="J203:K203"/>
+    <mergeCell ref="J204:K204"/>
+    <mergeCell ref="J205:K205"/>
+    <mergeCell ref="J206:K206"/>
+    <mergeCell ref="J207:K207"/>
+    <mergeCell ref="J208:K208"/>
+    <mergeCell ref="J209:K209"/>
+    <mergeCell ref="J210:K210"/>
+    <mergeCell ref="J211:K211"/>
+    <mergeCell ref="J194:K194"/>
+    <mergeCell ref="J195:K195"/>
+    <mergeCell ref="J196:K196"/>
+    <mergeCell ref="J197:K197"/>
+    <mergeCell ref="J198:K198"/>
+    <mergeCell ref="J199:K199"/>
+    <mergeCell ref="J200:K200"/>
+    <mergeCell ref="J201:K201"/>
+    <mergeCell ref="J202:K202"/>
+    <mergeCell ref="J185:K185"/>
+    <mergeCell ref="J186:K186"/>
+    <mergeCell ref="J187:K187"/>
+    <mergeCell ref="J188:K188"/>
+    <mergeCell ref="J189:K189"/>
+    <mergeCell ref="J190:K190"/>
+    <mergeCell ref="J191:K191"/>
+    <mergeCell ref="J192:K192"/>
+    <mergeCell ref="J193:K193"/>
+    <mergeCell ref="J176:K176"/>
+    <mergeCell ref="J177:K177"/>
+    <mergeCell ref="J178:K178"/>
+    <mergeCell ref="J179:K179"/>
+    <mergeCell ref="J180:K180"/>
+    <mergeCell ref="J181:K181"/>
+    <mergeCell ref="J182:K182"/>
+    <mergeCell ref="J183:K183"/>
+    <mergeCell ref="J184:K184"/>
+    <mergeCell ref="J167:K167"/>
+    <mergeCell ref="J168:K168"/>
+    <mergeCell ref="J169:K169"/>
+    <mergeCell ref="J170:K170"/>
+    <mergeCell ref="J171:K171"/>
+    <mergeCell ref="J172:K172"/>
+    <mergeCell ref="J173:K173"/>
+    <mergeCell ref="J174:K174"/>
+    <mergeCell ref="J175:K175"/>
+    <mergeCell ref="J158:K158"/>
+    <mergeCell ref="J159:K159"/>
+    <mergeCell ref="J160:K160"/>
+    <mergeCell ref="J161:K161"/>
+    <mergeCell ref="J162:K162"/>
+    <mergeCell ref="J163:K163"/>
+    <mergeCell ref="J164:K164"/>
+    <mergeCell ref="J165:K165"/>
+    <mergeCell ref="J166:K166"/>
+    <mergeCell ref="J149:K149"/>
+    <mergeCell ref="J150:K150"/>
+    <mergeCell ref="J151:K151"/>
+    <mergeCell ref="J152:K152"/>
+    <mergeCell ref="J153:K153"/>
+    <mergeCell ref="J154:K154"/>
+    <mergeCell ref="J155:K155"/>
+    <mergeCell ref="J156:K156"/>
+    <mergeCell ref="J157:K157"/>
+    <mergeCell ref="J140:K140"/>
+    <mergeCell ref="J141:K141"/>
+    <mergeCell ref="J142:K142"/>
+    <mergeCell ref="J143:K143"/>
+    <mergeCell ref="J144:K144"/>
+    <mergeCell ref="J145:K145"/>
+    <mergeCell ref="J146:K146"/>
+    <mergeCell ref="J147:K147"/>
+    <mergeCell ref="J148:K148"/>
+    <mergeCell ref="J131:K131"/>
+    <mergeCell ref="J132:K132"/>
+    <mergeCell ref="J133:K133"/>
+    <mergeCell ref="J134:K134"/>
+    <mergeCell ref="J135:K135"/>
+    <mergeCell ref="J136:K136"/>
+    <mergeCell ref="J137:K137"/>
+    <mergeCell ref="J138:K138"/>
+    <mergeCell ref="J139:K139"/>
+    <mergeCell ref="J122:K122"/>
+    <mergeCell ref="J123:K123"/>
+    <mergeCell ref="J124:K124"/>
+    <mergeCell ref="J125:K125"/>
+    <mergeCell ref="J126:K126"/>
+    <mergeCell ref="J127:K127"/>
+    <mergeCell ref="J128:K128"/>
+    <mergeCell ref="J129:K129"/>
+    <mergeCell ref="J130:K130"/>
+    <mergeCell ref="J113:K113"/>
+    <mergeCell ref="J114:K114"/>
+    <mergeCell ref="J115:K115"/>
+    <mergeCell ref="J116:K116"/>
+    <mergeCell ref="J117:K117"/>
+    <mergeCell ref="J118:K118"/>
+    <mergeCell ref="J119:K119"/>
+    <mergeCell ref="J120:K120"/>
+    <mergeCell ref="J121:K121"/>
+    <mergeCell ref="J104:K104"/>
+    <mergeCell ref="J105:K105"/>
+    <mergeCell ref="J106:K106"/>
+    <mergeCell ref="J107:K107"/>
+    <mergeCell ref="J108:K108"/>
+    <mergeCell ref="J109:K109"/>
+    <mergeCell ref="J110:K110"/>
+    <mergeCell ref="J111:K111"/>
+    <mergeCell ref="J112:K112"/>
+    <mergeCell ref="J95:K95"/>
+    <mergeCell ref="J96:K96"/>
+    <mergeCell ref="J97:K97"/>
+    <mergeCell ref="J98:K98"/>
+    <mergeCell ref="J99:K99"/>
+    <mergeCell ref="J100:K100"/>
+    <mergeCell ref="J101:K101"/>
+    <mergeCell ref="J102:K102"/>
+    <mergeCell ref="J103:K103"/>
+    <mergeCell ref="J88:K88"/>
+    <mergeCell ref="J89:K89"/>
+    <mergeCell ref="J73:K73"/>
+    <mergeCell ref="J74:K74"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="J75:K75"/>
+    <mergeCell ref="J76:K76"/>
+    <mergeCell ref="J77:K77"/>
+    <mergeCell ref="J78:K78"/>
+    <mergeCell ref="J79:K79"/>
+    <mergeCell ref="J80:K80"/>
+    <mergeCell ref="J55:K55"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="J59:K59"/>
+    <mergeCell ref="J61:K61"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="J63:K63"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J90:K90"/>
+    <mergeCell ref="J91:K91"/>
+    <mergeCell ref="J92:K92"/>
+    <mergeCell ref="J93:K93"/>
+    <mergeCell ref="J94:K94"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J71:K71"/>
+    <mergeCell ref="J72:K72"/>
+    <mergeCell ref="J81:K81"/>
+    <mergeCell ref="J82:K82"/>
+    <mergeCell ref="J83:K83"/>
+    <mergeCell ref="J84:K84"/>
+    <mergeCell ref="J85:K85"/>
+    <mergeCell ref="J86:K86"/>
+    <mergeCell ref="J87:K87"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="J52:K52"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="A27:K27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A20:K20"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
     <mergeCell ref="H36:I36"/>
     <mergeCell ref="H37:I37"/>
     <mergeCell ref="H38:I38"/>
@@ -6978,255 +7328,20 @@
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A20:K20"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="A27:K27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="J52:K52"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="J51:K51"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="J90:K90"/>
-    <mergeCell ref="J91:K91"/>
-    <mergeCell ref="J92:K92"/>
-    <mergeCell ref="J93:K93"/>
-    <mergeCell ref="J94:K94"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J67:K67"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="J71:K71"/>
-    <mergeCell ref="J72:K72"/>
-    <mergeCell ref="J81:K81"/>
-    <mergeCell ref="J82:K82"/>
-    <mergeCell ref="J83:K83"/>
-    <mergeCell ref="J84:K84"/>
-    <mergeCell ref="J85:K85"/>
-    <mergeCell ref="J86:K86"/>
-    <mergeCell ref="J87:K87"/>
-    <mergeCell ref="J88:K88"/>
-    <mergeCell ref="J89:K89"/>
-    <mergeCell ref="J73:K73"/>
-    <mergeCell ref="J74:K74"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="J75:K75"/>
-    <mergeCell ref="J76:K76"/>
-    <mergeCell ref="J77:K77"/>
-    <mergeCell ref="J78:K78"/>
-    <mergeCell ref="J79:K79"/>
-    <mergeCell ref="J80:K80"/>
-    <mergeCell ref="J55:K55"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="J59:K59"/>
-    <mergeCell ref="J61:K61"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="J63:K63"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="J95:K95"/>
-    <mergeCell ref="J96:K96"/>
-    <mergeCell ref="J97:K97"/>
-    <mergeCell ref="J98:K98"/>
-    <mergeCell ref="J99:K99"/>
-    <mergeCell ref="J100:K100"/>
-    <mergeCell ref="J101:K101"/>
-    <mergeCell ref="J102:K102"/>
-    <mergeCell ref="J103:K103"/>
-    <mergeCell ref="J104:K104"/>
-    <mergeCell ref="J105:K105"/>
-    <mergeCell ref="J106:K106"/>
-    <mergeCell ref="J107:K107"/>
-    <mergeCell ref="J108:K108"/>
-    <mergeCell ref="J109:K109"/>
-    <mergeCell ref="J110:K110"/>
-    <mergeCell ref="J111:K111"/>
-    <mergeCell ref="J112:K112"/>
-    <mergeCell ref="J113:K113"/>
-    <mergeCell ref="J114:K114"/>
-    <mergeCell ref="J115:K115"/>
-    <mergeCell ref="J116:K116"/>
-    <mergeCell ref="J117:K117"/>
-    <mergeCell ref="J118:K118"/>
-    <mergeCell ref="J119:K119"/>
-    <mergeCell ref="J120:K120"/>
-    <mergeCell ref="J121:K121"/>
-    <mergeCell ref="J122:K122"/>
-    <mergeCell ref="J123:K123"/>
-    <mergeCell ref="J124:K124"/>
-    <mergeCell ref="J125:K125"/>
-    <mergeCell ref="J126:K126"/>
-    <mergeCell ref="J127:K127"/>
-    <mergeCell ref="J128:K128"/>
-    <mergeCell ref="J129:K129"/>
-    <mergeCell ref="J130:K130"/>
-    <mergeCell ref="J131:K131"/>
-    <mergeCell ref="J132:K132"/>
-    <mergeCell ref="J133:K133"/>
-    <mergeCell ref="J134:K134"/>
-    <mergeCell ref="J135:K135"/>
-    <mergeCell ref="J136:K136"/>
-    <mergeCell ref="J137:K137"/>
-    <mergeCell ref="J138:K138"/>
-    <mergeCell ref="J139:K139"/>
-    <mergeCell ref="J140:K140"/>
-    <mergeCell ref="J141:K141"/>
-    <mergeCell ref="J142:K142"/>
-    <mergeCell ref="J143:K143"/>
-    <mergeCell ref="J144:K144"/>
-    <mergeCell ref="J145:K145"/>
-    <mergeCell ref="J146:K146"/>
-    <mergeCell ref="J147:K147"/>
-    <mergeCell ref="J148:K148"/>
-    <mergeCell ref="J149:K149"/>
-    <mergeCell ref="J150:K150"/>
-    <mergeCell ref="J151:K151"/>
-    <mergeCell ref="J152:K152"/>
-    <mergeCell ref="J153:K153"/>
-    <mergeCell ref="J154:K154"/>
-    <mergeCell ref="J155:K155"/>
-    <mergeCell ref="J156:K156"/>
-    <mergeCell ref="J157:K157"/>
-    <mergeCell ref="J158:K158"/>
-    <mergeCell ref="J159:K159"/>
-    <mergeCell ref="J160:K160"/>
-    <mergeCell ref="J161:K161"/>
-    <mergeCell ref="J162:K162"/>
-    <mergeCell ref="J163:K163"/>
-    <mergeCell ref="J164:K164"/>
-    <mergeCell ref="J165:K165"/>
-    <mergeCell ref="J166:K166"/>
-    <mergeCell ref="J167:K167"/>
-    <mergeCell ref="J168:K168"/>
-    <mergeCell ref="J169:K169"/>
-    <mergeCell ref="J170:K170"/>
-    <mergeCell ref="J171:K171"/>
-    <mergeCell ref="J172:K172"/>
-    <mergeCell ref="J173:K173"/>
-    <mergeCell ref="J174:K174"/>
-    <mergeCell ref="J175:K175"/>
-    <mergeCell ref="J176:K176"/>
-    <mergeCell ref="J177:K177"/>
-    <mergeCell ref="J178:K178"/>
-    <mergeCell ref="J179:K179"/>
-    <mergeCell ref="J180:K180"/>
-    <mergeCell ref="J181:K181"/>
-    <mergeCell ref="J182:K182"/>
-    <mergeCell ref="J183:K183"/>
-    <mergeCell ref="J184:K184"/>
-    <mergeCell ref="J185:K185"/>
-    <mergeCell ref="J186:K186"/>
-    <mergeCell ref="J187:K187"/>
-    <mergeCell ref="J188:K188"/>
-    <mergeCell ref="J189:K189"/>
-    <mergeCell ref="J190:K190"/>
-    <mergeCell ref="J191:K191"/>
-    <mergeCell ref="J192:K192"/>
-    <mergeCell ref="J193:K193"/>
-    <mergeCell ref="J194:K194"/>
-    <mergeCell ref="J195:K195"/>
-    <mergeCell ref="J196:K196"/>
-    <mergeCell ref="J197:K197"/>
-    <mergeCell ref="J198:K198"/>
-    <mergeCell ref="J199:K199"/>
-    <mergeCell ref="J200:K200"/>
-    <mergeCell ref="J201:K201"/>
-    <mergeCell ref="J202:K202"/>
-    <mergeCell ref="J203:K203"/>
-    <mergeCell ref="J204:K204"/>
-    <mergeCell ref="J205:K205"/>
-    <mergeCell ref="J206:K206"/>
-    <mergeCell ref="J207:K207"/>
-    <mergeCell ref="J208:K208"/>
-    <mergeCell ref="J209:K209"/>
-    <mergeCell ref="J210:K210"/>
-    <mergeCell ref="J211:K211"/>
-    <mergeCell ref="J212:K212"/>
-    <mergeCell ref="J213:K213"/>
-    <mergeCell ref="J214:K214"/>
-    <mergeCell ref="J215:K215"/>
-    <mergeCell ref="J216:K216"/>
-    <mergeCell ref="J217:K217"/>
-    <mergeCell ref="J218:K218"/>
-    <mergeCell ref="J219:K219"/>
-    <mergeCell ref="J220:K220"/>
-    <mergeCell ref="J230:K230"/>
-    <mergeCell ref="J231:K231"/>
-    <mergeCell ref="J221:K221"/>
-    <mergeCell ref="J222:K222"/>
-    <mergeCell ref="J223:K223"/>
-    <mergeCell ref="J224:K224"/>
-    <mergeCell ref="J225:K225"/>
-    <mergeCell ref="J226:K226"/>
-    <mergeCell ref="J227:K227"/>
-    <mergeCell ref="J228:K228"/>
-    <mergeCell ref="J229:K229"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="A60:K60"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Doc: Added Review comments for login and checkout pages
</commit_message>
<xml_diff>
--- a/Requirments/Review.xlsx
+++ b/Requirments/Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Requirments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CD1ED2-2FF2-4874-B4D5-3628277262C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1445C2B-C116-475F-8264-128BADA17388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="167">
   <si>
     <t>ID</t>
   </si>
@@ -506,6 +506,24 @@
   </si>
   <si>
     <t>Wireframe_Cart_005</t>
+  </si>
+  <si>
+    <t>Review_WF_Login_001</t>
+  </si>
+  <si>
+    <t>WireFrame_Login_002</t>
+  </si>
+  <si>
+    <t>Error message that should appear is Invalid username or Invalid password</t>
+  </si>
+  <si>
+    <t>5d5877d0f97c7ecefcf740d9e9d64c986b956837</t>
+  </si>
+  <si>
+    <t>Review_WF_Checkout_001</t>
+  </si>
+  <si>
+    <t>15849adea70087036301ed14388dce50211b8045</t>
   </si>
 </sst>
 </file>
@@ -796,12 +814,17 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -810,26 +833,21 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1057,8 +1075,8 @@
   </sheetPr>
   <dimension ref="A1:AC906"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="M65" sqref="M65"/>
+    <sheetView tabSelected="1" topLeftCell="B59" workbookViewId="0">
+      <selection activeCell="J67" sqref="J67:K67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1097,14 +1115,14 @@
       <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="37"/>
-      <c r="J1" s="36" t="s">
+      <c r="I1" s="46"/>
+      <c r="J1" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="K1" s="37"/>
+      <c r="K1" s="46"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -1125,19 +1143,19 @@
       <c r="AC1" s="1"/>
     </row>
     <row r="2" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -1179,12 +1197,12 @@
       <c r="G3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="40"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="38" t="s">
+      <c r="H3" s="42"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="K3" s="38"/>
+      <c r="K3" s="32"/>
     </row>
     <row r="4" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
@@ -1208,12 +1226,12 @@
       <c r="G4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="40"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="38" t="s">
+      <c r="H4" s="42"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="K4" s="38"/>
+      <c r="K4" s="32"/>
     </row>
     <row r="5" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
@@ -1237,12 +1255,12 @@
       <c r="G5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="40"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="38" t="s">
+      <c r="H5" s="42"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="K5" s="38"/>
+      <c r="K5" s="32"/>
     </row>
     <row r="6" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
@@ -1266,12 +1284,12 @@
       <c r="G6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="40"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="38" t="s">
+      <c r="H6" s="42"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="K6" s="38"/>
+      <c r="K6" s="32"/>
     </row>
     <row r="7" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -1295,12 +1313,12 @@
       <c r="G7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="40"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="38" t="s">
+      <c r="H7" s="42"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="K7" s="38"/>
+      <c r="K7" s="32"/>
     </row>
     <row r="8" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
@@ -1324,12 +1342,12 @@
       <c r="G8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="40"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="38" t="s">
+      <c r="H8" s="42"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="K8" s="38"/>
+      <c r="K8" s="32"/>
     </row>
     <row r="9" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
@@ -1353,12 +1371,12 @@
       <c r="G9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="40"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="38" t="s">
+      <c r="H9" s="42"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="K9" s="38"/>
+      <c r="K9" s="32"/>
     </row>
     <row r="10" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
@@ -1382,12 +1400,12 @@
       <c r="G10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="40"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="38" t="s">
+      <c r="H10" s="42"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="K10" s="38"/>
+      <c r="K10" s="32"/>
     </row>
     <row r="11" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
@@ -1411,12 +1429,12 @@
       <c r="G11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="40"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="38" t="s">
+      <c r="H11" s="42"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="K11" s="38"/>
+      <c r="K11" s="32"/>
     </row>
     <row r="12" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
@@ -1440,12 +1458,12 @@
       <c r="G12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="40"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="38" t="s">
+      <c r="H12" s="42"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="K12" s="38"/>
+      <c r="K12" s="32"/>
     </row>
     <row r="13" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
@@ -1469,12 +1487,12 @@
       <c r="G13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="40"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="38" t="s">
+      <c r="H13" s="42"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="K13" s="38"/>
+      <c r="K13" s="32"/>
     </row>
     <row r="14" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
@@ -1498,12 +1516,12 @@
       <c r="G14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="40"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="38" t="s">
+      <c r="H14" s="42"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="K14" s="38"/>
+      <c r="K14" s="32"/>
     </row>
     <row r="15" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
@@ -1525,12 +1543,12 @@
       <c r="G15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="40"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="38" t="s">
+      <c r="H15" s="42"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="38"/>
+      <c r="K15" s="32"/>
     </row>
     <row r="16" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
@@ -1554,12 +1572,12 @@
       <c r="G16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="40"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="38" t="s">
+      <c r="H16" s="42"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="K16" s="38"/>
+      <c r="K16" s="32"/>
     </row>
     <row r="17" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
@@ -1583,12 +1601,12 @@
       <c r="G17" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="40"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="38" t="s">
+      <c r="H17" s="42"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="38"/>
+      <c r="K17" s="32"/>
     </row>
     <row r="18" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
@@ -1612,12 +1630,12 @@
       <c r="G18" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="40"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="38" t="s">
+      <c r="H18" s="42"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="38"/>
+      <c r="K18" s="32"/>
     </row>
     <row r="19" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
@@ -1641,27 +1659,27 @@
       <c r="G19" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="40"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="38" t="s">
+      <c r="H19" s="42"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="K19" s="38"/>
+      <c r="K19" s="32"/>
     </row>
     <row r="20" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="35"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="38"/>
     </row>
     <row r="21" spans="1:11" s="16" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
@@ -1685,14 +1703,14 @@
       <c r="G21" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H21" s="30" t="s">
+      <c r="H21" s="44" t="s">
         <v>72</v>
       </c>
       <c r="I21" s="31"/>
-      <c r="J21" s="38" t="s">
+      <c r="J21" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="K21" s="38"/>
+      <c r="K21" s="32"/>
     </row>
     <row r="22" spans="1:11" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
@@ -1716,12 +1734,12 @@
       <c r="G22" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="32"/>
+      <c r="H22" s="30"/>
       <c r="I22" s="31"/>
-      <c r="J22" s="38" t="s">
+      <c r="J22" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="K22" s="38"/>
+      <c r="K22" s="32"/>
     </row>
     <row r="23" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
@@ -1745,14 +1763,14 @@
       <c r="G23" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="32" t="s">
+      <c r="H23" s="30" t="s">
         <v>73</v>
       </c>
       <c r="I23" s="31"/>
-      <c r="J23" s="38" t="s">
+      <c r="J23" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="K23" s="38"/>
+      <c r="K23" s="32"/>
     </row>
     <row r="24" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
@@ -1780,10 +1798,10 @@
         <v>74</v>
       </c>
       <c r="I24" s="25"/>
-      <c r="J24" s="38" t="s">
+      <c r="J24" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="K24" s="38"/>
+      <c r="K24" s="32"/>
     </row>
     <row r="25" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
@@ -1807,14 +1825,14 @@
       <c r="G25" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="32" t="s">
+      <c r="H25" s="30" t="s">
         <v>76</v>
       </c>
       <c r="I25" s="31"/>
-      <c r="J25" s="38" t="s">
+      <c r="J25" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="K25" s="38"/>
+      <c r="K25" s="32"/>
     </row>
     <row r="26" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
@@ -1838,27 +1856,27 @@
       <c r="G26" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H26" s="32"/>
+      <c r="H26" s="30"/>
       <c r="I26" s="31"/>
-      <c r="J26" s="38" t="s">
+      <c r="J26" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="K26" s="38"/>
+      <c r="K26" s="32"/>
     </row>
     <row r="27" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="35"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="38"/>
     </row>
     <row r="28" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
@@ -1882,12 +1900,12 @@
       <c r="G28" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H28" s="43"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="43" t="s">
+      <c r="H28" s="39"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="K28" s="44"/>
+      <c r="K28" s="40"/>
     </row>
     <row r="29" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
@@ -1911,14 +1929,14 @@
       <c r="G29" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="32" t="s">
+      <c r="H29" s="30" t="s">
         <v>90</v>
       </c>
       <c r="I29" s="31"/>
-      <c r="J29" s="39" t="s">
+      <c r="J29" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="K29" s="38"/>
+      <c r="K29" s="32"/>
     </row>
     <row r="30" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
@@ -1942,12 +1960,12 @@
       <c r="G30" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H30" s="32"/>
+      <c r="H30" s="30"/>
       <c r="I30" s="31"/>
-      <c r="J30" s="38" t="s">
+      <c r="J30" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="K30" s="38"/>
+      <c r="K30" s="32"/>
     </row>
     <row r="31" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
@@ -1973,10 +1991,10 @@
       </c>
       <c r="H31" s="24"/>
       <c r="I31" s="25"/>
-      <c r="J31" s="45" t="s">
+      <c r="J31" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="K31" s="44"/>
+      <c r="K31" s="40"/>
     </row>
     <row r="32" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
@@ -2000,27 +2018,27 @@
       <c r="G32" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H32" s="32"/>
+      <c r="H32" s="30"/>
       <c r="I32" s="31"/>
-      <c r="J32" s="38" t="s">
+      <c r="J32" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="K32" s="38"/>
+      <c r="K32" s="32"/>
     </row>
     <row r="33" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="35"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="38"/>
     </row>
     <row r="34" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
@@ -2044,12 +2062,12 @@
       <c r="G34" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H34" s="32"/>
+      <c r="H34" s="30"/>
       <c r="I34" s="31"/>
-      <c r="J34" s="39" t="s">
+      <c r="J34" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="K34" s="38"/>
+      <c r="K34" s="32"/>
     </row>
     <row r="35" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
@@ -2073,7 +2091,7 @@
       <c r="G35" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H35" s="32"/>
+      <c r="H35" s="30"/>
       <c r="I35" s="31"/>
       <c r="J35" s="28" t="s">
         <v>94</v>
@@ -2101,12 +2119,12 @@
       <c r="G36" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H36" s="32"/>
+      <c r="H36" s="30"/>
       <c r="I36" s="31"/>
-      <c r="J36" s="39" t="s">
+      <c r="J36" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="K36" s="38"/>
+      <c r="K36" s="32"/>
     </row>
     <row r="37" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
@@ -2130,12 +2148,12 @@
       <c r="G37" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H37" s="32"/>
+      <c r="H37" s="30"/>
       <c r="I37" s="31"/>
-      <c r="J37" s="39" t="s">
+      <c r="J37" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="K37" s="38"/>
+      <c r="K37" s="32"/>
     </row>
     <row r="38" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
@@ -2159,12 +2177,12 @@
       <c r="G38" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H38" s="32"/>
+      <c r="H38" s="30"/>
       <c r="I38" s="31"/>
-      <c r="J38" s="39" t="s">
+      <c r="J38" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="K38" s="38"/>
+      <c r="K38" s="32"/>
     </row>
     <row r="39" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
@@ -2188,12 +2206,12 @@
       <c r="G39" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H39" s="32"/>
+      <c r="H39" s="30"/>
       <c r="I39" s="31"/>
-      <c r="J39" s="39" t="s">
+      <c r="J39" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="K39" s="38"/>
+      <c r="K39" s="32"/>
     </row>
     <row r="40" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
@@ -2217,12 +2235,12 @@
       <c r="G40" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H40" s="32"/>
+      <c r="H40" s="30"/>
       <c r="I40" s="31"/>
-      <c r="J40" s="39" t="s">
+      <c r="J40" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="K40" s="38"/>
+      <c r="K40" s="32"/>
     </row>
     <row r="41" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
@@ -2246,12 +2264,12 @@
       <c r="G41" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H41" s="32"/>
+      <c r="H41" s="30"/>
       <c r="I41" s="31"/>
-      <c r="J41" s="39" t="s">
+      <c r="J41" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="K41" s="38"/>
+      <c r="K41" s="32"/>
     </row>
     <row r="42" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
@@ -2275,12 +2293,12 @@
       <c r="G42" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H42" s="32"/>
+      <c r="H42" s="30"/>
       <c r="I42" s="31"/>
-      <c r="J42" s="39" t="s">
+      <c r="J42" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="K42" s="38"/>
+      <c r="K42" s="32"/>
     </row>
     <row r="43" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
@@ -2304,12 +2322,12 @@
       <c r="G43" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H43" s="32"/>
+      <c r="H43" s="30"/>
       <c r="I43" s="31"/>
-      <c r="J43" s="39" t="s">
+      <c r="J43" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="K43" s="38"/>
+      <c r="K43" s="32"/>
     </row>
     <row r="44" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
@@ -2333,12 +2351,12 @@
       <c r="G44" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H44" s="32"/>
+      <c r="H44" s="30"/>
       <c r="I44" s="31"/>
-      <c r="J44" s="39" t="s">
+      <c r="J44" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="K44" s="38"/>
+      <c r="K44" s="32"/>
     </row>
     <row r="45" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
@@ -2362,12 +2380,12 @@
       <c r="G45" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H45" s="32"/>
+      <c r="H45" s="30"/>
       <c r="I45" s="31"/>
-      <c r="J45" s="39" t="s">
+      <c r="J45" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="K45" s="38"/>
+      <c r="K45" s="32"/>
     </row>
     <row r="46" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
@@ -2391,12 +2409,12 @@
       <c r="G46" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H46" s="32"/>
+      <c r="H46" s="30"/>
       <c r="I46" s="31"/>
-      <c r="J46" s="39" t="s">
+      <c r="J46" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="K46" s="38"/>
+      <c r="K46" s="32"/>
     </row>
     <row r="47" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
@@ -2420,12 +2438,12 @@
       <c r="G47" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H47" s="32"/>
+      <c r="H47" s="30"/>
       <c r="I47" s="31"/>
-      <c r="J47" s="39" t="s">
+      <c r="J47" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="K47" s="38"/>
+      <c r="K47" s="32"/>
     </row>
     <row r="48" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
@@ -2449,12 +2467,12 @@
       <c r="G48" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H48" s="32"/>
+      <c r="H48" s="30"/>
       <c r="I48" s="31"/>
-      <c r="J48" s="39" t="s">
+      <c r="J48" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="K48" s="38"/>
+      <c r="K48" s="32"/>
     </row>
     <row r="49" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
@@ -2478,12 +2496,12 @@
       <c r="G49" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H49" s="32"/>
+      <c r="H49" s="30"/>
       <c r="I49" s="31"/>
-      <c r="J49" s="38" t="s">
+      <c r="J49" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="K49" s="38"/>
+      <c r="K49" s="32"/>
     </row>
     <row r="50" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
@@ -2505,12 +2523,12 @@
       <c r="G50" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H50" s="32"/>
+      <c r="H50" s="30"/>
       <c r="I50" s="31"/>
-      <c r="J50" s="38" t="s">
+      <c r="J50" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="K50" s="38"/>
+      <c r="K50" s="32"/>
     </row>
     <row r="51" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
@@ -2532,12 +2550,12 @@
       <c r="G51" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H51" s="32"/>
+      <c r="H51" s="30"/>
       <c r="I51" s="31"/>
-      <c r="J51" s="38" t="s">
+      <c r="J51" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="K51" s="38"/>
+      <c r="K51" s="32"/>
     </row>
     <row r="52" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A52" s="13"/>
@@ -2547,10 +2565,10 @@
       <c r="E52" s="13"/>
       <c r="F52" s="13"/>
       <c r="G52" s="15"/>
-      <c r="H52" s="32"/>
+      <c r="H52" s="30"/>
       <c r="I52" s="31"/>
-      <c r="J52" s="38"/>
-      <c r="K52" s="38"/>
+      <c r="J52" s="32"/>
+      <c r="K52" s="32"/>
     </row>
     <row r="53" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A53" s="13"/>
@@ -2560,10 +2578,10 @@
       <c r="E53" s="13"/>
       <c r="F53" s="13"/>
       <c r="G53" s="15"/>
-      <c r="H53" s="32"/>
+      <c r="H53" s="30"/>
       <c r="I53" s="31"/>
-      <c r="J53" s="38"/>
-      <c r="K53" s="38"/>
+      <c r="J53" s="32"/>
+      <c r="K53" s="32"/>
     </row>
     <row r="54" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A54" s="13"/>
@@ -2573,10 +2591,10 @@
       <c r="E54" s="13"/>
       <c r="F54" s="13"/>
       <c r="G54" s="15"/>
-      <c r="H54" s="32"/>
+      <c r="H54" s="30"/>
       <c r="I54" s="31"/>
-      <c r="J54" s="38"/>
-      <c r="K54" s="38"/>
+      <c r="J54" s="32"/>
+      <c r="K54" s="32"/>
     </row>
     <row r="55" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A55" s="13"/>
@@ -2586,10 +2604,10 @@
       <c r="E55" s="13"/>
       <c r="F55" s="13"/>
       <c r="G55" s="15"/>
-      <c r="H55" s="32"/>
+      <c r="H55" s="30"/>
       <c r="I55" s="31"/>
-      <c r="J55" s="38"/>
-      <c r="K55" s="38"/>
+      <c r="J55" s="32"/>
+      <c r="K55" s="32"/>
     </row>
     <row r="56" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A56" s="13"/>
@@ -2599,10 +2617,10 @@
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
       <c r="G56" s="15"/>
-      <c r="H56" s="32"/>
+      <c r="H56" s="30"/>
       <c r="I56" s="31"/>
-      <c r="J56" s="38"/>
-      <c r="K56" s="38"/>
+      <c r="J56" s="32"/>
+      <c r="K56" s="32"/>
     </row>
     <row r="57" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A57" s="13"/>
@@ -2612,10 +2630,10 @@
       <c r="E57" s="13"/>
       <c r="F57" s="13"/>
       <c r="G57" s="15"/>
-      <c r="H57" s="32"/>
+      <c r="H57" s="30"/>
       <c r="I57" s="31"/>
-      <c r="J57" s="38"/>
-      <c r="K57" s="38"/>
+      <c r="J57" s="32"/>
+      <c r="K57" s="32"/>
     </row>
     <row r="58" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A58" s="13"/>
@@ -2625,10 +2643,10 @@
       <c r="E58" s="13"/>
       <c r="F58" s="13"/>
       <c r="G58" s="15"/>
-      <c r="H58" s="32"/>
+      <c r="H58" s="30"/>
       <c r="I58" s="31"/>
-      <c r="J58" s="38"/>
-      <c r="K58" s="38"/>
+      <c r="J58" s="32"/>
+      <c r="K58" s="32"/>
     </row>
     <row r="59" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A59" s="13"/>
@@ -2638,25 +2656,25 @@
       <c r="E59" s="13"/>
       <c r="F59" s="13"/>
       <c r="G59" s="15"/>
-      <c r="H59" s="32"/>
+      <c r="H59" s="30"/>
       <c r="I59" s="31"/>
-      <c r="J59" s="38"/>
-      <c r="K59" s="38"/>
+      <c r="J59" s="32"/>
+      <c r="K59" s="32"/>
     </row>
     <row r="60" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A60" s="33" t="s">
+      <c r="A60" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="B60" s="34"/>
-      <c r="C60" s="34"/>
-      <c r="D60" s="34"/>
-      <c r="E60" s="34"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="34"/>
-      <c r="H60" s="34"/>
-      <c r="I60" s="34"/>
-      <c r="J60" s="34"/>
-      <c r="K60" s="35"/>
+      <c r="B60" s="37"/>
+      <c r="C60" s="37"/>
+      <c r="D60" s="37"/>
+      <c r="E60" s="37"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="37"/>
+      <c r="I60" s="37"/>
+      <c r="J60" s="37"/>
+      <c r="K60" s="38"/>
     </row>
     <row r="61" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A61" s="13" t="s">
@@ -2680,12 +2698,12 @@
       <c r="G61" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H61" s="32"/>
+      <c r="H61" s="30"/>
       <c r="I61" s="31"/>
-      <c r="J61" s="38" t="s">
+      <c r="J61" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="K61" s="38"/>
+      <c r="K61" s="32"/>
     </row>
     <row r="62" spans="1:11" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
@@ -2709,14 +2727,14 @@
       <c r="G62" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="H62" s="30" t="s">
+      <c r="H62" s="44" t="s">
         <v>151</v>
       </c>
       <c r="I62" s="31"/>
-      <c r="J62" s="38" t="s">
+      <c r="J62" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="K62" s="38"/>
+      <c r="K62" s="32"/>
     </row>
     <row r="63" spans="1:11" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
@@ -2740,12 +2758,12 @@
       <c r="G63" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H63" s="32"/>
+      <c r="H63" s="30"/>
       <c r="I63" s="31"/>
-      <c r="J63" s="38" t="s">
+      <c r="J63" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="K63" s="38"/>
+      <c r="K63" s="32"/>
     </row>
     <row r="64" spans="1:11" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
@@ -2769,12 +2787,12 @@
       <c r="G64" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H64" s="32"/>
+      <c r="H64" s="30"/>
       <c r="I64" s="31"/>
-      <c r="J64" s="38" t="s">
+      <c r="J64" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="K64" s="38"/>
+      <c r="K64" s="32"/>
     </row>
     <row r="65" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
@@ -2798,38 +2816,68 @@
       <c r="G65" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H65" s="32"/>
+      <c r="H65" s="30"/>
       <c r="I65" s="31"/>
-      <c r="J65" s="38" t="s">
+      <c r="J65" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="K65" s="38"/>
+      <c r="K65" s="32"/>
     </row>
     <row r="66" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A66" s="13"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="13"/>
-      <c r="E66" s="13"/>
-      <c r="F66" s="13"/>
-      <c r="G66" s="15"/>
-      <c r="H66" s="32"/>
+      <c r="A66" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="B66" s="17">
+        <v>45772</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D66" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E66" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="F66" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="G66" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H66" s="30"/>
       <c r="I66" s="31"/>
-      <c r="J66" s="38"/>
-      <c r="K66" s="38"/>
+      <c r="J66" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="K66" s="32"/>
     </row>
     <row r="67" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A67" s="13"/>
-      <c r="B67" s="18"/>
-      <c r="C67" s="18"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="13"/>
+      <c r="A67" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="B67" s="17">
+        <v>45772</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E67" s="13" t="s">
+        <v>108</v>
+      </c>
       <c r="F67" s="13"/>
-      <c r="G67" s="15"/>
-      <c r="H67" s="32"/>
+      <c r="G67" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H67" s="30"/>
       <c r="I67" s="31"/>
-      <c r="J67" s="38"/>
-      <c r="K67" s="38"/>
+      <c r="J67" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="K67" s="32"/>
     </row>
     <row r="68" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A68" s="13"/>
@@ -2839,10 +2887,10 @@
       <c r="E68" s="13"/>
       <c r="F68" s="13"/>
       <c r="G68" s="15"/>
-      <c r="H68" s="32"/>
+      <c r="H68" s="30"/>
       <c r="I68" s="31"/>
-      <c r="J68" s="38"/>
-      <c r="K68" s="38"/>
+      <c r="J68" s="32"/>
+      <c r="K68" s="32"/>
     </row>
     <row r="69" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A69" s="13"/>
@@ -2852,10 +2900,10 @@
       <c r="E69" s="13"/>
       <c r="F69" s="13"/>
       <c r="G69" s="15"/>
-      <c r="H69" s="32"/>
+      <c r="H69" s="30"/>
       <c r="I69" s="31"/>
-      <c r="J69" s="38"/>
-      <c r="K69" s="38"/>
+      <c r="J69" s="32"/>
+      <c r="K69" s="32"/>
     </row>
     <row r="70" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A70" s="13"/>
@@ -2865,10 +2913,10 @@
       <c r="E70" s="13"/>
       <c r="F70" s="13"/>
       <c r="G70" s="15"/>
-      <c r="H70" s="32"/>
+      <c r="H70" s="30"/>
       <c r="I70" s="31"/>
-      <c r="J70" s="38"/>
-      <c r="K70" s="38"/>
+      <c r="J70" s="32"/>
+      <c r="K70" s="32"/>
     </row>
     <row r="71" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A71" s="13"/>
@@ -2878,10 +2926,10 @@
       <c r="E71" s="13"/>
       <c r="F71" s="13"/>
       <c r="G71" s="15"/>
-      <c r="H71" s="32"/>
+      <c r="H71" s="30"/>
       <c r="I71" s="31"/>
-      <c r="J71" s="38"/>
-      <c r="K71" s="38"/>
+      <c r="J71" s="32"/>
+      <c r="K71" s="32"/>
     </row>
     <row r="72" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A72" s="13"/>
@@ -2891,10 +2939,10 @@
       <c r="E72" s="13"/>
       <c r="F72" s="13"/>
       <c r="G72" s="15"/>
-      <c r="H72" s="32"/>
+      <c r="H72" s="30"/>
       <c r="I72" s="31"/>
-      <c r="J72" s="38"/>
-      <c r="K72" s="38"/>
+      <c r="J72" s="32"/>
+      <c r="K72" s="32"/>
     </row>
     <row r="73" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A73" s="13"/>
@@ -2904,10 +2952,10 @@
       <c r="E73" s="13"/>
       <c r="F73" s="13"/>
       <c r="G73" s="15"/>
-      <c r="H73" s="32"/>
+      <c r="H73" s="30"/>
       <c r="I73" s="31"/>
-      <c r="J73" s="38"/>
-      <c r="K73" s="38"/>
+      <c r="J73" s="32"/>
+      <c r="K73" s="32"/>
     </row>
     <row r="74" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A74" s="13"/>
@@ -2917,10 +2965,10 @@
       <c r="E74" s="13"/>
       <c r="F74" s="13"/>
       <c r="G74" s="15"/>
-      <c r="H74" s="32"/>
+      <c r="H74" s="30"/>
       <c r="I74" s="31"/>
-      <c r="J74" s="38"/>
-      <c r="K74" s="38"/>
+      <c r="J74" s="32"/>
+      <c r="K74" s="32"/>
     </row>
     <row r="75" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A75" s="13"/>
@@ -2930,10 +2978,10 @@
       <c r="E75" s="13"/>
       <c r="F75" s="13"/>
       <c r="G75" s="15"/>
-      <c r="H75" s="32"/>
+      <c r="H75" s="30"/>
       <c r="I75" s="31"/>
-      <c r="J75" s="38"/>
-      <c r="K75" s="38"/>
+      <c r="J75" s="32"/>
+      <c r="K75" s="32"/>
     </row>
     <row r="76" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A76" s="13"/>
@@ -2943,10 +2991,10 @@
       <c r="E76" s="13"/>
       <c r="F76" s="13"/>
       <c r="G76" s="15"/>
-      <c r="H76" s="32"/>
+      <c r="H76" s="30"/>
       <c r="I76" s="31"/>
-      <c r="J76" s="38"/>
-      <c r="K76" s="38"/>
+      <c r="J76" s="32"/>
+      <c r="K76" s="32"/>
     </row>
     <row r="77" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A77" s="13"/>
@@ -2956,10 +3004,10 @@
       <c r="E77" s="13"/>
       <c r="F77" s="13"/>
       <c r="G77" s="15"/>
-      <c r="H77" s="32"/>
+      <c r="H77" s="30"/>
       <c r="I77" s="31"/>
-      <c r="J77" s="38"/>
-      <c r="K77" s="38"/>
+      <c r="J77" s="32"/>
+      <c r="K77" s="32"/>
     </row>
     <row r="78" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A78" s="13"/>
@@ -2969,10 +3017,10 @@
       <c r="E78" s="13"/>
       <c r="F78" s="13"/>
       <c r="G78" s="15"/>
-      <c r="H78" s="32"/>
+      <c r="H78" s="30"/>
       <c r="I78" s="31"/>
-      <c r="J78" s="38"/>
-      <c r="K78" s="38"/>
+      <c r="J78" s="32"/>
+      <c r="K78" s="32"/>
     </row>
     <row r="79" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A79" s="13"/>
@@ -2982,10 +3030,10 @@
       <c r="E79" s="13"/>
       <c r="F79" s="13"/>
       <c r="G79" s="15"/>
-      <c r="H79" s="32"/>
+      <c r="H79" s="30"/>
       <c r="I79" s="31"/>
-      <c r="J79" s="38"/>
-      <c r="K79" s="38"/>
+      <c r="J79" s="32"/>
+      <c r="K79" s="32"/>
     </row>
     <row r="80" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A80" s="13"/>
@@ -2995,10 +3043,10 @@
       <c r="E80" s="13"/>
       <c r="F80" s="13"/>
       <c r="G80" s="15"/>
-      <c r="H80" s="32"/>
+      <c r="H80" s="30"/>
       <c r="I80" s="31"/>
-      <c r="J80" s="38"/>
-      <c r="K80" s="38"/>
+      <c r="J80" s="32"/>
+      <c r="K80" s="32"/>
     </row>
     <row r="81" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A81" s="13"/>
@@ -3008,10 +3056,10 @@
       <c r="E81" s="13"/>
       <c r="F81" s="13"/>
       <c r="G81" s="15"/>
-      <c r="H81" s="32"/>
+      <c r="H81" s="30"/>
       <c r="I81" s="31"/>
-      <c r="J81" s="38"/>
-      <c r="K81" s="38"/>
+      <c r="J81" s="32"/>
+      <c r="K81" s="32"/>
     </row>
     <row r="82" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A82" s="13"/>
@@ -3021,10 +3069,10 @@
       <c r="E82" s="13"/>
       <c r="F82" s="13"/>
       <c r="G82" s="15"/>
-      <c r="H82" s="32"/>
+      <c r="H82" s="30"/>
       <c r="I82" s="31"/>
-      <c r="J82" s="38"/>
-      <c r="K82" s="38"/>
+      <c r="J82" s="32"/>
+      <c r="K82" s="32"/>
     </row>
     <row r="83" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A83" s="13"/>
@@ -3034,10 +3082,10 @@
       <c r="E83" s="13"/>
       <c r="F83" s="13"/>
       <c r="G83" s="15"/>
-      <c r="H83" s="32"/>
+      <c r="H83" s="30"/>
       <c r="I83" s="31"/>
-      <c r="J83" s="38"/>
-      <c r="K83" s="38"/>
+      <c r="J83" s="32"/>
+      <c r="K83" s="32"/>
     </row>
     <row r="84" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A84" s="13"/>
@@ -3047,10 +3095,10 @@
       <c r="E84" s="13"/>
       <c r="F84" s="13"/>
       <c r="G84" s="15"/>
-      <c r="H84" s="32"/>
+      <c r="H84" s="30"/>
       <c r="I84" s="31"/>
-      <c r="J84" s="38"/>
-      <c r="K84" s="38"/>
+      <c r="J84" s="32"/>
+      <c r="K84" s="32"/>
     </row>
     <row r="85" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A85" s="13"/>
@@ -3060,10 +3108,10 @@
       <c r="E85" s="13"/>
       <c r="F85" s="13"/>
       <c r="G85" s="15"/>
-      <c r="H85" s="32"/>
+      <c r="H85" s="30"/>
       <c r="I85" s="31"/>
-      <c r="J85" s="38"/>
-      <c r="K85" s="38"/>
+      <c r="J85" s="32"/>
+      <c r="K85" s="32"/>
     </row>
     <row r="86" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A86" s="13"/>
@@ -3073,10 +3121,10 @@
       <c r="E86" s="13"/>
       <c r="F86" s="13"/>
       <c r="G86" s="15"/>
-      <c r="H86" s="32"/>
+      <c r="H86" s="30"/>
       <c r="I86" s="31"/>
-      <c r="J86" s="38"/>
-      <c r="K86" s="38"/>
+      <c r="J86" s="32"/>
+      <c r="K86" s="32"/>
     </row>
     <row r="87" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A87" s="13"/>
@@ -3086,10 +3134,10 @@
       <c r="E87" s="13"/>
       <c r="F87" s="13"/>
       <c r="G87" s="15"/>
-      <c r="H87" s="32"/>
+      <c r="H87" s="30"/>
       <c r="I87" s="31"/>
-      <c r="J87" s="38"/>
-      <c r="K87" s="38"/>
+      <c r="J87" s="32"/>
+      <c r="K87" s="32"/>
     </row>
     <row r="88" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A88" s="13"/>
@@ -3099,10 +3147,10 @@
       <c r="E88" s="13"/>
       <c r="F88" s="13"/>
       <c r="G88" s="15"/>
-      <c r="H88" s="32"/>
+      <c r="H88" s="30"/>
       <c r="I88" s="31"/>
-      <c r="J88" s="38"/>
-      <c r="K88" s="38"/>
+      <c r="J88" s="32"/>
+      <c r="K88" s="32"/>
     </row>
     <row r="89" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A89" s="13"/>
@@ -3112,10 +3160,10 @@
       <c r="E89" s="13"/>
       <c r="F89" s="13"/>
       <c r="G89" s="15"/>
-      <c r="H89" s="32"/>
+      <c r="H89" s="30"/>
       <c r="I89" s="31"/>
-      <c r="J89" s="38"/>
-      <c r="K89" s="38"/>
+      <c r="J89" s="32"/>
+      <c r="K89" s="32"/>
     </row>
     <row r="90" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A90" s="13"/>
@@ -3125,10 +3173,10 @@
       <c r="E90" s="13"/>
       <c r="F90" s="13"/>
       <c r="G90" s="15"/>
-      <c r="H90" s="32"/>
+      <c r="H90" s="30"/>
       <c r="I90" s="31"/>
-      <c r="J90" s="38"/>
-      <c r="K90" s="38"/>
+      <c r="J90" s="32"/>
+      <c r="K90" s="32"/>
     </row>
     <row r="91" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A91" s="13"/>
@@ -3138,10 +3186,10 @@
       <c r="E91" s="13"/>
       <c r="F91" s="13"/>
       <c r="G91" s="15"/>
-      <c r="H91" s="32"/>
+      <c r="H91" s="30"/>
       <c r="I91" s="31"/>
-      <c r="J91" s="38"/>
-      <c r="K91" s="38"/>
+      <c r="J91" s="32"/>
+      <c r="K91" s="32"/>
     </row>
     <row r="92" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A92" s="13"/>
@@ -3151,10 +3199,10 @@
       <c r="E92" s="13"/>
       <c r="F92" s="13"/>
       <c r="G92" s="15"/>
-      <c r="H92" s="32"/>
+      <c r="H92" s="30"/>
       <c r="I92" s="31"/>
-      <c r="J92" s="38"/>
-      <c r="K92" s="38"/>
+      <c r="J92" s="32"/>
+      <c r="K92" s="32"/>
     </row>
     <row r="93" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A93" s="13"/>
@@ -3164,10 +3212,10 @@
       <c r="E93" s="13"/>
       <c r="F93" s="13"/>
       <c r="G93" s="15"/>
-      <c r="H93" s="32"/>
+      <c r="H93" s="30"/>
       <c r="I93" s="31"/>
-      <c r="J93" s="38"/>
-      <c r="K93" s="38"/>
+      <c r="J93" s="32"/>
+      <c r="K93" s="32"/>
     </row>
     <row r="94" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A94" s="13"/>
@@ -3177,10 +3225,10 @@
       <c r="E94" s="13"/>
       <c r="F94" s="13"/>
       <c r="G94" s="15"/>
-      <c r="H94" s="32"/>
+      <c r="H94" s="30"/>
       <c r="I94" s="31"/>
-      <c r="J94" s="38"/>
-      <c r="K94" s="38"/>
+      <c r="J94" s="32"/>
+      <c r="K94" s="32"/>
     </row>
     <row r="95" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A95" s="13"/>
@@ -3190,10 +3238,10 @@
       <c r="E95" s="13"/>
       <c r="F95" s="13"/>
       <c r="G95" s="15"/>
-      <c r="H95" s="32"/>
+      <c r="H95" s="30"/>
       <c r="I95" s="31"/>
-      <c r="J95" s="38"/>
-      <c r="K95" s="38"/>
+      <c r="J95" s="32"/>
+      <c r="K95" s="32"/>
     </row>
     <row r="96" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A96" s="13"/>
@@ -3203,10 +3251,10 @@
       <c r="E96" s="13"/>
       <c r="F96" s="13"/>
       <c r="G96" s="15"/>
-      <c r="H96" s="32"/>
+      <c r="H96" s="30"/>
       <c r="I96" s="31"/>
-      <c r="J96" s="38"/>
-      <c r="K96" s="38"/>
+      <c r="J96" s="32"/>
+      <c r="K96" s="32"/>
     </row>
     <row r="97" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A97" s="13"/>
@@ -3216,10 +3264,10 @@
       <c r="E97" s="13"/>
       <c r="F97" s="13"/>
       <c r="G97" s="15"/>
-      <c r="H97" s="32"/>
+      <c r="H97" s="30"/>
       <c r="I97" s="31"/>
-      <c r="J97" s="38"/>
-      <c r="K97" s="38"/>
+      <c r="J97" s="32"/>
+      <c r="K97" s="32"/>
     </row>
     <row r="98" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A98" s="13"/>
@@ -3229,10 +3277,10 @@
       <c r="E98" s="13"/>
       <c r="F98" s="13"/>
       <c r="G98" s="15"/>
-      <c r="H98" s="32"/>
+      <c r="H98" s="30"/>
       <c r="I98" s="31"/>
-      <c r="J98" s="38"/>
-      <c r="K98" s="38"/>
+      <c r="J98" s="32"/>
+      <c r="K98" s="32"/>
     </row>
     <row r="99" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A99" s="13"/>
@@ -3242,10 +3290,10 @@
       <c r="E99" s="13"/>
       <c r="F99" s="13"/>
       <c r="G99" s="15"/>
-      <c r="H99" s="32"/>
+      <c r="H99" s="30"/>
       <c r="I99" s="31"/>
-      <c r="J99" s="38"/>
-      <c r="K99" s="38"/>
+      <c r="J99" s="32"/>
+      <c r="K99" s="32"/>
     </row>
     <row r="100" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A100" s="13"/>
@@ -3255,10 +3303,10 @@
       <c r="E100" s="13"/>
       <c r="F100" s="13"/>
       <c r="G100" s="15"/>
-      <c r="H100" s="32"/>
+      <c r="H100" s="30"/>
       <c r="I100" s="31"/>
-      <c r="J100" s="38"/>
-      <c r="K100" s="38"/>
+      <c r="J100" s="32"/>
+      <c r="K100" s="32"/>
     </row>
     <row r="101" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A101" s="13"/>
@@ -3268,10 +3316,10 @@
       <c r="E101" s="13"/>
       <c r="F101" s="13"/>
       <c r="G101" s="15"/>
-      <c r="H101" s="32"/>
+      <c r="H101" s="30"/>
       <c r="I101" s="31"/>
-      <c r="J101" s="38"/>
-      <c r="K101" s="38"/>
+      <c r="J101" s="32"/>
+      <c r="K101" s="32"/>
     </row>
     <row r="102" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A102" s="13"/>
@@ -3281,10 +3329,10 @@
       <c r="E102" s="13"/>
       <c r="F102" s="13"/>
       <c r="G102" s="15"/>
-      <c r="H102" s="32"/>
+      <c r="H102" s="30"/>
       <c r="I102" s="31"/>
-      <c r="J102" s="38"/>
-      <c r="K102" s="38"/>
+      <c r="J102" s="32"/>
+      <c r="K102" s="32"/>
     </row>
     <row r="103" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A103" s="13"/>
@@ -3294,10 +3342,10 @@
       <c r="E103" s="13"/>
       <c r="F103" s="13"/>
       <c r="G103" s="15"/>
-      <c r="H103" s="32"/>
+      <c r="H103" s="30"/>
       <c r="I103" s="31"/>
-      <c r="J103" s="38"/>
-      <c r="K103" s="38"/>
+      <c r="J103" s="32"/>
+      <c r="K103" s="32"/>
     </row>
     <row r="104" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A104" s="13"/>
@@ -3307,10 +3355,10 @@
       <c r="E104" s="13"/>
       <c r="F104" s="13"/>
       <c r="G104" s="15"/>
-      <c r="H104" s="32"/>
+      <c r="H104" s="30"/>
       <c r="I104" s="31"/>
-      <c r="J104" s="38"/>
-      <c r="K104" s="38"/>
+      <c r="J104" s="32"/>
+      <c r="K104" s="32"/>
     </row>
     <row r="105" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A105" s="13"/>
@@ -3320,10 +3368,10 @@
       <c r="E105" s="13"/>
       <c r="F105" s="13"/>
       <c r="G105" s="15"/>
-      <c r="H105" s="32"/>
+      <c r="H105" s="30"/>
       <c r="I105" s="31"/>
-      <c r="J105" s="38"/>
-      <c r="K105" s="38"/>
+      <c r="J105" s="32"/>
+      <c r="K105" s="32"/>
     </row>
     <row r="106" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A106" s="13"/>
@@ -3333,10 +3381,10 @@
       <c r="E106" s="13"/>
       <c r="F106" s="13"/>
       <c r="G106" s="15"/>
-      <c r="H106" s="32"/>
+      <c r="H106" s="30"/>
       <c r="I106" s="31"/>
-      <c r="J106" s="38"/>
-      <c r="K106" s="38"/>
+      <c r="J106" s="32"/>
+      <c r="K106" s="32"/>
     </row>
     <row r="107" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A107" s="13"/>
@@ -3346,10 +3394,10 @@
       <c r="E107" s="13"/>
       <c r="F107" s="13"/>
       <c r="G107" s="15"/>
-      <c r="H107" s="32"/>
+      <c r="H107" s="30"/>
       <c r="I107" s="31"/>
-      <c r="J107" s="38"/>
-      <c r="K107" s="38"/>
+      <c r="J107" s="32"/>
+      <c r="K107" s="32"/>
     </row>
     <row r="108" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A108" s="13"/>
@@ -3359,10 +3407,10 @@
       <c r="E108" s="13"/>
       <c r="F108" s="13"/>
       <c r="G108" s="15"/>
-      <c r="H108" s="32"/>
+      <c r="H108" s="30"/>
       <c r="I108" s="31"/>
-      <c r="J108" s="38"/>
-      <c r="K108" s="38"/>
+      <c r="J108" s="32"/>
+      <c r="K108" s="32"/>
     </row>
     <row r="109" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A109" s="13"/>
@@ -3372,10 +3420,10 @@
       <c r="E109" s="13"/>
       <c r="F109" s="13"/>
       <c r="G109" s="15"/>
-      <c r="H109" s="32"/>
+      <c r="H109" s="30"/>
       <c r="I109" s="31"/>
-      <c r="J109" s="38"/>
-      <c r="K109" s="38"/>
+      <c r="J109" s="32"/>
+      <c r="K109" s="32"/>
     </row>
     <row r="110" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A110" s="13"/>
@@ -3385,10 +3433,10 @@
       <c r="E110" s="13"/>
       <c r="F110" s="13"/>
       <c r="G110" s="15"/>
-      <c r="H110" s="32"/>
+      <c r="H110" s="30"/>
       <c r="I110" s="31"/>
-      <c r="J110" s="38"/>
-      <c r="K110" s="38"/>
+      <c r="J110" s="32"/>
+      <c r="K110" s="32"/>
     </row>
     <row r="111" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A111" s="13"/>
@@ -3398,10 +3446,10 @@
       <c r="E111" s="13"/>
       <c r="F111" s="13"/>
       <c r="G111" s="15"/>
-      <c r="H111" s="32"/>
+      <c r="H111" s="30"/>
       <c r="I111" s="31"/>
-      <c r="J111" s="38"/>
-      <c r="K111" s="38"/>
+      <c r="J111" s="32"/>
+      <c r="K111" s="32"/>
     </row>
     <row r="112" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A112" s="13"/>
@@ -3411,10 +3459,10 @@
       <c r="E112" s="13"/>
       <c r="F112" s="13"/>
       <c r="G112" s="15"/>
-      <c r="H112" s="32"/>
+      <c r="H112" s="30"/>
       <c r="I112" s="31"/>
-      <c r="J112" s="38"/>
-      <c r="K112" s="38"/>
+      <c r="J112" s="32"/>
+      <c r="K112" s="32"/>
     </row>
     <row r="113" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A113" s="13"/>
@@ -3424,10 +3472,10 @@
       <c r="E113" s="13"/>
       <c r="F113" s="13"/>
       <c r="G113" s="15"/>
-      <c r="H113" s="32"/>
+      <c r="H113" s="30"/>
       <c r="I113" s="31"/>
-      <c r="J113" s="38"/>
-      <c r="K113" s="38"/>
+      <c r="J113" s="32"/>
+      <c r="K113" s="32"/>
     </row>
     <row r="114" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A114" s="13"/>
@@ -3437,10 +3485,10 @@
       <c r="E114" s="13"/>
       <c r="F114" s="13"/>
       <c r="G114" s="15"/>
-      <c r="H114" s="32"/>
+      <c r="H114" s="30"/>
       <c r="I114" s="31"/>
-      <c r="J114" s="38"/>
-      <c r="K114" s="38"/>
+      <c r="J114" s="32"/>
+      <c r="K114" s="32"/>
     </row>
     <row r="115" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A115" s="13"/>
@@ -3450,10 +3498,10 @@
       <c r="E115" s="13"/>
       <c r="F115" s="13"/>
       <c r="G115" s="15"/>
-      <c r="H115" s="32"/>
+      <c r="H115" s="30"/>
       <c r="I115" s="31"/>
-      <c r="J115" s="38"/>
-      <c r="K115" s="38"/>
+      <c r="J115" s="32"/>
+      <c r="K115" s="32"/>
     </row>
     <row r="116" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A116" s="13"/>
@@ -3463,10 +3511,10 @@
       <c r="E116" s="13"/>
       <c r="F116" s="13"/>
       <c r="G116" s="15"/>
-      <c r="H116" s="32"/>
+      <c r="H116" s="30"/>
       <c r="I116" s="31"/>
-      <c r="J116" s="38"/>
-      <c r="K116" s="38"/>
+      <c r="J116" s="32"/>
+      <c r="K116" s="32"/>
     </row>
     <row r="117" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A117" s="13"/>
@@ -3476,10 +3524,10 @@
       <c r="E117" s="13"/>
       <c r="F117" s="13"/>
       <c r="G117" s="15"/>
-      <c r="H117" s="32"/>
+      <c r="H117" s="30"/>
       <c r="I117" s="31"/>
-      <c r="J117" s="38"/>
-      <c r="K117" s="38"/>
+      <c r="J117" s="32"/>
+      <c r="K117" s="32"/>
     </row>
     <row r="118" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A118" s="13"/>
@@ -3489,10 +3537,10 @@
       <c r="E118" s="13"/>
       <c r="F118" s="13"/>
       <c r="G118" s="15"/>
-      <c r="H118" s="32"/>
+      <c r="H118" s="30"/>
       <c r="I118" s="31"/>
-      <c r="J118" s="38"/>
-      <c r="K118" s="38"/>
+      <c r="J118" s="32"/>
+      <c r="K118" s="32"/>
     </row>
     <row r="119" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A119" s="13"/>
@@ -3502,10 +3550,10 @@
       <c r="E119" s="13"/>
       <c r="F119" s="13"/>
       <c r="G119" s="15"/>
-      <c r="H119" s="32"/>
+      <c r="H119" s="30"/>
       <c r="I119" s="31"/>
-      <c r="J119" s="38"/>
-      <c r="K119" s="38"/>
+      <c r="J119" s="32"/>
+      <c r="K119" s="32"/>
     </row>
     <row r="120" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A120" s="13"/>
@@ -3515,10 +3563,10 @@
       <c r="E120" s="13"/>
       <c r="F120" s="13"/>
       <c r="G120" s="15"/>
-      <c r="H120" s="32"/>
+      <c r="H120" s="30"/>
       <c r="I120" s="31"/>
-      <c r="J120" s="38"/>
-      <c r="K120" s="38"/>
+      <c r="J120" s="32"/>
+      <c r="K120" s="32"/>
     </row>
     <row r="121" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A121" s="13"/>
@@ -3528,10 +3576,10 @@
       <c r="E121" s="13"/>
       <c r="F121" s="13"/>
       <c r="G121" s="15"/>
-      <c r="H121" s="32"/>
+      <c r="H121" s="30"/>
       <c r="I121" s="31"/>
-      <c r="J121" s="38"/>
-      <c r="K121" s="38"/>
+      <c r="J121" s="32"/>
+      <c r="K121" s="32"/>
     </row>
     <row r="122" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A122" s="13"/>
@@ -3541,10 +3589,10 @@
       <c r="E122" s="13"/>
       <c r="F122" s="13"/>
       <c r="G122" s="15"/>
-      <c r="H122" s="32"/>
+      <c r="H122" s="30"/>
       <c r="I122" s="31"/>
-      <c r="J122" s="38"/>
-      <c r="K122" s="38"/>
+      <c r="J122" s="32"/>
+      <c r="K122" s="32"/>
     </row>
     <row r="123" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A123" s="13"/>
@@ -3554,10 +3602,10 @@
       <c r="E123" s="13"/>
       <c r="F123" s="13"/>
       <c r="G123" s="15"/>
-      <c r="H123" s="32"/>
+      <c r="H123" s="30"/>
       <c r="I123" s="31"/>
-      <c r="J123" s="38"/>
-      <c r="K123" s="38"/>
+      <c r="J123" s="32"/>
+      <c r="K123" s="32"/>
     </row>
     <row r="124" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A124" s="13"/>
@@ -3567,10 +3615,10 @@
       <c r="E124" s="13"/>
       <c r="F124" s="13"/>
       <c r="G124" s="15"/>
-      <c r="H124" s="32"/>
+      <c r="H124" s="30"/>
       <c r="I124" s="31"/>
-      <c r="J124" s="38"/>
-      <c r="K124" s="38"/>
+      <c r="J124" s="32"/>
+      <c r="K124" s="32"/>
     </row>
     <row r="125" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A125" s="13"/>
@@ -3580,10 +3628,10 @@
       <c r="E125" s="13"/>
       <c r="F125" s="13"/>
       <c r="G125" s="15"/>
-      <c r="H125" s="32"/>
+      <c r="H125" s="30"/>
       <c r="I125" s="31"/>
-      <c r="J125" s="38"/>
-      <c r="K125" s="38"/>
+      <c r="J125" s="32"/>
+      <c r="K125" s="32"/>
     </row>
     <row r="126" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A126" s="13"/>
@@ -3593,10 +3641,10 @@
       <c r="E126" s="13"/>
       <c r="F126" s="13"/>
       <c r="G126" s="15"/>
-      <c r="H126" s="32"/>
+      <c r="H126" s="30"/>
       <c r="I126" s="31"/>
-      <c r="J126" s="38"/>
-      <c r="K126" s="38"/>
+      <c r="J126" s="32"/>
+      <c r="K126" s="32"/>
     </row>
     <row r="127" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A127" s="13"/>
@@ -3606,10 +3654,10 @@
       <c r="E127" s="13"/>
       <c r="F127" s="13"/>
       <c r="G127" s="15"/>
-      <c r="H127" s="32"/>
+      <c r="H127" s="30"/>
       <c r="I127" s="31"/>
-      <c r="J127" s="38"/>
-      <c r="K127" s="38"/>
+      <c r="J127" s="32"/>
+      <c r="K127" s="32"/>
     </row>
     <row r="128" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A128" s="13"/>
@@ -3619,10 +3667,10 @@
       <c r="E128" s="13"/>
       <c r="F128" s="13"/>
       <c r="G128" s="15"/>
-      <c r="H128" s="32"/>
+      <c r="H128" s="30"/>
       <c r="I128" s="31"/>
-      <c r="J128" s="38"/>
-      <c r="K128" s="38"/>
+      <c r="J128" s="32"/>
+      <c r="K128" s="32"/>
     </row>
     <row r="129" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A129" s="13"/>
@@ -3632,10 +3680,10 @@
       <c r="E129" s="13"/>
       <c r="F129" s="13"/>
       <c r="G129" s="15"/>
-      <c r="H129" s="32"/>
+      <c r="H129" s="30"/>
       <c r="I129" s="31"/>
-      <c r="J129" s="38"/>
-      <c r="K129" s="38"/>
+      <c r="J129" s="32"/>
+      <c r="K129" s="32"/>
     </row>
     <row r="130" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A130" s="13"/>
@@ -3647,8 +3695,8 @@
       <c r="G130" s="15"/>
       <c r="H130" s="13"/>
       <c r="I130" s="13"/>
-      <c r="J130" s="38"/>
-      <c r="K130" s="38"/>
+      <c r="J130" s="32"/>
+      <c r="K130" s="32"/>
     </row>
     <row r="131" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A131" s="13"/>
@@ -3660,8 +3708,8 @@
       <c r="G131" s="15"/>
       <c r="H131" s="13"/>
       <c r="I131" s="13"/>
-      <c r="J131" s="38"/>
-      <c r="K131" s="38"/>
+      <c r="J131" s="32"/>
+      <c r="K131" s="32"/>
     </row>
     <row r="132" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A132" s="13"/>
@@ -3673,8 +3721,8 @@
       <c r="G132" s="15"/>
       <c r="H132" s="13"/>
       <c r="I132" s="13"/>
-      <c r="J132" s="38"/>
-      <c r="K132" s="38"/>
+      <c r="J132" s="32"/>
+      <c r="K132" s="32"/>
     </row>
     <row r="133" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A133" s="13"/>
@@ -3686,8 +3734,8 @@
       <c r="G133" s="15"/>
       <c r="H133" s="13"/>
       <c r="I133" s="13"/>
-      <c r="J133" s="38"/>
-      <c r="K133" s="38"/>
+      <c r="J133" s="32"/>
+      <c r="K133" s="32"/>
     </row>
     <row r="134" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A134" s="13"/>
@@ -3699,8 +3747,8 @@
       <c r="G134" s="15"/>
       <c r="H134" s="13"/>
       <c r="I134" s="13"/>
-      <c r="J134" s="38"/>
-      <c r="K134" s="38"/>
+      <c r="J134" s="32"/>
+      <c r="K134" s="32"/>
     </row>
     <row r="135" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A135" s="13"/>
@@ -3712,8 +3760,8 @@
       <c r="G135" s="15"/>
       <c r="H135" s="13"/>
       <c r="I135" s="13"/>
-      <c r="J135" s="38"/>
-      <c r="K135" s="38"/>
+      <c r="J135" s="32"/>
+      <c r="K135" s="32"/>
     </row>
     <row r="136" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A136" s="13"/>
@@ -3725,8 +3773,8 @@
       <c r="G136" s="15"/>
       <c r="H136" s="13"/>
       <c r="I136" s="13"/>
-      <c r="J136" s="38"/>
-      <c r="K136" s="38"/>
+      <c r="J136" s="32"/>
+      <c r="K136" s="32"/>
     </row>
     <row r="137" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A137" s="13"/>
@@ -3738,8 +3786,8 @@
       <c r="G137" s="15"/>
       <c r="H137" s="13"/>
       <c r="I137" s="13"/>
-      <c r="J137" s="38"/>
-      <c r="K137" s="38"/>
+      <c r="J137" s="32"/>
+      <c r="K137" s="32"/>
     </row>
     <row r="138" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A138" s="13"/>
@@ -3751,8 +3799,8 @@
       <c r="G138" s="15"/>
       <c r="H138" s="13"/>
       <c r="I138" s="13"/>
-      <c r="J138" s="38"/>
-      <c r="K138" s="38"/>
+      <c r="J138" s="32"/>
+      <c r="K138" s="32"/>
     </row>
     <row r="139" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A139" s="13"/>
@@ -3764,8 +3812,8 @@
       <c r="G139" s="15"/>
       <c r="H139" s="13"/>
       <c r="I139" s="13"/>
-      <c r="J139" s="38"/>
-      <c r="K139" s="38"/>
+      <c r="J139" s="32"/>
+      <c r="K139" s="32"/>
     </row>
     <row r="140" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A140" s="13"/>
@@ -3777,8 +3825,8 @@
       <c r="G140" s="15"/>
       <c r="H140" s="13"/>
       <c r="I140" s="13"/>
-      <c r="J140" s="38"/>
-      <c r="K140" s="38"/>
+      <c r="J140" s="32"/>
+      <c r="K140" s="32"/>
     </row>
     <row r="141" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A141" s="13"/>
@@ -3790,8 +3838,8 @@
       <c r="G141" s="15"/>
       <c r="H141" s="13"/>
       <c r="I141" s="13"/>
-      <c r="J141" s="38"/>
-      <c r="K141" s="38"/>
+      <c r="J141" s="32"/>
+      <c r="K141" s="32"/>
     </row>
     <row r="142" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A142" s="13"/>
@@ -3803,8 +3851,8 @@
       <c r="G142" s="15"/>
       <c r="H142" s="13"/>
       <c r="I142" s="13"/>
-      <c r="J142" s="38"/>
-      <c r="K142" s="38"/>
+      <c r="J142" s="32"/>
+      <c r="K142" s="32"/>
     </row>
     <row r="143" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A143" s="13"/>
@@ -3816,8 +3864,8 @@
       <c r="G143" s="15"/>
       <c r="H143" s="13"/>
       <c r="I143" s="13"/>
-      <c r="J143" s="38"/>
-      <c r="K143" s="38"/>
+      <c r="J143" s="32"/>
+      <c r="K143" s="32"/>
     </row>
     <row r="144" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A144" s="13"/>
@@ -3829,8 +3877,8 @@
       <c r="G144" s="15"/>
       <c r="H144" s="13"/>
       <c r="I144" s="13"/>
-      <c r="J144" s="38"/>
-      <c r="K144" s="38"/>
+      <c r="J144" s="32"/>
+      <c r="K144" s="32"/>
     </row>
     <row r="145" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A145" s="13"/>
@@ -3842,8 +3890,8 @@
       <c r="G145" s="15"/>
       <c r="H145" s="13"/>
       <c r="I145" s="13"/>
-      <c r="J145" s="38"/>
-      <c r="K145" s="38"/>
+      <c r="J145" s="32"/>
+      <c r="K145" s="32"/>
     </row>
     <row r="146" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A146" s="13"/>
@@ -3855,8 +3903,8 @@
       <c r="G146" s="15"/>
       <c r="H146" s="13"/>
       <c r="I146" s="13"/>
-      <c r="J146" s="38"/>
-      <c r="K146" s="38"/>
+      <c r="J146" s="32"/>
+      <c r="K146" s="32"/>
     </row>
     <row r="147" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A147" s="13"/>
@@ -3868,8 +3916,8 @@
       <c r="G147" s="15"/>
       <c r="H147" s="13"/>
       <c r="I147" s="13"/>
-      <c r="J147" s="38"/>
-      <c r="K147" s="38"/>
+      <c r="J147" s="32"/>
+      <c r="K147" s="32"/>
     </row>
     <row r="148" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A148" s="13"/>
@@ -3881,8 +3929,8 @@
       <c r="G148" s="15"/>
       <c r="H148" s="13"/>
       <c r="I148" s="13"/>
-      <c r="J148" s="38"/>
-      <c r="K148" s="38"/>
+      <c r="J148" s="32"/>
+      <c r="K148" s="32"/>
     </row>
     <row r="149" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A149" s="13"/>
@@ -3894,8 +3942,8 @@
       <c r="G149" s="15"/>
       <c r="H149" s="13"/>
       <c r="I149" s="13"/>
-      <c r="J149" s="38"/>
-      <c r="K149" s="38"/>
+      <c r="J149" s="32"/>
+      <c r="K149" s="32"/>
     </row>
     <row r="150" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A150" s="13"/>
@@ -3907,8 +3955,8 @@
       <c r="G150" s="15"/>
       <c r="H150" s="13"/>
       <c r="I150" s="13"/>
-      <c r="J150" s="38"/>
-      <c r="K150" s="38"/>
+      <c r="J150" s="32"/>
+      <c r="K150" s="32"/>
     </row>
     <row r="151" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A151" s="13"/>
@@ -3920,8 +3968,8 @@
       <c r="G151" s="15"/>
       <c r="H151" s="13"/>
       <c r="I151" s="13"/>
-      <c r="J151" s="38"/>
-      <c r="K151" s="38"/>
+      <c r="J151" s="32"/>
+      <c r="K151" s="32"/>
     </row>
     <row r="152" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A152" s="13"/>
@@ -3933,8 +3981,8 @@
       <c r="G152" s="15"/>
       <c r="H152" s="13"/>
       <c r="I152" s="13"/>
-      <c r="J152" s="38"/>
-      <c r="K152" s="38"/>
+      <c r="J152" s="32"/>
+      <c r="K152" s="32"/>
     </row>
     <row r="153" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A153" s="13"/>
@@ -3946,8 +3994,8 @@
       <c r="G153" s="15"/>
       <c r="H153" s="13"/>
       <c r="I153" s="13"/>
-      <c r="J153" s="38"/>
-      <c r="K153" s="38"/>
+      <c r="J153" s="32"/>
+      <c r="K153" s="32"/>
     </row>
     <row r="154" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A154" s="13"/>
@@ -3959,8 +4007,8 @@
       <c r="G154" s="15"/>
       <c r="H154" s="13"/>
       <c r="I154" s="13"/>
-      <c r="J154" s="38"/>
-      <c r="K154" s="38"/>
+      <c r="J154" s="32"/>
+      <c r="K154" s="32"/>
     </row>
     <row r="155" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A155" s="13"/>
@@ -3972,8 +4020,8 @@
       <c r="G155" s="15"/>
       <c r="H155" s="13"/>
       <c r="I155" s="13"/>
-      <c r="J155" s="38"/>
-      <c r="K155" s="38"/>
+      <c r="J155" s="32"/>
+      <c r="K155" s="32"/>
     </row>
     <row r="156" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A156" s="13"/>
@@ -3985,8 +4033,8 @@
       <c r="G156" s="15"/>
       <c r="H156" s="13"/>
       <c r="I156" s="13"/>
-      <c r="J156" s="38"/>
-      <c r="K156" s="38"/>
+      <c r="J156" s="32"/>
+      <c r="K156" s="32"/>
     </row>
     <row r="157" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A157" s="13"/>
@@ -3998,8 +4046,8 @@
       <c r="G157" s="15"/>
       <c r="H157" s="13"/>
       <c r="I157" s="13"/>
-      <c r="J157" s="38"/>
-      <c r="K157" s="38"/>
+      <c r="J157" s="32"/>
+      <c r="K157" s="32"/>
     </row>
     <row r="158" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A158" s="13"/>
@@ -4011,8 +4059,8 @@
       <c r="G158" s="15"/>
       <c r="H158" s="13"/>
       <c r="I158" s="13"/>
-      <c r="J158" s="38"/>
-      <c r="K158" s="38"/>
+      <c r="J158" s="32"/>
+      <c r="K158" s="32"/>
     </row>
     <row r="159" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A159" s="13"/>
@@ -4024,8 +4072,8 @@
       <c r="G159" s="15"/>
       <c r="H159" s="13"/>
       <c r="I159" s="13"/>
-      <c r="J159" s="38"/>
-      <c r="K159" s="38"/>
+      <c r="J159" s="32"/>
+      <c r="K159" s="32"/>
     </row>
     <row r="160" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A160" s="13"/>
@@ -4037,8 +4085,8 @@
       <c r="G160" s="15"/>
       <c r="H160" s="13"/>
       <c r="I160" s="13"/>
-      <c r="J160" s="38"/>
-      <c r="K160" s="38"/>
+      <c r="J160" s="32"/>
+      <c r="K160" s="32"/>
     </row>
     <row r="161" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A161" s="13"/>
@@ -4050,8 +4098,8 @@
       <c r="G161" s="15"/>
       <c r="H161" s="13"/>
       <c r="I161" s="13"/>
-      <c r="J161" s="38"/>
-      <c r="K161" s="38"/>
+      <c r="J161" s="32"/>
+      <c r="K161" s="32"/>
     </row>
     <row r="162" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A162" s="13"/>
@@ -4063,8 +4111,8 @@
       <c r="G162" s="15"/>
       <c r="H162" s="13"/>
       <c r="I162" s="13"/>
-      <c r="J162" s="38"/>
-      <c r="K162" s="38"/>
+      <c r="J162" s="32"/>
+      <c r="K162" s="32"/>
     </row>
     <row r="163" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A163" s="13"/>
@@ -4076,8 +4124,8 @@
       <c r="G163" s="15"/>
       <c r="H163" s="13"/>
       <c r="I163" s="13"/>
-      <c r="J163" s="38"/>
-      <c r="K163" s="38"/>
+      <c r="J163" s="32"/>
+      <c r="K163" s="32"/>
     </row>
     <row r="164" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A164" s="13"/>
@@ -4089,8 +4137,8 @@
       <c r="G164" s="15"/>
       <c r="H164" s="13"/>
       <c r="I164" s="13"/>
-      <c r="J164" s="38"/>
-      <c r="K164" s="38"/>
+      <c r="J164" s="32"/>
+      <c r="K164" s="32"/>
     </row>
     <row r="165" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A165" s="13"/>
@@ -4102,8 +4150,8 @@
       <c r="G165" s="15"/>
       <c r="H165" s="13"/>
       <c r="I165" s="13"/>
-      <c r="J165" s="38"/>
-      <c r="K165" s="38"/>
+      <c r="J165" s="32"/>
+      <c r="K165" s="32"/>
     </row>
     <row r="166" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A166" s="13"/>
@@ -4115,8 +4163,8 @@
       <c r="G166" s="15"/>
       <c r="H166" s="13"/>
       <c r="I166" s="13"/>
-      <c r="J166" s="38"/>
-      <c r="K166" s="38"/>
+      <c r="J166" s="32"/>
+      <c r="K166" s="32"/>
     </row>
     <row r="167" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A167" s="13"/>
@@ -4128,8 +4176,8 @@
       <c r="G167" s="15"/>
       <c r="H167" s="13"/>
       <c r="I167" s="13"/>
-      <c r="J167" s="38"/>
-      <c r="K167" s="38"/>
+      <c r="J167" s="32"/>
+      <c r="K167" s="32"/>
     </row>
     <row r="168" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A168" s="13"/>
@@ -4141,8 +4189,8 @@
       <c r="G168" s="15"/>
       <c r="H168" s="13"/>
       <c r="I168" s="13"/>
-      <c r="J168" s="38"/>
-      <c r="K168" s="38"/>
+      <c r="J168" s="32"/>
+      <c r="K168" s="32"/>
     </row>
     <row r="169" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A169" s="13"/>
@@ -4154,8 +4202,8 @@
       <c r="G169" s="15"/>
       <c r="H169" s="13"/>
       <c r="I169" s="13"/>
-      <c r="J169" s="38"/>
-      <c r="K169" s="38"/>
+      <c r="J169" s="32"/>
+      <c r="K169" s="32"/>
     </row>
     <row r="170" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A170" s="13"/>
@@ -4167,8 +4215,8 @@
       <c r="G170" s="15"/>
       <c r="H170" s="13"/>
       <c r="I170" s="13"/>
-      <c r="J170" s="38"/>
-      <c r="K170" s="38"/>
+      <c r="J170" s="32"/>
+      <c r="K170" s="32"/>
     </row>
     <row r="171" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A171" s="13"/>
@@ -4180,8 +4228,8 @@
       <c r="G171" s="15"/>
       <c r="H171" s="13"/>
       <c r="I171" s="13"/>
-      <c r="J171" s="38"/>
-      <c r="K171" s="38"/>
+      <c r="J171" s="32"/>
+      <c r="K171" s="32"/>
     </row>
     <row r="172" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A172" s="13"/>
@@ -4193,8 +4241,8 @@
       <c r="G172" s="15"/>
       <c r="H172" s="13"/>
       <c r="I172" s="13"/>
-      <c r="J172" s="38"/>
-      <c r="K172" s="38"/>
+      <c r="J172" s="32"/>
+      <c r="K172" s="32"/>
     </row>
     <row r="173" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A173" s="13"/>
@@ -4206,8 +4254,8 @@
       <c r="G173" s="15"/>
       <c r="H173" s="13"/>
       <c r="I173" s="13"/>
-      <c r="J173" s="38"/>
-      <c r="K173" s="38"/>
+      <c r="J173" s="32"/>
+      <c r="K173" s="32"/>
     </row>
     <row r="174" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A174" s="13"/>
@@ -4219,8 +4267,8 @@
       <c r="G174" s="15"/>
       <c r="H174" s="13"/>
       <c r="I174" s="13"/>
-      <c r="J174" s="38"/>
-      <c r="K174" s="38"/>
+      <c r="J174" s="32"/>
+      <c r="K174" s="32"/>
     </row>
     <row r="175" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A175" s="13"/>
@@ -4232,8 +4280,8 @@
       <c r="G175" s="15"/>
       <c r="H175" s="13"/>
       <c r="I175" s="13"/>
-      <c r="J175" s="38"/>
-      <c r="K175" s="38"/>
+      <c r="J175" s="32"/>
+      <c r="K175" s="32"/>
     </row>
     <row r="176" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A176" s="13"/>
@@ -4245,8 +4293,8 @@
       <c r="G176" s="15"/>
       <c r="H176" s="13"/>
       <c r="I176" s="13"/>
-      <c r="J176" s="38"/>
-      <c r="K176" s="38"/>
+      <c r="J176" s="32"/>
+      <c r="K176" s="32"/>
     </row>
     <row r="177" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A177" s="13"/>
@@ -4258,8 +4306,8 @@
       <c r="G177" s="15"/>
       <c r="H177" s="13"/>
       <c r="I177" s="13"/>
-      <c r="J177" s="38"/>
-      <c r="K177" s="38"/>
+      <c r="J177" s="32"/>
+      <c r="K177" s="32"/>
     </row>
     <row r="178" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A178" s="13"/>
@@ -4271,8 +4319,8 @@
       <c r="G178" s="15"/>
       <c r="H178" s="13"/>
       <c r="I178" s="13"/>
-      <c r="J178" s="38"/>
-      <c r="K178" s="38"/>
+      <c r="J178" s="32"/>
+      <c r="K178" s="32"/>
     </row>
     <row r="179" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A179" s="13"/>
@@ -4284,8 +4332,8 @@
       <c r="G179" s="15"/>
       <c r="H179" s="13"/>
       <c r="I179" s="13"/>
-      <c r="J179" s="38"/>
-      <c r="K179" s="38"/>
+      <c r="J179" s="32"/>
+      <c r="K179" s="32"/>
     </row>
     <row r="180" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A180" s="13"/>
@@ -4297,8 +4345,8 @@
       <c r="G180" s="15"/>
       <c r="H180" s="13"/>
       <c r="I180" s="13"/>
-      <c r="J180" s="38"/>
-      <c r="K180" s="38"/>
+      <c r="J180" s="32"/>
+      <c r="K180" s="32"/>
     </row>
     <row r="181" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A181" s="13"/>
@@ -4310,8 +4358,8 @@
       <c r="G181" s="15"/>
       <c r="H181" s="13"/>
       <c r="I181" s="13"/>
-      <c r="J181" s="38"/>
-      <c r="K181" s="38"/>
+      <c r="J181" s="32"/>
+      <c r="K181" s="32"/>
     </row>
     <row r="182" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A182" s="13"/>
@@ -4323,8 +4371,8 @@
       <c r="G182" s="15"/>
       <c r="H182" s="13"/>
       <c r="I182" s="13"/>
-      <c r="J182" s="38"/>
-      <c r="K182" s="38"/>
+      <c r="J182" s="32"/>
+      <c r="K182" s="32"/>
     </row>
     <row r="183" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A183" s="13"/>
@@ -4336,8 +4384,8 @@
       <c r="G183" s="15"/>
       <c r="H183" s="13"/>
       <c r="I183" s="13"/>
-      <c r="J183" s="38"/>
-      <c r="K183" s="38"/>
+      <c r="J183" s="32"/>
+      <c r="K183" s="32"/>
     </row>
     <row r="184" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A184" s="13"/>
@@ -4349,8 +4397,8 @@
       <c r="G184" s="15"/>
       <c r="H184" s="13"/>
       <c r="I184" s="13"/>
-      <c r="J184" s="38"/>
-      <c r="K184" s="38"/>
+      <c r="J184" s="32"/>
+      <c r="K184" s="32"/>
     </row>
     <row r="185" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A185" s="13"/>
@@ -4362,8 +4410,8 @@
       <c r="G185" s="15"/>
       <c r="H185" s="13"/>
       <c r="I185" s="13"/>
-      <c r="J185" s="38"/>
-      <c r="K185" s="38"/>
+      <c r="J185" s="32"/>
+      <c r="K185" s="32"/>
     </row>
     <row r="186" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A186" s="13"/>
@@ -4375,8 +4423,8 @@
       <c r="G186" s="15"/>
       <c r="H186" s="13"/>
       <c r="I186" s="13"/>
-      <c r="J186" s="38"/>
-      <c r="K186" s="38"/>
+      <c r="J186" s="32"/>
+      <c r="K186" s="32"/>
     </row>
     <row r="187" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A187" s="13"/>
@@ -4388,8 +4436,8 @@
       <c r="G187" s="15"/>
       <c r="H187" s="13"/>
       <c r="I187" s="13"/>
-      <c r="J187" s="38"/>
-      <c r="K187" s="38"/>
+      <c r="J187" s="32"/>
+      <c r="K187" s="32"/>
     </row>
     <row r="188" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A188" s="13"/>
@@ -4401,8 +4449,8 @@
       <c r="G188" s="15"/>
       <c r="H188" s="13"/>
       <c r="I188" s="13"/>
-      <c r="J188" s="38"/>
-      <c r="K188" s="38"/>
+      <c r="J188" s="32"/>
+      <c r="K188" s="32"/>
     </row>
     <row r="189" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A189" s="13"/>
@@ -4414,8 +4462,8 @@
       <c r="G189" s="15"/>
       <c r="H189" s="13"/>
       <c r="I189" s="13"/>
-      <c r="J189" s="38"/>
-      <c r="K189" s="38"/>
+      <c r="J189" s="32"/>
+      <c r="K189" s="32"/>
     </row>
     <row r="190" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A190" s="13"/>
@@ -4427,8 +4475,8 @@
       <c r="G190" s="15"/>
       <c r="H190" s="13"/>
       <c r="I190" s="13"/>
-      <c r="J190" s="38"/>
-      <c r="K190" s="38"/>
+      <c r="J190" s="32"/>
+      <c r="K190" s="32"/>
     </row>
     <row r="191" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A191" s="13"/>
@@ -4440,8 +4488,8 @@
       <c r="G191" s="15"/>
       <c r="H191" s="13"/>
       <c r="I191" s="13"/>
-      <c r="J191" s="38"/>
-      <c r="K191" s="38"/>
+      <c r="J191" s="32"/>
+      <c r="K191" s="32"/>
     </row>
     <row r="192" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A192" s="13"/>
@@ -4453,8 +4501,8 @@
       <c r="G192" s="15"/>
       <c r="H192" s="13"/>
       <c r="I192" s="13"/>
-      <c r="J192" s="38"/>
-      <c r="K192" s="38"/>
+      <c r="J192" s="32"/>
+      <c r="K192" s="32"/>
     </row>
     <row r="193" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A193" s="13"/>
@@ -4466,8 +4514,8 @@
       <c r="G193" s="15"/>
       <c r="H193" s="13"/>
       <c r="I193" s="13"/>
-      <c r="J193" s="38"/>
-      <c r="K193" s="38"/>
+      <c r="J193" s="32"/>
+      <c r="K193" s="32"/>
     </row>
     <row r="194" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A194" s="13"/>
@@ -4479,8 +4527,8 @@
       <c r="G194" s="15"/>
       <c r="H194" s="13"/>
       <c r="I194" s="13"/>
-      <c r="J194" s="38"/>
-      <c r="K194" s="38"/>
+      <c r="J194" s="32"/>
+      <c r="K194" s="32"/>
     </row>
     <row r="195" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A195" s="13"/>
@@ -4492,8 +4540,8 @@
       <c r="G195" s="15"/>
       <c r="H195" s="13"/>
       <c r="I195" s="13"/>
-      <c r="J195" s="38"/>
-      <c r="K195" s="38"/>
+      <c r="J195" s="32"/>
+      <c r="K195" s="32"/>
     </row>
     <row r="196" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A196" s="13"/>
@@ -4505,8 +4553,8 @@
       <c r="G196" s="15"/>
       <c r="H196" s="13"/>
       <c r="I196" s="13"/>
-      <c r="J196" s="38"/>
-      <c r="K196" s="38"/>
+      <c r="J196" s="32"/>
+      <c r="K196" s="32"/>
     </row>
     <row r="197" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A197" s="13"/>
@@ -4518,8 +4566,8 @@
       <c r="G197" s="15"/>
       <c r="H197" s="13"/>
       <c r="I197" s="13"/>
-      <c r="J197" s="38"/>
-      <c r="K197" s="38"/>
+      <c r="J197" s="32"/>
+      <c r="K197" s="32"/>
     </row>
     <row r="198" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A198" s="13"/>
@@ -4531,8 +4579,8 @@
       <c r="G198" s="15"/>
       <c r="H198" s="13"/>
       <c r="I198" s="13"/>
-      <c r="J198" s="38"/>
-      <c r="K198" s="38"/>
+      <c r="J198" s="32"/>
+      <c r="K198" s="32"/>
     </row>
     <row r="199" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A199" s="13"/>
@@ -4544,8 +4592,8 @@
       <c r="G199" s="15"/>
       <c r="H199" s="13"/>
       <c r="I199" s="13"/>
-      <c r="J199" s="38"/>
-      <c r="K199" s="38"/>
+      <c r="J199" s="32"/>
+      <c r="K199" s="32"/>
     </row>
     <row r="200" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A200" s="13"/>
@@ -4557,8 +4605,8 @@
       <c r="G200" s="15"/>
       <c r="H200" s="13"/>
       <c r="I200" s="13"/>
-      <c r="J200" s="38"/>
-      <c r="K200" s="38"/>
+      <c r="J200" s="32"/>
+      <c r="K200" s="32"/>
     </row>
     <row r="201" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A201" s="13"/>
@@ -4570,8 +4618,8 @@
       <c r="G201" s="15"/>
       <c r="H201" s="13"/>
       <c r="I201" s="13"/>
-      <c r="J201" s="38"/>
-      <c r="K201" s="38"/>
+      <c r="J201" s="32"/>
+      <c r="K201" s="32"/>
     </row>
     <row r="202" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A202" s="13"/>
@@ -4583,8 +4631,8 @@
       <c r="G202" s="15"/>
       <c r="H202" s="13"/>
       <c r="I202" s="13"/>
-      <c r="J202" s="38"/>
-      <c r="K202" s="38"/>
+      <c r="J202" s="32"/>
+      <c r="K202" s="32"/>
     </row>
     <row r="203" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A203" s="13"/>
@@ -4596,8 +4644,8 @@
       <c r="G203" s="15"/>
       <c r="H203" s="13"/>
       <c r="I203" s="13"/>
-      <c r="J203" s="38"/>
-      <c r="K203" s="38"/>
+      <c r="J203" s="32"/>
+      <c r="K203" s="32"/>
     </row>
     <row r="204" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A204" s="13"/>
@@ -4609,8 +4657,8 @@
       <c r="G204" s="15"/>
       <c r="H204" s="13"/>
       <c r="I204" s="13"/>
-      <c r="J204" s="38"/>
-      <c r="K204" s="38"/>
+      <c r="J204" s="32"/>
+      <c r="K204" s="32"/>
     </row>
     <row r="205" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A205" s="13"/>
@@ -4622,8 +4670,8 @@
       <c r="G205" s="15"/>
       <c r="H205" s="13"/>
       <c r="I205" s="13"/>
-      <c r="J205" s="38"/>
-      <c r="K205" s="38"/>
+      <c r="J205" s="32"/>
+      <c r="K205" s="32"/>
     </row>
     <row r="206" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A206" s="13"/>
@@ -4635,8 +4683,8 @@
       <c r="G206" s="15"/>
       <c r="H206" s="13"/>
       <c r="I206" s="13"/>
-      <c r="J206" s="38"/>
-      <c r="K206" s="38"/>
+      <c r="J206" s="32"/>
+      <c r="K206" s="32"/>
     </row>
     <row r="207" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A207" s="13"/>
@@ -4648,8 +4696,8 @@
       <c r="G207" s="15"/>
       <c r="H207" s="13"/>
       <c r="I207" s="13"/>
-      <c r="J207" s="38"/>
-      <c r="K207" s="38"/>
+      <c r="J207" s="32"/>
+      <c r="K207" s="32"/>
     </row>
     <row r="208" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A208" s="13"/>
@@ -4661,8 +4709,8 @@
       <c r="G208" s="15"/>
       <c r="H208" s="13"/>
       <c r="I208" s="13"/>
-      <c r="J208" s="38"/>
-      <c r="K208" s="38"/>
+      <c r="J208" s="32"/>
+      <c r="K208" s="32"/>
     </row>
     <row r="209" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A209" s="13"/>
@@ -4674,8 +4722,8 @@
       <c r="G209" s="15"/>
       <c r="H209" s="13"/>
       <c r="I209" s="13"/>
-      <c r="J209" s="38"/>
-      <c r="K209" s="38"/>
+      <c r="J209" s="32"/>
+      <c r="K209" s="32"/>
     </row>
     <row r="210" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A210" s="13"/>
@@ -4687,8 +4735,8 @@
       <c r="G210" s="15"/>
       <c r="H210" s="13"/>
       <c r="I210" s="13"/>
-      <c r="J210" s="38"/>
-      <c r="K210" s="38"/>
+      <c r="J210" s="32"/>
+      <c r="K210" s="32"/>
     </row>
     <row r="211" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A211" s="13"/>
@@ -4700,8 +4748,8 @@
       <c r="G211" s="15"/>
       <c r="H211" s="13"/>
       <c r="I211" s="13"/>
-      <c r="J211" s="38"/>
-      <c r="K211" s="38"/>
+      <c r="J211" s="32"/>
+      <c r="K211" s="32"/>
     </row>
     <row r="212" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A212" s="13"/>
@@ -4713,8 +4761,8 @@
       <c r="G212" s="15"/>
       <c r="H212" s="13"/>
       <c r="I212" s="13"/>
-      <c r="J212" s="38"/>
-      <c r="K212" s="38"/>
+      <c r="J212" s="32"/>
+      <c r="K212" s="32"/>
     </row>
     <row r="213" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A213" s="13"/>
@@ -4726,8 +4774,8 @@
       <c r="G213" s="15"/>
       <c r="H213" s="13"/>
       <c r="I213" s="13"/>
-      <c r="J213" s="38"/>
-      <c r="K213" s="38"/>
+      <c r="J213" s="32"/>
+      <c r="K213" s="32"/>
     </row>
     <row r="214" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A214" s="13"/>
@@ -4739,8 +4787,8 @@
       <c r="G214" s="15"/>
       <c r="H214" s="13"/>
       <c r="I214" s="13"/>
-      <c r="J214" s="38"/>
-      <c r="K214" s="38"/>
+      <c r="J214" s="32"/>
+      <c r="K214" s="32"/>
     </row>
     <row r="215" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A215" s="13"/>
@@ -4752,8 +4800,8 @@
       <c r="G215" s="15"/>
       <c r="H215" s="13"/>
       <c r="I215" s="13"/>
-      <c r="J215" s="38"/>
-      <c r="K215" s="38"/>
+      <c r="J215" s="32"/>
+      <c r="K215" s="32"/>
     </row>
     <row r="216" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A216" s="13"/>
@@ -4765,8 +4813,8 @@
       <c r="G216" s="15"/>
       <c r="H216" s="13"/>
       <c r="I216" s="13"/>
-      <c r="J216" s="38"/>
-      <c r="K216" s="38"/>
+      <c r="J216" s="32"/>
+      <c r="K216" s="32"/>
     </row>
     <row r="217" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A217" s="13"/>
@@ -4778,8 +4826,8 @@
       <c r="G217" s="15"/>
       <c r="H217" s="13"/>
       <c r="I217" s="13"/>
-      <c r="J217" s="38"/>
-      <c r="K217" s="38"/>
+      <c r="J217" s="32"/>
+      <c r="K217" s="32"/>
     </row>
     <row r="218" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A218" s="13"/>
@@ -4791,8 +4839,8 @@
       <c r="G218" s="15"/>
       <c r="H218" s="13"/>
       <c r="I218" s="13"/>
-      <c r="J218" s="38"/>
-      <c r="K218" s="38"/>
+      <c r="J218" s="32"/>
+      <c r="K218" s="32"/>
     </row>
     <row r="219" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A219" s="13"/>
@@ -4804,8 +4852,8 @@
       <c r="G219" s="15"/>
       <c r="H219" s="13"/>
       <c r="I219" s="13"/>
-      <c r="J219" s="38"/>
-      <c r="K219" s="38"/>
+      <c r="J219" s="32"/>
+      <c r="K219" s="32"/>
     </row>
     <row r="220" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A220" s="13"/>
@@ -4817,8 +4865,8 @@
       <c r="G220" s="15"/>
       <c r="H220" s="13"/>
       <c r="I220" s="13"/>
-      <c r="J220" s="38"/>
-      <c r="K220" s="38"/>
+      <c r="J220" s="32"/>
+      <c r="K220" s="32"/>
     </row>
     <row r="221" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A221" s="13"/>
@@ -4830,8 +4878,8 @@
       <c r="G221" s="15"/>
       <c r="H221" s="13"/>
       <c r="I221" s="13"/>
-      <c r="J221" s="38"/>
-      <c r="K221" s="38"/>
+      <c r="J221" s="32"/>
+      <c r="K221" s="32"/>
     </row>
     <row r="222" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A222" s="13"/>
@@ -4843,8 +4891,8 @@
       <c r="G222" s="15"/>
       <c r="H222" s="13"/>
       <c r="I222" s="13"/>
-      <c r="J222" s="38"/>
-      <c r="K222" s="38"/>
+      <c r="J222" s="32"/>
+      <c r="K222" s="32"/>
     </row>
     <row r="223" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A223" s="13"/>
@@ -4856,8 +4904,8 @@
       <c r="G223" s="15"/>
       <c r="H223" s="13"/>
       <c r="I223" s="13"/>
-      <c r="J223" s="38"/>
-      <c r="K223" s="38"/>
+      <c r="J223" s="32"/>
+      <c r="K223" s="32"/>
     </row>
     <row r="224" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A224" s="13"/>
@@ -4869,8 +4917,8 @@
       <c r="G224" s="15"/>
       <c r="H224" s="13"/>
       <c r="I224" s="13"/>
-      <c r="J224" s="38"/>
-      <c r="K224" s="38"/>
+      <c r="J224" s="32"/>
+      <c r="K224" s="32"/>
     </row>
     <row r="225" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A225" s="13"/>
@@ -4882,8 +4930,8 @@
       <c r="G225" s="15"/>
       <c r="H225" s="13"/>
       <c r="I225" s="13"/>
-      <c r="J225" s="38"/>
-      <c r="K225" s="38"/>
+      <c r="J225" s="32"/>
+      <c r="K225" s="32"/>
     </row>
     <row r="226" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A226" s="13"/>
@@ -4895,8 +4943,8 @@
       <c r="G226" s="15"/>
       <c r="H226" s="13"/>
       <c r="I226" s="13"/>
-      <c r="J226" s="38"/>
-      <c r="K226" s="38"/>
+      <c r="J226" s="32"/>
+      <c r="K226" s="32"/>
     </row>
     <row r="227" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A227" s="13"/>
@@ -4908,8 +4956,8 @@
       <c r="G227" s="15"/>
       <c r="H227" s="13"/>
       <c r="I227" s="13"/>
-      <c r="J227" s="38"/>
-      <c r="K227" s="38"/>
+      <c r="J227" s="32"/>
+      <c r="K227" s="32"/>
     </row>
     <row r="228" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A228" s="13"/>
@@ -4921,8 +4969,8 @@
       <c r="G228" s="15"/>
       <c r="H228" s="13"/>
       <c r="I228" s="13"/>
-      <c r="J228" s="38"/>
-      <c r="K228" s="38"/>
+      <c r="J228" s="32"/>
+      <c r="K228" s="32"/>
     </row>
     <row r="229" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A229" s="13"/>
@@ -4934,8 +4982,8 @@
       <c r="G229" s="15"/>
       <c r="H229" s="13"/>
       <c r="I229" s="13"/>
-      <c r="J229" s="38"/>
-      <c r="K229" s="38"/>
+      <c r="J229" s="32"/>
+      <c r="K229" s="32"/>
     </row>
     <row r="230" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A230" s="13"/>
@@ -4947,8 +4995,8 @@
       <c r="G230" s="15"/>
       <c r="H230" s="13"/>
       <c r="I230" s="13"/>
-      <c r="J230" s="38"/>
-      <c r="K230" s="38"/>
+      <c r="J230" s="32"/>
+      <c r="K230" s="32"/>
     </row>
     <row r="231" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A231" s="13"/>
@@ -4960,8 +5008,8 @@
       <c r="G231" s="15"/>
       <c r="H231" s="13"/>
       <c r="I231" s="13"/>
-      <c r="J231" s="38"/>
-      <c r="K231" s="38"/>
+      <c r="J231" s="32"/>
+      <c r="K231" s="32"/>
     </row>
     <row r="232" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G232" s="2"/>
@@ -6990,208 +7038,132 @@
     </row>
   </sheetData>
   <mergeCells count="352">
-    <mergeCell ref="H128:I128"/>
-    <mergeCell ref="H129:I129"/>
-    <mergeCell ref="H119:I119"/>
-    <mergeCell ref="H120:I120"/>
-    <mergeCell ref="H121:I121"/>
-    <mergeCell ref="H122:I122"/>
-    <mergeCell ref="H123:I123"/>
-    <mergeCell ref="H124:I124"/>
-    <mergeCell ref="H125:I125"/>
-    <mergeCell ref="H126:I126"/>
-    <mergeCell ref="H127:I127"/>
-    <mergeCell ref="H110:I110"/>
-    <mergeCell ref="H111:I111"/>
-    <mergeCell ref="H112:I112"/>
-    <mergeCell ref="H113:I113"/>
-    <mergeCell ref="H114:I114"/>
-    <mergeCell ref="H115:I115"/>
-    <mergeCell ref="H116:I116"/>
-    <mergeCell ref="H117:I117"/>
-    <mergeCell ref="H118:I118"/>
-    <mergeCell ref="H101:I101"/>
-    <mergeCell ref="H102:I102"/>
-    <mergeCell ref="H103:I103"/>
-    <mergeCell ref="H104:I104"/>
-    <mergeCell ref="H105:I105"/>
-    <mergeCell ref="H106:I106"/>
-    <mergeCell ref="H107:I107"/>
-    <mergeCell ref="H108:I108"/>
-    <mergeCell ref="H109:I109"/>
-    <mergeCell ref="H92:I92"/>
-    <mergeCell ref="H93:I93"/>
-    <mergeCell ref="H94:I94"/>
-    <mergeCell ref="H95:I95"/>
-    <mergeCell ref="H96:I96"/>
-    <mergeCell ref="H97:I97"/>
-    <mergeCell ref="H98:I98"/>
-    <mergeCell ref="H99:I99"/>
-    <mergeCell ref="H100:I100"/>
-    <mergeCell ref="H83:I83"/>
-    <mergeCell ref="H84:I84"/>
-    <mergeCell ref="H85:I85"/>
-    <mergeCell ref="H86:I86"/>
-    <mergeCell ref="H87:I87"/>
-    <mergeCell ref="H88:I88"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="H90:I90"/>
-    <mergeCell ref="H91:I91"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="H78:I78"/>
-    <mergeCell ref="H79:I79"/>
-    <mergeCell ref="H80:I80"/>
-    <mergeCell ref="H81:I81"/>
-    <mergeCell ref="H82:I82"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="H67:I67"/>
-    <mergeCell ref="H68:I68"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="H70:I70"/>
-    <mergeCell ref="H71:I71"/>
-    <mergeCell ref="H72:I72"/>
-    <mergeCell ref="H73:I73"/>
-    <mergeCell ref="J230:K230"/>
-    <mergeCell ref="J231:K231"/>
-    <mergeCell ref="J221:K221"/>
-    <mergeCell ref="J222:K222"/>
-    <mergeCell ref="J223:K223"/>
-    <mergeCell ref="J224:K224"/>
-    <mergeCell ref="J225:K225"/>
-    <mergeCell ref="J226:K226"/>
-    <mergeCell ref="J227:K227"/>
-    <mergeCell ref="J228:K228"/>
-    <mergeCell ref="J229:K229"/>
-    <mergeCell ref="J212:K212"/>
-    <mergeCell ref="J213:K213"/>
-    <mergeCell ref="J214:K214"/>
-    <mergeCell ref="J215:K215"/>
-    <mergeCell ref="J216:K216"/>
-    <mergeCell ref="J217:K217"/>
-    <mergeCell ref="J218:K218"/>
-    <mergeCell ref="J219:K219"/>
-    <mergeCell ref="J220:K220"/>
-    <mergeCell ref="J203:K203"/>
-    <mergeCell ref="J204:K204"/>
-    <mergeCell ref="J205:K205"/>
-    <mergeCell ref="J206:K206"/>
-    <mergeCell ref="J207:K207"/>
-    <mergeCell ref="J208:K208"/>
-    <mergeCell ref="J209:K209"/>
-    <mergeCell ref="J210:K210"/>
-    <mergeCell ref="J211:K211"/>
-    <mergeCell ref="J194:K194"/>
-    <mergeCell ref="J195:K195"/>
-    <mergeCell ref="J196:K196"/>
-    <mergeCell ref="J197:K197"/>
-    <mergeCell ref="J198:K198"/>
-    <mergeCell ref="J199:K199"/>
-    <mergeCell ref="J200:K200"/>
-    <mergeCell ref="J201:K201"/>
-    <mergeCell ref="J202:K202"/>
-    <mergeCell ref="J185:K185"/>
-    <mergeCell ref="J186:K186"/>
-    <mergeCell ref="J187:K187"/>
-    <mergeCell ref="J188:K188"/>
-    <mergeCell ref="J189:K189"/>
-    <mergeCell ref="J190:K190"/>
-    <mergeCell ref="J191:K191"/>
-    <mergeCell ref="J192:K192"/>
-    <mergeCell ref="J193:K193"/>
-    <mergeCell ref="J176:K176"/>
-    <mergeCell ref="J177:K177"/>
-    <mergeCell ref="J178:K178"/>
-    <mergeCell ref="J179:K179"/>
-    <mergeCell ref="J180:K180"/>
-    <mergeCell ref="J181:K181"/>
-    <mergeCell ref="J182:K182"/>
-    <mergeCell ref="J183:K183"/>
-    <mergeCell ref="J184:K184"/>
-    <mergeCell ref="J167:K167"/>
-    <mergeCell ref="J168:K168"/>
-    <mergeCell ref="J169:K169"/>
-    <mergeCell ref="J170:K170"/>
-    <mergeCell ref="J171:K171"/>
-    <mergeCell ref="J172:K172"/>
-    <mergeCell ref="J173:K173"/>
-    <mergeCell ref="J174:K174"/>
-    <mergeCell ref="J175:K175"/>
-    <mergeCell ref="J158:K158"/>
-    <mergeCell ref="J159:K159"/>
-    <mergeCell ref="J160:K160"/>
-    <mergeCell ref="J161:K161"/>
-    <mergeCell ref="J162:K162"/>
-    <mergeCell ref="J163:K163"/>
-    <mergeCell ref="J164:K164"/>
-    <mergeCell ref="J165:K165"/>
-    <mergeCell ref="J166:K166"/>
-    <mergeCell ref="J149:K149"/>
-    <mergeCell ref="J150:K150"/>
-    <mergeCell ref="J151:K151"/>
-    <mergeCell ref="J152:K152"/>
-    <mergeCell ref="J153:K153"/>
-    <mergeCell ref="J154:K154"/>
-    <mergeCell ref="J155:K155"/>
-    <mergeCell ref="J156:K156"/>
-    <mergeCell ref="J157:K157"/>
-    <mergeCell ref="J140:K140"/>
-    <mergeCell ref="J141:K141"/>
-    <mergeCell ref="J142:K142"/>
-    <mergeCell ref="J143:K143"/>
-    <mergeCell ref="J144:K144"/>
-    <mergeCell ref="J145:K145"/>
-    <mergeCell ref="J146:K146"/>
-    <mergeCell ref="J147:K147"/>
-    <mergeCell ref="J148:K148"/>
-    <mergeCell ref="J131:K131"/>
-    <mergeCell ref="J132:K132"/>
-    <mergeCell ref="J133:K133"/>
-    <mergeCell ref="J134:K134"/>
-    <mergeCell ref="J135:K135"/>
-    <mergeCell ref="J136:K136"/>
-    <mergeCell ref="J137:K137"/>
-    <mergeCell ref="J138:K138"/>
-    <mergeCell ref="J139:K139"/>
-    <mergeCell ref="J122:K122"/>
-    <mergeCell ref="J123:K123"/>
-    <mergeCell ref="J124:K124"/>
-    <mergeCell ref="J125:K125"/>
-    <mergeCell ref="J126:K126"/>
-    <mergeCell ref="J127:K127"/>
-    <mergeCell ref="J128:K128"/>
-    <mergeCell ref="J129:K129"/>
-    <mergeCell ref="J130:K130"/>
-    <mergeCell ref="J113:K113"/>
-    <mergeCell ref="J114:K114"/>
-    <mergeCell ref="J115:K115"/>
-    <mergeCell ref="J116:K116"/>
-    <mergeCell ref="J117:K117"/>
-    <mergeCell ref="J118:K118"/>
-    <mergeCell ref="J119:K119"/>
-    <mergeCell ref="J120:K120"/>
-    <mergeCell ref="J121:K121"/>
-    <mergeCell ref="J104:K104"/>
-    <mergeCell ref="J105:K105"/>
-    <mergeCell ref="J106:K106"/>
-    <mergeCell ref="J107:K107"/>
-    <mergeCell ref="J108:K108"/>
-    <mergeCell ref="J109:K109"/>
-    <mergeCell ref="J110:K110"/>
-    <mergeCell ref="J111:K111"/>
-    <mergeCell ref="J112:K112"/>
-    <mergeCell ref="J95:K95"/>
-    <mergeCell ref="J96:K96"/>
-    <mergeCell ref="J97:K97"/>
-    <mergeCell ref="J98:K98"/>
-    <mergeCell ref="J99:K99"/>
-    <mergeCell ref="J100:K100"/>
-    <mergeCell ref="J101:K101"/>
-    <mergeCell ref="J102:K102"/>
-    <mergeCell ref="J103:K103"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="A60:K60"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="A33:K33"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A20:K20"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="A27:K27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="J52:K52"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J90:K90"/>
+    <mergeCell ref="J91:K91"/>
+    <mergeCell ref="J92:K92"/>
+    <mergeCell ref="J93:K93"/>
+    <mergeCell ref="J94:K94"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J71:K71"/>
+    <mergeCell ref="J72:K72"/>
+    <mergeCell ref="J81:K81"/>
+    <mergeCell ref="J82:K82"/>
+    <mergeCell ref="J83:K83"/>
+    <mergeCell ref="J84:K84"/>
+    <mergeCell ref="J85:K85"/>
+    <mergeCell ref="J86:K86"/>
+    <mergeCell ref="J87:K87"/>
     <mergeCell ref="J88:K88"/>
     <mergeCell ref="J89:K89"/>
     <mergeCell ref="J73:K73"/>
@@ -7216,132 +7188,208 @@
     <mergeCell ref="J48:K48"/>
     <mergeCell ref="J49:K49"/>
     <mergeCell ref="J50:K50"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="J90:K90"/>
-    <mergeCell ref="J91:K91"/>
-    <mergeCell ref="J92:K92"/>
-    <mergeCell ref="J93:K93"/>
-    <mergeCell ref="J94:K94"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J67:K67"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="J71:K71"/>
-    <mergeCell ref="J72:K72"/>
-    <mergeCell ref="J81:K81"/>
-    <mergeCell ref="J82:K82"/>
-    <mergeCell ref="J83:K83"/>
-    <mergeCell ref="J84:K84"/>
-    <mergeCell ref="J85:K85"/>
-    <mergeCell ref="J86:K86"/>
-    <mergeCell ref="J87:K87"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="J52:K52"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="J51:K51"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="A27:K27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A20:K20"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="A33:K33"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="A60:K60"/>
+    <mergeCell ref="J95:K95"/>
+    <mergeCell ref="J96:K96"/>
+    <mergeCell ref="J97:K97"/>
+    <mergeCell ref="J98:K98"/>
+    <mergeCell ref="J99:K99"/>
+    <mergeCell ref="J100:K100"/>
+    <mergeCell ref="J101:K101"/>
+    <mergeCell ref="J102:K102"/>
+    <mergeCell ref="J103:K103"/>
+    <mergeCell ref="J104:K104"/>
+    <mergeCell ref="J105:K105"/>
+    <mergeCell ref="J106:K106"/>
+    <mergeCell ref="J107:K107"/>
+    <mergeCell ref="J108:K108"/>
+    <mergeCell ref="J109:K109"/>
+    <mergeCell ref="J110:K110"/>
+    <mergeCell ref="J111:K111"/>
+    <mergeCell ref="J112:K112"/>
+    <mergeCell ref="J113:K113"/>
+    <mergeCell ref="J114:K114"/>
+    <mergeCell ref="J115:K115"/>
+    <mergeCell ref="J116:K116"/>
+    <mergeCell ref="J117:K117"/>
+    <mergeCell ref="J118:K118"/>
+    <mergeCell ref="J119:K119"/>
+    <mergeCell ref="J120:K120"/>
+    <mergeCell ref="J121:K121"/>
+    <mergeCell ref="J122:K122"/>
+    <mergeCell ref="J123:K123"/>
+    <mergeCell ref="J124:K124"/>
+    <mergeCell ref="J125:K125"/>
+    <mergeCell ref="J126:K126"/>
+    <mergeCell ref="J127:K127"/>
+    <mergeCell ref="J128:K128"/>
+    <mergeCell ref="J129:K129"/>
+    <mergeCell ref="J130:K130"/>
+    <mergeCell ref="J131:K131"/>
+    <mergeCell ref="J132:K132"/>
+    <mergeCell ref="J133:K133"/>
+    <mergeCell ref="J134:K134"/>
+    <mergeCell ref="J135:K135"/>
+    <mergeCell ref="J136:K136"/>
+    <mergeCell ref="J137:K137"/>
+    <mergeCell ref="J138:K138"/>
+    <mergeCell ref="J139:K139"/>
+    <mergeCell ref="J140:K140"/>
+    <mergeCell ref="J141:K141"/>
+    <mergeCell ref="J142:K142"/>
+    <mergeCell ref="J143:K143"/>
+    <mergeCell ref="J144:K144"/>
+    <mergeCell ref="J145:K145"/>
+    <mergeCell ref="J146:K146"/>
+    <mergeCell ref="J147:K147"/>
+    <mergeCell ref="J148:K148"/>
+    <mergeCell ref="J149:K149"/>
+    <mergeCell ref="J150:K150"/>
+    <mergeCell ref="J151:K151"/>
+    <mergeCell ref="J152:K152"/>
+    <mergeCell ref="J153:K153"/>
+    <mergeCell ref="J154:K154"/>
+    <mergeCell ref="J155:K155"/>
+    <mergeCell ref="J156:K156"/>
+    <mergeCell ref="J157:K157"/>
+    <mergeCell ref="J158:K158"/>
+    <mergeCell ref="J159:K159"/>
+    <mergeCell ref="J160:K160"/>
+    <mergeCell ref="J161:K161"/>
+    <mergeCell ref="J162:K162"/>
+    <mergeCell ref="J163:K163"/>
+    <mergeCell ref="J164:K164"/>
+    <mergeCell ref="J165:K165"/>
+    <mergeCell ref="J166:K166"/>
+    <mergeCell ref="J167:K167"/>
+    <mergeCell ref="J168:K168"/>
+    <mergeCell ref="J169:K169"/>
+    <mergeCell ref="J170:K170"/>
+    <mergeCell ref="J171:K171"/>
+    <mergeCell ref="J172:K172"/>
+    <mergeCell ref="J173:K173"/>
+    <mergeCell ref="J174:K174"/>
+    <mergeCell ref="J175:K175"/>
+    <mergeCell ref="J176:K176"/>
+    <mergeCell ref="J177:K177"/>
+    <mergeCell ref="J178:K178"/>
+    <mergeCell ref="J179:K179"/>
+    <mergeCell ref="J180:K180"/>
+    <mergeCell ref="J181:K181"/>
+    <mergeCell ref="J182:K182"/>
+    <mergeCell ref="J183:K183"/>
+    <mergeCell ref="J184:K184"/>
+    <mergeCell ref="J185:K185"/>
+    <mergeCell ref="J186:K186"/>
+    <mergeCell ref="J187:K187"/>
+    <mergeCell ref="J188:K188"/>
+    <mergeCell ref="J189:K189"/>
+    <mergeCell ref="J190:K190"/>
+    <mergeCell ref="J191:K191"/>
+    <mergeCell ref="J192:K192"/>
+    <mergeCell ref="J193:K193"/>
+    <mergeCell ref="J194:K194"/>
+    <mergeCell ref="J195:K195"/>
+    <mergeCell ref="J196:K196"/>
+    <mergeCell ref="J197:K197"/>
+    <mergeCell ref="J198:K198"/>
+    <mergeCell ref="J199:K199"/>
+    <mergeCell ref="J200:K200"/>
+    <mergeCell ref="J201:K201"/>
+    <mergeCell ref="J202:K202"/>
+    <mergeCell ref="J203:K203"/>
+    <mergeCell ref="J204:K204"/>
+    <mergeCell ref="J205:K205"/>
+    <mergeCell ref="J206:K206"/>
+    <mergeCell ref="J207:K207"/>
+    <mergeCell ref="J208:K208"/>
+    <mergeCell ref="J209:K209"/>
+    <mergeCell ref="J210:K210"/>
+    <mergeCell ref="J211:K211"/>
+    <mergeCell ref="J212:K212"/>
+    <mergeCell ref="J213:K213"/>
+    <mergeCell ref="J214:K214"/>
+    <mergeCell ref="J215:K215"/>
+    <mergeCell ref="J216:K216"/>
+    <mergeCell ref="J217:K217"/>
+    <mergeCell ref="J218:K218"/>
+    <mergeCell ref="J219:K219"/>
+    <mergeCell ref="J220:K220"/>
+    <mergeCell ref="J230:K230"/>
+    <mergeCell ref="J231:K231"/>
+    <mergeCell ref="J221:K221"/>
+    <mergeCell ref="J222:K222"/>
+    <mergeCell ref="J223:K223"/>
+    <mergeCell ref="J224:K224"/>
+    <mergeCell ref="J225:K225"/>
+    <mergeCell ref="J226:K226"/>
+    <mergeCell ref="J227:K227"/>
+    <mergeCell ref="J228:K228"/>
+    <mergeCell ref="J229:K229"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="H68:I68"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="H78:I78"/>
+    <mergeCell ref="H79:I79"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="H82:I82"/>
+    <mergeCell ref="H83:I83"/>
+    <mergeCell ref="H84:I84"/>
+    <mergeCell ref="H85:I85"/>
+    <mergeCell ref="H86:I86"/>
+    <mergeCell ref="H87:I87"/>
+    <mergeCell ref="H88:I88"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="H90:I90"/>
+    <mergeCell ref="H91:I91"/>
+    <mergeCell ref="H92:I92"/>
+    <mergeCell ref="H93:I93"/>
+    <mergeCell ref="H94:I94"/>
+    <mergeCell ref="H95:I95"/>
+    <mergeCell ref="H96:I96"/>
+    <mergeCell ref="H97:I97"/>
+    <mergeCell ref="H98:I98"/>
+    <mergeCell ref="H99:I99"/>
+    <mergeCell ref="H100:I100"/>
+    <mergeCell ref="H101:I101"/>
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="H103:I103"/>
+    <mergeCell ref="H104:I104"/>
+    <mergeCell ref="H105:I105"/>
+    <mergeCell ref="H106:I106"/>
+    <mergeCell ref="H107:I107"/>
+    <mergeCell ref="H108:I108"/>
+    <mergeCell ref="H109:I109"/>
+    <mergeCell ref="H110:I110"/>
+    <mergeCell ref="H111:I111"/>
+    <mergeCell ref="H112:I112"/>
+    <mergeCell ref="H113:I113"/>
+    <mergeCell ref="H114:I114"/>
+    <mergeCell ref="H115:I115"/>
+    <mergeCell ref="H116:I116"/>
+    <mergeCell ref="H117:I117"/>
+    <mergeCell ref="H118:I118"/>
+    <mergeCell ref="H128:I128"/>
+    <mergeCell ref="H129:I129"/>
+    <mergeCell ref="H119:I119"/>
+    <mergeCell ref="H120:I120"/>
+    <mergeCell ref="H121:I121"/>
+    <mergeCell ref="H122:I122"/>
+    <mergeCell ref="H123:I123"/>
+    <mergeCell ref="H124:I124"/>
+    <mergeCell ref="H125:I125"/>
+    <mergeCell ref="H126:I126"/>
+    <mergeCell ref="H127:I127"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Doc: Added Review comments on system design for supplier home page and update produc page
</commit_message>
<xml_diff>
--- a/Requirments/Review.xlsx
+++ b/Requirments/Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Requirments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1445C2B-C116-475F-8264-128BADA17388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E33C4B-FBFD-40AA-B639-039D6291F496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="179">
   <si>
     <t>ID</t>
   </si>
@@ -524,6 +524,42 @@
   </si>
   <si>
     <t>15849adea70087036301ed14388dce50211b8045</t>
+  </si>
+  <si>
+    <t>System Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Design Review </t>
+  </si>
+  <si>
+    <t>No gaps</t>
+  </si>
+  <si>
+    <t>UI_SupplierHomePage</t>
+  </si>
+  <si>
+    <t>30ba2adae20c13b68c1897ef998de53712aafb01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review_UI_SupplierHomePage_001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review_SD_SupplierHomePage_002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">in sequence diagram we don’t have backend module in design </t>
+  </si>
+  <si>
+    <t>SequenceDiagram_SupplierHomePage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review_UI_UpdateProductPage_003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review_SD_updateProductPage_004 </t>
+  </si>
+  <si>
+    <t>SequenceDiagram_SupplierUpdatePage</t>
   </si>
 </sst>
 </file>
@@ -814,17 +850,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -833,21 +864,26 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1075,18 +1111,18 @@
   </sheetPr>
   <dimension ref="A1:AC906"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B59" workbookViewId="0">
-      <selection activeCell="J67" sqref="J67:K67"/>
+    <sheetView tabSelected="1" topLeftCell="F62" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="1" max="1" width="43" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" customWidth="1"/>
     <col min="5" max="5" width="97.140625" customWidth="1"/>
-    <col min="6" max="6" width="37.28515625" customWidth="1"/>
+    <col min="6" max="6" width="47.140625" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" customWidth="1"/>
     <col min="8" max="8" width="34.140625" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" customWidth="1"/>
@@ -1115,14 +1151,14 @@
       <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="45" t="s">
+      <c r="I1" s="37"/>
+      <c r="J1" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="K1" s="46"/>
+      <c r="K1" s="37"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -1143,19 +1179,19 @@
       <c r="AC1" s="1"/>
     </row>
     <row r="2" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -1197,12 +1233,12 @@
       <c r="G3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="42"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="32" t="s">
+      <c r="H3" s="40"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K3" s="32"/>
+      <c r="K3" s="38"/>
     </row>
     <row r="4" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
@@ -1226,12 +1262,12 @@
       <c r="G4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="42"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="32" t="s">
+      <c r="H4" s="40"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K4" s="32"/>
+      <c r="K4" s="38"/>
     </row>
     <row r="5" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
@@ -1255,12 +1291,12 @@
       <c r="G5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="42"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="32" t="s">
+      <c r="H5" s="40"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K5" s="32"/>
+      <c r="K5" s="38"/>
     </row>
     <row r="6" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
@@ -1284,12 +1320,12 @@
       <c r="G6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="42"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="32" t="s">
+      <c r="H6" s="40"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K6" s="32"/>
+      <c r="K6" s="38"/>
     </row>
     <row r="7" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -1313,12 +1349,12 @@
       <c r="G7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="42"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="32" t="s">
+      <c r="H7" s="40"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K7" s="32"/>
+      <c r="K7" s="38"/>
     </row>
     <row r="8" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
@@ -1342,12 +1378,12 @@
       <c r="G8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="42"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="32" t="s">
+      <c r="H8" s="40"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K8" s="32"/>
+      <c r="K8" s="38"/>
     </row>
     <row r="9" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
@@ -1371,12 +1407,12 @@
       <c r="G9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="42"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="32" t="s">
+      <c r="H9" s="40"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K9" s="32"/>
+      <c r="K9" s="38"/>
     </row>
     <row r="10" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
@@ -1400,12 +1436,12 @@
       <c r="G10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="42"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="32" t="s">
+      <c r="H10" s="40"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K10" s="32"/>
+      <c r="K10" s="38"/>
     </row>
     <row r="11" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
@@ -1429,12 +1465,12 @@
       <c r="G11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="42"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="32" t="s">
+      <c r="H11" s="40"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K11" s="32"/>
+      <c r="K11" s="38"/>
     </row>
     <row r="12" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
@@ -1458,12 +1494,12 @@
       <c r="G12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="42"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="32" t="s">
+      <c r="H12" s="40"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K12" s="32"/>
+      <c r="K12" s="38"/>
     </row>
     <row r="13" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
@@ -1487,12 +1523,12 @@
       <c r="G13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="42"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="32" t="s">
+      <c r="H13" s="40"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K13" s="32"/>
+      <c r="K13" s="38"/>
     </row>
     <row r="14" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
@@ -1516,12 +1552,12 @@
       <c r="G14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="42"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="32" t="s">
+      <c r="H14" s="40"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K14" s="32"/>
+      <c r="K14" s="38"/>
     </row>
     <row r="15" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
@@ -1543,12 +1579,12 @@
       <c r="G15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="42"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="32" t="s">
+      <c r="H15" s="40"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="32"/>
+      <c r="K15" s="38"/>
     </row>
     <row r="16" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
@@ -1572,12 +1608,12 @@
       <c r="G16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="42"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="32" t="s">
+      <c r="H16" s="40"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K16" s="32"/>
+      <c r="K16" s="38"/>
     </row>
     <row r="17" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
@@ -1601,12 +1637,12 @@
       <c r="G17" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="42"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="32" t="s">
+      <c r="H17" s="40"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="32"/>
+      <c r="K17" s="38"/>
     </row>
     <row r="18" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
@@ -1630,12 +1666,12 @@
       <c r="G18" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="42"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="32" t="s">
+      <c r="H18" s="40"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="32"/>
+      <c r="K18" s="38"/>
     </row>
     <row r="19" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
@@ -1659,27 +1695,27 @@
       <c r="G19" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="42"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="32" t="s">
+      <c r="H19" s="40"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="K19" s="32"/>
+      <c r="K19" s="38"/>
     </row>
     <row r="20" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="38"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="35"/>
     </row>
     <row r="21" spans="1:11" s="16" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
@@ -1703,14 +1739,14 @@
       <c r="G21" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H21" s="44" t="s">
+      <c r="H21" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I21" s="31"/>
-      <c r="J21" s="32" t="s">
+      <c r="J21" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="K21" s="32"/>
+      <c r="K21" s="38"/>
     </row>
     <row r="22" spans="1:11" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
@@ -1734,12 +1770,12 @@
       <c r="G22" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="30"/>
+      <c r="H22" s="32"/>
       <c r="I22" s="31"/>
-      <c r="J22" s="32" t="s">
+      <c r="J22" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="K22" s="32"/>
+      <c r="K22" s="38"/>
     </row>
     <row r="23" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
@@ -1763,14 +1799,14 @@
       <c r="G23" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="30" t="s">
+      <c r="H23" s="32" t="s">
         <v>73</v>
       </c>
       <c r="I23" s="31"/>
-      <c r="J23" s="32" t="s">
+      <c r="J23" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="K23" s="32"/>
+      <c r="K23" s="38"/>
     </row>
     <row r="24" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
@@ -1798,10 +1834,10 @@
         <v>74</v>
       </c>
       <c r="I24" s="25"/>
-      <c r="J24" s="32" t="s">
+      <c r="J24" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="K24" s="32"/>
+      <c r="K24" s="38"/>
     </row>
     <row r="25" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
@@ -1825,14 +1861,14 @@
       <c r="G25" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="30" t="s">
+      <c r="H25" s="32" t="s">
         <v>76</v>
       </c>
       <c r="I25" s="31"/>
-      <c r="J25" s="32" t="s">
+      <c r="J25" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="K25" s="32"/>
+      <c r="K25" s="38"/>
     </row>
     <row r="26" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
@@ -1856,27 +1892,27 @@
       <c r="G26" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H26" s="30"/>
+      <c r="H26" s="32"/>
       <c r="I26" s="31"/>
-      <c r="J26" s="32" t="s">
+      <c r="J26" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="K26" s="32"/>
+      <c r="K26" s="38"/>
     </row>
     <row r="27" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="38"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="35"/>
     </row>
     <row r="28" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
@@ -1900,12 +1936,12 @@
       <c r="G28" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H28" s="39"/>
-      <c r="I28" s="40"/>
-      <c r="J28" s="39" t="s">
+      <c r="H28" s="43"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="K28" s="40"/>
+      <c r="K28" s="44"/>
     </row>
     <row r="29" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
@@ -1929,14 +1965,14 @@
       <c r="G29" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="30" t="s">
+      <c r="H29" s="32" t="s">
         <v>90</v>
       </c>
       <c r="I29" s="31"/>
-      <c r="J29" s="35" t="s">
+      <c r="J29" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="K29" s="32"/>
+      <c r="K29" s="38"/>
     </row>
     <row r="30" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
@@ -1960,12 +1996,12 @@
       <c r="G30" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H30" s="30"/>
+      <c r="H30" s="32"/>
       <c r="I30" s="31"/>
-      <c r="J30" s="32" t="s">
+      <c r="J30" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="K30" s="32"/>
+      <c r="K30" s="38"/>
     </row>
     <row r="31" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
@@ -1991,10 +2027,10 @@
       </c>
       <c r="H31" s="24"/>
       <c r="I31" s="25"/>
-      <c r="J31" s="41" t="s">
+      <c r="J31" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="K31" s="40"/>
+      <c r="K31" s="44"/>
     </row>
     <row r="32" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
@@ -2018,27 +2054,27 @@
       <c r="G32" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H32" s="30"/>
+      <c r="H32" s="32"/>
       <c r="I32" s="31"/>
-      <c r="J32" s="32" t="s">
+      <c r="J32" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="K32" s="32"/>
+      <c r="K32" s="38"/>
     </row>
     <row r="33" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="38"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="35"/>
     </row>
     <row r="34" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
@@ -2062,12 +2098,12 @@
       <c r="G34" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H34" s="30"/>
+      <c r="H34" s="32"/>
       <c r="I34" s="31"/>
-      <c r="J34" s="35" t="s">
+      <c r="J34" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K34" s="32"/>
+      <c r="K34" s="38"/>
     </row>
     <row r="35" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
@@ -2091,7 +2127,7 @@
       <c r="G35" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H35" s="30"/>
+      <c r="H35" s="32"/>
       <c r="I35" s="31"/>
       <c r="J35" s="28" t="s">
         <v>94</v>
@@ -2119,12 +2155,12 @@
       <c r="G36" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H36" s="30"/>
+      <c r="H36" s="32"/>
       <c r="I36" s="31"/>
-      <c r="J36" s="35" t="s">
+      <c r="J36" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K36" s="32"/>
+      <c r="K36" s="38"/>
     </row>
     <row r="37" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
@@ -2148,12 +2184,12 @@
       <c r="G37" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H37" s="30"/>
+      <c r="H37" s="32"/>
       <c r="I37" s="31"/>
-      <c r="J37" s="35" t="s">
+      <c r="J37" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K37" s="32"/>
+      <c r="K37" s="38"/>
     </row>
     <row r="38" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
@@ -2177,12 +2213,12 @@
       <c r="G38" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H38" s="30"/>
+      <c r="H38" s="32"/>
       <c r="I38" s="31"/>
-      <c r="J38" s="35" t="s">
+      <c r="J38" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K38" s="32"/>
+      <c r="K38" s="38"/>
     </row>
     <row r="39" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
@@ -2206,12 +2242,12 @@
       <c r="G39" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H39" s="30"/>
+      <c r="H39" s="32"/>
       <c r="I39" s="31"/>
-      <c r="J39" s="35" t="s">
+      <c r="J39" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K39" s="32"/>
+      <c r="K39" s="38"/>
     </row>
     <row r="40" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
@@ -2235,12 +2271,12 @@
       <c r="G40" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H40" s="30"/>
+      <c r="H40" s="32"/>
       <c r="I40" s="31"/>
-      <c r="J40" s="35" t="s">
+      <c r="J40" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K40" s="32"/>
+      <c r="K40" s="38"/>
     </row>
     <row r="41" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
@@ -2264,12 +2300,12 @@
       <c r="G41" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H41" s="30"/>
+      <c r="H41" s="32"/>
       <c r="I41" s="31"/>
-      <c r="J41" s="35" t="s">
+      <c r="J41" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K41" s="32"/>
+      <c r="K41" s="38"/>
     </row>
     <row r="42" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
@@ -2293,12 +2329,12 @@
       <c r="G42" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H42" s="30"/>
+      <c r="H42" s="32"/>
       <c r="I42" s="31"/>
-      <c r="J42" s="35" t="s">
+      <c r="J42" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K42" s="32"/>
+      <c r="K42" s="38"/>
     </row>
     <row r="43" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
@@ -2322,12 +2358,12 @@
       <c r="G43" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H43" s="30"/>
+      <c r="H43" s="32"/>
       <c r="I43" s="31"/>
-      <c r="J43" s="35" t="s">
+      <c r="J43" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K43" s="32"/>
+      <c r="K43" s="38"/>
     </row>
     <row r="44" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
@@ -2351,12 +2387,12 @@
       <c r="G44" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H44" s="30"/>
+      <c r="H44" s="32"/>
       <c r="I44" s="31"/>
-      <c r="J44" s="35" t="s">
+      <c r="J44" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K44" s="32"/>
+      <c r="K44" s="38"/>
     </row>
     <row r="45" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
@@ -2380,12 +2416,12 @@
       <c r="G45" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H45" s="30"/>
+      <c r="H45" s="32"/>
       <c r="I45" s="31"/>
-      <c r="J45" s="35" t="s">
+      <c r="J45" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K45" s="32"/>
+      <c r="K45" s="38"/>
     </row>
     <row r="46" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
@@ -2409,12 +2445,12 @@
       <c r="G46" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H46" s="30"/>
+      <c r="H46" s="32"/>
       <c r="I46" s="31"/>
-      <c r="J46" s="35" t="s">
+      <c r="J46" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K46" s="32"/>
+      <c r="K46" s="38"/>
     </row>
     <row r="47" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
@@ -2438,12 +2474,12 @@
       <c r="G47" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H47" s="30"/>
+      <c r="H47" s="32"/>
       <c r="I47" s="31"/>
-      <c r="J47" s="35" t="s">
+      <c r="J47" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K47" s="32"/>
+      <c r="K47" s="38"/>
     </row>
     <row r="48" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
@@ -2467,12 +2503,12 @@
       <c r="G48" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H48" s="30"/>
+      <c r="H48" s="32"/>
       <c r="I48" s="31"/>
-      <c r="J48" s="35" t="s">
+      <c r="J48" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="K48" s="32"/>
+      <c r="K48" s="38"/>
     </row>
     <row r="49" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
@@ -2496,12 +2532,12 @@
       <c r="G49" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H49" s="30"/>
+      <c r="H49" s="32"/>
       <c r="I49" s="31"/>
-      <c r="J49" s="32" t="s">
+      <c r="J49" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="K49" s="32"/>
+      <c r="K49" s="38"/>
     </row>
     <row r="50" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
@@ -2523,12 +2559,12 @@
       <c r="G50" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H50" s="30"/>
+      <c r="H50" s="32"/>
       <c r="I50" s="31"/>
-      <c r="J50" s="32" t="s">
+      <c r="J50" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="K50" s="32"/>
+      <c r="K50" s="38"/>
     </row>
     <row r="51" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
@@ -2550,12 +2586,12 @@
       <c r="G51" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H51" s="30"/>
+      <c r="H51" s="32"/>
       <c r="I51" s="31"/>
-      <c r="J51" s="32" t="s">
+      <c r="J51" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="K51" s="32"/>
+      <c r="K51" s="38"/>
     </row>
     <row r="52" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A52" s="13"/>
@@ -2565,10 +2601,10 @@
       <c r="E52" s="13"/>
       <c r="F52" s="13"/>
       <c r="G52" s="15"/>
-      <c r="H52" s="30"/>
+      <c r="H52" s="32"/>
       <c r="I52" s="31"/>
-      <c r="J52" s="32"/>
-      <c r="K52" s="32"/>
+      <c r="J52" s="38"/>
+      <c r="K52" s="38"/>
     </row>
     <row r="53" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A53" s="13"/>
@@ -2578,10 +2614,10 @@
       <c r="E53" s="13"/>
       <c r="F53" s="13"/>
       <c r="G53" s="15"/>
-      <c r="H53" s="30"/>
+      <c r="H53" s="32"/>
       <c r="I53" s="31"/>
-      <c r="J53" s="32"/>
-      <c r="K53" s="32"/>
+      <c r="J53" s="38"/>
+      <c r="K53" s="38"/>
     </row>
     <row r="54" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A54" s="13"/>
@@ -2591,10 +2627,10 @@
       <c r="E54" s="13"/>
       <c r="F54" s="13"/>
       <c r="G54" s="15"/>
-      <c r="H54" s="30"/>
+      <c r="H54" s="32"/>
       <c r="I54" s="31"/>
-      <c r="J54" s="32"/>
-      <c r="K54" s="32"/>
+      <c r="J54" s="38"/>
+      <c r="K54" s="38"/>
     </row>
     <row r="55" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A55" s="13"/>
@@ -2604,10 +2640,10 @@
       <c r="E55" s="13"/>
       <c r="F55" s="13"/>
       <c r="G55" s="15"/>
-      <c r="H55" s="30"/>
+      <c r="H55" s="32"/>
       <c r="I55" s="31"/>
-      <c r="J55" s="32"/>
-      <c r="K55" s="32"/>
+      <c r="J55" s="38"/>
+      <c r="K55" s="38"/>
     </row>
     <row r="56" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A56" s="13"/>
@@ -2617,10 +2653,10 @@
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
       <c r="G56" s="15"/>
-      <c r="H56" s="30"/>
+      <c r="H56" s="32"/>
       <c r="I56" s="31"/>
-      <c r="J56" s="32"/>
-      <c r="K56" s="32"/>
+      <c r="J56" s="38"/>
+      <c r="K56" s="38"/>
     </row>
     <row r="57" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A57" s="13"/>
@@ -2630,10 +2666,10 @@
       <c r="E57" s="13"/>
       <c r="F57" s="13"/>
       <c r="G57" s="15"/>
-      <c r="H57" s="30"/>
+      <c r="H57" s="32"/>
       <c r="I57" s="31"/>
-      <c r="J57" s="32"/>
-      <c r="K57" s="32"/>
+      <c r="J57" s="38"/>
+      <c r="K57" s="38"/>
     </row>
     <row r="58" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A58" s="13"/>
@@ -2643,10 +2679,10 @@
       <c r="E58" s="13"/>
       <c r="F58" s="13"/>
       <c r="G58" s="15"/>
-      <c r="H58" s="30"/>
+      <c r="H58" s="32"/>
       <c r="I58" s="31"/>
-      <c r="J58" s="32"/>
-      <c r="K58" s="32"/>
+      <c r="J58" s="38"/>
+      <c r="K58" s="38"/>
     </row>
     <row r="59" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A59" s="13"/>
@@ -2656,25 +2692,25 @@
       <c r="E59" s="13"/>
       <c r="F59" s="13"/>
       <c r="G59" s="15"/>
-      <c r="H59" s="30"/>
+      <c r="H59" s="32"/>
       <c r="I59" s="31"/>
-      <c r="J59" s="32"/>
-      <c r="K59" s="32"/>
+      <c r="J59" s="38"/>
+      <c r="K59" s="38"/>
     </row>
     <row r="60" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A60" s="47" t="s">
+      <c r="A60" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="B60" s="37"/>
-      <c r="C60" s="37"/>
-      <c r="D60" s="37"/>
-      <c r="E60" s="37"/>
-      <c r="F60" s="37"/>
-      <c r="G60" s="37"/>
-      <c r="H60" s="37"/>
-      <c r="I60" s="37"/>
-      <c r="J60" s="37"/>
-      <c r="K60" s="38"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="34"/>
+      <c r="D60" s="34"/>
+      <c r="E60" s="34"/>
+      <c r="F60" s="34"/>
+      <c r="G60" s="34"/>
+      <c r="H60" s="34"/>
+      <c r="I60" s="34"/>
+      <c r="J60" s="34"/>
+      <c r="K60" s="35"/>
     </row>
     <row r="61" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A61" s="13" t="s">
@@ -2698,12 +2734,12 @@
       <c r="G61" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H61" s="30"/>
+      <c r="H61" s="32"/>
       <c r="I61" s="31"/>
-      <c r="J61" s="32" t="s">
+      <c r="J61" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="K61" s="32"/>
+      <c r="K61" s="38"/>
     </row>
     <row r="62" spans="1:11" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
@@ -2727,14 +2763,14 @@
       <c r="G62" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="H62" s="44" t="s">
+      <c r="H62" s="30" t="s">
         <v>151</v>
       </c>
       <c r="I62" s="31"/>
-      <c r="J62" s="32" t="s">
+      <c r="J62" s="38" t="s">
         <v>147</v>
       </c>
-      <c r="K62" s="32"/>
+      <c r="K62" s="38"/>
     </row>
     <row r="63" spans="1:11" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
@@ -2758,12 +2794,12 @@
       <c r="G63" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H63" s="30"/>
+      <c r="H63" s="32"/>
       <c r="I63" s="31"/>
-      <c r="J63" s="32" t="s">
+      <c r="J63" s="38" t="s">
         <v>147</v>
       </c>
-      <c r="K63" s="32"/>
+      <c r="K63" s="38"/>
     </row>
     <row r="64" spans="1:11" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
@@ -2787,12 +2823,12 @@
       <c r="G64" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H64" s="30"/>
+      <c r="H64" s="32"/>
       <c r="I64" s="31"/>
-      <c r="J64" s="32" t="s">
+      <c r="J64" s="38" t="s">
         <v>156</v>
       </c>
-      <c r="K64" s="32"/>
+      <c r="K64" s="38"/>
     </row>
     <row r="65" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
@@ -2816,12 +2852,12 @@
       <c r="G65" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H65" s="30"/>
+      <c r="H65" s="32"/>
       <c r="I65" s="31"/>
-      <c r="J65" s="32" t="s">
+      <c r="J65" s="38" t="s">
         <v>156</v>
       </c>
-      <c r="K65" s="32"/>
+      <c r="K65" s="38"/>
     </row>
     <row r="66" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
@@ -2845,12 +2881,12 @@
       <c r="G66" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H66" s="30"/>
+      <c r="H66" s="32"/>
       <c r="I66" s="31"/>
-      <c r="J66" s="32" t="s">
+      <c r="J66" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="K66" s="32"/>
+      <c r="K66" s="38"/>
     </row>
     <row r="67" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
@@ -2872,77 +2908,139 @@
       <c r="G67" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H67" s="30"/>
+      <c r="H67" s="32"/>
       <c r="I67" s="31"/>
-      <c r="J67" s="32" t="s">
+      <c r="J67" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="K67" s="32"/>
-    </row>
-    <row r="68" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A68" s="13"/>
-      <c r="B68" s="18"/>
-      <c r="C68" s="18"/>
-      <c r="D68" s="13"/>
-      <c r="E68" s="13"/>
-      <c r="F68" s="13"/>
-      <c r="G68" s="15"/>
-      <c r="H68" s="30"/>
-      <c r="I68" s="31"/>
-      <c r="J68" s="32"/>
-      <c r="K68" s="32"/>
+      <c r="K67" s="38"/>
+    </row>
+    <row r="68" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A68" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="B68" s="34"/>
+      <c r="C68" s="34"/>
+      <c r="D68" s="34"/>
+      <c r="E68" s="34"/>
+      <c r="F68" s="34"/>
+      <c r="G68" s="34"/>
+      <c r="H68" s="34"/>
+      <c r="I68" s="34"/>
+      <c r="J68" s="34"/>
+      <c r="K68" s="35"/>
     </row>
     <row r="69" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A69" s="13"/>
-      <c r="B69" s="18"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="13"/>
-      <c r="E69" s="13"/>
-      <c r="F69" s="13"/>
-      <c r="G69" s="15"/>
-      <c r="H69" s="30"/>
+      <c r="A69" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="B69" s="17">
+        <v>45776</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D69" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E69" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="F69" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="G69" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H69" s="32"/>
       <c r="I69" s="31"/>
-      <c r="J69" s="32"/>
-      <c r="K69" s="32"/>
+      <c r="J69" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="K69" s="38"/>
     </row>
     <row r="70" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A70" s="13"/>
-      <c r="B70" s="18"/>
-      <c r="C70" s="18"/>
-      <c r="D70" s="13"/>
-      <c r="E70" s="13"/>
-      <c r="F70" s="13"/>
+      <c r="A70" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="B70" s="17">
+        <v>45776</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D70" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E70" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="F70" s="13" t="s">
+        <v>175</v>
+      </c>
       <c r="G70" s="15"/>
-      <c r="H70" s="30"/>
+      <c r="H70" s="32"/>
       <c r="I70" s="31"/>
-      <c r="J70" s="32"/>
-      <c r="K70" s="32"/>
+      <c r="J70" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="K70" s="38"/>
     </row>
     <row r="71" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A71" s="13"/>
-      <c r="B71" s="18"/>
-      <c r="C71" s="18"/>
-      <c r="D71" s="13"/>
-      <c r="E71" s="13"/>
-      <c r="F71" s="13"/>
-      <c r="G71" s="15"/>
-      <c r="H71" s="30"/>
+      <c r="A71" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="B71" s="17">
+        <v>45776</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D71" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E71" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="F71" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="G71" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H71" s="32"/>
       <c r="I71" s="31"/>
-      <c r="J71" s="32"/>
-      <c r="K71" s="32"/>
+      <c r="J71" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="K71" s="38"/>
     </row>
     <row r="72" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A72" s="13"/>
-      <c r="B72" s="18"/>
-      <c r="C72" s="18"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="13"/>
+      <c r="A72" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="B72" s="17">
+        <v>45776</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D72" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E72" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="F72" s="13" t="s">
+        <v>178</v>
+      </c>
       <c r="G72" s="15"/>
-      <c r="H72" s="30"/>
+      <c r="H72" s="32"/>
       <c r="I72" s="31"/>
-      <c r="J72" s="32"/>
-      <c r="K72" s="32"/>
+      <c r="J72" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="K72" s="38"/>
     </row>
     <row r="73" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A73" s="13"/>
@@ -2952,10 +3050,10 @@
       <c r="E73" s="13"/>
       <c r="F73" s="13"/>
       <c r="G73" s="15"/>
-      <c r="H73" s="30"/>
+      <c r="H73" s="32"/>
       <c r="I73" s="31"/>
-      <c r="J73" s="32"/>
-      <c r="K73" s="32"/>
+      <c r="J73" s="38"/>
+      <c r="K73" s="38"/>
     </row>
     <row r="74" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A74" s="13"/>
@@ -2965,10 +3063,10 @@
       <c r="E74" s="13"/>
       <c r="F74" s="13"/>
       <c r="G74" s="15"/>
-      <c r="H74" s="30"/>
+      <c r="H74" s="32"/>
       <c r="I74" s="31"/>
-      <c r="J74" s="32"/>
-      <c r="K74" s="32"/>
+      <c r="J74" s="38"/>
+      <c r="K74" s="38"/>
     </row>
     <row r="75" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A75" s="13"/>
@@ -2978,10 +3076,10 @@
       <c r="E75" s="13"/>
       <c r="F75" s="13"/>
       <c r="G75" s="15"/>
-      <c r="H75" s="30"/>
+      <c r="H75" s="32"/>
       <c r="I75" s="31"/>
-      <c r="J75" s="32"/>
-      <c r="K75" s="32"/>
+      <c r="J75" s="38"/>
+      <c r="K75" s="38"/>
     </row>
     <row r="76" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A76" s="13"/>
@@ -2991,10 +3089,10 @@
       <c r="E76" s="13"/>
       <c r="F76" s="13"/>
       <c r="G76" s="15"/>
-      <c r="H76" s="30"/>
+      <c r="H76" s="32"/>
       <c r="I76" s="31"/>
-      <c r="J76" s="32"/>
-      <c r="K76" s="32"/>
+      <c r="J76" s="38"/>
+      <c r="K76" s="38"/>
     </row>
     <row r="77" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A77" s="13"/>
@@ -3004,10 +3102,10 @@
       <c r="E77" s="13"/>
       <c r="F77" s="13"/>
       <c r="G77" s="15"/>
-      <c r="H77" s="30"/>
+      <c r="H77" s="32"/>
       <c r="I77" s="31"/>
-      <c r="J77" s="32"/>
-      <c r="K77" s="32"/>
+      <c r="J77" s="38"/>
+      <c r="K77" s="38"/>
     </row>
     <row r="78" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A78" s="13"/>
@@ -3017,10 +3115,10 @@
       <c r="E78" s="13"/>
       <c r="F78" s="13"/>
       <c r="G78" s="15"/>
-      <c r="H78" s="30"/>
+      <c r="H78" s="32"/>
       <c r="I78" s="31"/>
-      <c r="J78" s="32"/>
-      <c r="K78" s="32"/>
+      <c r="J78" s="38"/>
+      <c r="K78" s="38"/>
     </row>
     <row r="79" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A79" s="13"/>
@@ -3030,10 +3128,10 @@
       <c r="E79" s="13"/>
       <c r="F79" s="13"/>
       <c r="G79" s="15"/>
-      <c r="H79" s="30"/>
+      <c r="H79" s="32"/>
       <c r="I79" s="31"/>
-      <c r="J79" s="32"/>
-      <c r="K79" s="32"/>
+      <c r="J79" s="38"/>
+      <c r="K79" s="38"/>
     </row>
     <row r="80" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A80" s="13"/>
@@ -3043,10 +3141,10 @@
       <c r="E80" s="13"/>
       <c r="F80" s="13"/>
       <c r="G80" s="15"/>
-      <c r="H80" s="30"/>
+      <c r="H80" s="32"/>
       <c r="I80" s="31"/>
-      <c r="J80" s="32"/>
-      <c r="K80" s="32"/>
+      <c r="J80" s="38"/>
+      <c r="K80" s="38"/>
     </row>
     <row r="81" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A81" s="13"/>
@@ -3056,10 +3154,10 @@
       <c r="E81" s="13"/>
       <c r="F81" s="13"/>
       <c r="G81" s="15"/>
-      <c r="H81" s="30"/>
+      <c r="H81" s="32"/>
       <c r="I81" s="31"/>
-      <c r="J81" s="32"/>
-      <c r="K81" s="32"/>
+      <c r="J81" s="38"/>
+      <c r="K81" s="38"/>
     </row>
     <row r="82" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A82" s="13"/>
@@ -3069,10 +3167,10 @@
       <c r="E82" s="13"/>
       <c r="F82" s="13"/>
       <c r="G82" s="15"/>
-      <c r="H82" s="30"/>
+      <c r="H82" s="32"/>
       <c r="I82" s="31"/>
-      <c r="J82" s="32"/>
-      <c r="K82" s="32"/>
+      <c r="J82" s="38"/>
+      <c r="K82" s="38"/>
     </row>
     <row r="83" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A83" s="13"/>
@@ -3082,10 +3180,10 @@
       <c r="E83" s="13"/>
       <c r="F83" s="13"/>
       <c r="G83" s="15"/>
-      <c r="H83" s="30"/>
+      <c r="H83" s="32"/>
       <c r="I83" s="31"/>
-      <c r="J83" s="32"/>
-      <c r="K83" s="32"/>
+      <c r="J83" s="38"/>
+      <c r="K83" s="38"/>
     </row>
     <row r="84" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A84" s="13"/>
@@ -3095,10 +3193,10 @@
       <c r="E84" s="13"/>
       <c r="F84" s="13"/>
       <c r="G84" s="15"/>
-      <c r="H84" s="30"/>
+      <c r="H84" s="32"/>
       <c r="I84" s="31"/>
-      <c r="J84" s="32"/>
-      <c r="K84" s="32"/>
+      <c r="J84" s="38"/>
+      <c r="K84" s="38"/>
     </row>
     <row r="85" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A85" s="13"/>
@@ -3108,10 +3206,10 @@
       <c r="E85" s="13"/>
       <c r="F85" s="13"/>
       <c r="G85" s="15"/>
-      <c r="H85" s="30"/>
+      <c r="H85" s="32"/>
       <c r="I85" s="31"/>
-      <c r="J85" s="32"/>
-      <c r="K85" s="32"/>
+      <c r="J85" s="38"/>
+      <c r="K85" s="38"/>
     </row>
     <row r="86" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A86" s="13"/>
@@ -3121,10 +3219,10 @@
       <c r="E86" s="13"/>
       <c r="F86" s="13"/>
       <c r="G86" s="15"/>
-      <c r="H86" s="30"/>
+      <c r="H86" s="32"/>
       <c r="I86" s="31"/>
-      <c r="J86" s="32"/>
-      <c r="K86" s="32"/>
+      <c r="J86" s="38"/>
+      <c r="K86" s="38"/>
     </row>
     <row r="87" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A87" s="13"/>
@@ -3134,10 +3232,10 @@
       <c r="E87" s="13"/>
       <c r="F87" s="13"/>
       <c r="G87" s="15"/>
-      <c r="H87" s="30"/>
+      <c r="H87" s="32"/>
       <c r="I87" s="31"/>
-      <c r="J87" s="32"/>
-      <c r="K87" s="32"/>
+      <c r="J87" s="38"/>
+      <c r="K87" s="38"/>
     </row>
     <row r="88" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A88" s="13"/>
@@ -3147,10 +3245,10 @@
       <c r="E88" s="13"/>
       <c r="F88" s="13"/>
       <c r="G88" s="15"/>
-      <c r="H88" s="30"/>
+      <c r="H88" s="32"/>
       <c r="I88" s="31"/>
-      <c r="J88" s="32"/>
-      <c r="K88" s="32"/>
+      <c r="J88" s="38"/>
+      <c r="K88" s="38"/>
     </row>
     <row r="89" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A89" s="13"/>
@@ -3160,10 +3258,10 @@
       <c r="E89" s="13"/>
       <c r="F89" s="13"/>
       <c r="G89" s="15"/>
-      <c r="H89" s="30"/>
+      <c r="H89" s="32"/>
       <c r="I89" s="31"/>
-      <c r="J89" s="32"/>
-      <c r="K89" s="32"/>
+      <c r="J89" s="38"/>
+      <c r="K89" s="38"/>
     </row>
     <row r="90" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A90" s="13"/>
@@ -3173,10 +3271,10 @@
       <c r="E90" s="13"/>
       <c r="F90" s="13"/>
       <c r="G90" s="15"/>
-      <c r="H90" s="30"/>
+      <c r="H90" s="32"/>
       <c r="I90" s="31"/>
-      <c r="J90" s="32"/>
-      <c r="K90" s="32"/>
+      <c r="J90" s="38"/>
+      <c r="K90" s="38"/>
     </row>
     <row r="91" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A91" s="13"/>
@@ -3186,10 +3284,10 @@
       <c r="E91" s="13"/>
       <c r="F91" s="13"/>
       <c r="G91" s="15"/>
-      <c r="H91" s="30"/>
+      <c r="H91" s="32"/>
       <c r="I91" s="31"/>
-      <c r="J91" s="32"/>
-      <c r="K91" s="32"/>
+      <c r="J91" s="38"/>
+      <c r="K91" s="38"/>
     </row>
     <row r="92" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A92" s="13"/>
@@ -3199,10 +3297,10 @@
       <c r="E92" s="13"/>
       <c r="F92" s="13"/>
       <c r="G92" s="15"/>
-      <c r="H92" s="30"/>
+      <c r="H92" s="32"/>
       <c r="I92" s="31"/>
-      <c r="J92" s="32"/>
-      <c r="K92" s="32"/>
+      <c r="J92" s="38"/>
+      <c r="K92" s="38"/>
     </row>
     <row r="93" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A93" s="13"/>
@@ -3212,10 +3310,10 @@
       <c r="E93" s="13"/>
       <c r="F93" s="13"/>
       <c r="G93" s="15"/>
-      <c r="H93" s="30"/>
+      <c r="H93" s="32"/>
       <c r="I93" s="31"/>
-      <c r="J93" s="32"/>
-      <c r="K93" s="32"/>
+      <c r="J93" s="38"/>
+      <c r="K93" s="38"/>
     </row>
     <row r="94" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A94" s="13"/>
@@ -3225,10 +3323,10 @@
       <c r="E94" s="13"/>
       <c r="F94" s="13"/>
       <c r="G94" s="15"/>
-      <c r="H94" s="30"/>
+      <c r="H94" s="32"/>
       <c r="I94" s="31"/>
-      <c r="J94" s="32"/>
-      <c r="K94" s="32"/>
+      <c r="J94" s="38"/>
+      <c r="K94" s="38"/>
     </row>
     <row r="95" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A95" s="13"/>
@@ -3238,10 +3336,10 @@
       <c r="E95" s="13"/>
       <c r="F95" s="13"/>
       <c r="G95" s="15"/>
-      <c r="H95" s="30"/>
+      <c r="H95" s="32"/>
       <c r="I95" s="31"/>
-      <c r="J95" s="32"/>
-      <c r="K95" s="32"/>
+      <c r="J95" s="38"/>
+      <c r="K95" s="38"/>
     </row>
     <row r="96" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A96" s="13"/>
@@ -3251,10 +3349,10 @@
       <c r="E96" s="13"/>
       <c r="F96" s="13"/>
       <c r="G96" s="15"/>
-      <c r="H96" s="30"/>
+      <c r="H96" s="32"/>
       <c r="I96" s="31"/>
-      <c r="J96" s="32"/>
-      <c r="K96" s="32"/>
+      <c r="J96" s="38"/>
+      <c r="K96" s="38"/>
     </row>
     <row r="97" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A97" s="13"/>
@@ -3264,10 +3362,10 @@
       <c r="E97" s="13"/>
       <c r="F97" s="13"/>
       <c r="G97" s="15"/>
-      <c r="H97" s="30"/>
+      <c r="H97" s="32"/>
       <c r="I97" s="31"/>
-      <c r="J97" s="32"/>
-      <c r="K97" s="32"/>
+      <c r="J97" s="38"/>
+      <c r="K97" s="38"/>
     </row>
     <row r="98" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A98" s="13"/>
@@ -3277,10 +3375,10 @@
       <c r="E98" s="13"/>
       <c r="F98" s="13"/>
       <c r="G98" s="15"/>
-      <c r="H98" s="30"/>
+      <c r="H98" s="32"/>
       <c r="I98" s="31"/>
-      <c r="J98" s="32"/>
-      <c r="K98" s="32"/>
+      <c r="J98" s="38"/>
+      <c r="K98" s="38"/>
     </row>
     <row r="99" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A99" s="13"/>
@@ -3290,10 +3388,10 @@
       <c r="E99" s="13"/>
       <c r="F99" s="13"/>
       <c r="G99" s="15"/>
-      <c r="H99" s="30"/>
+      <c r="H99" s="32"/>
       <c r="I99" s="31"/>
-      <c r="J99" s="32"/>
-      <c r="K99" s="32"/>
+      <c r="J99" s="38"/>
+      <c r="K99" s="38"/>
     </row>
     <row r="100" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A100" s="13"/>
@@ -3303,10 +3401,10 @@
       <c r="E100" s="13"/>
       <c r="F100" s="13"/>
       <c r="G100" s="15"/>
-      <c r="H100" s="30"/>
+      <c r="H100" s="32"/>
       <c r="I100" s="31"/>
-      <c r="J100" s="32"/>
-      <c r="K100" s="32"/>
+      <c r="J100" s="38"/>
+      <c r="K100" s="38"/>
     </row>
     <row r="101" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A101" s="13"/>
@@ -3316,10 +3414,10 @@
       <c r="E101" s="13"/>
       <c r="F101" s="13"/>
       <c r="G101" s="15"/>
-      <c r="H101" s="30"/>
+      <c r="H101" s="32"/>
       <c r="I101" s="31"/>
-      <c r="J101" s="32"/>
-      <c r="K101" s="32"/>
+      <c r="J101" s="38"/>
+      <c r="K101" s="38"/>
     </row>
     <row r="102" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A102" s="13"/>
@@ -3329,10 +3427,10 @@
       <c r="E102" s="13"/>
       <c r="F102" s="13"/>
       <c r="G102" s="15"/>
-      <c r="H102" s="30"/>
+      <c r="H102" s="32"/>
       <c r="I102" s="31"/>
-      <c r="J102" s="32"/>
-      <c r="K102" s="32"/>
+      <c r="J102" s="38"/>
+      <c r="K102" s="38"/>
     </row>
     <row r="103" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A103" s="13"/>
@@ -3342,10 +3440,10 @@
       <c r="E103" s="13"/>
       <c r="F103" s="13"/>
       <c r="G103" s="15"/>
-      <c r="H103" s="30"/>
+      <c r="H103" s="32"/>
       <c r="I103" s="31"/>
-      <c r="J103" s="32"/>
-      <c r="K103" s="32"/>
+      <c r="J103" s="38"/>
+      <c r="K103" s="38"/>
     </row>
     <row r="104" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A104" s="13"/>
@@ -3355,10 +3453,10 @@
       <c r="E104" s="13"/>
       <c r="F104" s="13"/>
       <c r="G104" s="15"/>
-      <c r="H104" s="30"/>
+      <c r="H104" s="32"/>
       <c r="I104" s="31"/>
-      <c r="J104" s="32"/>
-      <c r="K104" s="32"/>
+      <c r="J104" s="38"/>
+      <c r="K104" s="38"/>
     </row>
     <row r="105" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A105" s="13"/>
@@ -3368,10 +3466,10 @@
       <c r="E105" s="13"/>
       <c r="F105" s="13"/>
       <c r="G105" s="15"/>
-      <c r="H105" s="30"/>
+      <c r="H105" s="32"/>
       <c r="I105" s="31"/>
-      <c r="J105" s="32"/>
-      <c r="K105" s="32"/>
+      <c r="J105" s="38"/>
+      <c r="K105" s="38"/>
     </row>
     <row r="106" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A106" s="13"/>
@@ -3381,10 +3479,10 @@
       <c r="E106" s="13"/>
       <c r="F106" s="13"/>
       <c r="G106" s="15"/>
-      <c r="H106" s="30"/>
+      <c r="H106" s="32"/>
       <c r="I106" s="31"/>
-      <c r="J106" s="32"/>
-      <c r="K106" s="32"/>
+      <c r="J106" s="38"/>
+      <c r="K106" s="38"/>
     </row>
     <row r="107" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A107" s="13"/>
@@ -3394,10 +3492,10 @@
       <c r="E107" s="13"/>
       <c r="F107" s="13"/>
       <c r="G107" s="15"/>
-      <c r="H107" s="30"/>
+      <c r="H107" s="32"/>
       <c r="I107" s="31"/>
-      <c r="J107" s="32"/>
-      <c r="K107" s="32"/>
+      <c r="J107" s="38"/>
+      <c r="K107" s="38"/>
     </row>
     <row r="108" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A108" s="13"/>
@@ -3407,10 +3505,10 @@
       <c r="E108" s="13"/>
       <c r="F108" s="13"/>
       <c r="G108" s="15"/>
-      <c r="H108" s="30"/>
+      <c r="H108" s="32"/>
       <c r="I108" s="31"/>
-      <c r="J108" s="32"/>
-      <c r="K108" s="32"/>
+      <c r="J108" s="38"/>
+      <c r="K108" s="38"/>
     </row>
     <row r="109" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A109" s="13"/>
@@ -3420,10 +3518,10 @@
       <c r="E109" s="13"/>
       <c r="F109" s="13"/>
       <c r="G109" s="15"/>
-      <c r="H109" s="30"/>
+      <c r="H109" s="32"/>
       <c r="I109" s="31"/>
-      <c r="J109" s="32"/>
-      <c r="K109" s="32"/>
+      <c r="J109" s="38"/>
+      <c r="K109" s="38"/>
     </row>
     <row r="110" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A110" s="13"/>
@@ -3433,10 +3531,10 @@
       <c r="E110" s="13"/>
       <c r="F110" s="13"/>
       <c r="G110" s="15"/>
-      <c r="H110" s="30"/>
+      <c r="H110" s="32"/>
       <c r="I110" s="31"/>
-      <c r="J110" s="32"/>
-      <c r="K110" s="32"/>
+      <c r="J110" s="38"/>
+      <c r="K110" s="38"/>
     </row>
     <row r="111" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A111" s="13"/>
@@ -3446,10 +3544,10 @@
       <c r="E111" s="13"/>
       <c r="F111" s="13"/>
       <c r="G111" s="15"/>
-      <c r="H111" s="30"/>
+      <c r="H111" s="32"/>
       <c r="I111" s="31"/>
-      <c r="J111" s="32"/>
-      <c r="K111" s="32"/>
+      <c r="J111" s="38"/>
+      <c r="K111" s="38"/>
     </row>
     <row r="112" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A112" s="13"/>
@@ -3459,10 +3557,10 @@
       <c r="E112" s="13"/>
       <c r="F112" s="13"/>
       <c r="G112" s="15"/>
-      <c r="H112" s="30"/>
+      <c r="H112" s="32"/>
       <c r="I112" s="31"/>
-      <c r="J112" s="32"/>
-      <c r="K112" s="32"/>
+      <c r="J112" s="38"/>
+      <c r="K112" s="38"/>
     </row>
     <row r="113" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A113" s="13"/>
@@ -3472,10 +3570,10 @@
       <c r="E113" s="13"/>
       <c r="F113" s="13"/>
       <c r="G113" s="15"/>
-      <c r="H113" s="30"/>
+      <c r="H113" s="32"/>
       <c r="I113" s="31"/>
-      <c r="J113" s="32"/>
-      <c r="K113" s="32"/>
+      <c r="J113" s="38"/>
+      <c r="K113" s="38"/>
     </row>
     <row r="114" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A114" s="13"/>
@@ -3485,10 +3583,10 @@
       <c r="E114" s="13"/>
       <c r="F114" s="13"/>
       <c r="G114" s="15"/>
-      <c r="H114" s="30"/>
+      <c r="H114" s="32"/>
       <c r="I114" s="31"/>
-      <c r="J114" s="32"/>
-      <c r="K114" s="32"/>
+      <c r="J114" s="38"/>
+      <c r="K114" s="38"/>
     </row>
     <row r="115" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A115" s="13"/>
@@ -3498,10 +3596,10 @@
       <c r="E115" s="13"/>
       <c r="F115" s="13"/>
       <c r="G115" s="15"/>
-      <c r="H115" s="30"/>
+      <c r="H115" s="32"/>
       <c r="I115" s="31"/>
-      <c r="J115" s="32"/>
-      <c r="K115" s="32"/>
+      <c r="J115" s="38"/>
+      <c r="K115" s="38"/>
     </row>
     <row r="116" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A116" s="13"/>
@@ -3511,10 +3609,10 @@
       <c r="E116" s="13"/>
       <c r="F116" s="13"/>
       <c r="G116" s="15"/>
-      <c r="H116" s="30"/>
+      <c r="H116" s="32"/>
       <c r="I116" s="31"/>
-      <c r="J116" s="32"/>
-      <c r="K116" s="32"/>
+      <c r="J116" s="38"/>
+      <c r="K116" s="38"/>
     </row>
     <row r="117" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A117" s="13"/>
@@ -3524,10 +3622,10 @@
       <c r="E117" s="13"/>
       <c r="F117" s="13"/>
       <c r="G117" s="15"/>
-      <c r="H117" s="30"/>
+      <c r="H117" s="32"/>
       <c r="I117" s="31"/>
-      <c r="J117" s="32"/>
-      <c r="K117" s="32"/>
+      <c r="J117" s="38"/>
+      <c r="K117" s="38"/>
     </row>
     <row r="118" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A118" s="13"/>
@@ -3537,10 +3635,10 @@
       <c r="E118" s="13"/>
       <c r="F118" s="13"/>
       <c r="G118" s="15"/>
-      <c r="H118" s="30"/>
+      <c r="H118" s="32"/>
       <c r="I118" s="31"/>
-      <c r="J118" s="32"/>
-      <c r="K118" s="32"/>
+      <c r="J118" s="38"/>
+      <c r="K118" s="38"/>
     </row>
     <row r="119" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A119" s="13"/>
@@ -3550,10 +3648,10 @@
       <c r="E119" s="13"/>
       <c r="F119" s="13"/>
       <c r="G119" s="15"/>
-      <c r="H119" s="30"/>
+      <c r="H119" s="32"/>
       <c r="I119" s="31"/>
-      <c r="J119" s="32"/>
-      <c r="K119" s="32"/>
+      <c r="J119" s="38"/>
+      <c r="K119" s="38"/>
     </row>
     <row r="120" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A120" s="13"/>
@@ -3563,10 +3661,10 @@
       <c r="E120" s="13"/>
       <c r="F120" s="13"/>
       <c r="G120" s="15"/>
-      <c r="H120" s="30"/>
+      <c r="H120" s="32"/>
       <c r="I120" s="31"/>
-      <c r="J120" s="32"/>
-      <c r="K120" s="32"/>
+      <c r="J120" s="38"/>
+      <c r="K120" s="38"/>
     </row>
     <row r="121" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A121" s="13"/>
@@ -3576,10 +3674,10 @@
       <c r="E121" s="13"/>
       <c r="F121" s="13"/>
       <c r="G121" s="15"/>
-      <c r="H121" s="30"/>
+      <c r="H121" s="32"/>
       <c r="I121" s="31"/>
-      <c r="J121" s="32"/>
-      <c r="K121" s="32"/>
+      <c r="J121" s="38"/>
+      <c r="K121" s="38"/>
     </row>
     <row r="122" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A122" s="13"/>
@@ -3589,10 +3687,10 @@
       <c r="E122" s="13"/>
       <c r="F122" s="13"/>
       <c r="G122" s="15"/>
-      <c r="H122" s="30"/>
+      <c r="H122" s="32"/>
       <c r="I122" s="31"/>
-      <c r="J122" s="32"/>
-      <c r="K122" s="32"/>
+      <c r="J122" s="38"/>
+      <c r="K122" s="38"/>
     </row>
     <row r="123" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A123" s="13"/>
@@ -3602,10 +3700,10 @@
       <c r="E123" s="13"/>
       <c r="F123" s="13"/>
       <c r="G123" s="15"/>
-      <c r="H123" s="30"/>
+      <c r="H123" s="32"/>
       <c r="I123" s="31"/>
-      <c r="J123" s="32"/>
-      <c r="K123" s="32"/>
+      <c r="J123" s="38"/>
+      <c r="K123" s="38"/>
     </row>
     <row r="124" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A124" s="13"/>
@@ -3615,10 +3713,10 @@
       <c r="E124" s="13"/>
       <c r="F124" s="13"/>
       <c r="G124" s="15"/>
-      <c r="H124" s="30"/>
+      <c r="H124" s="32"/>
       <c r="I124" s="31"/>
-      <c r="J124" s="32"/>
-      <c r="K124" s="32"/>
+      <c r="J124" s="38"/>
+      <c r="K124" s="38"/>
     </row>
     <row r="125" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A125" s="13"/>
@@ -3628,10 +3726,10 @@
       <c r="E125" s="13"/>
       <c r="F125" s="13"/>
       <c r="G125" s="15"/>
-      <c r="H125" s="30"/>
+      <c r="H125" s="32"/>
       <c r="I125" s="31"/>
-      <c r="J125" s="32"/>
-      <c r="K125" s="32"/>
+      <c r="J125" s="38"/>
+      <c r="K125" s="38"/>
     </row>
     <row r="126" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A126" s="13"/>
@@ -3641,10 +3739,10 @@
       <c r="E126" s="13"/>
       <c r="F126" s="13"/>
       <c r="G126" s="15"/>
-      <c r="H126" s="30"/>
+      <c r="H126" s="32"/>
       <c r="I126" s="31"/>
-      <c r="J126" s="32"/>
-      <c r="K126" s="32"/>
+      <c r="J126" s="38"/>
+      <c r="K126" s="38"/>
     </row>
     <row r="127" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A127" s="13"/>
@@ -3654,10 +3752,10 @@
       <c r="E127" s="13"/>
       <c r="F127" s="13"/>
       <c r="G127" s="15"/>
-      <c r="H127" s="30"/>
+      <c r="H127" s="32"/>
       <c r="I127" s="31"/>
-      <c r="J127" s="32"/>
-      <c r="K127" s="32"/>
+      <c r="J127" s="38"/>
+      <c r="K127" s="38"/>
     </row>
     <row r="128" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A128" s="13"/>
@@ -3667,10 +3765,10 @@
       <c r="E128" s="13"/>
       <c r="F128" s="13"/>
       <c r="G128" s="15"/>
-      <c r="H128" s="30"/>
+      <c r="H128" s="32"/>
       <c r="I128" s="31"/>
-      <c r="J128" s="32"/>
-      <c r="K128" s="32"/>
+      <c r="J128" s="38"/>
+      <c r="K128" s="38"/>
     </row>
     <row r="129" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A129" s="13"/>
@@ -3680,10 +3778,10 @@
       <c r="E129" s="13"/>
       <c r="F129" s="13"/>
       <c r="G129" s="15"/>
-      <c r="H129" s="30"/>
+      <c r="H129" s="32"/>
       <c r="I129" s="31"/>
-      <c r="J129" s="32"/>
-      <c r="K129" s="32"/>
+      <c r="J129" s="38"/>
+      <c r="K129" s="38"/>
     </row>
     <row r="130" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A130" s="13"/>
@@ -3695,8 +3793,8 @@
       <c r="G130" s="15"/>
       <c r="H130" s="13"/>
       <c r="I130" s="13"/>
-      <c r="J130" s="32"/>
-      <c r="K130" s="32"/>
+      <c r="J130" s="38"/>
+      <c r="K130" s="38"/>
     </row>
     <row r="131" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A131" s="13"/>
@@ -3708,8 +3806,8 @@
       <c r="G131" s="15"/>
       <c r="H131" s="13"/>
       <c r="I131" s="13"/>
-      <c r="J131" s="32"/>
-      <c r="K131" s="32"/>
+      <c r="J131" s="38"/>
+      <c r="K131" s="38"/>
     </row>
     <row r="132" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A132" s="13"/>
@@ -3721,8 +3819,8 @@
       <c r="G132" s="15"/>
       <c r="H132" s="13"/>
       <c r="I132" s="13"/>
-      <c r="J132" s="32"/>
-      <c r="K132" s="32"/>
+      <c r="J132" s="38"/>
+      <c r="K132" s="38"/>
     </row>
     <row r="133" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A133" s="13"/>
@@ -3734,8 +3832,8 @@
       <c r="G133" s="15"/>
       <c r="H133" s="13"/>
       <c r="I133" s="13"/>
-      <c r="J133" s="32"/>
-      <c r="K133" s="32"/>
+      <c r="J133" s="38"/>
+      <c r="K133" s="38"/>
     </row>
     <row r="134" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A134" s="13"/>
@@ -3747,8 +3845,8 @@
       <c r="G134" s="15"/>
       <c r="H134" s="13"/>
       <c r="I134" s="13"/>
-      <c r="J134" s="32"/>
-      <c r="K134" s="32"/>
+      <c r="J134" s="38"/>
+      <c r="K134" s="38"/>
     </row>
     <row r="135" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A135" s="13"/>
@@ -3760,8 +3858,8 @@
       <c r="G135" s="15"/>
       <c r="H135" s="13"/>
       <c r="I135" s="13"/>
-      <c r="J135" s="32"/>
-      <c r="K135" s="32"/>
+      <c r="J135" s="38"/>
+      <c r="K135" s="38"/>
     </row>
     <row r="136" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A136" s="13"/>
@@ -3773,8 +3871,8 @@
       <c r="G136" s="15"/>
       <c r="H136" s="13"/>
       <c r="I136" s="13"/>
-      <c r="J136" s="32"/>
-      <c r="K136" s="32"/>
+      <c r="J136" s="38"/>
+      <c r="K136" s="38"/>
     </row>
     <row r="137" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A137" s="13"/>
@@ -3786,8 +3884,8 @@
       <c r="G137" s="15"/>
       <c r="H137" s="13"/>
       <c r="I137" s="13"/>
-      <c r="J137" s="32"/>
-      <c r="K137" s="32"/>
+      <c r="J137" s="38"/>
+      <c r="K137" s="38"/>
     </row>
     <row r="138" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A138" s="13"/>
@@ -3799,8 +3897,8 @@
       <c r="G138" s="15"/>
       <c r="H138" s="13"/>
       <c r="I138" s="13"/>
-      <c r="J138" s="32"/>
-      <c r="K138" s="32"/>
+      <c r="J138" s="38"/>
+      <c r="K138" s="38"/>
     </row>
     <row r="139" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A139" s="13"/>
@@ -3812,8 +3910,8 @@
       <c r="G139" s="15"/>
       <c r="H139" s="13"/>
       <c r="I139" s="13"/>
-      <c r="J139" s="32"/>
-      <c r="K139" s="32"/>
+      <c r="J139" s="38"/>
+      <c r="K139" s="38"/>
     </row>
     <row r="140" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A140" s="13"/>
@@ -3825,8 +3923,8 @@
       <c r="G140" s="15"/>
       <c r="H140" s="13"/>
       <c r="I140" s="13"/>
-      <c r="J140" s="32"/>
-      <c r="K140" s="32"/>
+      <c r="J140" s="38"/>
+      <c r="K140" s="38"/>
     </row>
     <row r="141" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A141" s="13"/>
@@ -3838,8 +3936,8 @@
       <c r="G141" s="15"/>
       <c r="H141" s="13"/>
       <c r="I141" s="13"/>
-      <c r="J141" s="32"/>
-      <c r="K141" s="32"/>
+      <c r="J141" s="38"/>
+      <c r="K141" s="38"/>
     </row>
     <row r="142" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A142" s="13"/>
@@ -3851,8 +3949,8 @@
       <c r="G142" s="15"/>
       <c r="H142" s="13"/>
       <c r="I142" s="13"/>
-      <c r="J142" s="32"/>
-      <c r="K142" s="32"/>
+      <c r="J142" s="38"/>
+      <c r="K142" s="38"/>
     </row>
     <row r="143" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A143" s="13"/>
@@ -3864,8 +3962,8 @@
       <c r="G143" s="15"/>
       <c r="H143" s="13"/>
       <c r="I143" s="13"/>
-      <c r="J143" s="32"/>
-      <c r="K143" s="32"/>
+      <c r="J143" s="38"/>
+      <c r="K143" s="38"/>
     </row>
     <row r="144" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A144" s="13"/>
@@ -3877,8 +3975,8 @@
       <c r="G144" s="15"/>
       <c r="H144" s="13"/>
       <c r="I144" s="13"/>
-      <c r="J144" s="32"/>
-      <c r="K144" s="32"/>
+      <c r="J144" s="38"/>
+      <c r="K144" s="38"/>
     </row>
     <row r="145" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A145" s="13"/>
@@ -3890,8 +3988,8 @@
       <c r="G145" s="15"/>
       <c r="H145" s="13"/>
       <c r="I145" s="13"/>
-      <c r="J145" s="32"/>
-      <c r="K145" s="32"/>
+      <c r="J145" s="38"/>
+      <c r="K145" s="38"/>
     </row>
     <row r="146" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A146" s="13"/>
@@ -3903,8 +4001,8 @@
       <c r="G146" s="15"/>
       <c r="H146" s="13"/>
       <c r="I146" s="13"/>
-      <c r="J146" s="32"/>
-      <c r="K146" s="32"/>
+      <c r="J146" s="38"/>
+      <c r="K146" s="38"/>
     </row>
     <row r="147" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A147" s="13"/>
@@ -3916,8 +4014,8 @@
       <c r="G147" s="15"/>
       <c r="H147" s="13"/>
       <c r="I147" s="13"/>
-      <c r="J147" s="32"/>
-      <c r="K147" s="32"/>
+      <c r="J147" s="38"/>
+      <c r="K147" s="38"/>
     </row>
     <row r="148" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A148" s="13"/>
@@ -3929,8 +4027,8 @@
       <c r="G148" s="15"/>
       <c r="H148" s="13"/>
       <c r="I148" s="13"/>
-      <c r="J148" s="32"/>
-      <c r="K148" s="32"/>
+      <c r="J148" s="38"/>
+      <c r="K148" s="38"/>
     </row>
     <row r="149" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A149" s="13"/>
@@ -3942,8 +4040,8 @@
       <c r="G149" s="15"/>
       <c r="H149" s="13"/>
       <c r="I149" s="13"/>
-      <c r="J149" s="32"/>
-      <c r="K149" s="32"/>
+      <c r="J149" s="38"/>
+      <c r="K149" s="38"/>
     </row>
     <row r="150" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A150" s="13"/>
@@ -3955,8 +4053,8 @@
       <c r="G150" s="15"/>
       <c r="H150" s="13"/>
       <c r="I150" s="13"/>
-      <c r="J150" s="32"/>
-      <c r="K150" s="32"/>
+      <c r="J150" s="38"/>
+      <c r="K150" s="38"/>
     </row>
     <row r="151" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A151" s="13"/>
@@ -3968,8 +4066,8 @@
       <c r="G151" s="15"/>
       <c r="H151" s="13"/>
       <c r="I151" s="13"/>
-      <c r="J151" s="32"/>
-      <c r="K151" s="32"/>
+      <c r="J151" s="38"/>
+      <c r="K151" s="38"/>
     </row>
     <row r="152" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A152" s="13"/>
@@ -3981,8 +4079,8 @@
       <c r="G152" s="15"/>
       <c r="H152" s="13"/>
       <c r="I152" s="13"/>
-      <c r="J152" s="32"/>
-      <c r="K152" s="32"/>
+      <c r="J152" s="38"/>
+      <c r="K152" s="38"/>
     </row>
     <row r="153" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A153" s="13"/>
@@ -3994,8 +4092,8 @@
       <c r="G153" s="15"/>
       <c r="H153" s="13"/>
       <c r="I153" s="13"/>
-      <c r="J153" s="32"/>
-      <c r="K153" s="32"/>
+      <c r="J153" s="38"/>
+      <c r="K153" s="38"/>
     </row>
     <row r="154" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A154" s="13"/>
@@ -4007,8 +4105,8 @@
       <c r="G154" s="15"/>
       <c r="H154" s="13"/>
       <c r="I154" s="13"/>
-      <c r="J154" s="32"/>
-      <c r="K154" s="32"/>
+      <c r="J154" s="38"/>
+      <c r="K154" s="38"/>
     </row>
     <row r="155" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A155" s="13"/>
@@ -4020,8 +4118,8 @@
       <c r="G155" s="15"/>
       <c r="H155" s="13"/>
       <c r="I155" s="13"/>
-      <c r="J155" s="32"/>
-      <c r="K155" s="32"/>
+      <c r="J155" s="38"/>
+      <c r="K155" s="38"/>
     </row>
     <row r="156" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A156" s="13"/>
@@ -4033,8 +4131,8 @@
       <c r="G156" s="15"/>
       <c r="H156" s="13"/>
       <c r="I156" s="13"/>
-      <c r="J156" s="32"/>
-      <c r="K156" s="32"/>
+      <c r="J156" s="38"/>
+      <c r="K156" s="38"/>
     </row>
     <row r="157" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A157" s="13"/>
@@ -4046,8 +4144,8 @@
       <c r="G157" s="15"/>
       <c r="H157" s="13"/>
       <c r="I157" s="13"/>
-      <c r="J157" s="32"/>
-      <c r="K157" s="32"/>
+      <c r="J157" s="38"/>
+      <c r="K157" s="38"/>
     </row>
     <row r="158" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A158" s="13"/>
@@ -4059,8 +4157,8 @@
       <c r="G158" s="15"/>
       <c r="H158" s="13"/>
       <c r="I158" s="13"/>
-      <c r="J158" s="32"/>
-      <c r="K158" s="32"/>
+      <c r="J158" s="38"/>
+      <c r="K158" s="38"/>
     </row>
     <row r="159" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A159" s="13"/>
@@ -4072,8 +4170,8 @@
       <c r="G159" s="15"/>
       <c r="H159" s="13"/>
       <c r="I159" s="13"/>
-      <c r="J159" s="32"/>
-      <c r="K159" s="32"/>
+      <c r="J159" s="38"/>
+      <c r="K159" s="38"/>
     </row>
     <row r="160" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A160" s="13"/>
@@ -4085,8 +4183,8 @@
       <c r="G160" s="15"/>
       <c r="H160" s="13"/>
       <c r="I160" s="13"/>
-      <c r="J160" s="32"/>
-      <c r="K160" s="32"/>
+      <c r="J160" s="38"/>
+      <c r="K160" s="38"/>
     </row>
     <row r="161" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A161" s="13"/>
@@ -4098,8 +4196,8 @@
       <c r="G161" s="15"/>
       <c r="H161" s="13"/>
       <c r="I161" s="13"/>
-      <c r="J161" s="32"/>
-      <c r="K161" s="32"/>
+      <c r="J161" s="38"/>
+      <c r="K161" s="38"/>
     </row>
     <row r="162" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A162" s="13"/>
@@ -4111,8 +4209,8 @@
       <c r="G162" s="15"/>
       <c r="H162" s="13"/>
       <c r="I162" s="13"/>
-      <c r="J162" s="32"/>
-      <c r="K162" s="32"/>
+      <c r="J162" s="38"/>
+      <c r="K162" s="38"/>
     </row>
     <row r="163" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A163" s="13"/>
@@ -4124,8 +4222,8 @@
       <c r="G163" s="15"/>
       <c r="H163" s="13"/>
       <c r="I163" s="13"/>
-      <c r="J163" s="32"/>
-      <c r="K163" s="32"/>
+      <c r="J163" s="38"/>
+      <c r="K163" s="38"/>
     </row>
     <row r="164" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A164" s="13"/>
@@ -4137,8 +4235,8 @@
       <c r="G164" s="15"/>
       <c r="H164" s="13"/>
       <c r="I164" s="13"/>
-      <c r="J164" s="32"/>
-      <c r="K164" s="32"/>
+      <c r="J164" s="38"/>
+      <c r="K164" s="38"/>
     </row>
     <row r="165" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A165" s="13"/>
@@ -4150,8 +4248,8 @@
       <c r="G165" s="15"/>
       <c r="H165" s="13"/>
       <c r="I165" s="13"/>
-      <c r="J165" s="32"/>
-      <c r="K165" s="32"/>
+      <c r="J165" s="38"/>
+      <c r="K165" s="38"/>
     </row>
     <row r="166" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A166" s="13"/>
@@ -4163,8 +4261,8 @@
       <c r="G166" s="15"/>
       <c r="H166" s="13"/>
       <c r="I166" s="13"/>
-      <c r="J166" s="32"/>
-      <c r="K166" s="32"/>
+      <c r="J166" s="38"/>
+      <c r="K166" s="38"/>
     </row>
     <row r="167" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A167" s="13"/>
@@ -4176,8 +4274,8 @@
       <c r="G167" s="15"/>
       <c r="H167" s="13"/>
       <c r="I167" s="13"/>
-      <c r="J167" s="32"/>
-      <c r="K167" s="32"/>
+      <c r="J167" s="38"/>
+      <c r="K167" s="38"/>
     </row>
     <row r="168" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A168" s="13"/>
@@ -4189,8 +4287,8 @@
       <c r="G168" s="15"/>
       <c r="H168" s="13"/>
       <c r="I168" s="13"/>
-      <c r="J168" s="32"/>
-      <c r="K168" s="32"/>
+      <c r="J168" s="38"/>
+      <c r="K168" s="38"/>
     </row>
     <row r="169" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A169" s="13"/>
@@ -4202,8 +4300,8 @@
       <c r="G169" s="15"/>
       <c r="H169" s="13"/>
       <c r="I169" s="13"/>
-      <c r="J169" s="32"/>
-      <c r="K169" s="32"/>
+      <c r="J169" s="38"/>
+      <c r="K169" s="38"/>
     </row>
     <row r="170" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A170" s="13"/>
@@ -4215,8 +4313,8 @@
       <c r="G170" s="15"/>
       <c r="H170" s="13"/>
       <c r="I170" s="13"/>
-      <c r="J170" s="32"/>
-      <c r="K170" s="32"/>
+      <c r="J170" s="38"/>
+      <c r="K170" s="38"/>
     </row>
     <row r="171" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A171" s="13"/>
@@ -4228,8 +4326,8 @@
       <c r="G171" s="15"/>
       <c r="H171" s="13"/>
       <c r="I171" s="13"/>
-      <c r="J171" s="32"/>
-      <c r="K171" s="32"/>
+      <c r="J171" s="38"/>
+      <c r="K171" s="38"/>
     </row>
     <row r="172" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A172" s="13"/>
@@ -4241,8 +4339,8 @@
       <c r="G172" s="15"/>
       <c r="H172" s="13"/>
       <c r="I172" s="13"/>
-      <c r="J172" s="32"/>
-      <c r="K172" s="32"/>
+      <c r="J172" s="38"/>
+      <c r="K172" s="38"/>
     </row>
     <row r="173" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A173" s="13"/>
@@ -4254,8 +4352,8 @@
       <c r="G173" s="15"/>
       <c r="H173" s="13"/>
       <c r="I173" s="13"/>
-      <c r="J173" s="32"/>
-      <c r="K173" s="32"/>
+      <c r="J173" s="38"/>
+      <c r="K173" s="38"/>
     </row>
     <row r="174" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A174" s="13"/>
@@ -4267,8 +4365,8 @@
       <c r="G174" s="15"/>
       <c r="H174" s="13"/>
       <c r="I174" s="13"/>
-      <c r="J174" s="32"/>
-      <c r="K174" s="32"/>
+      <c r="J174" s="38"/>
+      <c r="K174" s="38"/>
     </row>
     <row r="175" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A175" s="13"/>
@@ -4280,8 +4378,8 @@
       <c r="G175" s="15"/>
       <c r="H175" s="13"/>
       <c r="I175" s="13"/>
-      <c r="J175" s="32"/>
-      <c r="K175" s="32"/>
+      <c r="J175" s="38"/>
+      <c r="K175" s="38"/>
     </row>
     <row r="176" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A176" s="13"/>
@@ -4293,8 +4391,8 @@
       <c r="G176" s="15"/>
       <c r="H176" s="13"/>
       <c r="I176" s="13"/>
-      <c r="J176" s="32"/>
-      <c r="K176" s="32"/>
+      <c r="J176" s="38"/>
+      <c r="K176" s="38"/>
     </row>
     <row r="177" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A177" s="13"/>
@@ -4306,8 +4404,8 @@
       <c r="G177" s="15"/>
       <c r="H177" s="13"/>
       <c r="I177" s="13"/>
-      <c r="J177" s="32"/>
-      <c r="K177" s="32"/>
+      <c r="J177" s="38"/>
+      <c r="K177" s="38"/>
     </row>
     <row r="178" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A178" s="13"/>
@@ -4319,8 +4417,8 @@
       <c r="G178" s="15"/>
       <c r="H178" s="13"/>
       <c r="I178" s="13"/>
-      <c r="J178" s="32"/>
-      <c r="K178" s="32"/>
+      <c r="J178" s="38"/>
+      <c r="K178" s="38"/>
     </row>
     <row r="179" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A179" s="13"/>
@@ -4332,8 +4430,8 @@
       <c r="G179" s="15"/>
       <c r="H179" s="13"/>
       <c r="I179" s="13"/>
-      <c r="J179" s="32"/>
-      <c r="K179" s="32"/>
+      <c r="J179" s="38"/>
+      <c r="K179" s="38"/>
     </row>
     <row r="180" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A180" s="13"/>
@@ -4345,8 +4443,8 @@
       <c r="G180" s="15"/>
       <c r="H180" s="13"/>
       <c r="I180" s="13"/>
-      <c r="J180" s="32"/>
-      <c r="K180" s="32"/>
+      <c r="J180" s="38"/>
+      <c r="K180" s="38"/>
     </row>
     <row r="181" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A181" s="13"/>
@@ -4358,8 +4456,8 @@
       <c r="G181" s="15"/>
       <c r="H181" s="13"/>
       <c r="I181" s="13"/>
-      <c r="J181" s="32"/>
-      <c r="K181" s="32"/>
+      <c r="J181" s="38"/>
+      <c r="K181" s="38"/>
     </row>
     <row r="182" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A182" s="13"/>
@@ -4371,8 +4469,8 @@
       <c r="G182" s="15"/>
       <c r="H182" s="13"/>
       <c r="I182" s="13"/>
-      <c r="J182" s="32"/>
-      <c r="K182" s="32"/>
+      <c r="J182" s="38"/>
+      <c r="K182" s="38"/>
     </row>
     <row r="183" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A183" s="13"/>
@@ -4384,8 +4482,8 @@
       <c r="G183" s="15"/>
       <c r="H183" s="13"/>
       <c r="I183" s="13"/>
-      <c r="J183" s="32"/>
-      <c r="K183" s="32"/>
+      <c r="J183" s="38"/>
+      <c r="K183" s="38"/>
     </row>
     <row r="184" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A184" s="13"/>
@@ -4397,8 +4495,8 @@
       <c r="G184" s="15"/>
       <c r="H184" s="13"/>
       <c r="I184" s="13"/>
-      <c r="J184" s="32"/>
-      <c r="K184" s="32"/>
+      <c r="J184" s="38"/>
+      <c r="K184" s="38"/>
     </row>
     <row r="185" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A185" s="13"/>
@@ -4410,8 +4508,8 @@
       <c r="G185" s="15"/>
       <c r="H185" s="13"/>
       <c r="I185" s="13"/>
-      <c r="J185" s="32"/>
-      <c r="K185" s="32"/>
+      <c r="J185" s="38"/>
+      <c r="K185" s="38"/>
     </row>
     <row r="186" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A186" s="13"/>
@@ -4423,8 +4521,8 @@
       <c r="G186" s="15"/>
       <c r="H186" s="13"/>
       <c r="I186" s="13"/>
-      <c r="J186" s="32"/>
-      <c r="K186" s="32"/>
+      <c r="J186" s="38"/>
+      <c r="K186" s="38"/>
     </row>
     <row r="187" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A187" s="13"/>
@@ -4436,8 +4534,8 @@
       <c r="G187" s="15"/>
       <c r="H187" s="13"/>
       <c r="I187" s="13"/>
-      <c r="J187" s="32"/>
-      <c r="K187" s="32"/>
+      <c r="J187" s="38"/>
+      <c r="K187" s="38"/>
     </row>
     <row r="188" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A188" s="13"/>
@@ -4449,8 +4547,8 @@
       <c r="G188" s="15"/>
       <c r="H188" s="13"/>
       <c r="I188" s="13"/>
-      <c r="J188" s="32"/>
-      <c r="K188" s="32"/>
+      <c r="J188" s="38"/>
+      <c r="K188" s="38"/>
     </row>
     <row r="189" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A189" s="13"/>
@@ -4462,8 +4560,8 @@
       <c r="G189" s="15"/>
       <c r="H189" s="13"/>
       <c r="I189" s="13"/>
-      <c r="J189" s="32"/>
-      <c r="K189" s="32"/>
+      <c r="J189" s="38"/>
+      <c r="K189" s="38"/>
     </row>
     <row r="190" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A190" s="13"/>
@@ -4475,8 +4573,8 @@
       <c r="G190" s="15"/>
       <c r="H190" s="13"/>
       <c r="I190" s="13"/>
-      <c r="J190" s="32"/>
-      <c r="K190" s="32"/>
+      <c r="J190" s="38"/>
+      <c r="K190" s="38"/>
     </row>
     <row r="191" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A191" s="13"/>
@@ -4488,8 +4586,8 @@
       <c r="G191" s="15"/>
       <c r="H191" s="13"/>
       <c r="I191" s="13"/>
-      <c r="J191" s="32"/>
-      <c r="K191" s="32"/>
+      <c r="J191" s="38"/>
+      <c r="K191" s="38"/>
     </row>
     <row r="192" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A192" s="13"/>
@@ -4501,8 +4599,8 @@
       <c r="G192" s="15"/>
       <c r="H192" s="13"/>
       <c r="I192" s="13"/>
-      <c r="J192" s="32"/>
-      <c r="K192" s="32"/>
+      <c r="J192" s="38"/>
+      <c r="K192" s="38"/>
     </row>
     <row r="193" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A193" s="13"/>
@@ -4514,8 +4612,8 @@
       <c r="G193" s="15"/>
       <c r="H193" s="13"/>
       <c r="I193" s="13"/>
-      <c r="J193" s="32"/>
-      <c r="K193" s="32"/>
+      <c r="J193" s="38"/>
+      <c r="K193" s="38"/>
     </row>
     <row r="194" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A194" s="13"/>
@@ -4527,8 +4625,8 @@
       <c r="G194" s="15"/>
       <c r="H194" s="13"/>
       <c r="I194" s="13"/>
-      <c r="J194" s="32"/>
-      <c r="K194" s="32"/>
+      <c r="J194" s="38"/>
+      <c r="K194" s="38"/>
     </row>
     <row r="195" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A195" s="13"/>
@@ -4540,8 +4638,8 @@
       <c r="G195" s="15"/>
       <c r="H195" s="13"/>
       <c r="I195" s="13"/>
-      <c r="J195" s="32"/>
-      <c r="K195" s="32"/>
+      <c r="J195" s="38"/>
+      <c r="K195" s="38"/>
     </row>
     <row r="196" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A196" s="13"/>
@@ -4553,8 +4651,8 @@
       <c r="G196" s="15"/>
       <c r="H196" s="13"/>
       <c r="I196" s="13"/>
-      <c r="J196" s="32"/>
-      <c r="K196" s="32"/>
+      <c r="J196" s="38"/>
+      <c r="K196" s="38"/>
     </row>
     <row r="197" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A197" s="13"/>
@@ -4566,8 +4664,8 @@
       <c r="G197" s="15"/>
       <c r="H197" s="13"/>
       <c r="I197" s="13"/>
-      <c r="J197" s="32"/>
-      <c r="K197" s="32"/>
+      <c r="J197" s="38"/>
+      <c r="K197" s="38"/>
     </row>
     <row r="198" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A198" s="13"/>
@@ -4579,8 +4677,8 @@
       <c r="G198" s="15"/>
       <c r="H198" s="13"/>
       <c r="I198" s="13"/>
-      <c r="J198" s="32"/>
-      <c r="K198" s="32"/>
+      <c r="J198" s="38"/>
+      <c r="K198" s="38"/>
     </row>
     <row r="199" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A199" s="13"/>
@@ -4592,8 +4690,8 @@
       <c r="G199" s="15"/>
       <c r="H199" s="13"/>
       <c r="I199" s="13"/>
-      <c r="J199" s="32"/>
-      <c r="K199" s="32"/>
+      <c r="J199" s="38"/>
+      <c r="K199" s="38"/>
     </row>
     <row r="200" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A200" s="13"/>
@@ -4605,8 +4703,8 @@
       <c r="G200" s="15"/>
       <c r="H200" s="13"/>
       <c r="I200" s="13"/>
-      <c r="J200" s="32"/>
-      <c r="K200" s="32"/>
+      <c r="J200" s="38"/>
+      <c r="K200" s="38"/>
     </row>
     <row r="201" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A201" s="13"/>
@@ -4618,8 +4716,8 @@
       <c r="G201" s="15"/>
       <c r="H201" s="13"/>
       <c r="I201" s="13"/>
-      <c r="J201" s="32"/>
-      <c r="K201" s="32"/>
+      <c r="J201" s="38"/>
+      <c r="K201" s="38"/>
     </row>
     <row r="202" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A202" s="13"/>
@@ -4631,8 +4729,8 @@
       <c r="G202" s="15"/>
       <c r="H202" s="13"/>
       <c r="I202" s="13"/>
-      <c r="J202" s="32"/>
-      <c r="K202" s="32"/>
+      <c r="J202" s="38"/>
+      <c r="K202" s="38"/>
     </row>
     <row r="203" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A203" s="13"/>
@@ -4644,8 +4742,8 @@
       <c r="G203" s="15"/>
       <c r="H203" s="13"/>
       <c r="I203" s="13"/>
-      <c r="J203" s="32"/>
-      <c r="K203" s="32"/>
+      <c r="J203" s="38"/>
+      <c r="K203" s="38"/>
     </row>
     <row r="204" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A204" s="13"/>
@@ -4657,8 +4755,8 @@
       <c r="G204" s="15"/>
       <c r="H204" s="13"/>
       <c r="I204" s="13"/>
-      <c r="J204" s="32"/>
-      <c r="K204" s="32"/>
+      <c r="J204" s="38"/>
+      <c r="K204" s="38"/>
     </row>
     <row r="205" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A205" s="13"/>
@@ -4670,8 +4768,8 @@
       <c r="G205" s="15"/>
       <c r="H205" s="13"/>
       <c r="I205" s="13"/>
-      <c r="J205" s="32"/>
-      <c r="K205" s="32"/>
+      <c r="J205" s="38"/>
+      <c r="K205" s="38"/>
     </row>
     <row r="206" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A206" s="13"/>
@@ -4683,8 +4781,8 @@
       <c r="G206" s="15"/>
       <c r="H206" s="13"/>
       <c r="I206" s="13"/>
-      <c r="J206" s="32"/>
-      <c r="K206" s="32"/>
+      <c r="J206" s="38"/>
+      <c r="K206" s="38"/>
     </row>
     <row r="207" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A207" s="13"/>
@@ -4696,8 +4794,8 @@
       <c r="G207" s="15"/>
       <c r="H207" s="13"/>
       <c r="I207" s="13"/>
-      <c r="J207" s="32"/>
-      <c r="K207" s="32"/>
+      <c r="J207" s="38"/>
+      <c r="K207" s="38"/>
     </row>
     <row r="208" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A208" s="13"/>
@@ -4709,8 +4807,8 @@
       <c r="G208" s="15"/>
       <c r="H208" s="13"/>
       <c r="I208" s="13"/>
-      <c r="J208" s="32"/>
-      <c r="K208" s="32"/>
+      <c r="J208" s="38"/>
+      <c r="K208" s="38"/>
     </row>
     <row r="209" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A209" s="13"/>
@@ -4722,8 +4820,8 @@
       <c r="G209" s="15"/>
       <c r="H209" s="13"/>
       <c r="I209" s="13"/>
-      <c r="J209" s="32"/>
-      <c r="K209" s="32"/>
+      <c r="J209" s="38"/>
+      <c r="K209" s="38"/>
     </row>
     <row r="210" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A210" s="13"/>
@@ -4735,8 +4833,8 @@
       <c r="G210" s="15"/>
       <c r="H210" s="13"/>
       <c r="I210" s="13"/>
-      <c r="J210" s="32"/>
-      <c r="K210" s="32"/>
+      <c r="J210" s="38"/>
+      <c r="K210" s="38"/>
     </row>
     <row r="211" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A211" s="13"/>
@@ -4748,8 +4846,8 @@
       <c r="G211" s="15"/>
       <c r="H211" s="13"/>
       <c r="I211" s="13"/>
-      <c r="J211" s="32"/>
-      <c r="K211" s="32"/>
+      <c r="J211" s="38"/>
+      <c r="K211" s="38"/>
     </row>
     <row r="212" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A212" s="13"/>
@@ -4761,8 +4859,8 @@
       <c r="G212" s="15"/>
       <c r="H212" s="13"/>
       <c r="I212" s="13"/>
-      <c r="J212" s="32"/>
-      <c r="K212" s="32"/>
+      <c r="J212" s="38"/>
+      <c r="K212" s="38"/>
     </row>
     <row r="213" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A213" s="13"/>
@@ -4774,8 +4872,8 @@
       <c r="G213" s="15"/>
       <c r="H213" s="13"/>
       <c r="I213" s="13"/>
-      <c r="J213" s="32"/>
-      <c r="K213" s="32"/>
+      <c r="J213" s="38"/>
+      <c r="K213" s="38"/>
     </row>
     <row r="214" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A214" s="13"/>
@@ -4787,8 +4885,8 @@
       <c r="G214" s="15"/>
       <c r="H214" s="13"/>
       <c r="I214" s="13"/>
-      <c r="J214" s="32"/>
-      <c r="K214" s="32"/>
+      <c r="J214" s="38"/>
+      <c r="K214" s="38"/>
     </row>
     <row r="215" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A215" s="13"/>
@@ -4800,8 +4898,8 @@
       <c r="G215" s="15"/>
       <c r="H215" s="13"/>
       <c r="I215" s="13"/>
-      <c r="J215" s="32"/>
-      <c r="K215" s="32"/>
+      <c r="J215" s="38"/>
+      <c r="K215" s="38"/>
     </row>
     <row r="216" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A216" s="13"/>
@@ -4813,8 +4911,8 @@
       <c r="G216" s="15"/>
       <c r="H216" s="13"/>
       <c r="I216" s="13"/>
-      <c r="J216" s="32"/>
-      <c r="K216" s="32"/>
+      <c r="J216" s="38"/>
+      <c r="K216" s="38"/>
     </row>
     <row r="217" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A217" s="13"/>
@@ -4826,8 +4924,8 @@
       <c r="G217" s="15"/>
       <c r="H217" s="13"/>
       <c r="I217" s="13"/>
-      <c r="J217" s="32"/>
-      <c r="K217" s="32"/>
+      <c r="J217" s="38"/>
+      <c r="K217" s="38"/>
     </row>
     <row r="218" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A218" s="13"/>
@@ -4839,8 +4937,8 @@
       <c r="G218" s="15"/>
       <c r="H218" s="13"/>
       <c r="I218" s="13"/>
-      <c r="J218" s="32"/>
-      <c r="K218" s="32"/>
+      <c r="J218" s="38"/>
+      <c r="K218" s="38"/>
     </row>
     <row r="219" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A219" s="13"/>
@@ -4852,8 +4950,8 @@
       <c r="G219" s="15"/>
       <c r="H219" s="13"/>
       <c r="I219" s="13"/>
-      <c r="J219" s="32"/>
-      <c r="K219" s="32"/>
+      <c r="J219" s="38"/>
+      <c r="K219" s="38"/>
     </row>
     <row r="220" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A220" s="13"/>
@@ -4865,8 +4963,8 @@
       <c r="G220" s="15"/>
       <c r="H220" s="13"/>
       <c r="I220" s="13"/>
-      <c r="J220" s="32"/>
-      <c r="K220" s="32"/>
+      <c r="J220" s="38"/>
+      <c r="K220" s="38"/>
     </row>
     <row r="221" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A221" s="13"/>
@@ -4878,8 +4976,8 @@
       <c r="G221" s="15"/>
       <c r="H221" s="13"/>
       <c r="I221" s="13"/>
-      <c r="J221" s="32"/>
-      <c r="K221" s="32"/>
+      <c r="J221" s="38"/>
+      <c r="K221" s="38"/>
     </row>
     <row r="222" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A222" s="13"/>
@@ -4891,8 +4989,8 @@
       <c r="G222" s="15"/>
       <c r="H222" s="13"/>
       <c r="I222" s="13"/>
-      <c r="J222" s="32"/>
-      <c r="K222" s="32"/>
+      <c r="J222" s="38"/>
+      <c r="K222" s="38"/>
     </row>
     <row r="223" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A223" s="13"/>
@@ -4904,8 +5002,8 @@
       <c r="G223" s="15"/>
       <c r="H223" s="13"/>
       <c r="I223" s="13"/>
-      <c r="J223" s="32"/>
-      <c r="K223" s="32"/>
+      <c r="J223" s="38"/>
+      <c r="K223" s="38"/>
     </row>
     <row r="224" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A224" s="13"/>
@@ -4917,8 +5015,8 @@
       <c r="G224" s="15"/>
       <c r="H224" s="13"/>
       <c r="I224" s="13"/>
-      <c r="J224" s="32"/>
-      <c r="K224" s="32"/>
+      <c r="J224" s="38"/>
+      <c r="K224" s="38"/>
     </row>
     <row r="225" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A225" s="13"/>
@@ -4930,8 +5028,8 @@
       <c r="G225" s="15"/>
       <c r="H225" s="13"/>
       <c r="I225" s="13"/>
-      <c r="J225" s="32"/>
-      <c r="K225" s="32"/>
+      <c r="J225" s="38"/>
+      <c r="K225" s="38"/>
     </row>
     <row r="226" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A226" s="13"/>
@@ -4943,8 +5041,8 @@
       <c r="G226" s="15"/>
       <c r="H226" s="13"/>
       <c r="I226" s="13"/>
-      <c r="J226" s="32"/>
-      <c r="K226" s="32"/>
+      <c r="J226" s="38"/>
+      <c r="K226" s="38"/>
     </row>
     <row r="227" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A227" s="13"/>
@@ -4956,8 +5054,8 @@
       <c r="G227" s="15"/>
       <c r="H227" s="13"/>
       <c r="I227" s="13"/>
-      <c r="J227" s="32"/>
-      <c r="K227" s="32"/>
+      <c r="J227" s="38"/>
+      <c r="K227" s="38"/>
     </row>
     <row r="228" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A228" s="13"/>
@@ -4969,8 +5067,8 @@
       <c r="G228" s="15"/>
       <c r="H228" s="13"/>
       <c r="I228" s="13"/>
-      <c r="J228" s="32"/>
-      <c r="K228" s="32"/>
+      <c r="J228" s="38"/>
+      <c r="K228" s="38"/>
     </row>
     <row r="229" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A229" s="13"/>
@@ -4982,8 +5080,8 @@
       <c r="G229" s="15"/>
       <c r="H229" s="13"/>
       <c r="I229" s="13"/>
-      <c r="J229" s="32"/>
-      <c r="K229" s="32"/>
+      <c r="J229" s="38"/>
+      <c r="K229" s="38"/>
     </row>
     <row r="230" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A230" s="13"/>
@@ -4995,8 +5093,8 @@
       <c r="G230" s="15"/>
       <c r="H230" s="13"/>
       <c r="I230" s="13"/>
-      <c r="J230" s="32"/>
-      <c r="K230" s="32"/>
+      <c r="J230" s="38"/>
+      <c r="K230" s="38"/>
     </row>
     <row r="231" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A231" s="13"/>
@@ -5008,8 +5106,8 @@
       <c r="G231" s="15"/>
       <c r="H231" s="13"/>
       <c r="I231" s="13"/>
-      <c r="J231" s="32"/>
-      <c r="K231" s="32"/>
+      <c r="J231" s="38"/>
+      <c r="K231" s="38"/>
     </row>
     <row r="232" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="G232" s="2"/>
@@ -7037,21 +7135,320 @@
       <c r="G906" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="352">
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="A60:K60"/>
+  <mergeCells count="351">
+    <mergeCell ref="H128:I128"/>
+    <mergeCell ref="H129:I129"/>
+    <mergeCell ref="H119:I119"/>
+    <mergeCell ref="H120:I120"/>
+    <mergeCell ref="H121:I121"/>
+    <mergeCell ref="H122:I122"/>
+    <mergeCell ref="H123:I123"/>
+    <mergeCell ref="H124:I124"/>
+    <mergeCell ref="H125:I125"/>
+    <mergeCell ref="H126:I126"/>
+    <mergeCell ref="H127:I127"/>
+    <mergeCell ref="H110:I110"/>
+    <mergeCell ref="H111:I111"/>
+    <mergeCell ref="H112:I112"/>
+    <mergeCell ref="H113:I113"/>
+    <mergeCell ref="H114:I114"/>
+    <mergeCell ref="H115:I115"/>
+    <mergeCell ref="H116:I116"/>
+    <mergeCell ref="H117:I117"/>
+    <mergeCell ref="H118:I118"/>
+    <mergeCell ref="H101:I101"/>
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="H103:I103"/>
+    <mergeCell ref="H104:I104"/>
+    <mergeCell ref="H105:I105"/>
+    <mergeCell ref="H106:I106"/>
+    <mergeCell ref="H107:I107"/>
+    <mergeCell ref="H108:I108"/>
+    <mergeCell ref="H109:I109"/>
+    <mergeCell ref="H92:I92"/>
+    <mergeCell ref="H93:I93"/>
+    <mergeCell ref="H94:I94"/>
+    <mergeCell ref="H95:I95"/>
+    <mergeCell ref="H96:I96"/>
+    <mergeCell ref="H97:I97"/>
+    <mergeCell ref="H98:I98"/>
+    <mergeCell ref="H99:I99"/>
+    <mergeCell ref="H100:I100"/>
+    <mergeCell ref="H83:I83"/>
+    <mergeCell ref="H84:I84"/>
+    <mergeCell ref="H85:I85"/>
+    <mergeCell ref="H86:I86"/>
+    <mergeCell ref="H87:I87"/>
+    <mergeCell ref="H88:I88"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="H90:I90"/>
+    <mergeCell ref="H91:I91"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="H78:I78"/>
+    <mergeCell ref="H79:I79"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="H82:I82"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="A68:K68"/>
+    <mergeCell ref="J230:K230"/>
+    <mergeCell ref="J231:K231"/>
+    <mergeCell ref="J221:K221"/>
+    <mergeCell ref="J222:K222"/>
+    <mergeCell ref="J223:K223"/>
+    <mergeCell ref="J224:K224"/>
+    <mergeCell ref="J225:K225"/>
+    <mergeCell ref="J226:K226"/>
+    <mergeCell ref="J227:K227"/>
+    <mergeCell ref="J228:K228"/>
+    <mergeCell ref="J229:K229"/>
+    <mergeCell ref="J212:K212"/>
+    <mergeCell ref="J213:K213"/>
+    <mergeCell ref="J214:K214"/>
+    <mergeCell ref="J215:K215"/>
+    <mergeCell ref="J216:K216"/>
+    <mergeCell ref="J217:K217"/>
+    <mergeCell ref="J218:K218"/>
+    <mergeCell ref="J219:K219"/>
+    <mergeCell ref="J220:K220"/>
+    <mergeCell ref="J203:K203"/>
+    <mergeCell ref="J204:K204"/>
+    <mergeCell ref="J205:K205"/>
+    <mergeCell ref="J206:K206"/>
+    <mergeCell ref="J207:K207"/>
+    <mergeCell ref="J208:K208"/>
+    <mergeCell ref="J209:K209"/>
+    <mergeCell ref="J210:K210"/>
+    <mergeCell ref="J211:K211"/>
+    <mergeCell ref="J194:K194"/>
+    <mergeCell ref="J195:K195"/>
+    <mergeCell ref="J196:K196"/>
+    <mergeCell ref="J197:K197"/>
+    <mergeCell ref="J198:K198"/>
+    <mergeCell ref="J199:K199"/>
+    <mergeCell ref="J200:K200"/>
+    <mergeCell ref="J201:K201"/>
+    <mergeCell ref="J202:K202"/>
+    <mergeCell ref="J185:K185"/>
+    <mergeCell ref="J186:K186"/>
+    <mergeCell ref="J187:K187"/>
+    <mergeCell ref="J188:K188"/>
+    <mergeCell ref="J189:K189"/>
+    <mergeCell ref="J190:K190"/>
+    <mergeCell ref="J191:K191"/>
+    <mergeCell ref="J192:K192"/>
+    <mergeCell ref="J193:K193"/>
+    <mergeCell ref="J176:K176"/>
+    <mergeCell ref="J177:K177"/>
+    <mergeCell ref="J178:K178"/>
+    <mergeCell ref="J179:K179"/>
+    <mergeCell ref="J180:K180"/>
+    <mergeCell ref="J181:K181"/>
+    <mergeCell ref="J182:K182"/>
+    <mergeCell ref="J183:K183"/>
+    <mergeCell ref="J184:K184"/>
+    <mergeCell ref="J167:K167"/>
+    <mergeCell ref="J168:K168"/>
+    <mergeCell ref="J169:K169"/>
+    <mergeCell ref="J170:K170"/>
+    <mergeCell ref="J171:K171"/>
+    <mergeCell ref="J172:K172"/>
+    <mergeCell ref="J173:K173"/>
+    <mergeCell ref="J174:K174"/>
+    <mergeCell ref="J175:K175"/>
+    <mergeCell ref="J158:K158"/>
+    <mergeCell ref="J159:K159"/>
+    <mergeCell ref="J160:K160"/>
+    <mergeCell ref="J161:K161"/>
+    <mergeCell ref="J162:K162"/>
+    <mergeCell ref="J163:K163"/>
+    <mergeCell ref="J164:K164"/>
+    <mergeCell ref="J165:K165"/>
+    <mergeCell ref="J166:K166"/>
+    <mergeCell ref="J149:K149"/>
+    <mergeCell ref="J150:K150"/>
+    <mergeCell ref="J151:K151"/>
+    <mergeCell ref="J152:K152"/>
+    <mergeCell ref="J153:K153"/>
+    <mergeCell ref="J154:K154"/>
+    <mergeCell ref="J155:K155"/>
+    <mergeCell ref="J156:K156"/>
+    <mergeCell ref="J157:K157"/>
+    <mergeCell ref="J140:K140"/>
+    <mergeCell ref="J141:K141"/>
+    <mergeCell ref="J142:K142"/>
+    <mergeCell ref="J143:K143"/>
+    <mergeCell ref="J144:K144"/>
+    <mergeCell ref="J145:K145"/>
+    <mergeCell ref="J146:K146"/>
+    <mergeCell ref="J147:K147"/>
+    <mergeCell ref="J148:K148"/>
+    <mergeCell ref="J131:K131"/>
+    <mergeCell ref="J132:K132"/>
+    <mergeCell ref="J133:K133"/>
+    <mergeCell ref="J134:K134"/>
+    <mergeCell ref="J135:K135"/>
+    <mergeCell ref="J136:K136"/>
+    <mergeCell ref="J137:K137"/>
+    <mergeCell ref="J138:K138"/>
+    <mergeCell ref="J139:K139"/>
+    <mergeCell ref="J122:K122"/>
+    <mergeCell ref="J123:K123"/>
+    <mergeCell ref="J124:K124"/>
+    <mergeCell ref="J125:K125"/>
+    <mergeCell ref="J126:K126"/>
+    <mergeCell ref="J127:K127"/>
+    <mergeCell ref="J128:K128"/>
+    <mergeCell ref="J129:K129"/>
+    <mergeCell ref="J130:K130"/>
+    <mergeCell ref="J113:K113"/>
+    <mergeCell ref="J114:K114"/>
+    <mergeCell ref="J115:K115"/>
+    <mergeCell ref="J116:K116"/>
+    <mergeCell ref="J117:K117"/>
+    <mergeCell ref="J118:K118"/>
+    <mergeCell ref="J119:K119"/>
+    <mergeCell ref="J120:K120"/>
+    <mergeCell ref="J121:K121"/>
+    <mergeCell ref="J104:K104"/>
+    <mergeCell ref="J105:K105"/>
+    <mergeCell ref="J106:K106"/>
+    <mergeCell ref="J107:K107"/>
+    <mergeCell ref="J108:K108"/>
+    <mergeCell ref="J109:K109"/>
+    <mergeCell ref="J110:K110"/>
+    <mergeCell ref="J111:K111"/>
+    <mergeCell ref="J112:K112"/>
+    <mergeCell ref="J95:K95"/>
+    <mergeCell ref="J96:K96"/>
+    <mergeCell ref="J97:K97"/>
+    <mergeCell ref="J98:K98"/>
+    <mergeCell ref="J99:K99"/>
+    <mergeCell ref="J100:K100"/>
+    <mergeCell ref="J101:K101"/>
+    <mergeCell ref="J102:K102"/>
+    <mergeCell ref="J103:K103"/>
+    <mergeCell ref="J88:K88"/>
+    <mergeCell ref="J89:K89"/>
+    <mergeCell ref="J73:K73"/>
+    <mergeCell ref="J74:K74"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="J75:K75"/>
+    <mergeCell ref="J76:K76"/>
+    <mergeCell ref="J77:K77"/>
+    <mergeCell ref="J78:K78"/>
+    <mergeCell ref="J79:K79"/>
+    <mergeCell ref="J80:K80"/>
+    <mergeCell ref="J55:K55"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="J59:K59"/>
+    <mergeCell ref="J61:K61"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="J63:K63"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J90:K90"/>
+    <mergeCell ref="J91:K91"/>
+    <mergeCell ref="J92:K92"/>
+    <mergeCell ref="J93:K93"/>
+    <mergeCell ref="J94:K94"/>
+    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="J66:K66"/>
+    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J71:K71"/>
+    <mergeCell ref="J72:K72"/>
+    <mergeCell ref="J81:K81"/>
+    <mergeCell ref="J82:K82"/>
+    <mergeCell ref="J83:K83"/>
+    <mergeCell ref="J84:K84"/>
+    <mergeCell ref="J85:K85"/>
+    <mergeCell ref="J86:K86"/>
+    <mergeCell ref="J87:K87"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="J52:K52"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="A27:K27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A20:K20"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
     <mergeCell ref="H36:I36"/>
     <mergeCell ref="H37:I37"/>
     <mergeCell ref="H38:I38"/>
@@ -7076,324 +7473,24 @@
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A20:K20"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="A27:K27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="J52:K52"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="J51:K51"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="J90:K90"/>
-    <mergeCell ref="J91:K91"/>
-    <mergeCell ref="J92:K92"/>
-    <mergeCell ref="J93:K93"/>
-    <mergeCell ref="J94:K94"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="J66:K66"/>
-    <mergeCell ref="J67:K67"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="J71:K71"/>
-    <mergeCell ref="J72:K72"/>
-    <mergeCell ref="J81:K81"/>
-    <mergeCell ref="J82:K82"/>
-    <mergeCell ref="J83:K83"/>
-    <mergeCell ref="J84:K84"/>
-    <mergeCell ref="J85:K85"/>
-    <mergeCell ref="J86:K86"/>
-    <mergeCell ref="J87:K87"/>
-    <mergeCell ref="J88:K88"/>
-    <mergeCell ref="J89:K89"/>
-    <mergeCell ref="J73:K73"/>
-    <mergeCell ref="J74:K74"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="J75:K75"/>
-    <mergeCell ref="J76:K76"/>
-    <mergeCell ref="J77:K77"/>
-    <mergeCell ref="J78:K78"/>
-    <mergeCell ref="J79:K79"/>
-    <mergeCell ref="J80:K80"/>
-    <mergeCell ref="J55:K55"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="J59:K59"/>
-    <mergeCell ref="J61:K61"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="J63:K63"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="J95:K95"/>
-    <mergeCell ref="J96:K96"/>
-    <mergeCell ref="J97:K97"/>
-    <mergeCell ref="J98:K98"/>
-    <mergeCell ref="J99:K99"/>
-    <mergeCell ref="J100:K100"/>
-    <mergeCell ref="J101:K101"/>
-    <mergeCell ref="J102:K102"/>
-    <mergeCell ref="J103:K103"/>
-    <mergeCell ref="J104:K104"/>
-    <mergeCell ref="J105:K105"/>
-    <mergeCell ref="J106:K106"/>
-    <mergeCell ref="J107:K107"/>
-    <mergeCell ref="J108:K108"/>
-    <mergeCell ref="J109:K109"/>
-    <mergeCell ref="J110:K110"/>
-    <mergeCell ref="J111:K111"/>
-    <mergeCell ref="J112:K112"/>
-    <mergeCell ref="J113:K113"/>
-    <mergeCell ref="J114:K114"/>
-    <mergeCell ref="J115:K115"/>
-    <mergeCell ref="J116:K116"/>
-    <mergeCell ref="J117:K117"/>
-    <mergeCell ref="J118:K118"/>
-    <mergeCell ref="J119:K119"/>
-    <mergeCell ref="J120:K120"/>
-    <mergeCell ref="J121:K121"/>
-    <mergeCell ref="J122:K122"/>
-    <mergeCell ref="J123:K123"/>
-    <mergeCell ref="J124:K124"/>
-    <mergeCell ref="J125:K125"/>
-    <mergeCell ref="J126:K126"/>
-    <mergeCell ref="J127:K127"/>
-    <mergeCell ref="J128:K128"/>
-    <mergeCell ref="J129:K129"/>
-    <mergeCell ref="J130:K130"/>
-    <mergeCell ref="J131:K131"/>
-    <mergeCell ref="J132:K132"/>
-    <mergeCell ref="J133:K133"/>
-    <mergeCell ref="J134:K134"/>
-    <mergeCell ref="J135:K135"/>
-    <mergeCell ref="J136:K136"/>
-    <mergeCell ref="J137:K137"/>
-    <mergeCell ref="J138:K138"/>
-    <mergeCell ref="J139:K139"/>
-    <mergeCell ref="J140:K140"/>
-    <mergeCell ref="J141:K141"/>
-    <mergeCell ref="J142:K142"/>
-    <mergeCell ref="J143:K143"/>
-    <mergeCell ref="J144:K144"/>
-    <mergeCell ref="J145:K145"/>
-    <mergeCell ref="J146:K146"/>
-    <mergeCell ref="J147:K147"/>
-    <mergeCell ref="J148:K148"/>
-    <mergeCell ref="J149:K149"/>
-    <mergeCell ref="J150:K150"/>
-    <mergeCell ref="J151:K151"/>
-    <mergeCell ref="J152:K152"/>
-    <mergeCell ref="J153:K153"/>
-    <mergeCell ref="J154:K154"/>
-    <mergeCell ref="J155:K155"/>
-    <mergeCell ref="J156:K156"/>
-    <mergeCell ref="J157:K157"/>
-    <mergeCell ref="J158:K158"/>
-    <mergeCell ref="J159:K159"/>
-    <mergeCell ref="J160:K160"/>
-    <mergeCell ref="J161:K161"/>
-    <mergeCell ref="J162:K162"/>
-    <mergeCell ref="J163:K163"/>
-    <mergeCell ref="J164:K164"/>
-    <mergeCell ref="J165:K165"/>
-    <mergeCell ref="J166:K166"/>
-    <mergeCell ref="J167:K167"/>
-    <mergeCell ref="J168:K168"/>
-    <mergeCell ref="J169:K169"/>
-    <mergeCell ref="J170:K170"/>
-    <mergeCell ref="J171:K171"/>
-    <mergeCell ref="J172:K172"/>
-    <mergeCell ref="J173:K173"/>
-    <mergeCell ref="J174:K174"/>
-    <mergeCell ref="J175:K175"/>
-    <mergeCell ref="J176:K176"/>
-    <mergeCell ref="J177:K177"/>
-    <mergeCell ref="J178:K178"/>
-    <mergeCell ref="J179:K179"/>
-    <mergeCell ref="J180:K180"/>
-    <mergeCell ref="J181:K181"/>
-    <mergeCell ref="J182:K182"/>
-    <mergeCell ref="J183:K183"/>
-    <mergeCell ref="J184:K184"/>
-    <mergeCell ref="J185:K185"/>
-    <mergeCell ref="J186:K186"/>
-    <mergeCell ref="J187:K187"/>
-    <mergeCell ref="J188:K188"/>
-    <mergeCell ref="J189:K189"/>
-    <mergeCell ref="J190:K190"/>
-    <mergeCell ref="J191:K191"/>
-    <mergeCell ref="J192:K192"/>
-    <mergeCell ref="J193:K193"/>
-    <mergeCell ref="J194:K194"/>
-    <mergeCell ref="J195:K195"/>
-    <mergeCell ref="J196:K196"/>
-    <mergeCell ref="J197:K197"/>
-    <mergeCell ref="J198:K198"/>
-    <mergeCell ref="J199:K199"/>
-    <mergeCell ref="J200:K200"/>
-    <mergeCell ref="J201:K201"/>
-    <mergeCell ref="J202:K202"/>
-    <mergeCell ref="J203:K203"/>
-    <mergeCell ref="J204:K204"/>
-    <mergeCell ref="J205:K205"/>
-    <mergeCell ref="J206:K206"/>
-    <mergeCell ref="J207:K207"/>
-    <mergeCell ref="J208:K208"/>
-    <mergeCell ref="J209:K209"/>
-    <mergeCell ref="J210:K210"/>
-    <mergeCell ref="J211:K211"/>
-    <mergeCell ref="J212:K212"/>
-    <mergeCell ref="J213:K213"/>
-    <mergeCell ref="J214:K214"/>
-    <mergeCell ref="J215:K215"/>
-    <mergeCell ref="J216:K216"/>
-    <mergeCell ref="J217:K217"/>
-    <mergeCell ref="J218:K218"/>
-    <mergeCell ref="J219:K219"/>
-    <mergeCell ref="J220:K220"/>
-    <mergeCell ref="J230:K230"/>
-    <mergeCell ref="J231:K231"/>
-    <mergeCell ref="J221:K221"/>
-    <mergeCell ref="J222:K222"/>
-    <mergeCell ref="J223:K223"/>
-    <mergeCell ref="J224:K224"/>
-    <mergeCell ref="J225:K225"/>
-    <mergeCell ref="J226:K226"/>
-    <mergeCell ref="J227:K227"/>
-    <mergeCell ref="J228:K228"/>
-    <mergeCell ref="J229:K229"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="H67:I67"/>
-    <mergeCell ref="H68:I68"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="H70:I70"/>
-    <mergeCell ref="H71:I71"/>
-    <mergeCell ref="H72:I72"/>
-    <mergeCell ref="H73:I73"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="H78:I78"/>
-    <mergeCell ref="H79:I79"/>
-    <mergeCell ref="H80:I80"/>
-    <mergeCell ref="H81:I81"/>
-    <mergeCell ref="H82:I82"/>
-    <mergeCell ref="H83:I83"/>
-    <mergeCell ref="H84:I84"/>
-    <mergeCell ref="H85:I85"/>
-    <mergeCell ref="H86:I86"/>
-    <mergeCell ref="H87:I87"/>
-    <mergeCell ref="H88:I88"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="H90:I90"/>
-    <mergeCell ref="H91:I91"/>
-    <mergeCell ref="H92:I92"/>
-    <mergeCell ref="H93:I93"/>
-    <mergeCell ref="H94:I94"/>
-    <mergeCell ref="H95:I95"/>
-    <mergeCell ref="H96:I96"/>
-    <mergeCell ref="H97:I97"/>
-    <mergeCell ref="H98:I98"/>
-    <mergeCell ref="H99:I99"/>
-    <mergeCell ref="H100:I100"/>
-    <mergeCell ref="H101:I101"/>
-    <mergeCell ref="H102:I102"/>
-    <mergeCell ref="H103:I103"/>
-    <mergeCell ref="H104:I104"/>
-    <mergeCell ref="H105:I105"/>
-    <mergeCell ref="H106:I106"/>
-    <mergeCell ref="H107:I107"/>
-    <mergeCell ref="H108:I108"/>
-    <mergeCell ref="H109:I109"/>
-    <mergeCell ref="H110:I110"/>
-    <mergeCell ref="H111:I111"/>
-    <mergeCell ref="H112:I112"/>
-    <mergeCell ref="H113:I113"/>
-    <mergeCell ref="H114:I114"/>
-    <mergeCell ref="H115:I115"/>
-    <mergeCell ref="H116:I116"/>
-    <mergeCell ref="H117:I117"/>
-    <mergeCell ref="H118:I118"/>
-    <mergeCell ref="H128:I128"/>
-    <mergeCell ref="H129:I129"/>
-    <mergeCell ref="H119:I119"/>
-    <mergeCell ref="H120:I120"/>
-    <mergeCell ref="H121:I121"/>
-    <mergeCell ref="H122:I122"/>
-    <mergeCell ref="H123:I123"/>
-    <mergeCell ref="H124:I124"/>
-    <mergeCell ref="H125:I125"/>
-    <mergeCell ref="H126:I126"/>
-    <mergeCell ref="H127:I127"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="A60:K60"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G1 G3:G19 G21:G26 G28:G32 G61:G906 G34:G59" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G1 G3:G19 G21:G26 G28:G32 G34:G59 G61:G67 G69:G906" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Approved,Rejected,Pending"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>